<commit_message>
valid 0.7339873， LB 0.73979
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8625" tabRatio="993"/>
+    <workbookView windowWidth="28695" windowHeight="13305" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="特征选取" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42">
   <si>
     <r>
       <rPr>
@@ -358,12 +358,18 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">2017_checkname_diff_count
 </t>
     </r>
     <r>
       <rPr>
         <sz val="8"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>去掉</t>
@@ -386,9 +392,6 @@
   <si>
     <t>64</t>
   </si>
-  <si>
-    <t>fix “return 2” bug</t>
-  </si>
 </sst>
 </file>
 
@@ -397,13 +400,13 @@
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="0.00000_ "/>
     <numFmt numFmtId="177" formatCode="0.0000000_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="0.000000_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -436,9 +439,121 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -453,121 +568,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -583,10 +586,6 @@
     <font>
       <sz val="8"/>
       <name val="方正行楷_GBK"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -629,7 +628,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -641,7 +658,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,19 +730,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -677,85 +754,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -773,7 +778,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -785,19 +796,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -836,6 +835,45 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -846,21 +884,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -879,32 +902,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -913,130 +912,130 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1424,10 +1423,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AMP13"/>
+  <dimension ref="A1:AMP12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -4901,7 +4900,7 @@
       <c r="AMO8" s="19"/>
       <c r="AMP8" s="19"/>
     </row>
-    <row r="9" ht="31.5" spans="1:15">
+    <row r="9" ht="21" spans="1:15">
       <c r="A9" s="10" t="s">
         <v>35</v>
       </c>
@@ -6032,7 +6031,7 @@
         <v>0.27769</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" s="16" t="s">
         <v>40</v>
       </c>
@@ -6060,10 +6059,8 @@
       <c r="I12" s="4">
         <v>0.282156</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="1" t="s">
-        <v>42</v>
+      <c r="J12" s="6">
+        <v>0.73979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
valid 0.8407492,  cv test 0.8425299, LB 0.85900
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52">
   <si>
     <r>
       <rPr>
@@ -483,6 +483,64 @@
   </si>
   <si>
     <t>77</t>
+  </si>
+  <si>
+    <r>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <charset val="134"/>
+      </rPr>
+      <t>暂时不加这个特征</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>has_comment_flag</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">rating </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <charset val="134"/>
+      </rPr>
+      <t>统计信息，只保留</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> std</t>
+    </r>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>raing1,2,3,4,_ratio</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>scale_pos_weight = 1</t>
   </si>
 </sst>
 </file>
@@ -1558,10 +1616,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AMK20"/>
+  <dimension ref="A1:AMK24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -1571,7 +1629,7 @@
     <col min="3" max="3" width="9.51666666666667" style="6" customWidth="1"/>
     <col min="4" max="4" width="9.325" style="6" customWidth="1"/>
     <col min="5" max="6" width="11.1333333333333" style="6" customWidth="1"/>
-    <col min="7" max="7" width="9.325" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="7" customWidth="1"/>
     <col min="8" max="8" width="13.65" style="8" customWidth="1"/>
     <col min="9" max="9" width="12.0166666666667" style="8" customWidth="1"/>
     <col min="10" max="10" width="10.0916666666667" style="9" customWidth="1"/>
@@ -9147,24 +9205,113 @@
       <c r="AMJ19" s="29"/>
       <c r="AMK19" s="29"/>
     </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="22" t="s">
+    <row r="20" spans="1:7">
+      <c r="A20" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="21">
         <v>0.9265889</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="21">
         <v>0.8323145</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="21">
         <v>0.9253839</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="21">
         <v>0.8355919</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.9269827</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.8391829</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0.9284143</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.8415312</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="21">
+        <v>0.9334632</v>
+      </c>
+      <c r="D22" s="21">
+        <v>0.8392841</v>
+      </c>
+      <c r="E22" s="21">
+        <v>0.9282524</v>
+      </c>
+      <c r="F22" s="21">
+        <v>0.8414743</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.9318316</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.8393544</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0.9302583</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0.8415681</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.9117557</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.8407492</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0.9089489</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0.8425299</v>
+      </c>
+      <c r="G24" s="7">
+        <v>0.859</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
back to 0.86799 baseline
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79">
   <si>
     <r>
       <rPr>
@@ -573,6 +573,12 @@
     <t>85</t>
   </si>
   <si>
+    <t>days_from_nows = range(1, 5)</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
     <t>扩大训练集之后</t>
   </si>
   <si>
@@ -634,6 +640,9 @@
   </si>
   <si>
     <t>35</t>
+  </si>
+  <si>
+    <t>back to 0.86799 baseline</t>
   </si>
 </sst>
 </file>
@@ -1741,10 +1750,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AMH43"/>
+  <dimension ref="A1:AMH47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -11419,9 +11428,32 @@
       <c r="AMG27" s="37"/>
       <c r="AMH27" s="37"/>
     </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="8">
+        <v>0.9203679</v>
+      </c>
+      <c r="D28" s="8">
+        <v>0.848842</v>
+      </c>
+      <c r="E28" s="8">
+        <v>0.9157247</v>
+      </c>
+      <c r="F28" s="9">
+        <v>0.8505482</v>
+      </c>
+      <c r="G28" s="10">
+        <v>0.8678</v>
+      </c>
+    </row>
     <row r="32" spans="1:7">
       <c r="A32" s="12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -11431,7 +11463,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>8</v>
@@ -11454,10 +11486,10 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C34" s="8">
         <v>0.7168243</v>
@@ -11477,10 +11509,10 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C35" s="8">
         <v>0.7215203</v>
@@ -11497,10 +11529,10 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C36" s="8">
         <v>0.7355705</v>
@@ -11517,10 +11549,10 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C37" s="8">
         <v>0.7393779</v>
@@ -11540,10 +11572,10 @@
     </row>
     <row r="38" s="3" customFormat="1" spans="1:1022">
       <c r="A38" s="28" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C38" s="17">
         <v>0.7051926</v>
@@ -12578,10 +12610,10 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C39" s="8">
         <v>0.7279901</v>
@@ -12598,10 +12630,10 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="29" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C40" s="8">
         <v>0.7241441</v>
@@ -12618,10 +12650,10 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C41" s="8">
         <v>0.730688</v>
@@ -12638,10 +12670,10 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C42" s="8">
         <v>0.7248618</v>
@@ -12661,10 +12693,10 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C43" s="8">
         <v>0.7390101</v>
@@ -12680,6 +12712,29 @@
       </c>
       <c r="G43" s="10">
         <v>0.6641</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="8">
+        <v>0.9212036</v>
+      </c>
+      <c r="D47" s="8">
+        <v>0.8492135</v>
+      </c>
+      <c r="E47" s="8">
+        <v>0.9136246</v>
+      </c>
+      <c r="F47" s="9">
+        <v>0.8507061</v>
+      </c>
+      <c r="G47" s="10">
+        <v>0.86799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
距离上一次 pay money 操作到现在 actiontype 的比例， valid 0.8951611， cv 0.9004432
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91">
   <si>
     <r>
       <rPr>
@@ -751,6 +751,44 @@
   </si>
   <si>
     <t>133</t>
+  </si>
+  <si>
+    <r>
+      <t>距离上一次</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> pay money </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <charset val="134"/>
+      </rPr>
+      <t>操作到现在</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> actiontype </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的比例</t>
+    </r>
+  </si>
+  <si>
+    <t>139</t>
   </si>
 </sst>
 </file>
@@ -1858,10 +1896,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AMH52"/>
+  <dimension ref="A1:AMH53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -12951,6 +12989,26 @@
         <v>0.90399</v>
       </c>
     </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="8">
+        <v>0.9604394</v>
+      </c>
+      <c r="D53" s="8">
+        <v>0.8951611</v>
+      </c>
+      <c r="E53" s="8">
+        <v>0.9613578</v>
+      </c>
+      <c r="F53" s="9">
+        <v>0.9004432</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A32:G32"/>

</xml_diff>

<commit_message>
去掉 importance 很低的特征， LB 0.96859
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128">
   <si>
     <r>
       <rPr>
@@ -1115,20 +1115,61 @@
   <si>
     <t>400</t>
   </si>
+  <si>
+    <t>fix action_history_features6 bug</t>
+  </si>
+  <si>
+    <t>319</t>
+  </si>
+  <si>
+    <r>
+      <t>去掉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> importance </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <charset val="134"/>
+      </rPr>
+      <t>很低的特征</t>
+    </r>
+  </si>
+  <si>
+    <t>296</t>
+  </si>
+  <si>
+    <t>310</t>
+  </si>
+  <si>
+    <t>有用！</t>
+  </si>
+  <si>
+    <t>过采样处理样本不均衡</t>
+  </si>
+  <si>
+    <t>没啥用啊</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.0000000_ "/>
-    <numFmt numFmtId="177" formatCode="0.00000_ "/>
+    <numFmt numFmtId="176" formatCode="0.00000_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0.0000000_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1145,11 +1186,22 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="8"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1161,18 +1213,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1184,32 +1229,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1229,9 +1252,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1244,14 +1266,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -1260,7 +1274,39 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1281,9 +1327,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1311,7 +1356,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1350,7 +1395,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1362,19 +1515,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1386,13 +1533,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1404,7 +1545,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1416,121 +1581,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1548,7 +1599,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1557,7 +1623,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1577,32 +1658,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1612,17 +1674,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1646,142 +1697,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1809,16 +1860,16 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -1839,7 +1890,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1854,7 +1905,7 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1863,13 +1914,13 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1881,40 +1932,40 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -1930,6 +1981,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
@@ -2250,10 +2313,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AMH69"/>
+  <dimension ref="A1:AMH73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -7568,7 +7631,7 @@
       <c r="AMH13" s="46"/>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:1022">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="54" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="18" t="s">
@@ -16721,6 +16784,1116 @@
         <v>0.96749</v>
       </c>
     </row>
+    <row r="70" s="3" customFormat="1" spans="1:1022">
+      <c r="A70" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C70" s="19">
+        <v>0.9951934</v>
+      </c>
+      <c r="D70" s="19">
+        <v>0.9629157</v>
+      </c>
+      <c r="E70" s="19">
+        <v>0.9963413</v>
+      </c>
+      <c r="F70" s="19">
+        <v>0.966912</v>
+      </c>
+      <c r="G70" s="34">
+        <v>0.96789</v>
+      </c>
+      <c r="H70" s="35"/>
+      <c r="I70" s="45"/>
+      <c r="J70" s="45"/>
+      <c r="K70" s="45"/>
+      <c r="L70" s="45"/>
+      <c r="M70" s="45"/>
+      <c r="N70" s="45"/>
+      <c r="O70" s="45"/>
+      <c r="P70" s="45"/>
+      <c r="Q70" s="45"/>
+      <c r="R70" s="45"/>
+      <c r="S70" s="45"/>
+      <c r="T70" s="45"/>
+      <c r="U70" s="45"/>
+      <c r="V70" s="45"/>
+      <c r="W70" s="45"/>
+      <c r="X70" s="45"/>
+      <c r="Y70" s="45"/>
+      <c r="Z70" s="45"/>
+      <c r="AA70" s="45"/>
+      <c r="AB70" s="45"/>
+      <c r="AC70" s="45"/>
+      <c r="AD70" s="45"/>
+      <c r="AE70" s="45"/>
+      <c r="AF70" s="45"/>
+      <c r="AG70" s="45"/>
+      <c r="AH70" s="45"/>
+      <c r="AI70" s="45"/>
+      <c r="AJ70" s="45"/>
+      <c r="AK70" s="45"/>
+      <c r="AL70" s="45"/>
+      <c r="AM70" s="45"/>
+      <c r="AN70" s="45"/>
+      <c r="AO70" s="45"/>
+      <c r="AP70" s="45"/>
+      <c r="AQ70" s="45"/>
+      <c r="AR70" s="45"/>
+      <c r="AS70" s="45"/>
+      <c r="AT70" s="45"/>
+      <c r="AU70" s="45"/>
+      <c r="AV70" s="45"/>
+      <c r="AW70" s="45"/>
+      <c r="AX70" s="45"/>
+      <c r="AY70" s="45"/>
+      <c r="AZ70" s="45"/>
+      <c r="BA70" s="45"/>
+      <c r="BB70" s="45"/>
+      <c r="BC70" s="45"/>
+      <c r="BD70" s="45"/>
+      <c r="BE70" s="45"/>
+      <c r="BF70" s="45"/>
+      <c r="BG70" s="45"/>
+      <c r="BH70" s="45"/>
+      <c r="BI70" s="45"/>
+      <c r="BJ70" s="45"/>
+      <c r="BK70" s="45"/>
+      <c r="BL70" s="45"/>
+      <c r="BM70" s="45"/>
+      <c r="BN70" s="45"/>
+      <c r="BO70" s="45"/>
+      <c r="BP70" s="45"/>
+      <c r="BQ70" s="45"/>
+      <c r="BR70" s="45"/>
+      <c r="BS70" s="45"/>
+      <c r="BT70" s="45"/>
+      <c r="BU70" s="45"/>
+      <c r="BV70" s="45"/>
+      <c r="BW70" s="45"/>
+      <c r="BX70" s="45"/>
+      <c r="BY70" s="45"/>
+      <c r="BZ70" s="45"/>
+      <c r="CA70" s="45"/>
+      <c r="CB70" s="45"/>
+      <c r="CC70" s="45"/>
+      <c r="CD70" s="45"/>
+      <c r="CE70" s="45"/>
+      <c r="CF70" s="45"/>
+      <c r="CG70" s="45"/>
+      <c r="CH70" s="45"/>
+      <c r="CI70" s="45"/>
+      <c r="CJ70" s="45"/>
+      <c r="CK70" s="45"/>
+      <c r="CL70" s="45"/>
+      <c r="CM70" s="45"/>
+      <c r="CN70" s="45"/>
+      <c r="CO70" s="45"/>
+      <c r="CP70" s="45"/>
+      <c r="CQ70" s="45"/>
+      <c r="CR70" s="45"/>
+      <c r="CS70" s="45"/>
+      <c r="CT70" s="45"/>
+      <c r="CU70" s="45"/>
+      <c r="CV70" s="45"/>
+      <c r="CW70" s="45"/>
+      <c r="CX70" s="45"/>
+      <c r="CY70" s="45"/>
+      <c r="CZ70" s="45"/>
+      <c r="DA70" s="45"/>
+      <c r="DB70" s="45"/>
+      <c r="DC70" s="45"/>
+      <c r="DD70" s="45"/>
+      <c r="DE70" s="45"/>
+      <c r="DF70" s="45"/>
+      <c r="DG70" s="45"/>
+      <c r="DH70" s="45"/>
+      <c r="DI70" s="45"/>
+      <c r="DJ70" s="45"/>
+      <c r="DK70" s="45"/>
+      <c r="DL70" s="45"/>
+      <c r="DM70" s="45"/>
+      <c r="DN70" s="45"/>
+      <c r="DO70" s="45"/>
+      <c r="DP70" s="45"/>
+      <c r="DQ70" s="45"/>
+      <c r="DR70" s="45"/>
+      <c r="DS70" s="45"/>
+      <c r="DT70" s="45"/>
+      <c r="DU70" s="45"/>
+      <c r="DV70" s="45"/>
+      <c r="DW70" s="45"/>
+      <c r="DX70" s="45"/>
+      <c r="DY70" s="45"/>
+      <c r="DZ70" s="45"/>
+      <c r="EA70" s="45"/>
+      <c r="EB70" s="45"/>
+      <c r="EC70" s="45"/>
+      <c r="ED70" s="45"/>
+      <c r="EE70" s="45"/>
+      <c r="EF70" s="45"/>
+      <c r="EG70" s="45"/>
+      <c r="EH70" s="45"/>
+      <c r="EI70" s="45"/>
+      <c r="EJ70" s="45"/>
+      <c r="EK70" s="45"/>
+      <c r="EL70" s="45"/>
+      <c r="EM70" s="45"/>
+      <c r="EN70" s="45"/>
+      <c r="EO70" s="45"/>
+      <c r="EP70" s="45"/>
+      <c r="EQ70" s="45"/>
+      <c r="ER70" s="45"/>
+      <c r="ES70" s="45"/>
+      <c r="ET70" s="45"/>
+      <c r="EU70" s="45"/>
+      <c r="EV70" s="45"/>
+      <c r="EW70" s="45"/>
+      <c r="EX70" s="45"/>
+      <c r="EY70" s="45"/>
+      <c r="EZ70" s="45"/>
+      <c r="FA70" s="45"/>
+      <c r="FB70" s="45"/>
+      <c r="FC70" s="45"/>
+      <c r="FD70" s="45"/>
+      <c r="FE70" s="45"/>
+      <c r="FF70" s="45"/>
+      <c r="FG70" s="45"/>
+      <c r="FH70" s="45"/>
+      <c r="FI70" s="45"/>
+      <c r="FJ70" s="45"/>
+      <c r="FK70" s="45"/>
+      <c r="FL70" s="45"/>
+      <c r="FM70" s="45"/>
+      <c r="FN70" s="45"/>
+      <c r="FO70" s="45"/>
+      <c r="FP70" s="45"/>
+      <c r="FQ70" s="45"/>
+      <c r="FR70" s="45"/>
+      <c r="FS70" s="45"/>
+      <c r="FT70" s="45"/>
+      <c r="FU70" s="45"/>
+      <c r="FV70" s="45"/>
+      <c r="FW70" s="45"/>
+      <c r="FX70" s="45"/>
+      <c r="FY70" s="45"/>
+      <c r="FZ70" s="45"/>
+      <c r="GA70" s="45"/>
+      <c r="GB70" s="45"/>
+      <c r="GC70" s="45"/>
+      <c r="GD70" s="45"/>
+      <c r="GE70" s="45"/>
+      <c r="GF70" s="45"/>
+      <c r="GG70" s="45"/>
+      <c r="GH70" s="45"/>
+      <c r="GI70" s="45"/>
+      <c r="GJ70" s="45"/>
+      <c r="GK70" s="45"/>
+      <c r="GL70" s="45"/>
+      <c r="GM70" s="45"/>
+      <c r="GN70" s="45"/>
+      <c r="GO70" s="45"/>
+      <c r="GP70" s="45"/>
+      <c r="GQ70" s="45"/>
+      <c r="GR70" s="45"/>
+      <c r="GS70" s="45"/>
+      <c r="GT70" s="45"/>
+      <c r="GU70" s="45"/>
+      <c r="GV70" s="45"/>
+      <c r="GW70" s="45"/>
+      <c r="GX70" s="45"/>
+      <c r="GY70" s="45"/>
+      <c r="GZ70" s="45"/>
+      <c r="HA70" s="45"/>
+      <c r="HB70" s="45"/>
+      <c r="HC70" s="45"/>
+      <c r="HD70" s="45"/>
+      <c r="HE70" s="45"/>
+      <c r="HF70" s="45"/>
+      <c r="HG70" s="45"/>
+      <c r="HH70" s="45"/>
+      <c r="HI70" s="45"/>
+      <c r="HJ70" s="45"/>
+      <c r="HK70" s="45"/>
+      <c r="HL70" s="45"/>
+      <c r="HM70" s="45"/>
+      <c r="HN70" s="45"/>
+      <c r="HO70" s="45"/>
+      <c r="HP70" s="45"/>
+      <c r="HQ70" s="45"/>
+      <c r="HR70" s="45"/>
+      <c r="HS70" s="45"/>
+      <c r="HT70" s="45"/>
+      <c r="HU70" s="45"/>
+      <c r="HV70" s="45"/>
+      <c r="HW70" s="45"/>
+      <c r="HX70" s="45"/>
+      <c r="HY70" s="45"/>
+      <c r="HZ70" s="45"/>
+      <c r="IA70" s="45"/>
+      <c r="IB70" s="45"/>
+      <c r="IC70" s="45"/>
+      <c r="ID70" s="45"/>
+      <c r="IE70" s="45"/>
+      <c r="IF70" s="45"/>
+      <c r="IG70" s="45"/>
+      <c r="IH70" s="45"/>
+      <c r="II70" s="45"/>
+      <c r="IJ70" s="45"/>
+      <c r="IK70" s="45"/>
+      <c r="IL70" s="45"/>
+      <c r="IM70" s="45"/>
+      <c r="IN70" s="45"/>
+      <c r="IO70" s="45"/>
+      <c r="IP70" s="45"/>
+      <c r="IQ70" s="45"/>
+      <c r="IR70" s="45"/>
+      <c r="IS70" s="45"/>
+      <c r="IT70" s="45"/>
+      <c r="IU70" s="45"/>
+      <c r="IV70" s="45"/>
+      <c r="IW70" s="45"/>
+      <c r="IX70" s="45"/>
+      <c r="IY70" s="45"/>
+      <c r="IZ70" s="45"/>
+      <c r="JA70" s="45"/>
+      <c r="JB70" s="45"/>
+      <c r="JC70" s="45"/>
+      <c r="JD70" s="45"/>
+      <c r="JE70" s="45"/>
+      <c r="JF70" s="45"/>
+      <c r="JG70" s="45"/>
+      <c r="JH70" s="45"/>
+      <c r="JI70" s="45"/>
+      <c r="JJ70" s="45"/>
+      <c r="JK70" s="45"/>
+      <c r="JL70" s="45"/>
+      <c r="JM70" s="45"/>
+      <c r="JN70" s="45"/>
+      <c r="JO70" s="45"/>
+      <c r="JP70" s="45"/>
+      <c r="JQ70" s="45"/>
+      <c r="JR70" s="45"/>
+      <c r="JS70" s="45"/>
+      <c r="JT70" s="45"/>
+      <c r="JU70" s="45"/>
+      <c r="JV70" s="45"/>
+      <c r="JW70" s="45"/>
+      <c r="JX70" s="45"/>
+      <c r="JY70" s="45"/>
+      <c r="JZ70" s="45"/>
+      <c r="KA70" s="45"/>
+      <c r="KB70" s="45"/>
+      <c r="KC70" s="45"/>
+      <c r="KD70" s="45"/>
+      <c r="KE70" s="45"/>
+      <c r="KF70" s="45"/>
+      <c r="KG70" s="45"/>
+      <c r="KH70" s="45"/>
+      <c r="KI70" s="45"/>
+      <c r="KJ70" s="45"/>
+      <c r="KK70" s="45"/>
+      <c r="KL70" s="45"/>
+      <c r="KM70" s="45"/>
+      <c r="KN70" s="45"/>
+      <c r="KO70" s="45"/>
+      <c r="KP70" s="45"/>
+      <c r="KQ70" s="45"/>
+      <c r="KR70" s="45"/>
+      <c r="KS70" s="45"/>
+      <c r="KT70" s="45"/>
+      <c r="KU70" s="45"/>
+      <c r="KV70" s="45"/>
+      <c r="KW70" s="45"/>
+      <c r="KX70" s="45"/>
+      <c r="KY70" s="45"/>
+      <c r="KZ70" s="45"/>
+      <c r="LA70" s="45"/>
+      <c r="LB70" s="45"/>
+      <c r="LC70" s="45"/>
+      <c r="LD70" s="45"/>
+      <c r="LE70" s="45"/>
+      <c r="LF70" s="45"/>
+      <c r="LG70" s="45"/>
+      <c r="LH70" s="45"/>
+      <c r="LI70" s="45"/>
+      <c r="LJ70" s="45"/>
+      <c r="LK70" s="45"/>
+      <c r="LL70" s="45"/>
+      <c r="LM70" s="45"/>
+      <c r="LN70" s="45"/>
+      <c r="LO70" s="45"/>
+      <c r="LP70" s="45"/>
+      <c r="LQ70" s="45"/>
+      <c r="LR70" s="45"/>
+      <c r="LS70" s="45"/>
+      <c r="LT70" s="45"/>
+      <c r="LU70" s="45"/>
+      <c r="LV70" s="45"/>
+      <c r="LW70" s="45"/>
+      <c r="LX70" s="45"/>
+      <c r="LY70" s="45"/>
+      <c r="LZ70" s="45"/>
+      <c r="MA70" s="45"/>
+      <c r="MB70" s="45"/>
+      <c r="MC70" s="45"/>
+      <c r="MD70" s="45"/>
+      <c r="ME70" s="45"/>
+      <c r="MF70" s="45"/>
+      <c r="MG70" s="45"/>
+      <c r="MH70" s="45"/>
+      <c r="MI70" s="45"/>
+      <c r="MJ70" s="45"/>
+      <c r="MK70" s="45"/>
+      <c r="ML70" s="45"/>
+      <c r="MM70" s="45"/>
+      <c r="MN70" s="45"/>
+      <c r="MO70" s="45"/>
+      <c r="MP70" s="45"/>
+      <c r="MQ70" s="45"/>
+      <c r="MR70" s="45"/>
+      <c r="MS70" s="45"/>
+      <c r="MT70" s="45"/>
+      <c r="MU70" s="45"/>
+      <c r="MV70" s="45"/>
+      <c r="MW70" s="45"/>
+      <c r="MX70" s="45"/>
+      <c r="MY70" s="45"/>
+      <c r="MZ70" s="45"/>
+      <c r="NA70" s="45"/>
+      <c r="NB70" s="45"/>
+      <c r="NC70" s="45"/>
+      <c r="ND70" s="45"/>
+      <c r="NE70" s="45"/>
+      <c r="NF70" s="45"/>
+      <c r="NG70" s="45"/>
+      <c r="NH70" s="45"/>
+      <c r="NI70" s="45"/>
+      <c r="NJ70" s="45"/>
+      <c r="NK70" s="45"/>
+      <c r="NL70" s="45"/>
+      <c r="NM70" s="45"/>
+      <c r="NN70" s="45"/>
+      <c r="NO70" s="45"/>
+      <c r="NP70" s="45"/>
+      <c r="NQ70" s="45"/>
+      <c r="NR70" s="45"/>
+      <c r="NS70" s="45"/>
+      <c r="NT70" s="45"/>
+      <c r="NU70" s="45"/>
+      <c r="NV70" s="45"/>
+      <c r="NW70" s="45"/>
+      <c r="NX70" s="45"/>
+      <c r="NY70" s="45"/>
+      <c r="NZ70" s="45"/>
+      <c r="OA70" s="45"/>
+      <c r="OB70" s="45"/>
+      <c r="OC70" s="45"/>
+      <c r="OD70" s="45"/>
+      <c r="OE70" s="45"/>
+      <c r="OF70" s="45"/>
+      <c r="OG70" s="45"/>
+      <c r="OH70" s="45"/>
+      <c r="OI70" s="45"/>
+      <c r="OJ70" s="45"/>
+      <c r="OK70" s="45"/>
+      <c r="OL70" s="45"/>
+      <c r="OM70" s="45"/>
+      <c r="ON70" s="45"/>
+      <c r="OO70" s="45"/>
+      <c r="OP70" s="45"/>
+      <c r="OQ70" s="45"/>
+      <c r="OR70" s="45"/>
+      <c r="OS70" s="45"/>
+      <c r="OT70" s="45"/>
+      <c r="OU70" s="45"/>
+      <c r="OV70" s="45"/>
+      <c r="OW70" s="45"/>
+      <c r="OX70" s="45"/>
+      <c r="OY70" s="45"/>
+      <c r="OZ70" s="45"/>
+      <c r="PA70" s="45"/>
+      <c r="PB70" s="45"/>
+      <c r="PC70" s="45"/>
+      <c r="PD70" s="45"/>
+      <c r="PE70" s="45"/>
+      <c r="PF70" s="45"/>
+      <c r="PG70" s="45"/>
+      <c r="PH70" s="45"/>
+      <c r="PI70" s="45"/>
+      <c r="PJ70" s="45"/>
+      <c r="PK70" s="45"/>
+      <c r="PL70" s="45"/>
+      <c r="PM70" s="45"/>
+      <c r="PN70" s="45"/>
+      <c r="PO70" s="45"/>
+      <c r="PP70" s="45"/>
+      <c r="PQ70" s="45"/>
+      <c r="PR70" s="45"/>
+      <c r="PS70" s="45"/>
+      <c r="PT70" s="45"/>
+      <c r="PU70" s="45"/>
+      <c r="PV70" s="45"/>
+      <c r="PW70" s="45"/>
+      <c r="PX70" s="45"/>
+      <c r="PY70" s="45"/>
+      <c r="PZ70" s="45"/>
+      <c r="QA70" s="45"/>
+      <c r="QB70" s="45"/>
+      <c r="QC70" s="45"/>
+      <c r="QD70" s="45"/>
+      <c r="QE70" s="45"/>
+      <c r="QF70" s="45"/>
+      <c r="QG70" s="45"/>
+      <c r="QH70" s="45"/>
+      <c r="QI70" s="45"/>
+      <c r="QJ70" s="45"/>
+      <c r="QK70" s="45"/>
+      <c r="QL70" s="45"/>
+      <c r="QM70" s="45"/>
+      <c r="QN70" s="45"/>
+      <c r="QO70" s="45"/>
+      <c r="QP70" s="45"/>
+      <c r="QQ70" s="45"/>
+      <c r="QR70" s="45"/>
+      <c r="QS70" s="45"/>
+      <c r="QT70" s="45"/>
+      <c r="QU70" s="45"/>
+      <c r="QV70" s="45"/>
+      <c r="QW70" s="45"/>
+      <c r="QX70" s="45"/>
+      <c r="QY70" s="45"/>
+      <c r="QZ70" s="45"/>
+      <c r="RA70" s="45"/>
+      <c r="RB70" s="45"/>
+      <c r="RC70" s="45"/>
+      <c r="RD70" s="45"/>
+      <c r="RE70" s="45"/>
+      <c r="RF70" s="45"/>
+      <c r="RG70" s="45"/>
+      <c r="RH70" s="45"/>
+      <c r="RI70" s="45"/>
+      <c r="RJ70" s="45"/>
+      <c r="RK70" s="45"/>
+      <c r="RL70" s="45"/>
+      <c r="RM70" s="45"/>
+      <c r="RN70" s="45"/>
+      <c r="RO70" s="45"/>
+      <c r="RP70" s="45"/>
+      <c r="RQ70" s="45"/>
+      <c r="RR70" s="45"/>
+      <c r="RS70" s="45"/>
+      <c r="RT70" s="45"/>
+      <c r="RU70" s="45"/>
+      <c r="RV70" s="45"/>
+      <c r="RW70" s="45"/>
+      <c r="RX70" s="45"/>
+      <c r="RY70" s="45"/>
+      <c r="RZ70" s="45"/>
+      <c r="SA70" s="45"/>
+      <c r="SB70" s="45"/>
+      <c r="SC70" s="45"/>
+      <c r="SD70" s="45"/>
+      <c r="SE70" s="45"/>
+      <c r="SF70" s="45"/>
+      <c r="SG70" s="45"/>
+      <c r="SH70" s="45"/>
+      <c r="SI70" s="45"/>
+      <c r="SJ70" s="45"/>
+      <c r="SK70" s="45"/>
+      <c r="SL70" s="45"/>
+      <c r="SM70" s="45"/>
+      <c r="SN70" s="45"/>
+      <c r="SO70" s="45"/>
+      <c r="SP70" s="45"/>
+      <c r="SQ70" s="45"/>
+      <c r="SR70" s="45"/>
+      <c r="SS70" s="45"/>
+      <c r="ST70" s="45"/>
+      <c r="SU70" s="45"/>
+      <c r="SV70" s="45"/>
+      <c r="SW70" s="45"/>
+      <c r="SX70" s="45"/>
+      <c r="SY70" s="45"/>
+      <c r="SZ70" s="45"/>
+      <c r="TA70" s="45"/>
+      <c r="TB70" s="45"/>
+      <c r="TC70" s="45"/>
+      <c r="TD70" s="45"/>
+      <c r="TE70" s="45"/>
+      <c r="TF70" s="45"/>
+      <c r="TG70" s="45"/>
+      <c r="TH70" s="45"/>
+      <c r="TI70" s="45"/>
+      <c r="TJ70" s="45"/>
+      <c r="TK70" s="45"/>
+      <c r="TL70" s="45"/>
+      <c r="TM70" s="45"/>
+      <c r="TN70" s="45"/>
+      <c r="TO70" s="45"/>
+      <c r="TP70" s="45"/>
+      <c r="TQ70" s="45"/>
+      <c r="TR70" s="45"/>
+      <c r="TS70" s="45"/>
+      <c r="TT70" s="45"/>
+      <c r="TU70" s="45"/>
+      <c r="TV70" s="45"/>
+      <c r="TW70" s="45"/>
+      <c r="TX70" s="45"/>
+      <c r="TY70" s="45"/>
+      <c r="TZ70" s="45"/>
+      <c r="UA70" s="45"/>
+      <c r="UB70" s="45"/>
+      <c r="UC70" s="45"/>
+      <c r="UD70" s="45"/>
+      <c r="UE70" s="45"/>
+      <c r="UF70" s="45"/>
+      <c r="UG70" s="45"/>
+      <c r="UH70" s="45"/>
+      <c r="UI70" s="45"/>
+      <c r="UJ70" s="45"/>
+      <c r="UK70" s="45"/>
+      <c r="UL70" s="45"/>
+      <c r="UM70" s="45"/>
+      <c r="UN70" s="45"/>
+      <c r="UO70" s="45"/>
+      <c r="UP70" s="45"/>
+      <c r="UQ70" s="45"/>
+      <c r="UR70" s="45"/>
+      <c r="US70" s="45"/>
+      <c r="UT70" s="45"/>
+      <c r="UU70" s="45"/>
+      <c r="UV70" s="45"/>
+      <c r="UW70" s="45"/>
+      <c r="UX70" s="45"/>
+      <c r="UY70" s="45"/>
+      <c r="UZ70" s="45"/>
+      <c r="VA70" s="45"/>
+      <c r="VB70" s="45"/>
+      <c r="VC70" s="45"/>
+      <c r="VD70" s="45"/>
+      <c r="VE70" s="45"/>
+      <c r="VF70" s="45"/>
+      <c r="VG70" s="45"/>
+      <c r="VH70" s="45"/>
+      <c r="VI70" s="45"/>
+      <c r="VJ70" s="45"/>
+      <c r="VK70" s="45"/>
+      <c r="VL70" s="45"/>
+      <c r="VM70" s="45"/>
+      <c r="VN70" s="45"/>
+      <c r="VO70" s="45"/>
+      <c r="VP70" s="45"/>
+      <c r="VQ70" s="45"/>
+      <c r="VR70" s="45"/>
+      <c r="VS70" s="45"/>
+      <c r="VT70" s="45"/>
+      <c r="VU70" s="45"/>
+      <c r="VV70" s="45"/>
+      <c r="VW70" s="45"/>
+      <c r="VX70" s="45"/>
+      <c r="VY70" s="45"/>
+      <c r="VZ70" s="45"/>
+      <c r="WA70" s="45"/>
+      <c r="WB70" s="45"/>
+      <c r="WC70" s="45"/>
+      <c r="WD70" s="45"/>
+      <c r="WE70" s="45"/>
+      <c r="WF70" s="45"/>
+      <c r="WG70" s="45"/>
+      <c r="WH70" s="45"/>
+      <c r="WI70" s="45"/>
+      <c r="WJ70" s="45"/>
+      <c r="WK70" s="45"/>
+      <c r="WL70" s="45"/>
+      <c r="WM70" s="45"/>
+      <c r="WN70" s="45"/>
+      <c r="WO70" s="45"/>
+      <c r="WP70" s="45"/>
+      <c r="WQ70" s="45"/>
+      <c r="WR70" s="45"/>
+      <c r="WS70" s="45"/>
+      <c r="WT70" s="45"/>
+      <c r="WU70" s="45"/>
+      <c r="WV70" s="45"/>
+      <c r="WW70" s="45"/>
+      <c r="WX70" s="45"/>
+      <c r="WY70" s="45"/>
+      <c r="WZ70" s="45"/>
+      <c r="XA70" s="45"/>
+      <c r="XB70" s="45"/>
+      <c r="XC70" s="45"/>
+      <c r="XD70" s="45"/>
+      <c r="XE70" s="45"/>
+      <c r="XF70" s="45"/>
+      <c r="XG70" s="45"/>
+      <c r="XH70" s="45"/>
+      <c r="XI70" s="45"/>
+      <c r="XJ70" s="45"/>
+      <c r="XK70" s="45"/>
+      <c r="XL70" s="45"/>
+      <c r="XM70" s="45"/>
+      <c r="XN70" s="45"/>
+      <c r="XO70" s="45"/>
+      <c r="XP70" s="45"/>
+      <c r="XQ70" s="45"/>
+      <c r="XR70" s="45"/>
+      <c r="XS70" s="45"/>
+      <c r="XT70" s="45"/>
+      <c r="XU70" s="45"/>
+      <c r="XV70" s="45"/>
+      <c r="XW70" s="45"/>
+      <c r="XX70" s="45"/>
+      <c r="XY70" s="45"/>
+      <c r="XZ70" s="45"/>
+      <c r="YA70" s="45"/>
+      <c r="YB70" s="45"/>
+      <c r="YC70" s="45"/>
+      <c r="YD70" s="45"/>
+      <c r="YE70" s="45"/>
+      <c r="YF70" s="45"/>
+      <c r="YG70" s="45"/>
+      <c r="YH70" s="45"/>
+      <c r="YI70" s="45"/>
+      <c r="YJ70" s="45"/>
+      <c r="YK70" s="45"/>
+      <c r="YL70" s="45"/>
+      <c r="YM70" s="45"/>
+      <c r="YN70" s="45"/>
+      <c r="YO70" s="45"/>
+      <c r="YP70" s="45"/>
+      <c r="YQ70" s="45"/>
+      <c r="YR70" s="45"/>
+      <c r="YS70" s="45"/>
+      <c r="YT70" s="45"/>
+      <c r="YU70" s="45"/>
+      <c r="YV70" s="45"/>
+      <c r="YW70" s="45"/>
+      <c r="YX70" s="45"/>
+      <c r="YY70" s="45"/>
+      <c r="YZ70" s="45"/>
+      <c r="ZA70" s="45"/>
+      <c r="ZB70" s="45"/>
+      <c r="ZC70" s="45"/>
+      <c r="ZD70" s="45"/>
+      <c r="ZE70" s="45"/>
+      <c r="ZF70" s="45"/>
+      <c r="ZG70" s="45"/>
+      <c r="ZH70" s="45"/>
+      <c r="ZI70" s="45"/>
+      <c r="ZJ70" s="45"/>
+      <c r="ZK70" s="45"/>
+      <c r="ZL70" s="45"/>
+      <c r="ZM70" s="45"/>
+      <c r="ZN70" s="45"/>
+      <c r="ZO70" s="45"/>
+      <c r="ZP70" s="45"/>
+      <c r="ZQ70" s="45"/>
+      <c r="ZR70" s="45"/>
+      <c r="ZS70" s="45"/>
+      <c r="ZT70" s="45"/>
+      <c r="ZU70" s="45"/>
+      <c r="ZV70" s="45"/>
+      <c r="ZW70" s="45"/>
+      <c r="ZX70" s="45"/>
+      <c r="ZY70" s="45"/>
+      <c r="ZZ70" s="45"/>
+      <c r="AAA70" s="45"/>
+      <c r="AAB70" s="45"/>
+      <c r="AAC70" s="45"/>
+      <c r="AAD70" s="45"/>
+      <c r="AAE70" s="45"/>
+      <c r="AAF70" s="45"/>
+      <c r="AAG70" s="45"/>
+      <c r="AAH70" s="45"/>
+      <c r="AAI70" s="45"/>
+      <c r="AAJ70" s="45"/>
+      <c r="AAK70" s="45"/>
+      <c r="AAL70" s="45"/>
+      <c r="AAM70" s="45"/>
+      <c r="AAN70" s="45"/>
+      <c r="AAO70" s="45"/>
+      <c r="AAP70" s="45"/>
+      <c r="AAQ70" s="45"/>
+      <c r="AAR70" s="45"/>
+      <c r="AAS70" s="45"/>
+      <c r="AAT70" s="45"/>
+      <c r="AAU70" s="45"/>
+      <c r="AAV70" s="45"/>
+      <c r="AAW70" s="45"/>
+      <c r="AAX70" s="45"/>
+      <c r="AAY70" s="45"/>
+      <c r="AAZ70" s="45"/>
+      <c r="ABA70" s="45"/>
+      <c r="ABB70" s="45"/>
+      <c r="ABC70" s="45"/>
+      <c r="ABD70" s="45"/>
+      <c r="ABE70" s="45"/>
+      <c r="ABF70" s="45"/>
+      <c r="ABG70" s="45"/>
+      <c r="ABH70" s="45"/>
+      <c r="ABI70" s="45"/>
+      <c r="ABJ70" s="45"/>
+      <c r="ABK70" s="45"/>
+      <c r="ABL70" s="45"/>
+      <c r="ABM70" s="45"/>
+      <c r="ABN70" s="45"/>
+      <c r="ABO70" s="45"/>
+      <c r="ABP70" s="45"/>
+      <c r="ABQ70" s="45"/>
+      <c r="ABR70" s="45"/>
+      <c r="ABS70" s="45"/>
+      <c r="ABT70" s="45"/>
+      <c r="ABU70" s="45"/>
+      <c r="ABV70" s="45"/>
+      <c r="ABW70" s="45"/>
+      <c r="ABX70" s="45"/>
+      <c r="ABY70" s="45"/>
+      <c r="ABZ70" s="45"/>
+      <c r="ACA70" s="45"/>
+      <c r="ACB70" s="45"/>
+      <c r="ACC70" s="45"/>
+      <c r="ACD70" s="45"/>
+      <c r="ACE70" s="45"/>
+      <c r="ACF70" s="45"/>
+      <c r="ACG70" s="45"/>
+      <c r="ACH70" s="45"/>
+      <c r="ACI70" s="45"/>
+      <c r="ACJ70" s="45"/>
+      <c r="ACK70" s="45"/>
+      <c r="ACL70" s="45"/>
+      <c r="ACM70" s="45"/>
+      <c r="ACN70" s="45"/>
+      <c r="ACO70" s="45"/>
+      <c r="ACP70" s="45"/>
+      <c r="ACQ70" s="45"/>
+      <c r="ACR70" s="45"/>
+      <c r="ACS70" s="45"/>
+      <c r="ACT70" s="45"/>
+      <c r="ACU70" s="45"/>
+      <c r="ACV70" s="45"/>
+      <c r="ACW70" s="45"/>
+      <c r="ACX70" s="45"/>
+      <c r="ACY70" s="45"/>
+      <c r="ACZ70" s="45"/>
+      <c r="ADA70" s="45"/>
+      <c r="ADB70" s="45"/>
+      <c r="ADC70" s="45"/>
+      <c r="ADD70" s="45"/>
+      <c r="ADE70" s="45"/>
+      <c r="ADF70" s="45"/>
+      <c r="ADG70" s="45"/>
+      <c r="ADH70" s="45"/>
+      <c r="ADI70" s="45"/>
+      <c r="ADJ70" s="45"/>
+      <c r="ADK70" s="45"/>
+      <c r="ADL70" s="45"/>
+      <c r="ADM70" s="45"/>
+      <c r="ADN70" s="45"/>
+      <c r="ADO70" s="45"/>
+      <c r="ADP70" s="45"/>
+      <c r="ADQ70" s="45"/>
+      <c r="ADR70" s="45"/>
+      <c r="ADS70" s="45"/>
+      <c r="ADT70" s="45"/>
+      <c r="ADU70" s="45"/>
+      <c r="ADV70" s="45"/>
+      <c r="ADW70" s="45"/>
+      <c r="ADX70" s="45"/>
+      <c r="ADY70" s="45"/>
+      <c r="ADZ70" s="45"/>
+      <c r="AEA70" s="45"/>
+      <c r="AEB70" s="45"/>
+      <c r="AEC70" s="45"/>
+      <c r="AED70" s="45"/>
+      <c r="AEE70" s="45"/>
+      <c r="AEF70" s="45"/>
+      <c r="AEG70" s="45"/>
+      <c r="AEH70" s="45"/>
+      <c r="AEI70" s="45"/>
+      <c r="AEJ70" s="45"/>
+      <c r="AEK70" s="45"/>
+      <c r="AEL70" s="45"/>
+      <c r="AEM70" s="45"/>
+      <c r="AEN70" s="45"/>
+      <c r="AEO70" s="45"/>
+      <c r="AEP70" s="45"/>
+      <c r="AEQ70" s="45"/>
+      <c r="AER70" s="45"/>
+      <c r="AES70" s="45"/>
+      <c r="AET70" s="45"/>
+      <c r="AEU70" s="45"/>
+      <c r="AEV70" s="45"/>
+      <c r="AEW70" s="45"/>
+      <c r="AEX70" s="45"/>
+      <c r="AEY70" s="45"/>
+      <c r="AEZ70" s="45"/>
+      <c r="AFA70" s="45"/>
+      <c r="AFB70" s="45"/>
+      <c r="AFC70" s="45"/>
+      <c r="AFD70" s="45"/>
+      <c r="AFE70" s="45"/>
+      <c r="AFF70" s="45"/>
+      <c r="AFG70" s="45"/>
+      <c r="AFH70" s="45"/>
+      <c r="AFI70" s="45"/>
+      <c r="AFJ70" s="45"/>
+      <c r="AFK70" s="45"/>
+      <c r="AFL70" s="45"/>
+      <c r="AFM70" s="45"/>
+      <c r="AFN70" s="45"/>
+      <c r="AFO70" s="45"/>
+      <c r="AFP70" s="45"/>
+      <c r="AFQ70" s="45"/>
+      <c r="AFR70" s="45"/>
+      <c r="AFS70" s="45"/>
+      <c r="AFT70" s="45"/>
+      <c r="AFU70" s="45"/>
+      <c r="AFV70" s="45"/>
+      <c r="AFW70" s="45"/>
+      <c r="AFX70" s="45"/>
+      <c r="AFY70" s="45"/>
+      <c r="AFZ70" s="45"/>
+      <c r="AGA70" s="45"/>
+      <c r="AGB70" s="45"/>
+      <c r="AGC70" s="45"/>
+      <c r="AGD70" s="45"/>
+      <c r="AGE70" s="45"/>
+      <c r="AGF70" s="45"/>
+      <c r="AGG70" s="45"/>
+      <c r="AGH70" s="45"/>
+      <c r="AGI70" s="45"/>
+      <c r="AGJ70" s="45"/>
+      <c r="AGK70" s="45"/>
+      <c r="AGL70" s="45"/>
+      <c r="AGM70" s="45"/>
+      <c r="AGN70" s="45"/>
+      <c r="AGO70" s="45"/>
+      <c r="AGP70" s="45"/>
+      <c r="AGQ70" s="45"/>
+      <c r="AGR70" s="45"/>
+      <c r="AGS70" s="45"/>
+      <c r="AGT70" s="45"/>
+      <c r="AGU70" s="45"/>
+      <c r="AGV70" s="45"/>
+      <c r="AGW70" s="45"/>
+      <c r="AGX70" s="45"/>
+      <c r="AGY70" s="45"/>
+      <c r="AGZ70" s="45"/>
+      <c r="AHA70" s="45"/>
+      <c r="AHB70" s="45"/>
+      <c r="AHC70" s="45"/>
+      <c r="AHD70" s="45"/>
+      <c r="AHE70" s="45"/>
+      <c r="AHF70" s="45"/>
+      <c r="AHG70" s="45"/>
+      <c r="AHH70" s="45"/>
+      <c r="AHI70" s="45"/>
+      <c r="AHJ70" s="45"/>
+      <c r="AHK70" s="45"/>
+      <c r="AHL70" s="45"/>
+      <c r="AHM70" s="45"/>
+      <c r="AHN70" s="45"/>
+      <c r="AHO70" s="45"/>
+      <c r="AHP70" s="45"/>
+      <c r="AHQ70" s="45"/>
+      <c r="AHR70" s="45"/>
+      <c r="AHS70" s="45"/>
+      <c r="AHT70" s="45"/>
+      <c r="AHU70" s="45"/>
+      <c r="AHV70" s="45"/>
+      <c r="AHW70" s="45"/>
+      <c r="AHX70" s="45"/>
+      <c r="AHY70" s="45"/>
+      <c r="AHZ70" s="45"/>
+      <c r="AIA70" s="45"/>
+      <c r="AIB70" s="45"/>
+      <c r="AIC70" s="45"/>
+      <c r="AID70" s="45"/>
+      <c r="AIE70" s="45"/>
+      <c r="AIF70" s="45"/>
+      <c r="AIG70" s="45"/>
+      <c r="AIH70" s="45"/>
+      <c r="AII70" s="45"/>
+      <c r="AIJ70" s="45"/>
+      <c r="AIK70" s="45"/>
+      <c r="AIL70" s="45"/>
+      <c r="AIM70" s="45"/>
+      <c r="AIN70" s="45"/>
+      <c r="AIO70" s="45"/>
+      <c r="AIP70" s="45"/>
+      <c r="AIQ70" s="45"/>
+      <c r="AIR70" s="45"/>
+      <c r="AIS70" s="45"/>
+      <c r="AIT70" s="45"/>
+      <c r="AIU70" s="45"/>
+      <c r="AIV70" s="45"/>
+      <c r="AIW70" s="45"/>
+      <c r="AIX70" s="45"/>
+      <c r="AIY70" s="45"/>
+      <c r="AIZ70" s="45"/>
+      <c r="AJA70" s="45"/>
+      <c r="AJB70" s="45"/>
+      <c r="AJC70" s="45"/>
+      <c r="AJD70" s="45"/>
+      <c r="AJE70" s="45"/>
+      <c r="AJF70" s="45"/>
+      <c r="AJG70" s="45"/>
+      <c r="AJH70" s="45"/>
+      <c r="AJI70" s="45"/>
+      <c r="AJJ70" s="45"/>
+      <c r="AJK70" s="45"/>
+      <c r="AJL70" s="45"/>
+      <c r="AJM70" s="45"/>
+      <c r="AJN70" s="45"/>
+      <c r="AJO70" s="45"/>
+      <c r="AJP70" s="45"/>
+      <c r="AJQ70" s="45"/>
+      <c r="AJR70" s="45"/>
+      <c r="AJS70" s="45"/>
+      <c r="AJT70" s="45"/>
+      <c r="AJU70" s="45"/>
+      <c r="AJV70" s="45"/>
+      <c r="AJW70" s="45"/>
+      <c r="AJX70" s="45"/>
+      <c r="AJY70" s="45"/>
+      <c r="AJZ70" s="45"/>
+      <c r="AKA70" s="45"/>
+      <c r="AKB70" s="45"/>
+      <c r="AKC70" s="45"/>
+      <c r="AKD70" s="45"/>
+      <c r="AKE70" s="45"/>
+      <c r="AKF70" s="45"/>
+      <c r="AKG70" s="45"/>
+      <c r="AKH70" s="45"/>
+      <c r="AKI70" s="45"/>
+      <c r="AKJ70" s="45"/>
+      <c r="AKK70" s="45"/>
+      <c r="AKL70" s="45"/>
+      <c r="AKM70" s="45"/>
+      <c r="AKN70" s="45"/>
+      <c r="AKO70" s="45"/>
+      <c r="AKP70" s="45"/>
+      <c r="AKQ70" s="45"/>
+      <c r="AKR70" s="45"/>
+      <c r="AKS70" s="45"/>
+      <c r="AKT70" s="45"/>
+      <c r="AKU70" s="45"/>
+      <c r="AKV70" s="45"/>
+      <c r="AKW70" s="45"/>
+      <c r="AKX70" s="45"/>
+      <c r="AKY70" s="45"/>
+      <c r="AKZ70" s="45"/>
+      <c r="ALA70" s="45"/>
+      <c r="ALB70" s="45"/>
+      <c r="ALC70" s="45"/>
+      <c r="ALD70" s="45"/>
+      <c r="ALE70" s="45"/>
+      <c r="ALF70" s="45"/>
+      <c r="ALG70" s="45"/>
+      <c r="ALH70" s="45"/>
+      <c r="ALI70" s="45"/>
+      <c r="ALJ70" s="45"/>
+      <c r="ALK70" s="45"/>
+      <c r="ALL70" s="45"/>
+      <c r="ALM70" s="45"/>
+      <c r="ALN70" s="45"/>
+      <c r="ALO70" s="45"/>
+      <c r="ALP70" s="45"/>
+      <c r="ALQ70" s="45"/>
+      <c r="ALR70" s="45"/>
+      <c r="ALS70" s="45"/>
+      <c r="ALT70" s="45"/>
+      <c r="ALU70" s="45"/>
+      <c r="ALV70" s="45"/>
+      <c r="ALW70" s="45"/>
+      <c r="ALX70" s="45"/>
+      <c r="ALY70" s="45"/>
+      <c r="ALZ70" s="45"/>
+      <c r="AMA70" s="45"/>
+      <c r="AMB70" s="45"/>
+      <c r="AMC70" s="45"/>
+      <c r="AMD70" s="45"/>
+      <c r="AME70" s="45"/>
+      <c r="AMF70" s="45"/>
+      <c r="AMG70" s="45"/>
+      <c r="AMH70" s="45"/>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C71" s="9">
+        <v>0.9940074</v>
+      </c>
+      <c r="D71" s="9">
+        <v>0.9631354</v>
+      </c>
+      <c r="E71" s="9">
+        <v>0.9951506</v>
+      </c>
+      <c r="F71" s="10">
+        <v>0.9668159</v>
+      </c>
+      <c r="G71" s="11">
+        <v>0.9676</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C72" s="9">
+        <v>0.9947298</v>
+      </c>
+      <c r="D72" s="9">
+        <v>0.9635241</v>
+      </c>
+      <c r="E72" s="9">
+        <v>0.9970105</v>
+      </c>
+      <c r="F72" s="10">
+        <v>0.9671041</v>
+      </c>
+      <c r="G72" s="11">
+        <v>0.96859</v>
+      </c>
+      <c r="H72" s="53" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="C73" s="9">
+        <v>0.995564</v>
+      </c>
+      <c r="D73" s="9">
+        <v>0.9686082</v>
+      </c>
+      <c r="E73" s="9">
+        <v>0.9962035</v>
+      </c>
+      <c r="F73" s="10">
+        <v>0.9685502</v>
+      </c>
+      <c r="G73" s="11">
+        <v>0.9684</v>
+      </c>
+      <c r="H73" s="53" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A32:G32"/>

</xml_diff>

<commit_message>
back to new baseline, LB 0.96859
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137">
   <si>
     <r>
       <rPr>
@@ -1225,11 +1225,17 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
       <t>several_1</t>
     </r>
     <r>
       <rPr>
         <sz val="8"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>，</t>
@@ -1247,6 +1253,33 @@
   <si>
     <t>313</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0.96859 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <charset val="134"/>
+      </rPr>
+      <t>基础上添加</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> doc2vec, 
+size=100,window=2,min_count=2</t>
+    </r>
+  </si>
+  <si>
+    <t>410</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
 </sst>
 </file>
 
@@ -1254,9 +1287,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="0.00000_ "/>
+    <numFmt numFmtId="177" formatCode="0.0000000_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.0000000_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -1279,12 +1312,17 @@
     <font>
       <sz val="8"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFFF0000"/>
       <name val="DejaVu Sans Mono"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1295,9 +1333,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1311,41 +1348,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1356,31 +1362,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1400,6 +1391,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1408,17 +1415,41 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1430,17 +1461,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1467,12 +1505,8 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1517,13 +1551,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1535,37 +1623,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1583,31 +1641,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1619,85 +1731,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1711,52 +1751,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1785,15 +1784,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1808,147 +1798,197 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2111,13 +2151,28 @@
     <xf numFmtId="177" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
@@ -2438,10 +2493,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AMH76"/>
+  <dimension ref="A1:AMH80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -7756,7 +7811,7 @@
       <c r="AMH13" s="46"/>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:1022">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="18" t="s">
@@ -17992,7 +18047,7 @@
       <c r="G72" s="34">
         <v>0.96859</v>
       </c>
-      <c r="H72" s="54" t="s">
+      <c r="H72" s="58" t="s">
         <v>125</v>
       </c>
       <c r="I72" s="45"/>
@@ -19032,7 +19087,7 @@
       <c r="G73" s="11">
         <v>0.9684</v>
       </c>
-      <c r="H73" s="55" t="s">
+      <c r="H73" s="59" t="s">
         <v>127</v>
       </c>
     </row>
@@ -19080,7 +19135,7 @@
       </c>
     </row>
     <row r="76" ht="21" spans="1:7">
-      <c r="A76" s="16" t="s">
+      <c r="A76" s="21" t="s">
         <v>132</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -19089,17 +19144,63 @@
       <c r="C76" s="9">
         <v>0.995618</v>
       </c>
-      <c r="D76" s="9">
+      <c r="D76" s="19">
         <v>0.9638269</v>
       </c>
       <c r="E76" s="9">
         <v>0.995334</v>
       </c>
-      <c r="F76" s="10">
+      <c r="F76" s="19">
         <v>0.9671155</v>
       </c>
-      <c r="G76" s="56">
+      <c r="G76" s="60">
         <v>0.9682</v>
+      </c>
+    </row>
+    <row r="78" ht="21" spans="1:7">
+      <c r="A78" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="B78" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="C78" s="56">
+        <v>0.9962574</v>
+      </c>
+      <c r="D78" s="56">
+        <v>0.9633916</v>
+      </c>
+      <c r="E78" s="56">
+        <v>0.9963877</v>
+      </c>
+      <c r="F78" s="56">
+        <v>0.9666471</v>
+      </c>
+      <c r="G78" s="61">
+        <v>0.9678</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C80" s="19">
+        <v>0.9947298</v>
+      </c>
+      <c r="D80" s="19">
+        <v>0.9635241</v>
+      </c>
+      <c r="E80" s="19">
+        <v>0.9970105</v>
+      </c>
+      <c r="F80" s="19">
+        <v>0.9671041</v>
+      </c>
+      <c r="G80" s="34">
+        <v>0.96859</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
back to new baseline, LB 0.96869
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139">
   <si>
     <r>
       <rPr>
@@ -1280,6 +1280,12 @@
   <si>
     <t>baseline</t>
   </si>
+  <si>
+    <t>feature_percentile = 0.95</t>
+  </si>
+  <si>
+    <t>285</t>
+  </si>
 </sst>
 </file>
 
@@ -2493,10 +2499,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AMH80"/>
+  <dimension ref="A1:AMH81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -19203,6 +19209,29 @@
         <v>0.96859</v>
       </c>
     </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C81" s="9">
+        <v>0.9949835</v>
+      </c>
+      <c r="D81" s="9">
+        <v>0.9636112</v>
+      </c>
+      <c r="E81" s="9">
+        <v>0.9953615</v>
+      </c>
+      <c r="F81" s="10">
+        <v>0.9671736</v>
+      </c>
+      <c r="G81" s="11">
+        <v>0.96869</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A32:G32"/>

</xml_diff>

<commit_message>
simple lightgbm baseline， 0.96830
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145">
   <si>
     <r>
       <rPr>
@@ -1056,6 +1056,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>去掉</t>
     </r>
     <r>
@@ -1294,6 +1299,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>保留所有特征的</t>
     </r>
     <r>
@@ -1305,20 +1315,23 @@
       <t xml:space="preserve"> baseline</t>
     </r>
   </si>
+  <si>
+    <t>simple lightgbm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.0000000_ "/>
+    <numFmt numFmtId="176" formatCode="0.00000_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.00000_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0.0000000_ "/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="30">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1332,10 +1345,6 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1359,31 +1368,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1391,14 +1377,6 @@
     <font>
       <b/>
       <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1413,66 +1391,13 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1488,8 +1413,84 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1503,7 +1504,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1588,61 +1597,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1660,19 +1621,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1690,85 +1777,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1779,54 +1788,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1848,8 +1809,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1869,6 +1845,39 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1884,142 +1893,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2050,16 +2059,16 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -2080,7 +2089,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2095,7 +2104,7 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2104,13 +2113,13 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2122,40 +2131,40 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -2173,19 +2182,16 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2194,34 +2200,34 @@
     <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -2545,10 +2551,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AMH84"/>
+  <dimension ref="A1:AMH85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -7863,7 +7869,7 @@
       <c r="AMH13" s="47"/>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:1022">
-      <c r="A14" s="69" t="s">
+      <c r="A14" s="68" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="19" t="s">
@@ -16907,7 +16913,7 @@
       </c>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="51" t="s">
+      <c r="A65" s="15" t="s">
         <v>110</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -18099,7 +18105,7 @@
       <c r="G72" s="35">
         <v>0.96859</v>
       </c>
-      <c r="H72" s="62" t="s">
+      <c r="H72" s="61" t="s">
         <v>125</v>
       </c>
       <c r="I72" s="46"/>
@@ -19118,28 +19124,28 @@
       <c r="AMH72" s="46"/>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="52" t="s">
+      <c r="A73" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="B73" s="53" t="s">
+      <c r="B73" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="C73" s="54">
+      <c r="C73" s="53">
         <v>0.995564</v>
       </c>
-      <c r="D73" s="55">
+      <c r="D73" s="54">
         <v>0.9686082</v>
       </c>
-      <c r="E73" s="54">
+      <c r="E73" s="53">
         <v>0.9962035</v>
       </c>
-      <c r="F73" s="55">
+      <c r="F73" s="54">
         <v>0.9685502</v>
       </c>
       <c r="G73" s="12">
         <v>0.9684</v>
       </c>
-      <c r="H73" s="63" t="s">
+      <c r="H73" s="62" t="s">
         <v>127</v>
       </c>
     </row>
@@ -19205,30 +19211,30 @@
       <c r="F76" s="20">
         <v>0.9671155</v>
       </c>
-      <c r="G76" s="64">
+      <c r="G76" s="63">
         <v>0.9682</v>
       </c>
     </row>
     <row r="78" ht="21" spans="1:7">
-      <c r="A78" s="56" t="s">
+      <c r="A78" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="B78" s="57" t="s">
+      <c r="B78" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="C78" s="58">
+      <c r="C78" s="57">
         <v>0.9962574</v>
       </c>
-      <c r="D78" s="58">
+      <c r="D78" s="57">
         <v>0.9633916</v>
       </c>
-      <c r="E78" s="58">
+      <c r="E78" s="57">
         <v>0.9963877</v>
       </c>
-      <c r="F78" s="58">
+      <c r="F78" s="57">
         <v>0.9666471</v>
       </c>
-      <c r="G78" s="65">
+      <c r="G78" s="64">
         <v>0.9678</v>
       </c>
     </row>
@@ -19325,1042 +19331,1056 @@
       </c>
     </row>
     <row r="84" s="9" customFormat="1" spans="1:1022">
-      <c r="A84" s="59" t="s">
+      <c r="A84" s="58" t="s">
         <v>143</v>
       </c>
-      <c r="B84" s="60" t="s">
+      <c r="B84" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="C84" s="61">
+      <c r="C84" s="60">
         <v>0.9942723</v>
       </c>
-      <c r="D84" s="61">
+      <c r="D84" s="60">
         <v>0.9633743</v>
       </c>
-      <c r="E84" s="61">
+      <c r="E84" s="60">
         <v>0.9959016</v>
       </c>
-      <c r="F84" s="61">
+      <c r="F84" s="60">
         <v>0.9673051</v>
       </c>
-      <c r="G84" s="66">
+      <c r="G84" s="65">
         <v>0.9686</v>
       </c>
-      <c r="H84" s="67"/>
-      <c r="I84" s="68"/>
-      <c r="J84" s="68"/>
-      <c r="K84" s="68"/>
-      <c r="L84" s="68"/>
-      <c r="M84" s="68"/>
-      <c r="N84" s="68"/>
-      <c r="O84" s="68"/>
-      <c r="P84" s="68"/>
-      <c r="Q84" s="68"/>
-      <c r="R84" s="68"/>
-      <c r="S84" s="68"/>
-      <c r="T84" s="68"/>
-      <c r="U84" s="68"/>
-      <c r="V84" s="68"/>
-      <c r="W84" s="68"/>
-      <c r="X84" s="68"/>
-      <c r="Y84" s="68"/>
-      <c r="Z84" s="68"/>
-      <c r="AA84" s="68"/>
-      <c r="AB84" s="68"/>
-      <c r="AC84" s="68"/>
-      <c r="AD84" s="68"/>
-      <c r="AE84" s="68"/>
-      <c r="AF84" s="68"/>
-      <c r="AG84" s="68"/>
-      <c r="AH84" s="68"/>
-      <c r="AI84" s="68"/>
-      <c r="AJ84" s="68"/>
-      <c r="AK84" s="68"/>
-      <c r="AL84" s="68"/>
-      <c r="AM84" s="68"/>
-      <c r="AN84" s="68"/>
-      <c r="AO84" s="68"/>
-      <c r="AP84" s="68"/>
-      <c r="AQ84" s="68"/>
-      <c r="AR84" s="68"/>
-      <c r="AS84" s="68"/>
-      <c r="AT84" s="68"/>
-      <c r="AU84" s="68"/>
-      <c r="AV84" s="68"/>
-      <c r="AW84" s="68"/>
-      <c r="AX84" s="68"/>
-      <c r="AY84" s="68"/>
-      <c r="AZ84" s="68"/>
-      <c r="BA84" s="68"/>
-      <c r="BB84" s="68"/>
-      <c r="BC84" s="68"/>
-      <c r="BD84" s="68"/>
-      <c r="BE84" s="68"/>
-      <c r="BF84" s="68"/>
-      <c r="BG84" s="68"/>
-      <c r="BH84" s="68"/>
-      <c r="BI84" s="68"/>
-      <c r="BJ84" s="68"/>
-      <c r="BK84" s="68"/>
-      <c r="BL84" s="68"/>
-      <c r="BM84" s="68"/>
-      <c r="BN84" s="68"/>
-      <c r="BO84" s="68"/>
-      <c r="BP84" s="68"/>
-      <c r="BQ84" s="68"/>
-      <c r="BR84" s="68"/>
-      <c r="BS84" s="68"/>
-      <c r="BT84" s="68"/>
-      <c r="BU84" s="68"/>
-      <c r="BV84" s="68"/>
-      <c r="BW84" s="68"/>
-      <c r="BX84" s="68"/>
-      <c r="BY84" s="68"/>
-      <c r="BZ84" s="68"/>
-      <c r="CA84" s="68"/>
-      <c r="CB84" s="68"/>
-      <c r="CC84" s="68"/>
-      <c r="CD84" s="68"/>
-      <c r="CE84" s="68"/>
-      <c r="CF84" s="68"/>
-      <c r="CG84" s="68"/>
-      <c r="CH84" s="68"/>
-      <c r="CI84" s="68"/>
-      <c r="CJ84" s="68"/>
-      <c r="CK84" s="68"/>
-      <c r="CL84" s="68"/>
-      <c r="CM84" s="68"/>
-      <c r="CN84" s="68"/>
-      <c r="CO84" s="68"/>
-      <c r="CP84" s="68"/>
-      <c r="CQ84" s="68"/>
-      <c r="CR84" s="68"/>
-      <c r="CS84" s="68"/>
-      <c r="CT84" s="68"/>
-      <c r="CU84" s="68"/>
-      <c r="CV84" s="68"/>
-      <c r="CW84" s="68"/>
-      <c r="CX84" s="68"/>
-      <c r="CY84" s="68"/>
-      <c r="CZ84" s="68"/>
-      <c r="DA84" s="68"/>
-      <c r="DB84" s="68"/>
-      <c r="DC84" s="68"/>
-      <c r="DD84" s="68"/>
-      <c r="DE84" s="68"/>
-      <c r="DF84" s="68"/>
-      <c r="DG84" s="68"/>
-      <c r="DH84" s="68"/>
-      <c r="DI84" s="68"/>
-      <c r="DJ84" s="68"/>
-      <c r="DK84" s="68"/>
-      <c r="DL84" s="68"/>
-      <c r="DM84" s="68"/>
-      <c r="DN84" s="68"/>
-      <c r="DO84" s="68"/>
-      <c r="DP84" s="68"/>
-      <c r="DQ84" s="68"/>
-      <c r="DR84" s="68"/>
-      <c r="DS84" s="68"/>
-      <c r="DT84" s="68"/>
-      <c r="DU84" s="68"/>
-      <c r="DV84" s="68"/>
-      <c r="DW84" s="68"/>
-      <c r="DX84" s="68"/>
-      <c r="DY84" s="68"/>
-      <c r="DZ84" s="68"/>
-      <c r="EA84" s="68"/>
-      <c r="EB84" s="68"/>
-      <c r="EC84" s="68"/>
-      <c r="ED84" s="68"/>
-      <c r="EE84" s="68"/>
-      <c r="EF84" s="68"/>
-      <c r="EG84" s="68"/>
-      <c r="EH84" s="68"/>
-      <c r="EI84" s="68"/>
-      <c r="EJ84" s="68"/>
-      <c r="EK84" s="68"/>
-      <c r="EL84" s="68"/>
-      <c r="EM84" s="68"/>
-      <c r="EN84" s="68"/>
-      <c r="EO84" s="68"/>
-      <c r="EP84" s="68"/>
-      <c r="EQ84" s="68"/>
-      <c r="ER84" s="68"/>
-      <c r="ES84" s="68"/>
-      <c r="ET84" s="68"/>
-      <c r="EU84" s="68"/>
-      <c r="EV84" s="68"/>
-      <c r="EW84" s="68"/>
-      <c r="EX84" s="68"/>
-      <c r="EY84" s="68"/>
-      <c r="EZ84" s="68"/>
-      <c r="FA84" s="68"/>
-      <c r="FB84" s="68"/>
-      <c r="FC84" s="68"/>
-      <c r="FD84" s="68"/>
-      <c r="FE84" s="68"/>
-      <c r="FF84" s="68"/>
-      <c r="FG84" s="68"/>
-      <c r="FH84" s="68"/>
-      <c r="FI84" s="68"/>
-      <c r="FJ84" s="68"/>
-      <c r="FK84" s="68"/>
-      <c r="FL84" s="68"/>
-      <c r="FM84" s="68"/>
-      <c r="FN84" s="68"/>
-      <c r="FO84" s="68"/>
-      <c r="FP84" s="68"/>
-      <c r="FQ84" s="68"/>
-      <c r="FR84" s="68"/>
-      <c r="FS84" s="68"/>
-      <c r="FT84" s="68"/>
-      <c r="FU84" s="68"/>
-      <c r="FV84" s="68"/>
-      <c r="FW84" s="68"/>
-      <c r="FX84" s="68"/>
-      <c r="FY84" s="68"/>
-      <c r="FZ84" s="68"/>
-      <c r="GA84" s="68"/>
-      <c r="GB84" s="68"/>
-      <c r="GC84" s="68"/>
-      <c r="GD84" s="68"/>
-      <c r="GE84" s="68"/>
-      <c r="GF84" s="68"/>
-      <c r="GG84" s="68"/>
-      <c r="GH84" s="68"/>
-      <c r="GI84" s="68"/>
-      <c r="GJ84" s="68"/>
-      <c r="GK84" s="68"/>
-      <c r="GL84" s="68"/>
-      <c r="GM84" s="68"/>
-      <c r="GN84" s="68"/>
-      <c r="GO84" s="68"/>
-      <c r="GP84" s="68"/>
-      <c r="GQ84" s="68"/>
-      <c r="GR84" s="68"/>
-      <c r="GS84" s="68"/>
-      <c r="GT84" s="68"/>
-      <c r="GU84" s="68"/>
-      <c r="GV84" s="68"/>
-      <c r="GW84" s="68"/>
-      <c r="GX84" s="68"/>
-      <c r="GY84" s="68"/>
-      <c r="GZ84" s="68"/>
-      <c r="HA84" s="68"/>
-      <c r="HB84" s="68"/>
-      <c r="HC84" s="68"/>
-      <c r="HD84" s="68"/>
-      <c r="HE84" s="68"/>
-      <c r="HF84" s="68"/>
-      <c r="HG84" s="68"/>
-      <c r="HH84" s="68"/>
-      <c r="HI84" s="68"/>
-      <c r="HJ84" s="68"/>
-      <c r="HK84" s="68"/>
-      <c r="HL84" s="68"/>
-      <c r="HM84" s="68"/>
-      <c r="HN84" s="68"/>
-      <c r="HO84" s="68"/>
-      <c r="HP84" s="68"/>
-      <c r="HQ84" s="68"/>
-      <c r="HR84" s="68"/>
-      <c r="HS84" s="68"/>
-      <c r="HT84" s="68"/>
-      <c r="HU84" s="68"/>
-      <c r="HV84" s="68"/>
-      <c r="HW84" s="68"/>
-      <c r="HX84" s="68"/>
-      <c r="HY84" s="68"/>
-      <c r="HZ84" s="68"/>
-      <c r="IA84" s="68"/>
-      <c r="IB84" s="68"/>
-      <c r="IC84" s="68"/>
-      <c r="ID84" s="68"/>
-      <c r="IE84" s="68"/>
-      <c r="IF84" s="68"/>
-      <c r="IG84" s="68"/>
-      <c r="IH84" s="68"/>
-      <c r="II84" s="68"/>
-      <c r="IJ84" s="68"/>
-      <c r="IK84" s="68"/>
-      <c r="IL84" s="68"/>
-      <c r="IM84" s="68"/>
-      <c r="IN84" s="68"/>
-      <c r="IO84" s="68"/>
-      <c r="IP84" s="68"/>
-      <c r="IQ84" s="68"/>
-      <c r="IR84" s="68"/>
-      <c r="IS84" s="68"/>
-      <c r="IT84" s="68"/>
-      <c r="IU84" s="68"/>
-      <c r="IV84" s="68"/>
-      <c r="IW84" s="68"/>
-      <c r="IX84" s="68"/>
-      <c r="IY84" s="68"/>
-      <c r="IZ84" s="68"/>
-      <c r="JA84" s="68"/>
-      <c r="JB84" s="68"/>
-      <c r="JC84" s="68"/>
-      <c r="JD84" s="68"/>
-      <c r="JE84" s="68"/>
-      <c r="JF84" s="68"/>
-      <c r="JG84" s="68"/>
-      <c r="JH84" s="68"/>
-      <c r="JI84" s="68"/>
-      <c r="JJ84" s="68"/>
-      <c r="JK84" s="68"/>
-      <c r="JL84" s="68"/>
-      <c r="JM84" s="68"/>
-      <c r="JN84" s="68"/>
-      <c r="JO84" s="68"/>
-      <c r="JP84" s="68"/>
-      <c r="JQ84" s="68"/>
-      <c r="JR84" s="68"/>
-      <c r="JS84" s="68"/>
-      <c r="JT84" s="68"/>
-      <c r="JU84" s="68"/>
-      <c r="JV84" s="68"/>
-      <c r="JW84" s="68"/>
-      <c r="JX84" s="68"/>
-      <c r="JY84" s="68"/>
-      <c r="JZ84" s="68"/>
-      <c r="KA84" s="68"/>
-      <c r="KB84" s="68"/>
-      <c r="KC84" s="68"/>
-      <c r="KD84" s="68"/>
-      <c r="KE84" s="68"/>
-      <c r="KF84" s="68"/>
-      <c r="KG84" s="68"/>
-      <c r="KH84" s="68"/>
-      <c r="KI84" s="68"/>
-      <c r="KJ84" s="68"/>
-      <c r="KK84" s="68"/>
-      <c r="KL84" s="68"/>
-      <c r="KM84" s="68"/>
-      <c r="KN84" s="68"/>
-      <c r="KO84" s="68"/>
-      <c r="KP84" s="68"/>
-      <c r="KQ84" s="68"/>
-      <c r="KR84" s="68"/>
-      <c r="KS84" s="68"/>
-      <c r="KT84" s="68"/>
-      <c r="KU84" s="68"/>
-      <c r="KV84" s="68"/>
-      <c r="KW84" s="68"/>
-      <c r="KX84" s="68"/>
-      <c r="KY84" s="68"/>
-      <c r="KZ84" s="68"/>
-      <c r="LA84" s="68"/>
-      <c r="LB84" s="68"/>
-      <c r="LC84" s="68"/>
-      <c r="LD84" s="68"/>
-      <c r="LE84" s="68"/>
-      <c r="LF84" s="68"/>
-      <c r="LG84" s="68"/>
-      <c r="LH84" s="68"/>
-      <c r="LI84" s="68"/>
-      <c r="LJ84" s="68"/>
-      <c r="LK84" s="68"/>
-      <c r="LL84" s="68"/>
-      <c r="LM84" s="68"/>
-      <c r="LN84" s="68"/>
-      <c r="LO84" s="68"/>
-      <c r="LP84" s="68"/>
-      <c r="LQ84" s="68"/>
-      <c r="LR84" s="68"/>
-      <c r="LS84" s="68"/>
-      <c r="LT84" s="68"/>
-      <c r="LU84" s="68"/>
-      <c r="LV84" s="68"/>
-      <c r="LW84" s="68"/>
-      <c r="LX84" s="68"/>
-      <c r="LY84" s="68"/>
-      <c r="LZ84" s="68"/>
-      <c r="MA84" s="68"/>
-      <c r="MB84" s="68"/>
-      <c r="MC84" s="68"/>
-      <c r="MD84" s="68"/>
-      <c r="ME84" s="68"/>
-      <c r="MF84" s="68"/>
-      <c r="MG84" s="68"/>
-      <c r="MH84" s="68"/>
-      <c r="MI84" s="68"/>
-      <c r="MJ84" s="68"/>
-      <c r="MK84" s="68"/>
-      <c r="ML84" s="68"/>
-      <c r="MM84" s="68"/>
-      <c r="MN84" s="68"/>
-      <c r="MO84" s="68"/>
-      <c r="MP84" s="68"/>
-      <c r="MQ84" s="68"/>
-      <c r="MR84" s="68"/>
-      <c r="MS84" s="68"/>
-      <c r="MT84" s="68"/>
-      <c r="MU84" s="68"/>
-      <c r="MV84" s="68"/>
-      <c r="MW84" s="68"/>
-      <c r="MX84" s="68"/>
-      <c r="MY84" s="68"/>
-      <c r="MZ84" s="68"/>
-      <c r="NA84" s="68"/>
-      <c r="NB84" s="68"/>
-      <c r="NC84" s="68"/>
-      <c r="ND84" s="68"/>
-      <c r="NE84" s="68"/>
-      <c r="NF84" s="68"/>
-      <c r="NG84" s="68"/>
-      <c r="NH84" s="68"/>
-      <c r="NI84" s="68"/>
-      <c r="NJ84" s="68"/>
-      <c r="NK84" s="68"/>
-      <c r="NL84" s="68"/>
-      <c r="NM84" s="68"/>
-      <c r="NN84" s="68"/>
-      <c r="NO84" s="68"/>
-      <c r="NP84" s="68"/>
-      <c r="NQ84" s="68"/>
-      <c r="NR84" s="68"/>
-      <c r="NS84" s="68"/>
-      <c r="NT84" s="68"/>
-      <c r="NU84" s="68"/>
-      <c r="NV84" s="68"/>
-      <c r="NW84" s="68"/>
-      <c r="NX84" s="68"/>
-      <c r="NY84" s="68"/>
-      <c r="NZ84" s="68"/>
-      <c r="OA84" s="68"/>
-      <c r="OB84" s="68"/>
-      <c r="OC84" s="68"/>
-      <c r="OD84" s="68"/>
-      <c r="OE84" s="68"/>
-      <c r="OF84" s="68"/>
-      <c r="OG84" s="68"/>
-      <c r="OH84" s="68"/>
-      <c r="OI84" s="68"/>
-      <c r="OJ84" s="68"/>
-      <c r="OK84" s="68"/>
-      <c r="OL84" s="68"/>
-      <c r="OM84" s="68"/>
-      <c r="ON84" s="68"/>
-      <c r="OO84" s="68"/>
-      <c r="OP84" s="68"/>
-      <c r="OQ84" s="68"/>
-      <c r="OR84" s="68"/>
-      <c r="OS84" s="68"/>
-      <c r="OT84" s="68"/>
-      <c r="OU84" s="68"/>
-      <c r="OV84" s="68"/>
-      <c r="OW84" s="68"/>
-      <c r="OX84" s="68"/>
-      <c r="OY84" s="68"/>
-      <c r="OZ84" s="68"/>
-      <c r="PA84" s="68"/>
-      <c r="PB84" s="68"/>
-      <c r="PC84" s="68"/>
-      <c r="PD84" s="68"/>
-      <c r="PE84" s="68"/>
-      <c r="PF84" s="68"/>
-      <c r="PG84" s="68"/>
-      <c r="PH84" s="68"/>
-      <c r="PI84" s="68"/>
-      <c r="PJ84" s="68"/>
-      <c r="PK84" s="68"/>
-      <c r="PL84" s="68"/>
-      <c r="PM84" s="68"/>
-      <c r="PN84" s="68"/>
-      <c r="PO84" s="68"/>
-      <c r="PP84" s="68"/>
-      <c r="PQ84" s="68"/>
-      <c r="PR84" s="68"/>
-      <c r="PS84" s="68"/>
-      <c r="PT84" s="68"/>
-      <c r="PU84" s="68"/>
-      <c r="PV84" s="68"/>
-      <c r="PW84" s="68"/>
-      <c r="PX84" s="68"/>
-      <c r="PY84" s="68"/>
-      <c r="PZ84" s="68"/>
-      <c r="QA84" s="68"/>
-      <c r="QB84" s="68"/>
-      <c r="QC84" s="68"/>
-      <c r="QD84" s="68"/>
-      <c r="QE84" s="68"/>
-      <c r="QF84" s="68"/>
-      <c r="QG84" s="68"/>
-      <c r="QH84" s="68"/>
-      <c r="QI84" s="68"/>
-      <c r="QJ84" s="68"/>
-      <c r="QK84" s="68"/>
-      <c r="QL84" s="68"/>
-      <c r="QM84" s="68"/>
-      <c r="QN84" s="68"/>
-      <c r="QO84" s="68"/>
-      <c r="QP84" s="68"/>
-      <c r="QQ84" s="68"/>
-      <c r="QR84" s="68"/>
-      <c r="QS84" s="68"/>
-      <c r="QT84" s="68"/>
-      <c r="QU84" s="68"/>
-      <c r="QV84" s="68"/>
-      <c r="QW84" s="68"/>
-      <c r="QX84" s="68"/>
-      <c r="QY84" s="68"/>
-      <c r="QZ84" s="68"/>
-      <c r="RA84" s="68"/>
-      <c r="RB84" s="68"/>
-      <c r="RC84" s="68"/>
-      <c r="RD84" s="68"/>
-      <c r="RE84" s="68"/>
-      <c r="RF84" s="68"/>
-      <c r="RG84" s="68"/>
-      <c r="RH84" s="68"/>
-      <c r="RI84" s="68"/>
-      <c r="RJ84" s="68"/>
-      <c r="RK84" s="68"/>
-      <c r="RL84" s="68"/>
-      <c r="RM84" s="68"/>
-      <c r="RN84" s="68"/>
-      <c r="RO84" s="68"/>
-      <c r="RP84" s="68"/>
-      <c r="RQ84" s="68"/>
-      <c r="RR84" s="68"/>
-      <c r="RS84" s="68"/>
-      <c r="RT84" s="68"/>
-      <c r="RU84" s="68"/>
-      <c r="RV84" s="68"/>
-      <c r="RW84" s="68"/>
-      <c r="RX84" s="68"/>
-      <c r="RY84" s="68"/>
-      <c r="RZ84" s="68"/>
-      <c r="SA84" s="68"/>
-      <c r="SB84" s="68"/>
-      <c r="SC84" s="68"/>
-      <c r="SD84" s="68"/>
-      <c r="SE84" s="68"/>
-      <c r="SF84" s="68"/>
-      <c r="SG84" s="68"/>
-      <c r="SH84" s="68"/>
-      <c r="SI84" s="68"/>
-      <c r="SJ84" s="68"/>
-      <c r="SK84" s="68"/>
-      <c r="SL84" s="68"/>
-      <c r="SM84" s="68"/>
-      <c r="SN84" s="68"/>
-      <c r="SO84" s="68"/>
-      <c r="SP84" s="68"/>
-      <c r="SQ84" s="68"/>
-      <c r="SR84" s="68"/>
-      <c r="SS84" s="68"/>
-      <c r="ST84" s="68"/>
-      <c r="SU84" s="68"/>
-      <c r="SV84" s="68"/>
-      <c r="SW84" s="68"/>
-      <c r="SX84" s="68"/>
-      <c r="SY84" s="68"/>
-      <c r="SZ84" s="68"/>
-      <c r="TA84" s="68"/>
-      <c r="TB84" s="68"/>
-      <c r="TC84" s="68"/>
-      <c r="TD84" s="68"/>
-      <c r="TE84" s="68"/>
-      <c r="TF84" s="68"/>
-      <c r="TG84" s="68"/>
-      <c r="TH84" s="68"/>
-      <c r="TI84" s="68"/>
-      <c r="TJ84" s="68"/>
-      <c r="TK84" s="68"/>
-      <c r="TL84" s="68"/>
-      <c r="TM84" s="68"/>
-      <c r="TN84" s="68"/>
-      <c r="TO84" s="68"/>
-      <c r="TP84" s="68"/>
-      <c r="TQ84" s="68"/>
-      <c r="TR84" s="68"/>
-      <c r="TS84" s="68"/>
-      <c r="TT84" s="68"/>
-      <c r="TU84" s="68"/>
-      <c r="TV84" s="68"/>
-      <c r="TW84" s="68"/>
-      <c r="TX84" s="68"/>
-      <c r="TY84" s="68"/>
-      <c r="TZ84" s="68"/>
-      <c r="UA84" s="68"/>
-      <c r="UB84" s="68"/>
-      <c r="UC84" s="68"/>
-      <c r="UD84" s="68"/>
-      <c r="UE84" s="68"/>
-      <c r="UF84" s="68"/>
-      <c r="UG84" s="68"/>
-      <c r="UH84" s="68"/>
-      <c r="UI84" s="68"/>
-      <c r="UJ84" s="68"/>
-      <c r="UK84" s="68"/>
-      <c r="UL84" s="68"/>
-      <c r="UM84" s="68"/>
-      <c r="UN84" s="68"/>
-      <c r="UO84" s="68"/>
-      <c r="UP84" s="68"/>
-      <c r="UQ84" s="68"/>
-      <c r="UR84" s="68"/>
-      <c r="US84" s="68"/>
-      <c r="UT84" s="68"/>
-      <c r="UU84" s="68"/>
-      <c r="UV84" s="68"/>
-      <c r="UW84" s="68"/>
-      <c r="UX84" s="68"/>
-      <c r="UY84" s="68"/>
-      <c r="UZ84" s="68"/>
-      <c r="VA84" s="68"/>
-      <c r="VB84" s="68"/>
-      <c r="VC84" s="68"/>
-      <c r="VD84" s="68"/>
-      <c r="VE84" s="68"/>
-      <c r="VF84" s="68"/>
-      <c r="VG84" s="68"/>
-      <c r="VH84" s="68"/>
-      <c r="VI84" s="68"/>
-      <c r="VJ84" s="68"/>
-      <c r="VK84" s="68"/>
-      <c r="VL84" s="68"/>
-      <c r="VM84" s="68"/>
-      <c r="VN84" s="68"/>
-      <c r="VO84" s="68"/>
-      <c r="VP84" s="68"/>
-      <c r="VQ84" s="68"/>
-      <c r="VR84" s="68"/>
-      <c r="VS84" s="68"/>
-      <c r="VT84" s="68"/>
-      <c r="VU84" s="68"/>
-      <c r="VV84" s="68"/>
-      <c r="VW84" s="68"/>
-      <c r="VX84" s="68"/>
-      <c r="VY84" s="68"/>
-      <c r="VZ84" s="68"/>
-      <c r="WA84" s="68"/>
-      <c r="WB84" s="68"/>
-      <c r="WC84" s="68"/>
-      <c r="WD84" s="68"/>
-      <c r="WE84" s="68"/>
-      <c r="WF84" s="68"/>
-      <c r="WG84" s="68"/>
-      <c r="WH84" s="68"/>
-      <c r="WI84" s="68"/>
-      <c r="WJ84" s="68"/>
-      <c r="WK84" s="68"/>
-      <c r="WL84" s="68"/>
-      <c r="WM84" s="68"/>
-      <c r="WN84" s="68"/>
-      <c r="WO84" s="68"/>
-      <c r="WP84" s="68"/>
-      <c r="WQ84" s="68"/>
-      <c r="WR84" s="68"/>
-      <c r="WS84" s="68"/>
-      <c r="WT84" s="68"/>
-      <c r="WU84" s="68"/>
-      <c r="WV84" s="68"/>
-      <c r="WW84" s="68"/>
-      <c r="WX84" s="68"/>
-      <c r="WY84" s="68"/>
-      <c r="WZ84" s="68"/>
-      <c r="XA84" s="68"/>
-      <c r="XB84" s="68"/>
-      <c r="XC84" s="68"/>
-      <c r="XD84" s="68"/>
-      <c r="XE84" s="68"/>
-      <c r="XF84" s="68"/>
-      <c r="XG84" s="68"/>
-      <c r="XH84" s="68"/>
-      <c r="XI84" s="68"/>
-      <c r="XJ84" s="68"/>
-      <c r="XK84" s="68"/>
-      <c r="XL84" s="68"/>
-      <c r="XM84" s="68"/>
-      <c r="XN84" s="68"/>
-      <c r="XO84" s="68"/>
-      <c r="XP84" s="68"/>
-      <c r="XQ84" s="68"/>
-      <c r="XR84" s="68"/>
-      <c r="XS84" s="68"/>
-      <c r="XT84" s="68"/>
-      <c r="XU84" s="68"/>
-      <c r="XV84" s="68"/>
-      <c r="XW84" s="68"/>
-      <c r="XX84" s="68"/>
-      <c r="XY84" s="68"/>
-      <c r="XZ84" s="68"/>
-      <c r="YA84" s="68"/>
-      <c r="YB84" s="68"/>
-      <c r="YC84" s="68"/>
-      <c r="YD84" s="68"/>
-      <c r="YE84" s="68"/>
-      <c r="YF84" s="68"/>
-      <c r="YG84" s="68"/>
-      <c r="YH84" s="68"/>
-      <c r="YI84" s="68"/>
-      <c r="YJ84" s="68"/>
-      <c r="YK84" s="68"/>
-      <c r="YL84" s="68"/>
-      <c r="YM84" s="68"/>
-      <c r="YN84" s="68"/>
-      <c r="YO84" s="68"/>
-      <c r="YP84" s="68"/>
-      <c r="YQ84" s="68"/>
-      <c r="YR84" s="68"/>
-      <c r="YS84" s="68"/>
-      <c r="YT84" s="68"/>
-      <c r="YU84" s="68"/>
-      <c r="YV84" s="68"/>
-      <c r="YW84" s="68"/>
-      <c r="YX84" s="68"/>
-      <c r="YY84" s="68"/>
-      <c r="YZ84" s="68"/>
-      <c r="ZA84" s="68"/>
-      <c r="ZB84" s="68"/>
-      <c r="ZC84" s="68"/>
-      <c r="ZD84" s="68"/>
-      <c r="ZE84" s="68"/>
-      <c r="ZF84" s="68"/>
-      <c r="ZG84" s="68"/>
-      <c r="ZH84" s="68"/>
-      <c r="ZI84" s="68"/>
-      <c r="ZJ84" s="68"/>
-      <c r="ZK84" s="68"/>
-      <c r="ZL84" s="68"/>
-      <c r="ZM84" s="68"/>
-      <c r="ZN84" s="68"/>
-      <c r="ZO84" s="68"/>
-      <c r="ZP84" s="68"/>
-      <c r="ZQ84" s="68"/>
-      <c r="ZR84" s="68"/>
-      <c r="ZS84" s="68"/>
-      <c r="ZT84" s="68"/>
-      <c r="ZU84" s="68"/>
-      <c r="ZV84" s="68"/>
-      <c r="ZW84" s="68"/>
-      <c r="ZX84" s="68"/>
-      <c r="ZY84" s="68"/>
-      <c r="ZZ84" s="68"/>
-      <c r="AAA84" s="68"/>
-      <c r="AAB84" s="68"/>
-      <c r="AAC84" s="68"/>
-      <c r="AAD84" s="68"/>
-      <c r="AAE84" s="68"/>
-      <c r="AAF84" s="68"/>
-      <c r="AAG84" s="68"/>
-      <c r="AAH84" s="68"/>
-      <c r="AAI84" s="68"/>
-      <c r="AAJ84" s="68"/>
-      <c r="AAK84" s="68"/>
-      <c r="AAL84" s="68"/>
-      <c r="AAM84" s="68"/>
-      <c r="AAN84" s="68"/>
-      <c r="AAO84" s="68"/>
-      <c r="AAP84" s="68"/>
-      <c r="AAQ84" s="68"/>
-      <c r="AAR84" s="68"/>
-      <c r="AAS84" s="68"/>
-      <c r="AAT84" s="68"/>
-      <c r="AAU84" s="68"/>
-      <c r="AAV84" s="68"/>
-      <c r="AAW84" s="68"/>
-      <c r="AAX84" s="68"/>
-      <c r="AAY84" s="68"/>
-      <c r="AAZ84" s="68"/>
-      <c r="ABA84" s="68"/>
-      <c r="ABB84" s="68"/>
-      <c r="ABC84" s="68"/>
-      <c r="ABD84" s="68"/>
-      <c r="ABE84" s="68"/>
-      <c r="ABF84" s="68"/>
-      <c r="ABG84" s="68"/>
-      <c r="ABH84" s="68"/>
-      <c r="ABI84" s="68"/>
-      <c r="ABJ84" s="68"/>
-      <c r="ABK84" s="68"/>
-      <c r="ABL84" s="68"/>
-      <c r="ABM84" s="68"/>
-      <c r="ABN84" s="68"/>
-      <c r="ABO84" s="68"/>
-      <c r="ABP84" s="68"/>
-      <c r="ABQ84" s="68"/>
-      <c r="ABR84" s="68"/>
-      <c r="ABS84" s="68"/>
-      <c r="ABT84" s="68"/>
-      <c r="ABU84" s="68"/>
-      <c r="ABV84" s="68"/>
-      <c r="ABW84" s="68"/>
-      <c r="ABX84" s="68"/>
-      <c r="ABY84" s="68"/>
-      <c r="ABZ84" s="68"/>
-      <c r="ACA84" s="68"/>
-      <c r="ACB84" s="68"/>
-      <c r="ACC84" s="68"/>
-      <c r="ACD84" s="68"/>
-      <c r="ACE84" s="68"/>
-      <c r="ACF84" s="68"/>
-      <c r="ACG84" s="68"/>
-      <c r="ACH84" s="68"/>
-      <c r="ACI84" s="68"/>
-      <c r="ACJ84" s="68"/>
-      <c r="ACK84" s="68"/>
-      <c r="ACL84" s="68"/>
-      <c r="ACM84" s="68"/>
-      <c r="ACN84" s="68"/>
-      <c r="ACO84" s="68"/>
-      <c r="ACP84" s="68"/>
-      <c r="ACQ84" s="68"/>
-      <c r="ACR84" s="68"/>
-      <c r="ACS84" s="68"/>
-      <c r="ACT84" s="68"/>
-      <c r="ACU84" s="68"/>
-      <c r="ACV84" s="68"/>
-      <c r="ACW84" s="68"/>
-      <c r="ACX84" s="68"/>
-      <c r="ACY84" s="68"/>
-      <c r="ACZ84" s="68"/>
-      <c r="ADA84" s="68"/>
-      <c r="ADB84" s="68"/>
-      <c r="ADC84" s="68"/>
-      <c r="ADD84" s="68"/>
-      <c r="ADE84" s="68"/>
-      <c r="ADF84" s="68"/>
-      <c r="ADG84" s="68"/>
-      <c r="ADH84" s="68"/>
-      <c r="ADI84" s="68"/>
-      <c r="ADJ84" s="68"/>
-      <c r="ADK84" s="68"/>
-      <c r="ADL84" s="68"/>
-      <c r="ADM84" s="68"/>
-      <c r="ADN84" s="68"/>
-      <c r="ADO84" s="68"/>
-      <c r="ADP84" s="68"/>
-      <c r="ADQ84" s="68"/>
-      <c r="ADR84" s="68"/>
-      <c r="ADS84" s="68"/>
-      <c r="ADT84" s="68"/>
-      <c r="ADU84" s="68"/>
-      <c r="ADV84" s="68"/>
-      <c r="ADW84" s="68"/>
-      <c r="ADX84" s="68"/>
-      <c r="ADY84" s="68"/>
-      <c r="ADZ84" s="68"/>
-      <c r="AEA84" s="68"/>
-      <c r="AEB84" s="68"/>
-      <c r="AEC84" s="68"/>
-      <c r="AED84" s="68"/>
-      <c r="AEE84" s="68"/>
-      <c r="AEF84" s="68"/>
-      <c r="AEG84" s="68"/>
-      <c r="AEH84" s="68"/>
-      <c r="AEI84" s="68"/>
-      <c r="AEJ84" s="68"/>
-      <c r="AEK84" s="68"/>
-      <c r="AEL84" s="68"/>
-      <c r="AEM84" s="68"/>
-      <c r="AEN84" s="68"/>
-      <c r="AEO84" s="68"/>
-      <c r="AEP84" s="68"/>
-      <c r="AEQ84" s="68"/>
-      <c r="AER84" s="68"/>
-      <c r="AES84" s="68"/>
-      <c r="AET84" s="68"/>
-      <c r="AEU84" s="68"/>
-      <c r="AEV84" s="68"/>
-      <c r="AEW84" s="68"/>
-      <c r="AEX84" s="68"/>
-      <c r="AEY84" s="68"/>
-      <c r="AEZ84" s="68"/>
-      <c r="AFA84" s="68"/>
-      <c r="AFB84" s="68"/>
-      <c r="AFC84" s="68"/>
-      <c r="AFD84" s="68"/>
-      <c r="AFE84" s="68"/>
-      <c r="AFF84" s="68"/>
-      <c r="AFG84" s="68"/>
-      <c r="AFH84" s="68"/>
-      <c r="AFI84" s="68"/>
-      <c r="AFJ84" s="68"/>
-      <c r="AFK84" s="68"/>
-      <c r="AFL84" s="68"/>
-      <c r="AFM84" s="68"/>
-      <c r="AFN84" s="68"/>
-      <c r="AFO84" s="68"/>
-      <c r="AFP84" s="68"/>
-      <c r="AFQ84" s="68"/>
-      <c r="AFR84" s="68"/>
-      <c r="AFS84" s="68"/>
-      <c r="AFT84" s="68"/>
-      <c r="AFU84" s="68"/>
-      <c r="AFV84" s="68"/>
-      <c r="AFW84" s="68"/>
-      <c r="AFX84" s="68"/>
-      <c r="AFY84" s="68"/>
-      <c r="AFZ84" s="68"/>
-      <c r="AGA84" s="68"/>
-      <c r="AGB84" s="68"/>
-      <c r="AGC84" s="68"/>
-      <c r="AGD84" s="68"/>
-      <c r="AGE84" s="68"/>
-      <c r="AGF84" s="68"/>
-      <c r="AGG84" s="68"/>
-      <c r="AGH84" s="68"/>
-      <c r="AGI84" s="68"/>
-      <c r="AGJ84" s="68"/>
-      <c r="AGK84" s="68"/>
-      <c r="AGL84" s="68"/>
-      <c r="AGM84" s="68"/>
-      <c r="AGN84" s="68"/>
-      <c r="AGO84" s="68"/>
-      <c r="AGP84" s="68"/>
-      <c r="AGQ84" s="68"/>
-      <c r="AGR84" s="68"/>
-      <c r="AGS84" s="68"/>
-      <c r="AGT84" s="68"/>
-      <c r="AGU84" s="68"/>
-      <c r="AGV84" s="68"/>
-      <c r="AGW84" s="68"/>
-      <c r="AGX84" s="68"/>
-      <c r="AGY84" s="68"/>
-      <c r="AGZ84" s="68"/>
-      <c r="AHA84" s="68"/>
-      <c r="AHB84" s="68"/>
-      <c r="AHC84" s="68"/>
-      <c r="AHD84" s="68"/>
-      <c r="AHE84" s="68"/>
-      <c r="AHF84" s="68"/>
-      <c r="AHG84" s="68"/>
-      <c r="AHH84" s="68"/>
-      <c r="AHI84" s="68"/>
-      <c r="AHJ84" s="68"/>
-      <c r="AHK84" s="68"/>
-      <c r="AHL84" s="68"/>
-      <c r="AHM84" s="68"/>
-      <c r="AHN84" s="68"/>
-      <c r="AHO84" s="68"/>
-      <c r="AHP84" s="68"/>
-      <c r="AHQ84" s="68"/>
-      <c r="AHR84" s="68"/>
-      <c r="AHS84" s="68"/>
-      <c r="AHT84" s="68"/>
-      <c r="AHU84" s="68"/>
-      <c r="AHV84" s="68"/>
-      <c r="AHW84" s="68"/>
-      <c r="AHX84" s="68"/>
-      <c r="AHY84" s="68"/>
-      <c r="AHZ84" s="68"/>
-      <c r="AIA84" s="68"/>
-      <c r="AIB84" s="68"/>
-      <c r="AIC84" s="68"/>
-      <c r="AID84" s="68"/>
-      <c r="AIE84" s="68"/>
-      <c r="AIF84" s="68"/>
-      <c r="AIG84" s="68"/>
-      <c r="AIH84" s="68"/>
-      <c r="AII84" s="68"/>
-      <c r="AIJ84" s="68"/>
-      <c r="AIK84" s="68"/>
-      <c r="AIL84" s="68"/>
-      <c r="AIM84" s="68"/>
-      <c r="AIN84" s="68"/>
-      <c r="AIO84" s="68"/>
-      <c r="AIP84" s="68"/>
-      <c r="AIQ84" s="68"/>
-      <c r="AIR84" s="68"/>
-      <c r="AIS84" s="68"/>
-      <c r="AIT84" s="68"/>
-      <c r="AIU84" s="68"/>
-      <c r="AIV84" s="68"/>
-      <c r="AIW84" s="68"/>
-      <c r="AIX84" s="68"/>
-      <c r="AIY84" s="68"/>
-      <c r="AIZ84" s="68"/>
-      <c r="AJA84" s="68"/>
-      <c r="AJB84" s="68"/>
-      <c r="AJC84" s="68"/>
-      <c r="AJD84" s="68"/>
-      <c r="AJE84" s="68"/>
-      <c r="AJF84" s="68"/>
-      <c r="AJG84" s="68"/>
-      <c r="AJH84" s="68"/>
-      <c r="AJI84" s="68"/>
-      <c r="AJJ84" s="68"/>
-      <c r="AJK84" s="68"/>
-      <c r="AJL84" s="68"/>
-      <c r="AJM84" s="68"/>
-      <c r="AJN84" s="68"/>
-      <c r="AJO84" s="68"/>
-      <c r="AJP84" s="68"/>
-      <c r="AJQ84" s="68"/>
-      <c r="AJR84" s="68"/>
-      <c r="AJS84" s="68"/>
-      <c r="AJT84" s="68"/>
-      <c r="AJU84" s="68"/>
-      <c r="AJV84" s="68"/>
-      <c r="AJW84" s="68"/>
-      <c r="AJX84" s="68"/>
-      <c r="AJY84" s="68"/>
-      <c r="AJZ84" s="68"/>
-      <c r="AKA84" s="68"/>
-      <c r="AKB84" s="68"/>
-      <c r="AKC84" s="68"/>
-      <c r="AKD84" s="68"/>
-      <c r="AKE84" s="68"/>
-      <c r="AKF84" s="68"/>
-      <c r="AKG84" s="68"/>
-      <c r="AKH84" s="68"/>
-      <c r="AKI84" s="68"/>
-      <c r="AKJ84" s="68"/>
-      <c r="AKK84" s="68"/>
-      <c r="AKL84" s="68"/>
-      <c r="AKM84" s="68"/>
-      <c r="AKN84" s="68"/>
-      <c r="AKO84" s="68"/>
-      <c r="AKP84" s="68"/>
-      <c r="AKQ84" s="68"/>
-      <c r="AKR84" s="68"/>
-      <c r="AKS84" s="68"/>
-      <c r="AKT84" s="68"/>
-      <c r="AKU84" s="68"/>
-      <c r="AKV84" s="68"/>
-      <c r="AKW84" s="68"/>
-      <c r="AKX84" s="68"/>
-      <c r="AKY84" s="68"/>
-      <c r="AKZ84" s="68"/>
-      <c r="ALA84" s="68"/>
-      <c r="ALB84" s="68"/>
-      <c r="ALC84" s="68"/>
-      <c r="ALD84" s="68"/>
-      <c r="ALE84" s="68"/>
-      <c r="ALF84" s="68"/>
-      <c r="ALG84" s="68"/>
-      <c r="ALH84" s="68"/>
-      <c r="ALI84" s="68"/>
-      <c r="ALJ84" s="68"/>
-      <c r="ALK84" s="68"/>
-      <c r="ALL84" s="68"/>
-      <c r="ALM84" s="68"/>
-      <c r="ALN84" s="68"/>
-      <c r="ALO84" s="68"/>
-      <c r="ALP84" s="68"/>
-      <c r="ALQ84" s="68"/>
-      <c r="ALR84" s="68"/>
-      <c r="ALS84" s="68"/>
-      <c r="ALT84" s="68"/>
-      <c r="ALU84" s="68"/>
-      <c r="ALV84" s="68"/>
-      <c r="ALW84" s="68"/>
-      <c r="ALX84" s="68"/>
-      <c r="ALY84" s="68"/>
-      <c r="ALZ84" s="68"/>
-      <c r="AMA84" s="68"/>
-      <c r="AMB84" s="68"/>
-      <c r="AMC84" s="68"/>
-      <c r="AMD84" s="68"/>
-      <c r="AME84" s="68"/>
-      <c r="AMF84" s="68"/>
-      <c r="AMG84" s="68"/>
-      <c r="AMH84" s="68"/>
+      <c r="H84" s="66"/>
+      <c r="I84" s="67"/>
+      <c r="J84" s="67"/>
+      <c r="K84" s="67"/>
+      <c r="L84" s="67"/>
+      <c r="M84" s="67"/>
+      <c r="N84" s="67"/>
+      <c r="O84" s="67"/>
+      <c r="P84" s="67"/>
+      <c r="Q84" s="67"/>
+      <c r="R84" s="67"/>
+      <c r="S84" s="67"/>
+      <c r="T84" s="67"/>
+      <c r="U84" s="67"/>
+      <c r="V84" s="67"/>
+      <c r="W84" s="67"/>
+      <c r="X84" s="67"/>
+      <c r="Y84" s="67"/>
+      <c r="Z84" s="67"/>
+      <c r="AA84" s="67"/>
+      <c r="AB84" s="67"/>
+      <c r="AC84" s="67"/>
+      <c r="AD84" s="67"/>
+      <c r="AE84" s="67"/>
+      <c r="AF84" s="67"/>
+      <c r="AG84" s="67"/>
+      <c r="AH84" s="67"/>
+      <c r="AI84" s="67"/>
+      <c r="AJ84" s="67"/>
+      <c r="AK84" s="67"/>
+      <c r="AL84" s="67"/>
+      <c r="AM84" s="67"/>
+      <c r="AN84" s="67"/>
+      <c r="AO84" s="67"/>
+      <c r="AP84" s="67"/>
+      <c r="AQ84" s="67"/>
+      <c r="AR84" s="67"/>
+      <c r="AS84" s="67"/>
+      <c r="AT84" s="67"/>
+      <c r="AU84" s="67"/>
+      <c r="AV84" s="67"/>
+      <c r="AW84" s="67"/>
+      <c r="AX84" s="67"/>
+      <c r="AY84" s="67"/>
+      <c r="AZ84" s="67"/>
+      <c r="BA84" s="67"/>
+      <c r="BB84" s="67"/>
+      <c r="BC84" s="67"/>
+      <c r="BD84" s="67"/>
+      <c r="BE84" s="67"/>
+      <c r="BF84" s="67"/>
+      <c r="BG84" s="67"/>
+      <c r="BH84" s="67"/>
+      <c r="BI84" s="67"/>
+      <c r="BJ84" s="67"/>
+      <c r="BK84" s="67"/>
+      <c r="BL84" s="67"/>
+      <c r="BM84" s="67"/>
+      <c r="BN84" s="67"/>
+      <c r="BO84" s="67"/>
+      <c r="BP84" s="67"/>
+      <c r="BQ84" s="67"/>
+      <c r="BR84" s="67"/>
+      <c r="BS84" s="67"/>
+      <c r="BT84" s="67"/>
+      <c r="BU84" s="67"/>
+      <c r="BV84" s="67"/>
+      <c r="BW84" s="67"/>
+      <c r="BX84" s="67"/>
+      <c r="BY84" s="67"/>
+      <c r="BZ84" s="67"/>
+      <c r="CA84" s="67"/>
+      <c r="CB84" s="67"/>
+      <c r="CC84" s="67"/>
+      <c r="CD84" s="67"/>
+      <c r="CE84" s="67"/>
+      <c r="CF84" s="67"/>
+      <c r="CG84" s="67"/>
+      <c r="CH84" s="67"/>
+      <c r="CI84" s="67"/>
+      <c r="CJ84" s="67"/>
+      <c r="CK84" s="67"/>
+      <c r="CL84" s="67"/>
+      <c r="CM84" s="67"/>
+      <c r="CN84" s="67"/>
+      <c r="CO84" s="67"/>
+      <c r="CP84" s="67"/>
+      <c r="CQ84" s="67"/>
+      <c r="CR84" s="67"/>
+      <c r="CS84" s="67"/>
+      <c r="CT84" s="67"/>
+      <c r="CU84" s="67"/>
+      <c r="CV84" s="67"/>
+      <c r="CW84" s="67"/>
+      <c r="CX84" s="67"/>
+      <c r="CY84" s="67"/>
+      <c r="CZ84" s="67"/>
+      <c r="DA84" s="67"/>
+      <c r="DB84" s="67"/>
+      <c r="DC84" s="67"/>
+      <c r="DD84" s="67"/>
+      <c r="DE84" s="67"/>
+      <c r="DF84" s="67"/>
+      <c r="DG84" s="67"/>
+      <c r="DH84" s="67"/>
+      <c r="DI84" s="67"/>
+      <c r="DJ84" s="67"/>
+      <c r="DK84" s="67"/>
+      <c r="DL84" s="67"/>
+      <c r="DM84" s="67"/>
+      <c r="DN84" s="67"/>
+      <c r="DO84" s="67"/>
+      <c r="DP84" s="67"/>
+      <c r="DQ84" s="67"/>
+      <c r="DR84" s="67"/>
+      <c r="DS84" s="67"/>
+      <c r="DT84" s="67"/>
+      <c r="DU84" s="67"/>
+      <c r="DV84" s="67"/>
+      <c r="DW84" s="67"/>
+      <c r="DX84" s="67"/>
+      <c r="DY84" s="67"/>
+      <c r="DZ84" s="67"/>
+      <c r="EA84" s="67"/>
+      <c r="EB84" s="67"/>
+      <c r="EC84" s="67"/>
+      <c r="ED84" s="67"/>
+      <c r="EE84" s="67"/>
+      <c r="EF84" s="67"/>
+      <c r="EG84" s="67"/>
+      <c r="EH84" s="67"/>
+      <c r="EI84" s="67"/>
+      <c r="EJ84" s="67"/>
+      <c r="EK84" s="67"/>
+      <c r="EL84" s="67"/>
+      <c r="EM84" s="67"/>
+      <c r="EN84" s="67"/>
+      <c r="EO84" s="67"/>
+      <c r="EP84" s="67"/>
+      <c r="EQ84" s="67"/>
+      <c r="ER84" s="67"/>
+      <c r="ES84" s="67"/>
+      <c r="ET84" s="67"/>
+      <c r="EU84" s="67"/>
+      <c r="EV84" s="67"/>
+      <c r="EW84" s="67"/>
+      <c r="EX84" s="67"/>
+      <c r="EY84" s="67"/>
+      <c r="EZ84" s="67"/>
+      <c r="FA84" s="67"/>
+      <c r="FB84" s="67"/>
+      <c r="FC84" s="67"/>
+      <c r="FD84" s="67"/>
+      <c r="FE84" s="67"/>
+      <c r="FF84" s="67"/>
+      <c r="FG84" s="67"/>
+      <c r="FH84" s="67"/>
+      <c r="FI84" s="67"/>
+      <c r="FJ84" s="67"/>
+      <c r="FK84" s="67"/>
+      <c r="FL84" s="67"/>
+      <c r="FM84" s="67"/>
+      <c r="FN84" s="67"/>
+      <c r="FO84" s="67"/>
+      <c r="FP84" s="67"/>
+      <c r="FQ84" s="67"/>
+      <c r="FR84" s="67"/>
+      <c r="FS84" s="67"/>
+      <c r="FT84" s="67"/>
+      <c r="FU84" s="67"/>
+      <c r="FV84" s="67"/>
+      <c r="FW84" s="67"/>
+      <c r="FX84" s="67"/>
+      <c r="FY84" s="67"/>
+      <c r="FZ84" s="67"/>
+      <c r="GA84" s="67"/>
+      <c r="GB84" s="67"/>
+      <c r="GC84" s="67"/>
+      <c r="GD84" s="67"/>
+      <c r="GE84" s="67"/>
+      <c r="GF84" s="67"/>
+      <c r="GG84" s="67"/>
+      <c r="GH84" s="67"/>
+      <c r="GI84" s="67"/>
+      <c r="GJ84" s="67"/>
+      <c r="GK84" s="67"/>
+      <c r="GL84" s="67"/>
+      <c r="GM84" s="67"/>
+      <c r="GN84" s="67"/>
+      <c r="GO84" s="67"/>
+      <c r="GP84" s="67"/>
+      <c r="GQ84" s="67"/>
+      <c r="GR84" s="67"/>
+      <c r="GS84" s="67"/>
+      <c r="GT84" s="67"/>
+      <c r="GU84" s="67"/>
+      <c r="GV84" s="67"/>
+      <c r="GW84" s="67"/>
+      <c r="GX84" s="67"/>
+      <c r="GY84" s="67"/>
+      <c r="GZ84" s="67"/>
+      <c r="HA84" s="67"/>
+      <c r="HB84" s="67"/>
+      <c r="HC84" s="67"/>
+      <c r="HD84" s="67"/>
+      <c r="HE84" s="67"/>
+      <c r="HF84" s="67"/>
+      <c r="HG84" s="67"/>
+      <c r="HH84" s="67"/>
+      <c r="HI84" s="67"/>
+      <c r="HJ84" s="67"/>
+      <c r="HK84" s="67"/>
+      <c r="HL84" s="67"/>
+      <c r="HM84" s="67"/>
+      <c r="HN84" s="67"/>
+      <c r="HO84" s="67"/>
+      <c r="HP84" s="67"/>
+      <c r="HQ84" s="67"/>
+      <c r="HR84" s="67"/>
+      <c r="HS84" s="67"/>
+      <c r="HT84" s="67"/>
+      <c r="HU84" s="67"/>
+      <c r="HV84" s="67"/>
+      <c r="HW84" s="67"/>
+      <c r="HX84" s="67"/>
+      <c r="HY84" s="67"/>
+      <c r="HZ84" s="67"/>
+      <c r="IA84" s="67"/>
+      <c r="IB84" s="67"/>
+      <c r="IC84" s="67"/>
+      <c r="ID84" s="67"/>
+      <c r="IE84" s="67"/>
+      <c r="IF84" s="67"/>
+      <c r="IG84" s="67"/>
+      <c r="IH84" s="67"/>
+      <c r="II84" s="67"/>
+      <c r="IJ84" s="67"/>
+      <c r="IK84" s="67"/>
+      <c r="IL84" s="67"/>
+      <c r="IM84" s="67"/>
+      <c r="IN84" s="67"/>
+      <c r="IO84" s="67"/>
+      <c r="IP84" s="67"/>
+      <c r="IQ84" s="67"/>
+      <c r="IR84" s="67"/>
+      <c r="IS84" s="67"/>
+      <c r="IT84" s="67"/>
+      <c r="IU84" s="67"/>
+      <c r="IV84" s="67"/>
+      <c r="IW84" s="67"/>
+      <c r="IX84" s="67"/>
+      <c r="IY84" s="67"/>
+      <c r="IZ84" s="67"/>
+      <c r="JA84" s="67"/>
+      <c r="JB84" s="67"/>
+      <c r="JC84" s="67"/>
+      <c r="JD84" s="67"/>
+      <c r="JE84" s="67"/>
+      <c r="JF84" s="67"/>
+      <c r="JG84" s="67"/>
+      <c r="JH84" s="67"/>
+      <c r="JI84" s="67"/>
+      <c r="JJ84" s="67"/>
+      <c r="JK84" s="67"/>
+      <c r="JL84" s="67"/>
+      <c r="JM84" s="67"/>
+      <c r="JN84" s="67"/>
+      <c r="JO84" s="67"/>
+      <c r="JP84" s="67"/>
+      <c r="JQ84" s="67"/>
+      <c r="JR84" s="67"/>
+      <c r="JS84" s="67"/>
+      <c r="JT84" s="67"/>
+      <c r="JU84" s="67"/>
+      <c r="JV84" s="67"/>
+      <c r="JW84" s="67"/>
+      <c r="JX84" s="67"/>
+      <c r="JY84" s="67"/>
+      <c r="JZ84" s="67"/>
+      <c r="KA84" s="67"/>
+      <c r="KB84" s="67"/>
+      <c r="KC84" s="67"/>
+      <c r="KD84" s="67"/>
+      <c r="KE84" s="67"/>
+      <c r="KF84" s="67"/>
+      <c r="KG84" s="67"/>
+      <c r="KH84" s="67"/>
+      <c r="KI84" s="67"/>
+      <c r="KJ84" s="67"/>
+      <c r="KK84" s="67"/>
+      <c r="KL84" s="67"/>
+      <c r="KM84" s="67"/>
+      <c r="KN84" s="67"/>
+      <c r="KO84" s="67"/>
+      <c r="KP84" s="67"/>
+      <c r="KQ84" s="67"/>
+      <c r="KR84" s="67"/>
+      <c r="KS84" s="67"/>
+      <c r="KT84" s="67"/>
+      <c r="KU84" s="67"/>
+      <c r="KV84" s="67"/>
+      <c r="KW84" s="67"/>
+      <c r="KX84" s="67"/>
+      <c r="KY84" s="67"/>
+      <c r="KZ84" s="67"/>
+      <c r="LA84" s="67"/>
+      <c r="LB84" s="67"/>
+      <c r="LC84" s="67"/>
+      <c r="LD84" s="67"/>
+      <c r="LE84" s="67"/>
+      <c r="LF84" s="67"/>
+      <c r="LG84" s="67"/>
+      <c r="LH84" s="67"/>
+      <c r="LI84" s="67"/>
+      <c r="LJ84" s="67"/>
+      <c r="LK84" s="67"/>
+      <c r="LL84" s="67"/>
+      <c r="LM84" s="67"/>
+      <c r="LN84" s="67"/>
+      <c r="LO84" s="67"/>
+      <c r="LP84" s="67"/>
+      <c r="LQ84" s="67"/>
+      <c r="LR84" s="67"/>
+      <c r="LS84" s="67"/>
+      <c r="LT84" s="67"/>
+      <c r="LU84" s="67"/>
+      <c r="LV84" s="67"/>
+      <c r="LW84" s="67"/>
+      <c r="LX84" s="67"/>
+      <c r="LY84" s="67"/>
+      <c r="LZ84" s="67"/>
+      <c r="MA84" s="67"/>
+      <c r="MB84" s="67"/>
+      <c r="MC84" s="67"/>
+      <c r="MD84" s="67"/>
+      <c r="ME84" s="67"/>
+      <c r="MF84" s="67"/>
+      <c r="MG84" s="67"/>
+      <c r="MH84" s="67"/>
+      <c r="MI84" s="67"/>
+      <c r="MJ84" s="67"/>
+      <c r="MK84" s="67"/>
+      <c r="ML84" s="67"/>
+      <c r="MM84" s="67"/>
+      <c r="MN84" s="67"/>
+      <c r="MO84" s="67"/>
+      <c r="MP84" s="67"/>
+      <c r="MQ84" s="67"/>
+      <c r="MR84" s="67"/>
+      <c r="MS84" s="67"/>
+      <c r="MT84" s="67"/>
+      <c r="MU84" s="67"/>
+      <c r="MV84" s="67"/>
+      <c r="MW84" s="67"/>
+      <c r="MX84" s="67"/>
+      <c r="MY84" s="67"/>
+      <c r="MZ84" s="67"/>
+      <c r="NA84" s="67"/>
+      <c r="NB84" s="67"/>
+      <c r="NC84" s="67"/>
+      <c r="ND84" s="67"/>
+      <c r="NE84" s="67"/>
+      <c r="NF84" s="67"/>
+      <c r="NG84" s="67"/>
+      <c r="NH84" s="67"/>
+      <c r="NI84" s="67"/>
+      <c r="NJ84" s="67"/>
+      <c r="NK84" s="67"/>
+      <c r="NL84" s="67"/>
+      <c r="NM84" s="67"/>
+      <c r="NN84" s="67"/>
+      <c r="NO84" s="67"/>
+      <c r="NP84" s="67"/>
+      <c r="NQ84" s="67"/>
+      <c r="NR84" s="67"/>
+      <c r="NS84" s="67"/>
+      <c r="NT84" s="67"/>
+      <c r="NU84" s="67"/>
+      <c r="NV84" s="67"/>
+      <c r="NW84" s="67"/>
+      <c r="NX84" s="67"/>
+      <c r="NY84" s="67"/>
+      <c r="NZ84" s="67"/>
+      <c r="OA84" s="67"/>
+      <c r="OB84" s="67"/>
+      <c r="OC84" s="67"/>
+      <c r="OD84" s="67"/>
+      <c r="OE84" s="67"/>
+      <c r="OF84" s="67"/>
+      <c r="OG84" s="67"/>
+      <c r="OH84" s="67"/>
+      <c r="OI84" s="67"/>
+      <c r="OJ84" s="67"/>
+      <c r="OK84" s="67"/>
+      <c r="OL84" s="67"/>
+      <c r="OM84" s="67"/>
+      <c r="ON84" s="67"/>
+      <c r="OO84" s="67"/>
+      <c r="OP84" s="67"/>
+      <c r="OQ84" s="67"/>
+      <c r="OR84" s="67"/>
+      <c r="OS84" s="67"/>
+      <c r="OT84" s="67"/>
+      <c r="OU84" s="67"/>
+      <c r="OV84" s="67"/>
+      <c r="OW84" s="67"/>
+      <c r="OX84" s="67"/>
+      <c r="OY84" s="67"/>
+      <c r="OZ84" s="67"/>
+      <c r="PA84" s="67"/>
+      <c r="PB84" s="67"/>
+      <c r="PC84" s="67"/>
+      <c r="PD84" s="67"/>
+      <c r="PE84" s="67"/>
+      <c r="PF84" s="67"/>
+      <c r="PG84" s="67"/>
+      <c r="PH84" s="67"/>
+      <c r="PI84" s="67"/>
+      <c r="PJ84" s="67"/>
+      <c r="PK84" s="67"/>
+      <c r="PL84" s="67"/>
+      <c r="PM84" s="67"/>
+      <c r="PN84" s="67"/>
+      <c r="PO84" s="67"/>
+      <c r="PP84" s="67"/>
+      <c r="PQ84" s="67"/>
+      <c r="PR84" s="67"/>
+      <c r="PS84" s="67"/>
+      <c r="PT84" s="67"/>
+      <c r="PU84" s="67"/>
+      <c r="PV84" s="67"/>
+      <c r="PW84" s="67"/>
+      <c r="PX84" s="67"/>
+      <c r="PY84" s="67"/>
+      <c r="PZ84" s="67"/>
+      <c r="QA84" s="67"/>
+      <c r="QB84" s="67"/>
+      <c r="QC84" s="67"/>
+      <c r="QD84" s="67"/>
+      <c r="QE84" s="67"/>
+      <c r="QF84" s="67"/>
+      <c r="QG84" s="67"/>
+      <c r="QH84" s="67"/>
+      <c r="QI84" s="67"/>
+      <c r="QJ84" s="67"/>
+      <c r="QK84" s="67"/>
+      <c r="QL84" s="67"/>
+      <c r="QM84" s="67"/>
+      <c r="QN84" s="67"/>
+      <c r="QO84" s="67"/>
+      <c r="QP84" s="67"/>
+      <c r="QQ84" s="67"/>
+      <c r="QR84" s="67"/>
+      <c r="QS84" s="67"/>
+      <c r="QT84" s="67"/>
+      <c r="QU84" s="67"/>
+      <c r="QV84" s="67"/>
+      <c r="QW84" s="67"/>
+      <c r="QX84" s="67"/>
+      <c r="QY84" s="67"/>
+      <c r="QZ84" s="67"/>
+      <c r="RA84" s="67"/>
+      <c r="RB84" s="67"/>
+      <c r="RC84" s="67"/>
+      <c r="RD84" s="67"/>
+      <c r="RE84" s="67"/>
+      <c r="RF84" s="67"/>
+      <c r="RG84" s="67"/>
+      <c r="RH84" s="67"/>
+      <c r="RI84" s="67"/>
+      <c r="RJ84" s="67"/>
+      <c r="RK84" s="67"/>
+      <c r="RL84" s="67"/>
+      <c r="RM84" s="67"/>
+      <c r="RN84" s="67"/>
+      <c r="RO84" s="67"/>
+      <c r="RP84" s="67"/>
+      <c r="RQ84" s="67"/>
+      <c r="RR84" s="67"/>
+      <c r="RS84" s="67"/>
+      <c r="RT84" s="67"/>
+      <c r="RU84" s="67"/>
+      <c r="RV84" s="67"/>
+      <c r="RW84" s="67"/>
+      <c r="RX84" s="67"/>
+      <c r="RY84" s="67"/>
+      <c r="RZ84" s="67"/>
+      <c r="SA84" s="67"/>
+      <c r="SB84" s="67"/>
+      <c r="SC84" s="67"/>
+      <c r="SD84" s="67"/>
+      <c r="SE84" s="67"/>
+      <c r="SF84" s="67"/>
+      <c r="SG84" s="67"/>
+      <c r="SH84" s="67"/>
+      <c r="SI84" s="67"/>
+      <c r="SJ84" s="67"/>
+      <c r="SK84" s="67"/>
+      <c r="SL84" s="67"/>
+      <c r="SM84" s="67"/>
+      <c r="SN84" s="67"/>
+      <c r="SO84" s="67"/>
+      <c r="SP84" s="67"/>
+      <c r="SQ84" s="67"/>
+      <c r="SR84" s="67"/>
+      <c r="SS84" s="67"/>
+      <c r="ST84" s="67"/>
+      <c r="SU84" s="67"/>
+      <c r="SV84" s="67"/>
+      <c r="SW84" s="67"/>
+      <c r="SX84" s="67"/>
+      <c r="SY84" s="67"/>
+      <c r="SZ84" s="67"/>
+      <c r="TA84" s="67"/>
+      <c r="TB84" s="67"/>
+      <c r="TC84" s="67"/>
+      <c r="TD84" s="67"/>
+      <c r="TE84" s="67"/>
+      <c r="TF84" s="67"/>
+      <c r="TG84" s="67"/>
+      <c r="TH84" s="67"/>
+      <c r="TI84" s="67"/>
+      <c r="TJ84" s="67"/>
+      <c r="TK84" s="67"/>
+      <c r="TL84" s="67"/>
+      <c r="TM84" s="67"/>
+      <c r="TN84" s="67"/>
+      <c r="TO84" s="67"/>
+      <c r="TP84" s="67"/>
+      <c r="TQ84" s="67"/>
+      <c r="TR84" s="67"/>
+      <c r="TS84" s="67"/>
+      <c r="TT84" s="67"/>
+      <c r="TU84" s="67"/>
+      <c r="TV84" s="67"/>
+      <c r="TW84" s="67"/>
+      <c r="TX84" s="67"/>
+      <c r="TY84" s="67"/>
+      <c r="TZ84" s="67"/>
+      <c r="UA84" s="67"/>
+      <c r="UB84" s="67"/>
+      <c r="UC84" s="67"/>
+      <c r="UD84" s="67"/>
+      <c r="UE84" s="67"/>
+      <c r="UF84" s="67"/>
+      <c r="UG84" s="67"/>
+      <c r="UH84" s="67"/>
+      <c r="UI84" s="67"/>
+      <c r="UJ84" s="67"/>
+      <c r="UK84" s="67"/>
+      <c r="UL84" s="67"/>
+      <c r="UM84" s="67"/>
+      <c r="UN84" s="67"/>
+      <c r="UO84" s="67"/>
+      <c r="UP84" s="67"/>
+      <c r="UQ84" s="67"/>
+      <c r="UR84" s="67"/>
+      <c r="US84" s="67"/>
+      <c r="UT84" s="67"/>
+      <c r="UU84" s="67"/>
+      <c r="UV84" s="67"/>
+      <c r="UW84" s="67"/>
+      <c r="UX84" s="67"/>
+      <c r="UY84" s="67"/>
+      <c r="UZ84" s="67"/>
+      <c r="VA84" s="67"/>
+      <c r="VB84" s="67"/>
+      <c r="VC84" s="67"/>
+      <c r="VD84" s="67"/>
+      <c r="VE84" s="67"/>
+      <c r="VF84" s="67"/>
+      <c r="VG84" s="67"/>
+      <c r="VH84" s="67"/>
+      <c r="VI84" s="67"/>
+      <c r="VJ84" s="67"/>
+      <c r="VK84" s="67"/>
+      <c r="VL84" s="67"/>
+      <c r="VM84" s="67"/>
+      <c r="VN84" s="67"/>
+      <c r="VO84" s="67"/>
+      <c r="VP84" s="67"/>
+      <c r="VQ84" s="67"/>
+      <c r="VR84" s="67"/>
+      <c r="VS84" s="67"/>
+      <c r="VT84" s="67"/>
+      <c r="VU84" s="67"/>
+      <c r="VV84" s="67"/>
+      <c r="VW84" s="67"/>
+      <c r="VX84" s="67"/>
+      <c r="VY84" s="67"/>
+      <c r="VZ84" s="67"/>
+      <c r="WA84" s="67"/>
+      <c r="WB84" s="67"/>
+      <c r="WC84" s="67"/>
+      <c r="WD84" s="67"/>
+      <c r="WE84" s="67"/>
+      <c r="WF84" s="67"/>
+      <c r="WG84" s="67"/>
+      <c r="WH84" s="67"/>
+      <c r="WI84" s="67"/>
+      <c r="WJ84" s="67"/>
+      <c r="WK84" s="67"/>
+      <c r="WL84" s="67"/>
+      <c r="WM84" s="67"/>
+      <c r="WN84" s="67"/>
+      <c r="WO84" s="67"/>
+      <c r="WP84" s="67"/>
+      <c r="WQ84" s="67"/>
+      <c r="WR84" s="67"/>
+      <c r="WS84" s="67"/>
+      <c r="WT84" s="67"/>
+      <c r="WU84" s="67"/>
+      <c r="WV84" s="67"/>
+      <c r="WW84" s="67"/>
+      <c r="WX84" s="67"/>
+      <c r="WY84" s="67"/>
+      <c r="WZ84" s="67"/>
+      <c r="XA84" s="67"/>
+      <c r="XB84" s="67"/>
+      <c r="XC84" s="67"/>
+      <c r="XD84" s="67"/>
+      <c r="XE84" s="67"/>
+      <c r="XF84" s="67"/>
+      <c r="XG84" s="67"/>
+      <c r="XH84" s="67"/>
+      <c r="XI84" s="67"/>
+      <c r="XJ84" s="67"/>
+      <c r="XK84" s="67"/>
+      <c r="XL84" s="67"/>
+      <c r="XM84" s="67"/>
+      <c r="XN84" s="67"/>
+      <c r="XO84" s="67"/>
+      <c r="XP84" s="67"/>
+      <c r="XQ84" s="67"/>
+      <c r="XR84" s="67"/>
+      <c r="XS84" s="67"/>
+      <c r="XT84" s="67"/>
+      <c r="XU84" s="67"/>
+      <c r="XV84" s="67"/>
+      <c r="XW84" s="67"/>
+      <c r="XX84" s="67"/>
+      <c r="XY84" s="67"/>
+      <c r="XZ84" s="67"/>
+      <c r="YA84" s="67"/>
+      <c r="YB84" s="67"/>
+      <c r="YC84" s="67"/>
+      <c r="YD84" s="67"/>
+      <c r="YE84" s="67"/>
+      <c r="YF84" s="67"/>
+      <c r="YG84" s="67"/>
+      <c r="YH84" s="67"/>
+      <c r="YI84" s="67"/>
+      <c r="YJ84" s="67"/>
+      <c r="YK84" s="67"/>
+      <c r="YL84" s="67"/>
+      <c r="YM84" s="67"/>
+      <c r="YN84" s="67"/>
+      <c r="YO84" s="67"/>
+      <c r="YP84" s="67"/>
+      <c r="YQ84" s="67"/>
+      <c r="YR84" s="67"/>
+      <c r="YS84" s="67"/>
+      <c r="YT84" s="67"/>
+      <c r="YU84" s="67"/>
+      <c r="YV84" s="67"/>
+      <c r="YW84" s="67"/>
+      <c r="YX84" s="67"/>
+      <c r="YY84" s="67"/>
+      <c r="YZ84" s="67"/>
+      <c r="ZA84" s="67"/>
+      <c r="ZB84" s="67"/>
+      <c r="ZC84" s="67"/>
+      <c r="ZD84" s="67"/>
+      <c r="ZE84" s="67"/>
+      <c r="ZF84" s="67"/>
+      <c r="ZG84" s="67"/>
+      <c r="ZH84" s="67"/>
+      <c r="ZI84" s="67"/>
+      <c r="ZJ84" s="67"/>
+      <c r="ZK84" s="67"/>
+      <c r="ZL84" s="67"/>
+      <c r="ZM84" s="67"/>
+      <c r="ZN84" s="67"/>
+      <c r="ZO84" s="67"/>
+      <c r="ZP84" s="67"/>
+      <c r="ZQ84" s="67"/>
+      <c r="ZR84" s="67"/>
+      <c r="ZS84" s="67"/>
+      <c r="ZT84" s="67"/>
+      <c r="ZU84" s="67"/>
+      <c r="ZV84" s="67"/>
+      <c r="ZW84" s="67"/>
+      <c r="ZX84" s="67"/>
+      <c r="ZY84" s="67"/>
+      <c r="ZZ84" s="67"/>
+      <c r="AAA84" s="67"/>
+      <c r="AAB84" s="67"/>
+      <c r="AAC84" s="67"/>
+      <c r="AAD84" s="67"/>
+      <c r="AAE84" s="67"/>
+      <c r="AAF84" s="67"/>
+      <c r="AAG84" s="67"/>
+      <c r="AAH84" s="67"/>
+      <c r="AAI84" s="67"/>
+      <c r="AAJ84" s="67"/>
+      <c r="AAK84" s="67"/>
+      <c r="AAL84" s="67"/>
+      <c r="AAM84" s="67"/>
+      <c r="AAN84" s="67"/>
+      <c r="AAO84" s="67"/>
+      <c r="AAP84" s="67"/>
+      <c r="AAQ84" s="67"/>
+      <c r="AAR84" s="67"/>
+      <c r="AAS84" s="67"/>
+      <c r="AAT84" s="67"/>
+      <c r="AAU84" s="67"/>
+      <c r="AAV84" s="67"/>
+      <c r="AAW84" s="67"/>
+      <c r="AAX84" s="67"/>
+      <c r="AAY84" s="67"/>
+      <c r="AAZ84" s="67"/>
+      <c r="ABA84" s="67"/>
+      <c r="ABB84" s="67"/>
+      <c r="ABC84" s="67"/>
+      <c r="ABD84" s="67"/>
+      <c r="ABE84" s="67"/>
+      <c r="ABF84" s="67"/>
+      <c r="ABG84" s="67"/>
+      <c r="ABH84" s="67"/>
+      <c r="ABI84" s="67"/>
+      <c r="ABJ84" s="67"/>
+      <c r="ABK84" s="67"/>
+      <c r="ABL84" s="67"/>
+      <c r="ABM84" s="67"/>
+      <c r="ABN84" s="67"/>
+      <c r="ABO84" s="67"/>
+      <c r="ABP84" s="67"/>
+      <c r="ABQ84" s="67"/>
+      <c r="ABR84" s="67"/>
+      <c r="ABS84" s="67"/>
+      <c r="ABT84" s="67"/>
+      <c r="ABU84" s="67"/>
+      <c r="ABV84" s="67"/>
+      <c r="ABW84" s="67"/>
+      <c r="ABX84" s="67"/>
+      <c r="ABY84" s="67"/>
+      <c r="ABZ84" s="67"/>
+      <c r="ACA84" s="67"/>
+      <c r="ACB84" s="67"/>
+      <c r="ACC84" s="67"/>
+      <c r="ACD84" s="67"/>
+      <c r="ACE84" s="67"/>
+      <c r="ACF84" s="67"/>
+      <c r="ACG84" s="67"/>
+      <c r="ACH84" s="67"/>
+      <c r="ACI84" s="67"/>
+      <c r="ACJ84" s="67"/>
+      <c r="ACK84" s="67"/>
+      <c r="ACL84" s="67"/>
+      <c r="ACM84" s="67"/>
+      <c r="ACN84" s="67"/>
+      <c r="ACO84" s="67"/>
+      <c r="ACP84" s="67"/>
+      <c r="ACQ84" s="67"/>
+      <c r="ACR84" s="67"/>
+      <c r="ACS84" s="67"/>
+      <c r="ACT84" s="67"/>
+      <c r="ACU84" s="67"/>
+      <c r="ACV84" s="67"/>
+      <c r="ACW84" s="67"/>
+      <c r="ACX84" s="67"/>
+      <c r="ACY84" s="67"/>
+      <c r="ACZ84" s="67"/>
+      <c r="ADA84" s="67"/>
+      <c r="ADB84" s="67"/>
+      <c r="ADC84" s="67"/>
+      <c r="ADD84" s="67"/>
+      <c r="ADE84" s="67"/>
+      <c r="ADF84" s="67"/>
+      <c r="ADG84" s="67"/>
+      <c r="ADH84" s="67"/>
+      <c r="ADI84" s="67"/>
+      <c r="ADJ84" s="67"/>
+      <c r="ADK84" s="67"/>
+      <c r="ADL84" s="67"/>
+      <c r="ADM84" s="67"/>
+      <c r="ADN84" s="67"/>
+      <c r="ADO84" s="67"/>
+      <c r="ADP84" s="67"/>
+      <c r="ADQ84" s="67"/>
+      <c r="ADR84" s="67"/>
+      <c r="ADS84" s="67"/>
+      <c r="ADT84" s="67"/>
+      <c r="ADU84" s="67"/>
+      <c r="ADV84" s="67"/>
+      <c r="ADW84" s="67"/>
+      <c r="ADX84" s="67"/>
+      <c r="ADY84" s="67"/>
+      <c r="ADZ84" s="67"/>
+      <c r="AEA84" s="67"/>
+      <c r="AEB84" s="67"/>
+      <c r="AEC84" s="67"/>
+      <c r="AED84" s="67"/>
+      <c r="AEE84" s="67"/>
+      <c r="AEF84" s="67"/>
+      <c r="AEG84" s="67"/>
+      <c r="AEH84" s="67"/>
+      <c r="AEI84" s="67"/>
+      <c r="AEJ84" s="67"/>
+      <c r="AEK84" s="67"/>
+      <c r="AEL84" s="67"/>
+      <c r="AEM84" s="67"/>
+      <c r="AEN84" s="67"/>
+      <c r="AEO84" s="67"/>
+      <c r="AEP84" s="67"/>
+      <c r="AEQ84" s="67"/>
+      <c r="AER84" s="67"/>
+      <c r="AES84" s="67"/>
+      <c r="AET84" s="67"/>
+      <c r="AEU84" s="67"/>
+      <c r="AEV84" s="67"/>
+      <c r="AEW84" s="67"/>
+      <c r="AEX84" s="67"/>
+      <c r="AEY84" s="67"/>
+      <c r="AEZ84" s="67"/>
+      <c r="AFA84" s="67"/>
+      <c r="AFB84" s="67"/>
+      <c r="AFC84" s="67"/>
+      <c r="AFD84" s="67"/>
+      <c r="AFE84" s="67"/>
+      <c r="AFF84" s="67"/>
+      <c r="AFG84" s="67"/>
+      <c r="AFH84" s="67"/>
+      <c r="AFI84" s="67"/>
+      <c r="AFJ84" s="67"/>
+      <c r="AFK84" s="67"/>
+      <c r="AFL84" s="67"/>
+      <c r="AFM84" s="67"/>
+      <c r="AFN84" s="67"/>
+      <c r="AFO84" s="67"/>
+      <c r="AFP84" s="67"/>
+      <c r="AFQ84" s="67"/>
+      <c r="AFR84" s="67"/>
+      <c r="AFS84" s="67"/>
+      <c r="AFT84" s="67"/>
+      <c r="AFU84" s="67"/>
+      <c r="AFV84" s="67"/>
+      <c r="AFW84" s="67"/>
+      <c r="AFX84" s="67"/>
+      <c r="AFY84" s="67"/>
+      <c r="AFZ84" s="67"/>
+      <c r="AGA84" s="67"/>
+      <c r="AGB84" s="67"/>
+      <c r="AGC84" s="67"/>
+      <c r="AGD84" s="67"/>
+      <c r="AGE84" s="67"/>
+      <c r="AGF84" s="67"/>
+      <c r="AGG84" s="67"/>
+      <c r="AGH84" s="67"/>
+      <c r="AGI84" s="67"/>
+      <c r="AGJ84" s="67"/>
+      <c r="AGK84" s="67"/>
+      <c r="AGL84" s="67"/>
+      <c r="AGM84" s="67"/>
+      <c r="AGN84" s="67"/>
+      <c r="AGO84" s="67"/>
+      <c r="AGP84" s="67"/>
+      <c r="AGQ84" s="67"/>
+      <c r="AGR84" s="67"/>
+      <c r="AGS84" s="67"/>
+      <c r="AGT84" s="67"/>
+      <c r="AGU84" s="67"/>
+      <c r="AGV84" s="67"/>
+      <c r="AGW84" s="67"/>
+      <c r="AGX84" s="67"/>
+      <c r="AGY84" s="67"/>
+      <c r="AGZ84" s="67"/>
+      <c r="AHA84" s="67"/>
+      <c r="AHB84" s="67"/>
+      <c r="AHC84" s="67"/>
+      <c r="AHD84" s="67"/>
+      <c r="AHE84" s="67"/>
+      <c r="AHF84" s="67"/>
+      <c r="AHG84" s="67"/>
+      <c r="AHH84" s="67"/>
+      <c r="AHI84" s="67"/>
+      <c r="AHJ84" s="67"/>
+      <c r="AHK84" s="67"/>
+      <c r="AHL84" s="67"/>
+      <c r="AHM84" s="67"/>
+      <c r="AHN84" s="67"/>
+      <c r="AHO84" s="67"/>
+      <c r="AHP84" s="67"/>
+      <c r="AHQ84" s="67"/>
+      <c r="AHR84" s="67"/>
+      <c r="AHS84" s="67"/>
+      <c r="AHT84" s="67"/>
+      <c r="AHU84" s="67"/>
+      <c r="AHV84" s="67"/>
+      <c r="AHW84" s="67"/>
+      <c r="AHX84" s="67"/>
+      <c r="AHY84" s="67"/>
+      <c r="AHZ84" s="67"/>
+      <c r="AIA84" s="67"/>
+      <c r="AIB84" s="67"/>
+      <c r="AIC84" s="67"/>
+      <c r="AID84" s="67"/>
+      <c r="AIE84" s="67"/>
+      <c r="AIF84" s="67"/>
+      <c r="AIG84" s="67"/>
+      <c r="AIH84" s="67"/>
+      <c r="AII84" s="67"/>
+      <c r="AIJ84" s="67"/>
+      <c r="AIK84" s="67"/>
+      <c r="AIL84" s="67"/>
+      <c r="AIM84" s="67"/>
+      <c r="AIN84" s="67"/>
+      <c r="AIO84" s="67"/>
+      <c r="AIP84" s="67"/>
+      <c r="AIQ84" s="67"/>
+      <c r="AIR84" s="67"/>
+      <c r="AIS84" s="67"/>
+      <c r="AIT84" s="67"/>
+      <c r="AIU84" s="67"/>
+      <c r="AIV84" s="67"/>
+      <c r="AIW84" s="67"/>
+      <c r="AIX84" s="67"/>
+      <c r="AIY84" s="67"/>
+      <c r="AIZ84" s="67"/>
+      <c r="AJA84" s="67"/>
+      <c r="AJB84" s="67"/>
+      <c r="AJC84" s="67"/>
+      <c r="AJD84" s="67"/>
+      <c r="AJE84" s="67"/>
+      <c r="AJF84" s="67"/>
+      <c r="AJG84" s="67"/>
+      <c r="AJH84" s="67"/>
+      <c r="AJI84" s="67"/>
+      <c r="AJJ84" s="67"/>
+      <c r="AJK84" s="67"/>
+      <c r="AJL84" s="67"/>
+      <c r="AJM84" s="67"/>
+      <c r="AJN84" s="67"/>
+      <c r="AJO84" s="67"/>
+      <c r="AJP84" s="67"/>
+      <c r="AJQ84" s="67"/>
+      <c r="AJR84" s="67"/>
+      <c r="AJS84" s="67"/>
+      <c r="AJT84" s="67"/>
+      <c r="AJU84" s="67"/>
+      <c r="AJV84" s="67"/>
+      <c r="AJW84" s="67"/>
+      <c r="AJX84" s="67"/>
+      <c r="AJY84" s="67"/>
+      <c r="AJZ84" s="67"/>
+      <c r="AKA84" s="67"/>
+      <c r="AKB84" s="67"/>
+      <c r="AKC84" s="67"/>
+      <c r="AKD84" s="67"/>
+      <c r="AKE84" s="67"/>
+      <c r="AKF84" s="67"/>
+      <c r="AKG84" s="67"/>
+      <c r="AKH84" s="67"/>
+      <c r="AKI84" s="67"/>
+      <c r="AKJ84" s="67"/>
+      <c r="AKK84" s="67"/>
+      <c r="AKL84" s="67"/>
+      <c r="AKM84" s="67"/>
+      <c r="AKN84" s="67"/>
+      <c r="AKO84" s="67"/>
+      <c r="AKP84" s="67"/>
+      <c r="AKQ84" s="67"/>
+      <c r="AKR84" s="67"/>
+      <c r="AKS84" s="67"/>
+      <c r="AKT84" s="67"/>
+      <c r="AKU84" s="67"/>
+      <c r="AKV84" s="67"/>
+      <c r="AKW84" s="67"/>
+      <c r="AKX84" s="67"/>
+      <c r="AKY84" s="67"/>
+      <c r="AKZ84" s="67"/>
+      <c r="ALA84" s="67"/>
+      <c r="ALB84" s="67"/>
+      <c r="ALC84" s="67"/>
+      <c r="ALD84" s="67"/>
+      <c r="ALE84" s="67"/>
+      <c r="ALF84" s="67"/>
+      <c r="ALG84" s="67"/>
+      <c r="ALH84" s="67"/>
+      <c r="ALI84" s="67"/>
+      <c r="ALJ84" s="67"/>
+      <c r="ALK84" s="67"/>
+      <c r="ALL84" s="67"/>
+      <c r="ALM84" s="67"/>
+      <c r="ALN84" s="67"/>
+      <c r="ALO84" s="67"/>
+      <c r="ALP84" s="67"/>
+      <c r="ALQ84" s="67"/>
+      <c r="ALR84" s="67"/>
+      <c r="ALS84" s="67"/>
+      <c r="ALT84" s="67"/>
+      <c r="ALU84" s="67"/>
+      <c r="ALV84" s="67"/>
+      <c r="ALW84" s="67"/>
+      <c r="ALX84" s="67"/>
+      <c r="ALY84" s="67"/>
+      <c r="ALZ84" s="67"/>
+      <c r="AMA84" s="67"/>
+      <c r="AMB84" s="67"/>
+      <c r="AMC84" s="67"/>
+      <c r="AMD84" s="67"/>
+      <c r="AME84" s="67"/>
+      <c r="AMF84" s="67"/>
+      <c r="AMG84" s="67"/>
+      <c r="AMH84" s="67"/>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F85" s="11">
+        <v>0.968174</v>
+      </c>
+      <c r="G85" s="12">
+        <v>0.9683</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
i don't know what to do
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149">
   <si>
     <r>
       <rPr>
@@ -1318,6 +1318,18 @@
   <si>
     <t>simple lightgbm</t>
   </si>
+  <si>
+    <t>province_economic</t>
+  </si>
+  <si>
+    <t>328</t>
+  </si>
+  <si>
+    <t>是否好评好评次数</t>
+  </si>
+  <si>
+    <t>331</t>
+  </si>
 </sst>
 </file>
 
@@ -1325,13 +1337,13 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="0.00000_ "/>
+    <numFmt numFmtId="177" formatCode="0.0000000_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.0000000_ "/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1360,6 +1372,10 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="8"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="8"/>
       <color rgb="FFFF0000"/>
@@ -1376,15 +1392,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1398,8 +1407,83 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1415,40 +1499,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1460,59 +1521,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1603,7 +1619,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1615,7 +1691,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1627,37 +1763,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1669,43 +1775,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1717,61 +1787,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1808,9 +1824,29 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1826,6 +1862,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1859,176 +1904,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2212,10 +2228,13 @@
     <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2551,10 +2570,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AMH85"/>
+  <dimension ref="A1:AMH87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+      <selection activeCell="A88" sqref="$A88:$XFD88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -7869,7 +7888,7 @@
       <c r="AMH13" s="47"/>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:1022">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="69" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="19" t="s">
@@ -18105,7 +18124,7 @@
       <c r="G72" s="35">
         <v>0.96859</v>
       </c>
-      <c r="H72" s="61" t="s">
+      <c r="H72" s="62" t="s">
         <v>125</v>
       </c>
       <c r="I72" s="46"/>
@@ -19145,7 +19164,7 @@
       <c r="G73" s="12">
         <v>0.9684</v>
       </c>
-      <c r="H73" s="62" t="s">
+      <c r="H73" s="63" t="s">
         <v>127</v>
       </c>
     </row>
@@ -19211,7 +19230,7 @@
       <c r="F76" s="20">
         <v>0.9671155</v>
       </c>
-      <c r="G76" s="63">
+      <c r="G76" s="64">
         <v>0.9682</v>
       </c>
     </row>
@@ -19234,7 +19253,7 @@
       <c r="F78" s="57">
         <v>0.9666471</v>
       </c>
-      <c r="G78" s="64">
+      <c r="G78" s="65">
         <v>0.9678</v>
       </c>
     </row>
@@ -19349,1024 +19368,1024 @@
       <c r="F84" s="60">
         <v>0.9673051</v>
       </c>
-      <c r="G84" s="65">
+      <c r="G84" s="66">
         <v>0.9686</v>
       </c>
-      <c r="H84" s="66"/>
-      <c r="I84" s="67"/>
-      <c r="J84" s="67"/>
-      <c r="K84" s="67"/>
-      <c r="L84" s="67"/>
-      <c r="M84" s="67"/>
-      <c r="N84" s="67"/>
-      <c r="O84" s="67"/>
-      <c r="P84" s="67"/>
-      <c r="Q84" s="67"/>
-      <c r="R84" s="67"/>
-      <c r="S84" s="67"/>
-      <c r="T84" s="67"/>
-      <c r="U84" s="67"/>
-      <c r="V84" s="67"/>
-      <c r="W84" s="67"/>
-      <c r="X84" s="67"/>
-      <c r="Y84" s="67"/>
-      <c r="Z84" s="67"/>
-      <c r="AA84" s="67"/>
-      <c r="AB84" s="67"/>
-      <c r="AC84" s="67"/>
-      <c r="AD84" s="67"/>
-      <c r="AE84" s="67"/>
-      <c r="AF84" s="67"/>
-      <c r="AG84" s="67"/>
-      <c r="AH84" s="67"/>
-      <c r="AI84" s="67"/>
-      <c r="AJ84" s="67"/>
-      <c r="AK84" s="67"/>
-      <c r="AL84" s="67"/>
-      <c r="AM84" s="67"/>
-      <c r="AN84" s="67"/>
-      <c r="AO84" s="67"/>
-      <c r="AP84" s="67"/>
-      <c r="AQ84" s="67"/>
-      <c r="AR84" s="67"/>
-      <c r="AS84" s="67"/>
-      <c r="AT84" s="67"/>
-      <c r="AU84" s="67"/>
-      <c r="AV84" s="67"/>
-      <c r="AW84" s="67"/>
-      <c r="AX84" s="67"/>
-      <c r="AY84" s="67"/>
-      <c r="AZ84" s="67"/>
-      <c r="BA84" s="67"/>
-      <c r="BB84" s="67"/>
-      <c r="BC84" s="67"/>
-      <c r="BD84" s="67"/>
-      <c r="BE84" s="67"/>
-      <c r="BF84" s="67"/>
-      <c r="BG84" s="67"/>
-      <c r="BH84" s="67"/>
-      <c r="BI84" s="67"/>
-      <c r="BJ84" s="67"/>
-      <c r="BK84" s="67"/>
-      <c r="BL84" s="67"/>
-      <c r="BM84" s="67"/>
-      <c r="BN84" s="67"/>
-      <c r="BO84" s="67"/>
-      <c r="BP84" s="67"/>
-      <c r="BQ84" s="67"/>
-      <c r="BR84" s="67"/>
-      <c r="BS84" s="67"/>
-      <c r="BT84" s="67"/>
-      <c r="BU84" s="67"/>
-      <c r="BV84" s="67"/>
-      <c r="BW84" s="67"/>
-      <c r="BX84" s="67"/>
-      <c r="BY84" s="67"/>
-      <c r="BZ84" s="67"/>
-      <c r="CA84" s="67"/>
-      <c r="CB84" s="67"/>
-      <c r="CC84" s="67"/>
-      <c r="CD84" s="67"/>
-      <c r="CE84" s="67"/>
-      <c r="CF84" s="67"/>
-      <c r="CG84" s="67"/>
-      <c r="CH84" s="67"/>
-      <c r="CI84" s="67"/>
-      <c r="CJ84" s="67"/>
-      <c r="CK84" s="67"/>
-      <c r="CL84" s="67"/>
-      <c r="CM84" s="67"/>
-      <c r="CN84" s="67"/>
-      <c r="CO84" s="67"/>
-      <c r="CP84" s="67"/>
-      <c r="CQ84" s="67"/>
-      <c r="CR84" s="67"/>
-      <c r="CS84" s="67"/>
-      <c r="CT84" s="67"/>
-      <c r="CU84" s="67"/>
-      <c r="CV84" s="67"/>
-      <c r="CW84" s="67"/>
-      <c r="CX84" s="67"/>
-      <c r="CY84" s="67"/>
-      <c r="CZ84" s="67"/>
-      <c r="DA84" s="67"/>
-      <c r="DB84" s="67"/>
-      <c r="DC84" s="67"/>
-      <c r="DD84" s="67"/>
-      <c r="DE84" s="67"/>
-      <c r="DF84" s="67"/>
-      <c r="DG84" s="67"/>
-      <c r="DH84" s="67"/>
-      <c r="DI84" s="67"/>
-      <c r="DJ84" s="67"/>
-      <c r="DK84" s="67"/>
-      <c r="DL84" s="67"/>
-      <c r="DM84" s="67"/>
-      <c r="DN84" s="67"/>
-      <c r="DO84" s="67"/>
-      <c r="DP84" s="67"/>
-      <c r="DQ84" s="67"/>
-      <c r="DR84" s="67"/>
-      <c r="DS84" s="67"/>
-      <c r="DT84" s="67"/>
-      <c r="DU84" s="67"/>
-      <c r="DV84" s="67"/>
-      <c r="DW84" s="67"/>
-      <c r="DX84" s="67"/>
-      <c r="DY84" s="67"/>
-      <c r="DZ84" s="67"/>
-      <c r="EA84" s="67"/>
-      <c r="EB84" s="67"/>
-      <c r="EC84" s="67"/>
-      <c r="ED84" s="67"/>
-      <c r="EE84" s="67"/>
-      <c r="EF84" s="67"/>
-      <c r="EG84" s="67"/>
-      <c r="EH84" s="67"/>
-      <c r="EI84" s="67"/>
-      <c r="EJ84" s="67"/>
-      <c r="EK84" s="67"/>
-      <c r="EL84" s="67"/>
-      <c r="EM84" s="67"/>
-      <c r="EN84" s="67"/>
-      <c r="EO84" s="67"/>
-      <c r="EP84" s="67"/>
-      <c r="EQ84" s="67"/>
-      <c r="ER84" s="67"/>
-      <c r="ES84" s="67"/>
-      <c r="ET84" s="67"/>
-      <c r="EU84" s="67"/>
-      <c r="EV84" s="67"/>
-      <c r="EW84" s="67"/>
-      <c r="EX84" s="67"/>
-      <c r="EY84" s="67"/>
-      <c r="EZ84" s="67"/>
-      <c r="FA84" s="67"/>
-      <c r="FB84" s="67"/>
-      <c r="FC84" s="67"/>
-      <c r="FD84" s="67"/>
-      <c r="FE84" s="67"/>
-      <c r="FF84" s="67"/>
-      <c r="FG84" s="67"/>
-      <c r="FH84" s="67"/>
-      <c r="FI84" s="67"/>
-      <c r="FJ84" s="67"/>
-      <c r="FK84" s="67"/>
-      <c r="FL84" s="67"/>
-      <c r="FM84" s="67"/>
-      <c r="FN84" s="67"/>
-      <c r="FO84" s="67"/>
-      <c r="FP84" s="67"/>
-      <c r="FQ84" s="67"/>
-      <c r="FR84" s="67"/>
-      <c r="FS84" s="67"/>
-      <c r="FT84" s="67"/>
-      <c r="FU84" s="67"/>
-      <c r="FV84" s="67"/>
-      <c r="FW84" s="67"/>
-      <c r="FX84" s="67"/>
-      <c r="FY84" s="67"/>
-      <c r="FZ84" s="67"/>
-      <c r="GA84" s="67"/>
-      <c r="GB84" s="67"/>
-      <c r="GC84" s="67"/>
-      <c r="GD84" s="67"/>
-      <c r="GE84" s="67"/>
-      <c r="GF84" s="67"/>
-      <c r="GG84" s="67"/>
-      <c r="GH84" s="67"/>
-      <c r="GI84" s="67"/>
-      <c r="GJ84" s="67"/>
-      <c r="GK84" s="67"/>
-      <c r="GL84" s="67"/>
-      <c r="GM84" s="67"/>
-      <c r="GN84" s="67"/>
-      <c r="GO84" s="67"/>
-      <c r="GP84" s="67"/>
-      <c r="GQ84" s="67"/>
-      <c r="GR84" s="67"/>
-      <c r="GS84" s="67"/>
-      <c r="GT84" s="67"/>
-      <c r="GU84" s="67"/>
-      <c r="GV84" s="67"/>
-      <c r="GW84" s="67"/>
-      <c r="GX84" s="67"/>
-      <c r="GY84" s="67"/>
-      <c r="GZ84" s="67"/>
-      <c r="HA84" s="67"/>
-      <c r="HB84" s="67"/>
-      <c r="HC84" s="67"/>
-      <c r="HD84" s="67"/>
-      <c r="HE84" s="67"/>
-      <c r="HF84" s="67"/>
-      <c r="HG84" s="67"/>
-      <c r="HH84" s="67"/>
-      <c r="HI84" s="67"/>
-      <c r="HJ84" s="67"/>
-      <c r="HK84" s="67"/>
-      <c r="HL84" s="67"/>
-      <c r="HM84" s="67"/>
-      <c r="HN84" s="67"/>
-      <c r="HO84" s="67"/>
-      <c r="HP84" s="67"/>
-      <c r="HQ84" s="67"/>
-      <c r="HR84" s="67"/>
-      <c r="HS84" s="67"/>
-      <c r="HT84" s="67"/>
-      <c r="HU84" s="67"/>
-      <c r="HV84" s="67"/>
-      <c r="HW84" s="67"/>
-      <c r="HX84" s="67"/>
-      <c r="HY84" s="67"/>
-      <c r="HZ84" s="67"/>
-      <c r="IA84" s="67"/>
-      <c r="IB84" s="67"/>
-      <c r="IC84" s="67"/>
-      <c r="ID84" s="67"/>
-      <c r="IE84" s="67"/>
-      <c r="IF84" s="67"/>
-      <c r="IG84" s="67"/>
-      <c r="IH84" s="67"/>
-      <c r="II84" s="67"/>
-      <c r="IJ84" s="67"/>
-      <c r="IK84" s="67"/>
-      <c r="IL84" s="67"/>
-      <c r="IM84" s="67"/>
-      <c r="IN84" s="67"/>
-      <c r="IO84" s="67"/>
-      <c r="IP84" s="67"/>
-      <c r="IQ84" s="67"/>
-      <c r="IR84" s="67"/>
-      <c r="IS84" s="67"/>
-      <c r="IT84" s="67"/>
-      <c r="IU84" s="67"/>
-      <c r="IV84" s="67"/>
-      <c r="IW84" s="67"/>
-      <c r="IX84" s="67"/>
-      <c r="IY84" s="67"/>
-      <c r="IZ84" s="67"/>
-      <c r="JA84" s="67"/>
-      <c r="JB84" s="67"/>
-      <c r="JC84" s="67"/>
-      <c r="JD84" s="67"/>
-      <c r="JE84" s="67"/>
-      <c r="JF84" s="67"/>
-      <c r="JG84" s="67"/>
-      <c r="JH84" s="67"/>
-      <c r="JI84" s="67"/>
-      <c r="JJ84" s="67"/>
-      <c r="JK84" s="67"/>
-      <c r="JL84" s="67"/>
-      <c r="JM84" s="67"/>
-      <c r="JN84" s="67"/>
-      <c r="JO84" s="67"/>
-      <c r="JP84" s="67"/>
-      <c r="JQ84" s="67"/>
-      <c r="JR84" s="67"/>
-      <c r="JS84" s="67"/>
-      <c r="JT84" s="67"/>
-      <c r="JU84" s="67"/>
-      <c r="JV84" s="67"/>
-      <c r="JW84" s="67"/>
-      <c r="JX84" s="67"/>
-      <c r="JY84" s="67"/>
-      <c r="JZ84" s="67"/>
-      <c r="KA84" s="67"/>
-      <c r="KB84" s="67"/>
-      <c r="KC84" s="67"/>
-      <c r="KD84" s="67"/>
-      <c r="KE84" s="67"/>
-      <c r="KF84" s="67"/>
-      <c r="KG84" s="67"/>
-      <c r="KH84" s="67"/>
-      <c r="KI84" s="67"/>
-      <c r="KJ84" s="67"/>
-      <c r="KK84" s="67"/>
-      <c r="KL84" s="67"/>
-      <c r="KM84" s="67"/>
-      <c r="KN84" s="67"/>
-      <c r="KO84" s="67"/>
-      <c r="KP84" s="67"/>
-      <c r="KQ84" s="67"/>
-      <c r="KR84" s="67"/>
-      <c r="KS84" s="67"/>
-      <c r="KT84" s="67"/>
-      <c r="KU84" s="67"/>
-      <c r="KV84" s="67"/>
-      <c r="KW84" s="67"/>
-      <c r="KX84" s="67"/>
-      <c r="KY84" s="67"/>
-      <c r="KZ84" s="67"/>
-      <c r="LA84" s="67"/>
-      <c r="LB84" s="67"/>
-      <c r="LC84" s="67"/>
-      <c r="LD84" s="67"/>
-      <c r="LE84" s="67"/>
-      <c r="LF84" s="67"/>
-      <c r="LG84" s="67"/>
-      <c r="LH84" s="67"/>
-      <c r="LI84" s="67"/>
-      <c r="LJ84" s="67"/>
-      <c r="LK84" s="67"/>
-      <c r="LL84" s="67"/>
-      <c r="LM84" s="67"/>
-      <c r="LN84" s="67"/>
-      <c r="LO84" s="67"/>
-      <c r="LP84" s="67"/>
-      <c r="LQ84" s="67"/>
-      <c r="LR84" s="67"/>
-      <c r="LS84" s="67"/>
-      <c r="LT84" s="67"/>
-      <c r="LU84" s="67"/>
-      <c r="LV84" s="67"/>
-      <c r="LW84" s="67"/>
-      <c r="LX84" s="67"/>
-      <c r="LY84" s="67"/>
-      <c r="LZ84" s="67"/>
-      <c r="MA84" s="67"/>
-      <c r="MB84" s="67"/>
-      <c r="MC84" s="67"/>
-      <c r="MD84" s="67"/>
-      <c r="ME84" s="67"/>
-      <c r="MF84" s="67"/>
-      <c r="MG84" s="67"/>
-      <c r="MH84" s="67"/>
-      <c r="MI84" s="67"/>
-      <c r="MJ84" s="67"/>
-      <c r="MK84" s="67"/>
-      <c r="ML84" s="67"/>
-      <c r="MM84" s="67"/>
-      <c r="MN84" s="67"/>
-      <c r="MO84" s="67"/>
-      <c r="MP84" s="67"/>
-      <c r="MQ84" s="67"/>
-      <c r="MR84" s="67"/>
-      <c r="MS84" s="67"/>
-      <c r="MT84" s="67"/>
-      <c r="MU84" s="67"/>
-      <c r="MV84" s="67"/>
-      <c r="MW84" s="67"/>
-      <c r="MX84" s="67"/>
-      <c r="MY84" s="67"/>
-      <c r="MZ84" s="67"/>
-      <c r="NA84" s="67"/>
-      <c r="NB84" s="67"/>
-      <c r="NC84" s="67"/>
-      <c r="ND84" s="67"/>
-      <c r="NE84" s="67"/>
-      <c r="NF84" s="67"/>
-      <c r="NG84" s="67"/>
-      <c r="NH84" s="67"/>
-      <c r="NI84" s="67"/>
-      <c r="NJ84" s="67"/>
-      <c r="NK84" s="67"/>
-      <c r="NL84" s="67"/>
-      <c r="NM84" s="67"/>
-      <c r="NN84" s="67"/>
-      <c r="NO84" s="67"/>
-      <c r="NP84" s="67"/>
-      <c r="NQ84" s="67"/>
-      <c r="NR84" s="67"/>
-      <c r="NS84" s="67"/>
-      <c r="NT84" s="67"/>
-      <c r="NU84" s="67"/>
-      <c r="NV84" s="67"/>
-      <c r="NW84" s="67"/>
-      <c r="NX84" s="67"/>
-      <c r="NY84" s="67"/>
-      <c r="NZ84" s="67"/>
-      <c r="OA84" s="67"/>
-      <c r="OB84" s="67"/>
-      <c r="OC84" s="67"/>
-      <c r="OD84" s="67"/>
-      <c r="OE84" s="67"/>
-      <c r="OF84" s="67"/>
-      <c r="OG84" s="67"/>
-      <c r="OH84" s="67"/>
-      <c r="OI84" s="67"/>
-      <c r="OJ84" s="67"/>
-      <c r="OK84" s="67"/>
-      <c r="OL84" s="67"/>
-      <c r="OM84" s="67"/>
-      <c r="ON84" s="67"/>
-      <c r="OO84" s="67"/>
-      <c r="OP84" s="67"/>
-      <c r="OQ84" s="67"/>
-      <c r="OR84" s="67"/>
-      <c r="OS84" s="67"/>
-      <c r="OT84" s="67"/>
-      <c r="OU84" s="67"/>
-      <c r="OV84" s="67"/>
-      <c r="OW84" s="67"/>
-      <c r="OX84" s="67"/>
-      <c r="OY84" s="67"/>
-      <c r="OZ84" s="67"/>
-      <c r="PA84" s="67"/>
-      <c r="PB84" s="67"/>
-      <c r="PC84" s="67"/>
-      <c r="PD84" s="67"/>
-      <c r="PE84" s="67"/>
-      <c r="PF84" s="67"/>
-      <c r="PG84" s="67"/>
-      <c r="PH84" s="67"/>
-      <c r="PI84" s="67"/>
-      <c r="PJ84" s="67"/>
-      <c r="PK84" s="67"/>
-      <c r="PL84" s="67"/>
-      <c r="PM84" s="67"/>
-      <c r="PN84" s="67"/>
-      <c r="PO84" s="67"/>
-      <c r="PP84" s="67"/>
-      <c r="PQ84" s="67"/>
-      <c r="PR84" s="67"/>
-      <c r="PS84" s="67"/>
-      <c r="PT84" s="67"/>
-      <c r="PU84" s="67"/>
-      <c r="PV84" s="67"/>
-      <c r="PW84" s="67"/>
-      <c r="PX84" s="67"/>
-      <c r="PY84" s="67"/>
-      <c r="PZ84" s="67"/>
-      <c r="QA84" s="67"/>
-      <c r="QB84" s="67"/>
-      <c r="QC84" s="67"/>
-      <c r="QD84" s="67"/>
-      <c r="QE84" s="67"/>
-      <c r="QF84" s="67"/>
-      <c r="QG84" s="67"/>
-      <c r="QH84" s="67"/>
-      <c r="QI84" s="67"/>
-      <c r="QJ84" s="67"/>
-      <c r="QK84" s="67"/>
-      <c r="QL84" s="67"/>
-      <c r="QM84" s="67"/>
-      <c r="QN84" s="67"/>
-      <c r="QO84" s="67"/>
-      <c r="QP84" s="67"/>
-      <c r="QQ84" s="67"/>
-      <c r="QR84" s="67"/>
-      <c r="QS84" s="67"/>
-      <c r="QT84" s="67"/>
-      <c r="QU84" s="67"/>
-      <c r="QV84" s="67"/>
-      <c r="QW84" s="67"/>
-      <c r="QX84" s="67"/>
-      <c r="QY84" s="67"/>
-      <c r="QZ84" s="67"/>
-      <c r="RA84" s="67"/>
-      <c r="RB84" s="67"/>
-      <c r="RC84" s="67"/>
-      <c r="RD84" s="67"/>
-      <c r="RE84" s="67"/>
-      <c r="RF84" s="67"/>
-      <c r="RG84" s="67"/>
-      <c r="RH84" s="67"/>
-      <c r="RI84" s="67"/>
-      <c r="RJ84" s="67"/>
-      <c r="RK84" s="67"/>
-      <c r="RL84" s="67"/>
-      <c r="RM84" s="67"/>
-      <c r="RN84" s="67"/>
-      <c r="RO84" s="67"/>
-      <c r="RP84" s="67"/>
-      <c r="RQ84" s="67"/>
-      <c r="RR84" s="67"/>
-      <c r="RS84" s="67"/>
-      <c r="RT84" s="67"/>
-      <c r="RU84" s="67"/>
-      <c r="RV84" s="67"/>
-      <c r="RW84" s="67"/>
-      <c r="RX84" s="67"/>
-      <c r="RY84" s="67"/>
-      <c r="RZ84" s="67"/>
-      <c r="SA84" s="67"/>
-      <c r="SB84" s="67"/>
-      <c r="SC84" s="67"/>
-      <c r="SD84" s="67"/>
-      <c r="SE84" s="67"/>
-      <c r="SF84" s="67"/>
-      <c r="SG84" s="67"/>
-      <c r="SH84" s="67"/>
-      <c r="SI84" s="67"/>
-      <c r="SJ84" s="67"/>
-      <c r="SK84" s="67"/>
-      <c r="SL84" s="67"/>
-      <c r="SM84" s="67"/>
-      <c r="SN84" s="67"/>
-      <c r="SO84" s="67"/>
-      <c r="SP84" s="67"/>
-      <c r="SQ84" s="67"/>
-      <c r="SR84" s="67"/>
-      <c r="SS84" s="67"/>
-      <c r="ST84" s="67"/>
-      <c r="SU84" s="67"/>
-      <c r="SV84" s="67"/>
-      <c r="SW84" s="67"/>
-      <c r="SX84" s="67"/>
-      <c r="SY84" s="67"/>
-      <c r="SZ84" s="67"/>
-      <c r="TA84" s="67"/>
-      <c r="TB84" s="67"/>
-      <c r="TC84" s="67"/>
-      <c r="TD84" s="67"/>
-      <c r="TE84" s="67"/>
-      <c r="TF84" s="67"/>
-      <c r="TG84" s="67"/>
-      <c r="TH84" s="67"/>
-      <c r="TI84" s="67"/>
-      <c r="TJ84" s="67"/>
-      <c r="TK84" s="67"/>
-      <c r="TL84" s="67"/>
-      <c r="TM84" s="67"/>
-      <c r="TN84" s="67"/>
-      <c r="TO84" s="67"/>
-      <c r="TP84" s="67"/>
-      <c r="TQ84" s="67"/>
-      <c r="TR84" s="67"/>
-      <c r="TS84" s="67"/>
-      <c r="TT84" s="67"/>
-      <c r="TU84" s="67"/>
-      <c r="TV84" s="67"/>
-      <c r="TW84" s="67"/>
-      <c r="TX84" s="67"/>
-      <c r="TY84" s="67"/>
-      <c r="TZ84" s="67"/>
-      <c r="UA84" s="67"/>
-      <c r="UB84" s="67"/>
-      <c r="UC84" s="67"/>
-      <c r="UD84" s="67"/>
-      <c r="UE84" s="67"/>
-      <c r="UF84" s="67"/>
-      <c r="UG84" s="67"/>
-      <c r="UH84" s="67"/>
-      <c r="UI84" s="67"/>
-      <c r="UJ84" s="67"/>
-      <c r="UK84" s="67"/>
-      <c r="UL84" s="67"/>
-      <c r="UM84" s="67"/>
-      <c r="UN84" s="67"/>
-      <c r="UO84" s="67"/>
-      <c r="UP84" s="67"/>
-      <c r="UQ84" s="67"/>
-      <c r="UR84" s="67"/>
-      <c r="US84" s="67"/>
-      <c r="UT84" s="67"/>
-      <c r="UU84" s="67"/>
-      <c r="UV84" s="67"/>
-      <c r="UW84" s="67"/>
-      <c r="UX84" s="67"/>
-      <c r="UY84" s="67"/>
-      <c r="UZ84" s="67"/>
-      <c r="VA84" s="67"/>
-      <c r="VB84" s="67"/>
-      <c r="VC84" s="67"/>
-      <c r="VD84" s="67"/>
-      <c r="VE84" s="67"/>
-      <c r="VF84" s="67"/>
-      <c r="VG84" s="67"/>
-      <c r="VH84" s="67"/>
-      <c r="VI84" s="67"/>
-      <c r="VJ84" s="67"/>
-      <c r="VK84" s="67"/>
-      <c r="VL84" s="67"/>
-      <c r="VM84" s="67"/>
-      <c r="VN84" s="67"/>
-      <c r="VO84" s="67"/>
-      <c r="VP84" s="67"/>
-      <c r="VQ84" s="67"/>
-      <c r="VR84" s="67"/>
-      <c r="VS84" s="67"/>
-      <c r="VT84" s="67"/>
-      <c r="VU84" s="67"/>
-      <c r="VV84" s="67"/>
-      <c r="VW84" s="67"/>
-      <c r="VX84" s="67"/>
-      <c r="VY84" s="67"/>
-      <c r="VZ84" s="67"/>
-      <c r="WA84" s="67"/>
-      <c r="WB84" s="67"/>
-      <c r="WC84" s="67"/>
-      <c r="WD84" s="67"/>
-      <c r="WE84" s="67"/>
-      <c r="WF84" s="67"/>
-      <c r="WG84" s="67"/>
-      <c r="WH84" s="67"/>
-      <c r="WI84" s="67"/>
-      <c r="WJ84" s="67"/>
-      <c r="WK84" s="67"/>
-      <c r="WL84" s="67"/>
-      <c r="WM84" s="67"/>
-      <c r="WN84" s="67"/>
-      <c r="WO84" s="67"/>
-      <c r="WP84" s="67"/>
-      <c r="WQ84" s="67"/>
-      <c r="WR84" s="67"/>
-      <c r="WS84" s="67"/>
-      <c r="WT84" s="67"/>
-      <c r="WU84" s="67"/>
-      <c r="WV84" s="67"/>
-      <c r="WW84" s="67"/>
-      <c r="WX84" s="67"/>
-      <c r="WY84" s="67"/>
-      <c r="WZ84" s="67"/>
-      <c r="XA84" s="67"/>
-      <c r="XB84" s="67"/>
-      <c r="XC84" s="67"/>
-      <c r="XD84" s="67"/>
-      <c r="XE84" s="67"/>
-      <c r="XF84" s="67"/>
-      <c r="XG84" s="67"/>
-      <c r="XH84" s="67"/>
-      <c r="XI84" s="67"/>
-      <c r="XJ84" s="67"/>
-      <c r="XK84" s="67"/>
-      <c r="XL84" s="67"/>
-      <c r="XM84" s="67"/>
-      <c r="XN84" s="67"/>
-      <c r="XO84" s="67"/>
-      <c r="XP84" s="67"/>
-      <c r="XQ84" s="67"/>
-      <c r="XR84" s="67"/>
-      <c r="XS84" s="67"/>
-      <c r="XT84" s="67"/>
-      <c r="XU84" s="67"/>
-      <c r="XV84" s="67"/>
-      <c r="XW84" s="67"/>
-      <c r="XX84" s="67"/>
-      <c r="XY84" s="67"/>
-      <c r="XZ84" s="67"/>
-      <c r="YA84" s="67"/>
-      <c r="YB84" s="67"/>
-      <c r="YC84" s="67"/>
-      <c r="YD84" s="67"/>
-      <c r="YE84" s="67"/>
-      <c r="YF84" s="67"/>
-      <c r="YG84" s="67"/>
-      <c r="YH84" s="67"/>
-      <c r="YI84" s="67"/>
-      <c r="YJ84" s="67"/>
-      <c r="YK84" s="67"/>
-      <c r="YL84" s="67"/>
-      <c r="YM84" s="67"/>
-      <c r="YN84" s="67"/>
-      <c r="YO84" s="67"/>
-      <c r="YP84" s="67"/>
-      <c r="YQ84" s="67"/>
-      <c r="YR84" s="67"/>
-      <c r="YS84" s="67"/>
-      <c r="YT84" s="67"/>
-      <c r="YU84" s="67"/>
-      <c r="YV84" s="67"/>
-      <c r="YW84" s="67"/>
-      <c r="YX84" s="67"/>
-      <c r="YY84" s="67"/>
-      <c r="YZ84" s="67"/>
-      <c r="ZA84" s="67"/>
-      <c r="ZB84" s="67"/>
-      <c r="ZC84" s="67"/>
-      <c r="ZD84" s="67"/>
-      <c r="ZE84" s="67"/>
-      <c r="ZF84" s="67"/>
-      <c r="ZG84" s="67"/>
-      <c r="ZH84" s="67"/>
-      <c r="ZI84" s="67"/>
-      <c r="ZJ84" s="67"/>
-      <c r="ZK84" s="67"/>
-      <c r="ZL84" s="67"/>
-      <c r="ZM84" s="67"/>
-      <c r="ZN84" s="67"/>
-      <c r="ZO84" s="67"/>
-      <c r="ZP84" s="67"/>
-      <c r="ZQ84" s="67"/>
-      <c r="ZR84" s="67"/>
-      <c r="ZS84" s="67"/>
-      <c r="ZT84" s="67"/>
-      <c r="ZU84" s="67"/>
-      <c r="ZV84" s="67"/>
-      <c r="ZW84" s="67"/>
-      <c r="ZX84" s="67"/>
-      <c r="ZY84" s="67"/>
-      <c r="ZZ84" s="67"/>
-      <c r="AAA84" s="67"/>
-      <c r="AAB84" s="67"/>
-      <c r="AAC84" s="67"/>
-      <c r="AAD84" s="67"/>
-      <c r="AAE84" s="67"/>
-      <c r="AAF84" s="67"/>
-      <c r="AAG84" s="67"/>
-      <c r="AAH84" s="67"/>
-      <c r="AAI84" s="67"/>
-      <c r="AAJ84" s="67"/>
-      <c r="AAK84" s="67"/>
-      <c r="AAL84" s="67"/>
-      <c r="AAM84" s="67"/>
-      <c r="AAN84" s="67"/>
-      <c r="AAO84" s="67"/>
-      <c r="AAP84" s="67"/>
-      <c r="AAQ84" s="67"/>
-      <c r="AAR84" s="67"/>
-      <c r="AAS84" s="67"/>
-      <c r="AAT84" s="67"/>
-      <c r="AAU84" s="67"/>
-      <c r="AAV84" s="67"/>
-      <c r="AAW84" s="67"/>
-      <c r="AAX84" s="67"/>
-      <c r="AAY84" s="67"/>
-      <c r="AAZ84" s="67"/>
-      <c r="ABA84" s="67"/>
-      <c r="ABB84" s="67"/>
-      <c r="ABC84" s="67"/>
-      <c r="ABD84" s="67"/>
-      <c r="ABE84" s="67"/>
-      <c r="ABF84" s="67"/>
-      <c r="ABG84" s="67"/>
-      <c r="ABH84" s="67"/>
-      <c r="ABI84" s="67"/>
-      <c r="ABJ84" s="67"/>
-      <c r="ABK84" s="67"/>
-      <c r="ABL84" s="67"/>
-      <c r="ABM84" s="67"/>
-      <c r="ABN84" s="67"/>
-      <c r="ABO84" s="67"/>
-      <c r="ABP84" s="67"/>
-      <c r="ABQ84" s="67"/>
-      <c r="ABR84" s="67"/>
-      <c r="ABS84" s="67"/>
-      <c r="ABT84" s="67"/>
-      <c r="ABU84" s="67"/>
-      <c r="ABV84" s="67"/>
-      <c r="ABW84" s="67"/>
-      <c r="ABX84" s="67"/>
-      <c r="ABY84" s="67"/>
-      <c r="ABZ84" s="67"/>
-      <c r="ACA84" s="67"/>
-      <c r="ACB84" s="67"/>
-      <c r="ACC84" s="67"/>
-      <c r="ACD84" s="67"/>
-      <c r="ACE84" s="67"/>
-      <c r="ACF84" s="67"/>
-      <c r="ACG84" s="67"/>
-      <c r="ACH84" s="67"/>
-      <c r="ACI84" s="67"/>
-      <c r="ACJ84" s="67"/>
-      <c r="ACK84" s="67"/>
-      <c r="ACL84" s="67"/>
-      <c r="ACM84" s="67"/>
-      <c r="ACN84" s="67"/>
-      <c r="ACO84" s="67"/>
-      <c r="ACP84" s="67"/>
-      <c r="ACQ84" s="67"/>
-      <c r="ACR84" s="67"/>
-      <c r="ACS84" s="67"/>
-      <c r="ACT84" s="67"/>
-      <c r="ACU84" s="67"/>
-      <c r="ACV84" s="67"/>
-      <c r="ACW84" s="67"/>
-      <c r="ACX84" s="67"/>
-      <c r="ACY84" s="67"/>
-      <c r="ACZ84" s="67"/>
-      <c r="ADA84" s="67"/>
-      <c r="ADB84" s="67"/>
-      <c r="ADC84" s="67"/>
-      <c r="ADD84" s="67"/>
-      <c r="ADE84" s="67"/>
-      <c r="ADF84" s="67"/>
-      <c r="ADG84" s="67"/>
-      <c r="ADH84" s="67"/>
-      <c r="ADI84" s="67"/>
-      <c r="ADJ84" s="67"/>
-      <c r="ADK84" s="67"/>
-      <c r="ADL84" s="67"/>
-      <c r="ADM84" s="67"/>
-      <c r="ADN84" s="67"/>
-      <c r="ADO84" s="67"/>
-      <c r="ADP84" s="67"/>
-      <c r="ADQ84" s="67"/>
-      <c r="ADR84" s="67"/>
-      <c r="ADS84" s="67"/>
-      <c r="ADT84" s="67"/>
-      <c r="ADU84" s="67"/>
-      <c r="ADV84" s="67"/>
-      <c r="ADW84" s="67"/>
-      <c r="ADX84" s="67"/>
-      <c r="ADY84" s="67"/>
-      <c r="ADZ84" s="67"/>
-      <c r="AEA84" s="67"/>
-      <c r="AEB84" s="67"/>
-      <c r="AEC84" s="67"/>
-      <c r="AED84" s="67"/>
-      <c r="AEE84" s="67"/>
-      <c r="AEF84" s="67"/>
-      <c r="AEG84" s="67"/>
-      <c r="AEH84" s="67"/>
-      <c r="AEI84" s="67"/>
-      <c r="AEJ84" s="67"/>
-      <c r="AEK84" s="67"/>
-      <c r="AEL84" s="67"/>
-      <c r="AEM84" s="67"/>
-      <c r="AEN84" s="67"/>
-      <c r="AEO84" s="67"/>
-      <c r="AEP84" s="67"/>
-      <c r="AEQ84" s="67"/>
-      <c r="AER84" s="67"/>
-      <c r="AES84" s="67"/>
-      <c r="AET84" s="67"/>
-      <c r="AEU84" s="67"/>
-      <c r="AEV84" s="67"/>
-      <c r="AEW84" s="67"/>
-      <c r="AEX84" s="67"/>
-      <c r="AEY84" s="67"/>
-      <c r="AEZ84" s="67"/>
-      <c r="AFA84" s="67"/>
-      <c r="AFB84" s="67"/>
-      <c r="AFC84" s="67"/>
-      <c r="AFD84" s="67"/>
-      <c r="AFE84" s="67"/>
-      <c r="AFF84" s="67"/>
-      <c r="AFG84" s="67"/>
-      <c r="AFH84" s="67"/>
-      <c r="AFI84" s="67"/>
-      <c r="AFJ84" s="67"/>
-      <c r="AFK84" s="67"/>
-      <c r="AFL84" s="67"/>
-      <c r="AFM84" s="67"/>
-      <c r="AFN84" s="67"/>
-      <c r="AFO84" s="67"/>
-      <c r="AFP84" s="67"/>
-      <c r="AFQ84" s="67"/>
-      <c r="AFR84" s="67"/>
-      <c r="AFS84" s="67"/>
-      <c r="AFT84" s="67"/>
-      <c r="AFU84" s="67"/>
-      <c r="AFV84" s="67"/>
-      <c r="AFW84" s="67"/>
-      <c r="AFX84" s="67"/>
-      <c r="AFY84" s="67"/>
-      <c r="AFZ84" s="67"/>
-      <c r="AGA84" s="67"/>
-      <c r="AGB84" s="67"/>
-      <c r="AGC84" s="67"/>
-      <c r="AGD84" s="67"/>
-      <c r="AGE84" s="67"/>
-      <c r="AGF84" s="67"/>
-      <c r="AGG84" s="67"/>
-      <c r="AGH84" s="67"/>
-      <c r="AGI84" s="67"/>
-      <c r="AGJ84" s="67"/>
-      <c r="AGK84" s="67"/>
-      <c r="AGL84" s="67"/>
-      <c r="AGM84" s="67"/>
-      <c r="AGN84" s="67"/>
-      <c r="AGO84" s="67"/>
-      <c r="AGP84" s="67"/>
-      <c r="AGQ84" s="67"/>
-      <c r="AGR84" s="67"/>
-      <c r="AGS84" s="67"/>
-      <c r="AGT84" s="67"/>
-      <c r="AGU84" s="67"/>
-      <c r="AGV84" s="67"/>
-      <c r="AGW84" s="67"/>
-      <c r="AGX84" s="67"/>
-      <c r="AGY84" s="67"/>
-      <c r="AGZ84" s="67"/>
-      <c r="AHA84" s="67"/>
-      <c r="AHB84" s="67"/>
-      <c r="AHC84" s="67"/>
-      <c r="AHD84" s="67"/>
-      <c r="AHE84" s="67"/>
-      <c r="AHF84" s="67"/>
-      <c r="AHG84" s="67"/>
-      <c r="AHH84" s="67"/>
-      <c r="AHI84" s="67"/>
-      <c r="AHJ84" s="67"/>
-      <c r="AHK84" s="67"/>
-      <c r="AHL84" s="67"/>
-      <c r="AHM84" s="67"/>
-      <c r="AHN84" s="67"/>
-      <c r="AHO84" s="67"/>
-      <c r="AHP84" s="67"/>
-      <c r="AHQ84" s="67"/>
-      <c r="AHR84" s="67"/>
-      <c r="AHS84" s="67"/>
-      <c r="AHT84" s="67"/>
-      <c r="AHU84" s="67"/>
-      <c r="AHV84" s="67"/>
-      <c r="AHW84" s="67"/>
-      <c r="AHX84" s="67"/>
-      <c r="AHY84" s="67"/>
-      <c r="AHZ84" s="67"/>
-      <c r="AIA84" s="67"/>
-      <c r="AIB84" s="67"/>
-      <c r="AIC84" s="67"/>
-      <c r="AID84" s="67"/>
-      <c r="AIE84" s="67"/>
-      <c r="AIF84" s="67"/>
-      <c r="AIG84" s="67"/>
-      <c r="AIH84" s="67"/>
-      <c r="AII84" s="67"/>
-      <c r="AIJ84" s="67"/>
-      <c r="AIK84" s="67"/>
-      <c r="AIL84" s="67"/>
-      <c r="AIM84" s="67"/>
-      <c r="AIN84" s="67"/>
-      <c r="AIO84" s="67"/>
-      <c r="AIP84" s="67"/>
-      <c r="AIQ84" s="67"/>
-      <c r="AIR84" s="67"/>
-      <c r="AIS84" s="67"/>
-      <c r="AIT84" s="67"/>
-      <c r="AIU84" s="67"/>
-      <c r="AIV84" s="67"/>
-      <c r="AIW84" s="67"/>
-      <c r="AIX84" s="67"/>
-      <c r="AIY84" s="67"/>
-      <c r="AIZ84" s="67"/>
-      <c r="AJA84" s="67"/>
-      <c r="AJB84" s="67"/>
-      <c r="AJC84" s="67"/>
-      <c r="AJD84" s="67"/>
-      <c r="AJE84" s="67"/>
-      <c r="AJF84" s="67"/>
-      <c r="AJG84" s="67"/>
-      <c r="AJH84" s="67"/>
-      <c r="AJI84" s="67"/>
-      <c r="AJJ84" s="67"/>
-      <c r="AJK84" s="67"/>
-      <c r="AJL84" s="67"/>
-      <c r="AJM84" s="67"/>
-      <c r="AJN84" s="67"/>
-      <c r="AJO84" s="67"/>
-      <c r="AJP84" s="67"/>
-      <c r="AJQ84" s="67"/>
-      <c r="AJR84" s="67"/>
-      <c r="AJS84" s="67"/>
-      <c r="AJT84" s="67"/>
-      <c r="AJU84" s="67"/>
-      <c r="AJV84" s="67"/>
-      <c r="AJW84" s="67"/>
-      <c r="AJX84" s="67"/>
-      <c r="AJY84" s="67"/>
-      <c r="AJZ84" s="67"/>
-      <c r="AKA84" s="67"/>
-      <c r="AKB84" s="67"/>
-      <c r="AKC84" s="67"/>
-      <c r="AKD84" s="67"/>
-      <c r="AKE84" s="67"/>
-      <c r="AKF84" s="67"/>
-      <c r="AKG84" s="67"/>
-      <c r="AKH84" s="67"/>
-      <c r="AKI84" s="67"/>
-      <c r="AKJ84" s="67"/>
-      <c r="AKK84" s="67"/>
-      <c r="AKL84" s="67"/>
-      <c r="AKM84" s="67"/>
-      <c r="AKN84" s="67"/>
-      <c r="AKO84" s="67"/>
-      <c r="AKP84" s="67"/>
-      <c r="AKQ84" s="67"/>
-      <c r="AKR84" s="67"/>
-      <c r="AKS84" s="67"/>
-      <c r="AKT84" s="67"/>
-      <c r="AKU84" s="67"/>
-      <c r="AKV84" s="67"/>
-      <c r="AKW84" s="67"/>
-      <c r="AKX84" s="67"/>
-      <c r="AKY84" s="67"/>
-      <c r="AKZ84" s="67"/>
-      <c r="ALA84" s="67"/>
-      <c r="ALB84" s="67"/>
-      <c r="ALC84" s="67"/>
-      <c r="ALD84" s="67"/>
-      <c r="ALE84" s="67"/>
-      <c r="ALF84" s="67"/>
-      <c r="ALG84" s="67"/>
-      <c r="ALH84" s="67"/>
-      <c r="ALI84" s="67"/>
-      <c r="ALJ84" s="67"/>
-      <c r="ALK84" s="67"/>
-      <c r="ALL84" s="67"/>
-      <c r="ALM84" s="67"/>
-      <c r="ALN84" s="67"/>
-      <c r="ALO84" s="67"/>
-      <c r="ALP84" s="67"/>
-      <c r="ALQ84" s="67"/>
-      <c r="ALR84" s="67"/>
-      <c r="ALS84" s="67"/>
-      <c r="ALT84" s="67"/>
-      <c r="ALU84" s="67"/>
-      <c r="ALV84" s="67"/>
-      <c r="ALW84" s="67"/>
-      <c r="ALX84" s="67"/>
-      <c r="ALY84" s="67"/>
-      <c r="ALZ84" s="67"/>
-      <c r="AMA84" s="67"/>
-      <c r="AMB84" s="67"/>
-      <c r="AMC84" s="67"/>
-      <c r="AMD84" s="67"/>
-      <c r="AME84" s="67"/>
-      <c r="AMF84" s="67"/>
-      <c r="AMG84" s="67"/>
-      <c r="AMH84" s="67"/>
+      <c r="H84" s="67"/>
+      <c r="I84" s="68"/>
+      <c r="J84" s="68"/>
+      <c r="K84" s="68"/>
+      <c r="L84" s="68"/>
+      <c r="M84" s="68"/>
+      <c r="N84" s="68"/>
+      <c r="O84" s="68"/>
+      <c r="P84" s="68"/>
+      <c r="Q84" s="68"/>
+      <c r="R84" s="68"/>
+      <c r="S84" s="68"/>
+      <c r="T84" s="68"/>
+      <c r="U84" s="68"/>
+      <c r="V84" s="68"/>
+      <c r="W84" s="68"/>
+      <c r="X84" s="68"/>
+      <c r="Y84" s="68"/>
+      <c r="Z84" s="68"/>
+      <c r="AA84" s="68"/>
+      <c r="AB84" s="68"/>
+      <c r="AC84" s="68"/>
+      <c r="AD84" s="68"/>
+      <c r="AE84" s="68"/>
+      <c r="AF84" s="68"/>
+      <c r="AG84" s="68"/>
+      <c r="AH84" s="68"/>
+      <c r="AI84" s="68"/>
+      <c r="AJ84" s="68"/>
+      <c r="AK84" s="68"/>
+      <c r="AL84" s="68"/>
+      <c r="AM84" s="68"/>
+      <c r="AN84" s="68"/>
+      <c r="AO84" s="68"/>
+      <c r="AP84" s="68"/>
+      <c r="AQ84" s="68"/>
+      <c r="AR84" s="68"/>
+      <c r="AS84" s="68"/>
+      <c r="AT84" s="68"/>
+      <c r="AU84" s="68"/>
+      <c r="AV84" s="68"/>
+      <c r="AW84" s="68"/>
+      <c r="AX84" s="68"/>
+      <c r="AY84" s="68"/>
+      <c r="AZ84" s="68"/>
+      <c r="BA84" s="68"/>
+      <c r="BB84" s="68"/>
+      <c r="BC84" s="68"/>
+      <c r="BD84" s="68"/>
+      <c r="BE84" s="68"/>
+      <c r="BF84" s="68"/>
+      <c r="BG84" s="68"/>
+      <c r="BH84" s="68"/>
+      <c r="BI84" s="68"/>
+      <c r="BJ84" s="68"/>
+      <c r="BK84" s="68"/>
+      <c r="BL84" s="68"/>
+      <c r="BM84" s="68"/>
+      <c r="BN84" s="68"/>
+      <c r="BO84" s="68"/>
+      <c r="BP84" s="68"/>
+      <c r="BQ84" s="68"/>
+      <c r="BR84" s="68"/>
+      <c r="BS84" s="68"/>
+      <c r="BT84" s="68"/>
+      <c r="BU84" s="68"/>
+      <c r="BV84" s="68"/>
+      <c r="BW84" s="68"/>
+      <c r="BX84" s="68"/>
+      <c r="BY84" s="68"/>
+      <c r="BZ84" s="68"/>
+      <c r="CA84" s="68"/>
+      <c r="CB84" s="68"/>
+      <c r="CC84" s="68"/>
+      <c r="CD84" s="68"/>
+      <c r="CE84" s="68"/>
+      <c r="CF84" s="68"/>
+      <c r="CG84" s="68"/>
+      <c r="CH84" s="68"/>
+      <c r="CI84" s="68"/>
+      <c r="CJ84" s="68"/>
+      <c r="CK84" s="68"/>
+      <c r="CL84" s="68"/>
+      <c r="CM84" s="68"/>
+      <c r="CN84" s="68"/>
+      <c r="CO84" s="68"/>
+      <c r="CP84" s="68"/>
+      <c r="CQ84" s="68"/>
+      <c r="CR84" s="68"/>
+      <c r="CS84" s="68"/>
+      <c r="CT84" s="68"/>
+      <c r="CU84" s="68"/>
+      <c r="CV84" s="68"/>
+      <c r="CW84" s="68"/>
+      <c r="CX84" s="68"/>
+      <c r="CY84" s="68"/>
+      <c r="CZ84" s="68"/>
+      <c r="DA84" s="68"/>
+      <c r="DB84" s="68"/>
+      <c r="DC84" s="68"/>
+      <c r="DD84" s="68"/>
+      <c r="DE84" s="68"/>
+      <c r="DF84" s="68"/>
+      <c r="DG84" s="68"/>
+      <c r="DH84" s="68"/>
+      <c r="DI84" s="68"/>
+      <c r="DJ84" s="68"/>
+      <c r="DK84" s="68"/>
+      <c r="DL84" s="68"/>
+      <c r="DM84" s="68"/>
+      <c r="DN84" s="68"/>
+      <c r="DO84" s="68"/>
+      <c r="DP84" s="68"/>
+      <c r="DQ84" s="68"/>
+      <c r="DR84" s="68"/>
+      <c r="DS84" s="68"/>
+      <c r="DT84" s="68"/>
+      <c r="DU84" s="68"/>
+      <c r="DV84" s="68"/>
+      <c r="DW84" s="68"/>
+      <c r="DX84" s="68"/>
+      <c r="DY84" s="68"/>
+      <c r="DZ84" s="68"/>
+      <c r="EA84" s="68"/>
+      <c r="EB84" s="68"/>
+      <c r="EC84" s="68"/>
+      <c r="ED84" s="68"/>
+      <c r="EE84" s="68"/>
+      <c r="EF84" s="68"/>
+      <c r="EG84" s="68"/>
+      <c r="EH84" s="68"/>
+      <c r="EI84" s="68"/>
+      <c r="EJ84" s="68"/>
+      <c r="EK84" s="68"/>
+      <c r="EL84" s="68"/>
+      <c r="EM84" s="68"/>
+      <c r="EN84" s="68"/>
+      <c r="EO84" s="68"/>
+      <c r="EP84" s="68"/>
+      <c r="EQ84" s="68"/>
+      <c r="ER84" s="68"/>
+      <c r="ES84" s="68"/>
+      <c r="ET84" s="68"/>
+      <c r="EU84" s="68"/>
+      <c r="EV84" s="68"/>
+      <c r="EW84" s="68"/>
+      <c r="EX84" s="68"/>
+      <c r="EY84" s="68"/>
+      <c r="EZ84" s="68"/>
+      <c r="FA84" s="68"/>
+      <c r="FB84" s="68"/>
+      <c r="FC84" s="68"/>
+      <c r="FD84" s="68"/>
+      <c r="FE84" s="68"/>
+      <c r="FF84" s="68"/>
+      <c r="FG84" s="68"/>
+      <c r="FH84" s="68"/>
+      <c r="FI84" s="68"/>
+      <c r="FJ84" s="68"/>
+      <c r="FK84" s="68"/>
+      <c r="FL84" s="68"/>
+      <c r="FM84" s="68"/>
+      <c r="FN84" s="68"/>
+      <c r="FO84" s="68"/>
+      <c r="FP84" s="68"/>
+      <c r="FQ84" s="68"/>
+      <c r="FR84" s="68"/>
+      <c r="FS84" s="68"/>
+      <c r="FT84" s="68"/>
+      <c r="FU84" s="68"/>
+      <c r="FV84" s="68"/>
+      <c r="FW84" s="68"/>
+      <c r="FX84" s="68"/>
+      <c r="FY84" s="68"/>
+      <c r="FZ84" s="68"/>
+      <c r="GA84" s="68"/>
+      <c r="GB84" s="68"/>
+      <c r="GC84" s="68"/>
+      <c r="GD84" s="68"/>
+      <c r="GE84" s="68"/>
+      <c r="GF84" s="68"/>
+      <c r="GG84" s="68"/>
+      <c r="GH84" s="68"/>
+      <c r="GI84" s="68"/>
+      <c r="GJ84" s="68"/>
+      <c r="GK84" s="68"/>
+      <c r="GL84" s="68"/>
+      <c r="GM84" s="68"/>
+      <c r="GN84" s="68"/>
+      <c r="GO84" s="68"/>
+      <c r="GP84" s="68"/>
+      <c r="GQ84" s="68"/>
+      <c r="GR84" s="68"/>
+      <c r="GS84" s="68"/>
+      <c r="GT84" s="68"/>
+      <c r="GU84" s="68"/>
+      <c r="GV84" s="68"/>
+      <c r="GW84" s="68"/>
+      <c r="GX84" s="68"/>
+      <c r="GY84" s="68"/>
+      <c r="GZ84" s="68"/>
+      <c r="HA84" s="68"/>
+      <c r="HB84" s="68"/>
+      <c r="HC84" s="68"/>
+      <c r="HD84" s="68"/>
+      <c r="HE84" s="68"/>
+      <c r="HF84" s="68"/>
+      <c r="HG84" s="68"/>
+      <c r="HH84" s="68"/>
+      <c r="HI84" s="68"/>
+      <c r="HJ84" s="68"/>
+      <c r="HK84" s="68"/>
+      <c r="HL84" s="68"/>
+      <c r="HM84" s="68"/>
+      <c r="HN84" s="68"/>
+      <c r="HO84" s="68"/>
+      <c r="HP84" s="68"/>
+      <c r="HQ84" s="68"/>
+      <c r="HR84" s="68"/>
+      <c r="HS84" s="68"/>
+      <c r="HT84" s="68"/>
+      <c r="HU84" s="68"/>
+      <c r="HV84" s="68"/>
+      <c r="HW84" s="68"/>
+      <c r="HX84" s="68"/>
+      <c r="HY84" s="68"/>
+      <c r="HZ84" s="68"/>
+      <c r="IA84" s="68"/>
+      <c r="IB84" s="68"/>
+      <c r="IC84" s="68"/>
+      <c r="ID84" s="68"/>
+      <c r="IE84" s="68"/>
+      <c r="IF84" s="68"/>
+      <c r="IG84" s="68"/>
+      <c r="IH84" s="68"/>
+      <c r="II84" s="68"/>
+      <c r="IJ84" s="68"/>
+      <c r="IK84" s="68"/>
+      <c r="IL84" s="68"/>
+      <c r="IM84" s="68"/>
+      <c r="IN84" s="68"/>
+      <c r="IO84" s="68"/>
+      <c r="IP84" s="68"/>
+      <c r="IQ84" s="68"/>
+      <c r="IR84" s="68"/>
+      <c r="IS84" s="68"/>
+      <c r="IT84" s="68"/>
+      <c r="IU84" s="68"/>
+      <c r="IV84" s="68"/>
+      <c r="IW84" s="68"/>
+      <c r="IX84" s="68"/>
+      <c r="IY84" s="68"/>
+      <c r="IZ84" s="68"/>
+      <c r="JA84" s="68"/>
+      <c r="JB84" s="68"/>
+      <c r="JC84" s="68"/>
+      <c r="JD84" s="68"/>
+      <c r="JE84" s="68"/>
+      <c r="JF84" s="68"/>
+      <c r="JG84" s="68"/>
+      <c r="JH84" s="68"/>
+      <c r="JI84" s="68"/>
+      <c r="JJ84" s="68"/>
+      <c r="JK84" s="68"/>
+      <c r="JL84" s="68"/>
+      <c r="JM84" s="68"/>
+      <c r="JN84" s="68"/>
+      <c r="JO84" s="68"/>
+      <c r="JP84" s="68"/>
+      <c r="JQ84" s="68"/>
+      <c r="JR84" s="68"/>
+      <c r="JS84" s="68"/>
+      <c r="JT84" s="68"/>
+      <c r="JU84" s="68"/>
+      <c r="JV84" s="68"/>
+      <c r="JW84" s="68"/>
+      <c r="JX84" s="68"/>
+      <c r="JY84" s="68"/>
+      <c r="JZ84" s="68"/>
+      <c r="KA84" s="68"/>
+      <c r="KB84" s="68"/>
+      <c r="KC84" s="68"/>
+      <c r="KD84" s="68"/>
+      <c r="KE84" s="68"/>
+      <c r="KF84" s="68"/>
+      <c r="KG84" s="68"/>
+      <c r="KH84" s="68"/>
+      <c r="KI84" s="68"/>
+      <c r="KJ84" s="68"/>
+      <c r="KK84" s="68"/>
+      <c r="KL84" s="68"/>
+      <c r="KM84" s="68"/>
+      <c r="KN84" s="68"/>
+      <c r="KO84" s="68"/>
+      <c r="KP84" s="68"/>
+      <c r="KQ84" s="68"/>
+      <c r="KR84" s="68"/>
+      <c r="KS84" s="68"/>
+      <c r="KT84" s="68"/>
+      <c r="KU84" s="68"/>
+      <c r="KV84" s="68"/>
+      <c r="KW84" s="68"/>
+      <c r="KX84" s="68"/>
+      <c r="KY84" s="68"/>
+      <c r="KZ84" s="68"/>
+      <c r="LA84" s="68"/>
+      <c r="LB84" s="68"/>
+      <c r="LC84" s="68"/>
+      <c r="LD84" s="68"/>
+      <c r="LE84" s="68"/>
+      <c r="LF84" s="68"/>
+      <c r="LG84" s="68"/>
+      <c r="LH84" s="68"/>
+      <c r="LI84" s="68"/>
+      <c r="LJ84" s="68"/>
+      <c r="LK84" s="68"/>
+      <c r="LL84" s="68"/>
+      <c r="LM84" s="68"/>
+      <c r="LN84" s="68"/>
+      <c r="LO84" s="68"/>
+      <c r="LP84" s="68"/>
+      <c r="LQ84" s="68"/>
+      <c r="LR84" s="68"/>
+      <c r="LS84" s="68"/>
+      <c r="LT84" s="68"/>
+      <c r="LU84" s="68"/>
+      <c r="LV84" s="68"/>
+      <c r="LW84" s="68"/>
+      <c r="LX84" s="68"/>
+      <c r="LY84" s="68"/>
+      <c r="LZ84" s="68"/>
+      <c r="MA84" s="68"/>
+      <c r="MB84" s="68"/>
+      <c r="MC84" s="68"/>
+      <c r="MD84" s="68"/>
+      <c r="ME84" s="68"/>
+      <c r="MF84" s="68"/>
+      <c r="MG84" s="68"/>
+      <c r="MH84" s="68"/>
+      <c r="MI84" s="68"/>
+      <c r="MJ84" s="68"/>
+      <c r="MK84" s="68"/>
+      <c r="ML84" s="68"/>
+      <c r="MM84" s="68"/>
+      <c r="MN84" s="68"/>
+      <c r="MO84" s="68"/>
+      <c r="MP84" s="68"/>
+      <c r="MQ84" s="68"/>
+      <c r="MR84" s="68"/>
+      <c r="MS84" s="68"/>
+      <c r="MT84" s="68"/>
+      <c r="MU84" s="68"/>
+      <c r="MV84" s="68"/>
+      <c r="MW84" s="68"/>
+      <c r="MX84" s="68"/>
+      <c r="MY84" s="68"/>
+      <c r="MZ84" s="68"/>
+      <c r="NA84" s="68"/>
+      <c r="NB84" s="68"/>
+      <c r="NC84" s="68"/>
+      <c r="ND84" s="68"/>
+      <c r="NE84" s="68"/>
+      <c r="NF84" s="68"/>
+      <c r="NG84" s="68"/>
+      <c r="NH84" s="68"/>
+      <c r="NI84" s="68"/>
+      <c r="NJ84" s="68"/>
+      <c r="NK84" s="68"/>
+      <c r="NL84" s="68"/>
+      <c r="NM84" s="68"/>
+      <c r="NN84" s="68"/>
+      <c r="NO84" s="68"/>
+      <c r="NP84" s="68"/>
+      <c r="NQ84" s="68"/>
+      <c r="NR84" s="68"/>
+      <c r="NS84" s="68"/>
+      <c r="NT84" s="68"/>
+      <c r="NU84" s="68"/>
+      <c r="NV84" s="68"/>
+      <c r="NW84" s="68"/>
+      <c r="NX84" s="68"/>
+      <c r="NY84" s="68"/>
+      <c r="NZ84" s="68"/>
+      <c r="OA84" s="68"/>
+      <c r="OB84" s="68"/>
+      <c r="OC84" s="68"/>
+      <c r="OD84" s="68"/>
+      <c r="OE84" s="68"/>
+      <c r="OF84" s="68"/>
+      <c r="OG84" s="68"/>
+      <c r="OH84" s="68"/>
+      <c r="OI84" s="68"/>
+      <c r="OJ84" s="68"/>
+      <c r="OK84" s="68"/>
+      <c r="OL84" s="68"/>
+      <c r="OM84" s="68"/>
+      <c r="ON84" s="68"/>
+      <c r="OO84" s="68"/>
+      <c r="OP84" s="68"/>
+      <c r="OQ84" s="68"/>
+      <c r="OR84" s="68"/>
+      <c r="OS84" s="68"/>
+      <c r="OT84" s="68"/>
+      <c r="OU84" s="68"/>
+      <c r="OV84" s="68"/>
+      <c r="OW84" s="68"/>
+      <c r="OX84" s="68"/>
+      <c r="OY84" s="68"/>
+      <c r="OZ84" s="68"/>
+      <c r="PA84" s="68"/>
+      <c r="PB84" s="68"/>
+      <c r="PC84" s="68"/>
+      <c r="PD84" s="68"/>
+      <c r="PE84" s="68"/>
+      <c r="PF84" s="68"/>
+      <c r="PG84" s="68"/>
+      <c r="PH84" s="68"/>
+      <c r="PI84" s="68"/>
+      <c r="PJ84" s="68"/>
+      <c r="PK84" s="68"/>
+      <c r="PL84" s="68"/>
+      <c r="PM84" s="68"/>
+      <c r="PN84" s="68"/>
+      <c r="PO84" s="68"/>
+      <c r="PP84" s="68"/>
+      <c r="PQ84" s="68"/>
+      <c r="PR84" s="68"/>
+      <c r="PS84" s="68"/>
+      <c r="PT84" s="68"/>
+      <c r="PU84" s="68"/>
+      <c r="PV84" s="68"/>
+      <c r="PW84" s="68"/>
+      <c r="PX84" s="68"/>
+      <c r="PY84" s="68"/>
+      <c r="PZ84" s="68"/>
+      <c r="QA84" s="68"/>
+      <c r="QB84" s="68"/>
+      <c r="QC84" s="68"/>
+      <c r="QD84" s="68"/>
+      <c r="QE84" s="68"/>
+      <c r="QF84" s="68"/>
+      <c r="QG84" s="68"/>
+      <c r="QH84" s="68"/>
+      <c r="QI84" s="68"/>
+      <c r="QJ84" s="68"/>
+      <c r="QK84" s="68"/>
+      <c r="QL84" s="68"/>
+      <c r="QM84" s="68"/>
+      <c r="QN84" s="68"/>
+      <c r="QO84" s="68"/>
+      <c r="QP84" s="68"/>
+      <c r="QQ84" s="68"/>
+      <c r="QR84" s="68"/>
+      <c r="QS84" s="68"/>
+      <c r="QT84" s="68"/>
+      <c r="QU84" s="68"/>
+      <c r="QV84" s="68"/>
+      <c r="QW84" s="68"/>
+      <c r="QX84" s="68"/>
+      <c r="QY84" s="68"/>
+      <c r="QZ84" s="68"/>
+      <c r="RA84" s="68"/>
+      <c r="RB84" s="68"/>
+      <c r="RC84" s="68"/>
+      <c r="RD84" s="68"/>
+      <c r="RE84" s="68"/>
+      <c r="RF84" s="68"/>
+      <c r="RG84" s="68"/>
+      <c r="RH84" s="68"/>
+      <c r="RI84" s="68"/>
+      <c r="RJ84" s="68"/>
+      <c r="RK84" s="68"/>
+      <c r="RL84" s="68"/>
+      <c r="RM84" s="68"/>
+      <c r="RN84" s="68"/>
+      <c r="RO84" s="68"/>
+      <c r="RP84" s="68"/>
+      <c r="RQ84" s="68"/>
+      <c r="RR84" s="68"/>
+      <c r="RS84" s="68"/>
+      <c r="RT84" s="68"/>
+      <c r="RU84" s="68"/>
+      <c r="RV84" s="68"/>
+      <c r="RW84" s="68"/>
+      <c r="RX84" s="68"/>
+      <c r="RY84" s="68"/>
+      <c r="RZ84" s="68"/>
+      <c r="SA84" s="68"/>
+      <c r="SB84" s="68"/>
+      <c r="SC84" s="68"/>
+      <c r="SD84" s="68"/>
+      <c r="SE84" s="68"/>
+      <c r="SF84" s="68"/>
+      <c r="SG84" s="68"/>
+      <c r="SH84" s="68"/>
+      <c r="SI84" s="68"/>
+      <c r="SJ84" s="68"/>
+      <c r="SK84" s="68"/>
+      <c r="SL84" s="68"/>
+      <c r="SM84" s="68"/>
+      <c r="SN84" s="68"/>
+      <c r="SO84" s="68"/>
+      <c r="SP84" s="68"/>
+      <c r="SQ84" s="68"/>
+      <c r="SR84" s="68"/>
+      <c r="SS84" s="68"/>
+      <c r="ST84" s="68"/>
+      <c r="SU84" s="68"/>
+      <c r="SV84" s="68"/>
+      <c r="SW84" s="68"/>
+      <c r="SX84" s="68"/>
+      <c r="SY84" s="68"/>
+      <c r="SZ84" s="68"/>
+      <c r="TA84" s="68"/>
+      <c r="TB84" s="68"/>
+      <c r="TC84" s="68"/>
+      <c r="TD84" s="68"/>
+      <c r="TE84" s="68"/>
+      <c r="TF84" s="68"/>
+      <c r="TG84" s="68"/>
+      <c r="TH84" s="68"/>
+      <c r="TI84" s="68"/>
+      <c r="TJ84" s="68"/>
+      <c r="TK84" s="68"/>
+      <c r="TL84" s="68"/>
+      <c r="TM84" s="68"/>
+      <c r="TN84" s="68"/>
+      <c r="TO84" s="68"/>
+      <c r="TP84" s="68"/>
+      <c r="TQ84" s="68"/>
+      <c r="TR84" s="68"/>
+      <c r="TS84" s="68"/>
+      <c r="TT84" s="68"/>
+      <c r="TU84" s="68"/>
+      <c r="TV84" s="68"/>
+      <c r="TW84" s="68"/>
+      <c r="TX84" s="68"/>
+      <c r="TY84" s="68"/>
+      <c r="TZ84" s="68"/>
+      <c r="UA84" s="68"/>
+      <c r="UB84" s="68"/>
+      <c r="UC84" s="68"/>
+      <c r="UD84" s="68"/>
+      <c r="UE84" s="68"/>
+      <c r="UF84" s="68"/>
+      <c r="UG84" s="68"/>
+      <c r="UH84" s="68"/>
+      <c r="UI84" s="68"/>
+      <c r="UJ84" s="68"/>
+      <c r="UK84" s="68"/>
+      <c r="UL84" s="68"/>
+      <c r="UM84" s="68"/>
+      <c r="UN84" s="68"/>
+      <c r="UO84" s="68"/>
+      <c r="UP84" s="68"/>
+      <c r="UQ84" s="68"/>
+      <c r="UR84" s="68"/>
+      <c r="US84" s="68"/>
+      <c r="UT84" s="68"/>
+      <c r="UU84" s="68"/>
+      <c r="UV84" s="68"/>
+      <c r="UW84" s="68"/>
+      <c r="UX84" s="68"/>
+      <c r="UY84" s="68"/>
+      <c r="UZ84" s="68"/>
+      <c r="VA84" s="68"/>
+      <c r="VB84" s="68"/>
+      <c r="VC84" s="68"/>
+      <c r="VD84" s="68"/>
+      <c r="VE84" s="68"/>
+      <c r="VF84" s="68"/>
+      <c r="VG84" s="68"/>
+      <c r="VH84" s="68"/>
+      <c r="VI84" s="68"/>
+      <c r="VJ84" s="68"/>
+      <c r="VK84" s="68"/>
+      <c r="VL84" s="68"/>
+      <c r="VM84" s="68"/>
+      <c r="VN84" s="68"/>
+      <c r="VO84" s="68"/>
+      <c r="VP84" s="68"/>
+      <c r="VQ84" s="68"/>
+      <c r="VR84" s="68"/>
+      <c r="VS84" s="68"/>
+      <c r="VT84" s="68"/>
+      <c r="VU84" s="68"/>
+      <c r="VV84" s="68"/>
+      <c r="VW84" s="68"/>
+      <c r="VX84" s="68"/>
+      <c r="VY84" s="68"/>
+      <c r="VZ84" s="68"/>
+      <c r="WA84" s="68"/>
+      <c r="WB84" s="68"/>
+      <c r="WC84" s="68"/>
+      <c r="WD84" s="68"/>
+      <c r="WE84" s="68"/>
+      <c r="WF84" s="68"/>
+      <c r="WG84" s="68"/>
+      <c r="WH84" s="68"/>
+      <c r="WI84" s="68"/>
+      <c r="WJ84" s="68"/>
+      <c r="WK84" s="68"/>
+      <c r="WL84" s="68"/>
+      <c r="WM84" s="68"/>
+      <c r="WN84" s="68"/>
+      <c r="WO84" s="68"/>
+      <c r="WP84" s="68"/>
+      <c r="WQ84" s="68"/>
+      <c r="WR84" s="68"/>
+      <c r="WS84" s="68"/>
+      <c r="WT84" s="68"/>
+      <c r="WU84" s="68"/>
+      <c r="WV84" s="68"/>
+      <c r="WW84" s="68"/>
+      <c r="WX84" s="68"/>
+      <c r="WY84" s="68"/>
+      <c r="WZ84" s="68"/>
+      <c r="XA84" s="68"/>
+      <c r="XB84" s="68"/>
+      <c r="XC84" s="68"/>
+      <c r="XD84" s="68"/>
+      <c r="XE84" s="68"/>
+      <c r="XF84" s="68"/>
+      <c r="XG84" s="68"/>
+      <c r="XH84" s="68"/>
+      <c r="XI84" s="68"/>
+      <c r="XJ84" s="68"/>
+      <c r="XK84" s="68"/>
+      <c r="XL84" s="68"/>
+      <c r="XM84" s="68"/>
+      <c r="XN84" s="68"/>
+      <c r="XO84" s="68"/>
+      <c r="XP84" s="68"/>
+      <c r="XQ84" s="68"/>
+      <c r="XR84" s="68"/>
+      <c r="XS84" s="68"/>
+      <c r="XT84" s="68"/>
+      <c r="XU84" s="68"/>
+      <c r="XV84" s="68"/>
+      <c r="XW84" s="68"/>
+      <c r="XX84" s="68"/>
+      <c r="XY84" s="68"/>
+      <c r="XZ84" s="68"/>
+      <c r="YA84" s="68"/>
+      <c r="YB84" s="68"/>
+      <c r="YC84" s="68"/>
+      <c r="YD84" s="68"/>
+      <c r="YE84" s="68"/>
+      <c r="YF84" s="68"/>
+      <c r="YG84" s="68"/>
+      <c r="YH84" s="68"/>
+      <c r="YI84" s="68"/>
+      <c r="YJ84" s="68"/>
+      <c r="YK84" s="68"/>
+      <c r="YL84" s="68"/>
+      <c r="YM84" s="68"/>
+      <c r="YN84" s="68"/>
+      <c r="YO84" s="68"/>
+      <c r="YP84" s="68"/>
+      <c r="YQ84" s="68"/>
+      <c r="YR84" s="68"/>
+      <c r="YS84" s="68"/>
+      <c r="YT84" s="68"/>
+      <c r="YU84" s="68"/>
+      <c r="YV84" s="68"/>
+      <c r="YW84" s="68"/>
+      <c r="YX84" s="68"/>
+      <c r="YY84" s="68"/>
+      <c r="YZ84" s="68"/>
+      <c r="ZA84" s="68"/>
+      <c r="ZB84" s="68"/>
+      <c r="ZC84" s="68"/>
+      <c r="ZD84" s="68"/>
+      <c r="ZE84" s="68"/>
+      <c r="ZF84" s="68"/>
+      <c r="ZG84" s="68"/>
+      <c r="ZH84" s="68"/>
+      <c r="ZI84" s="68"/>
+      <c r="ZJ84" s="68"/>
+      <c r="ZK84" s="68"/>
+      <c r="ZL84" s="68"/>
+      <c r="ZM84" s="68"/>
+      <c r="ZN84" s="68"/>
+      <c r="ZO84" s="68"/>
+      <c r="ZP84" s="68"/>
+      <c r="ZQ84" s="68"/>
+      <c r="ZR84" s="68"/>
+      <c r="ZS84" s="68"/>
+      <c r="ZT84" s="68"/>
+      <c r="ZU84" s="68"/>
+      <c r="ZV84" s="68"/>
+      <c r="ZW84" s="68"/>
+      <c r="ZX84" s="68"/>
+      <c r="ZY84" s="68"/>
+      <c r="ZZ84" s="68"/>
+      <c r="AAA84" s="68"/>
+      <c r="AAB84" s="68"/>
+      <c r="AAC84" s="68"/>
+      <c r="AAD84" s="68"/>
+      <c r="AAE84" s="68"/>
+      <c r="AAF84" s="68"/>
+      <c r="AAG84" s="68"/>
+      <c r="AAH84" s="68"/>
+      <c r="AAI84" s="68"/>
+      <c r="AAJ84" s="68"/>
+      <c r="AAK84" s="68"/>
+      <c r="AAL84" s="68"/>
+      <c r="AAM84" s="68"/>
+      <c r="AAN84" s="68"/>
+      <c r="AAO84" s="68"/>
+      <c r="AAP84" s="68"/>
+      <c r="AAQ84" s="68"/>
+      <c r="AAR84" s="68"/>
+      <c r="AAS84" s="68"/>
+      <c r="AAT84" s="68"/>
+      <c r="AAU84" s="68"/>
+      <c r="AAV84" s="68"/>
+      <c r="AAW84" s="68"/>
+      <c r="AAX84" s="68"/>
+      <c r="AAY84" s="68"/>
+      <c r="AAZ84" s="68"/>
+      <c r="ABA84" s="68"/>
+      <c r="ABB84" s="68"/>
+      <c r="ABC84" s="68"/>
+      <c r="ABD84" s="68"/>
+      <c r="ABE84" s="68"/>
+      <c r="ABF84" s="68"/>
+      <c r="ABG84" s="68"/>
+      <c r="ABH84" s="68"/>
+      <c r="ABI84" s="68"/>
+      <c r="ABJ84" s="68"/>
+      <c r="ABK84" s="68"/>
+      <c r="ABL84" s="68"/>
+      <c r="ABM84" s="68"/>
+      <c r="ABN84" s="68"/>
+      <c r="ABO84" s="68"/>
+      <c r="ABP84" s="68"/>
+      <c r="ABQ84" s="68"/>
+      <c r="ABR84" s="68"/>
+      <c r="ABS84" s="68"/>
+      <c r="ABT84" s="68"/>
+      <c r="ABU84" s="68"/>
+      <c r="ABV84" s="68"/>
+      <c r="ABW84" s="68"/>
+      <c r="ABX84" s="68"/>
+      <c r="ABY84" s="68"/>
+      <c r="ABZ84" s="68"/>
+      <c r="ACA84" s="68"/>
+      <c r="ACB84" s="68"/>
+      <c r="ACC84" s="68"/>
+      <c r="ACD84" s="68"/>
+      <c r="ACE84" s="68"/>
+      <c r="ACF84" s="68"/>
+      <c r="ACG84" s="68"/>
+      <c r="ACH84" s="68"/>
+      <c r="ACI84" s="68"/>
+      <c r="ACJ84" s="68"/>
+      <c r="ACK84" s="68"/>
+      <c r="ACL84" s="68"/>
+      <c r="ACM84" s="68"/>
+      <c r="ACN84" s="68"/>
+      <c r="ACO84" s="68"/>
+      <c r="ACP84" s="68"/>
+      <c r="ACQ84" s="68"/>
+      <c r="ACR84" s="68"/>
+      <c r="ACS84" s="68"/>
+      <c r="ACT84" s="68"/>
+      <c r="ACU84" s="68"/>
+      <c r="ACV84" s="68"/>
+      <c r="ACW84" s="68"/>
+      <c r="ACX84" s="68"/>
+      <c r="ACY84" s="68"/>
+      <c r="ACZ84" s="68"/>
+      <c r="ADA84" s="68"/>
+      <c r="ADB84" s="68"/>
+      <c r="ADC84" s="68"/>
+      <c r="ADD84" s="68"/>
+      <c r="ADE84" s="68"/>
+      <c r="ADF84" s="68"/>
+      <c r="ADG84" s="68"/>
+      <c r="ADH84" s="68"/>
+      <c r="ADI84" s="68"/>
+      <c r="ADJ84" s="68"/>
+      <c r="ADK84" s="68"/>
+      <c r="ADL84" s="68"/>
+      <c r="ADM84" s="68"/>
+      <c r="ADN84" s="68"/>
+      <c r="ADO84" s="68"/>
+      <c r="ADP84" s="68"/>
+      <c r="ADQ84" s="68"/>
+      <c r="ADR84" s="68"/>
+      <c r="ADS84" s="68"/>
+      <c r="ADT84" s="68"/>
+      <c r="ADU84" s="68"/>
+      <c r="ADV84" s="68"/>
+      <c r="ADW84" s="68"/>
+      <c r="ADX84" s="68"/>
+      <c r="ADY84" s="68"/>
+      <c r="ADZ84" s="68"/>
+      <c r="AEA84" s="68"/>
+      <c r="AEB84" s="68"/>
+      <c r="AEC84" s="68"/>
+      <c r="AED84" s="68"/>
+      <c r="AEE84" s="68"/>
+      <c r="AEF84" s="68"/>
+      <c r="AEG84" s="68"/>
+      <c r="AEH84" s="68"/>
+      <c r="AEI84" s="68"/>
+      <c r="AEJ84" s="68"/>
+      <c r="AEK84" s="68"/>
+      <c r="AEL84" s="68"/>
+      <c r="AEM84" s="68"/>
+      <c r="AEN84" s="68"/>
+      <c r="AEO84" s="68"/>
+      <c r="AEP84" s="68"/>
+      <c r="AEQ84" s="68"/>
+      <c r="AER84" s="68"/>
+      <c r="AES84" s="68"/>
+      <c r="AET84" s="68"/>
+      <c r="AEU84" s="68"/>
+      <c r="AEV84" s="68"/>
+      <c r="AEW84" s="68"/>
+      <c r="AEX84" s="68"/>
+      <c r="AEY84" s="68"/>
+      <c r="AEZ84" s="68"/>
+      <c r="AFA84" s="68"/>
+      <c r="AFB84" s="68"/>
+      <c r="AFC84" s="68"/>
+      <c r="AFD84" s="68"/>
+      <c r="AFE84" s="68"/>
+      <c r="AFF84" s="68"/>
+      <c r="AFG84" s="68"/>
+      <c r="AFH84" s="68"/>
+      <c r="AFI84" s="68"/>
+      <c r="AFJ84" s="68"/>
+      <c r="AFK84" s="68"/>
+      <c r="AFL84" s="68"/>
+      <c r="AFM84" s="68"/>
+      <c r="AFN84" s="68"/>
+      <c r="AFO84" s="68"/>
+      <c r="AFP84" s="68"/>
+      <c r="AFQ84" s="68"/>
+      <c r="AFR84" s="68"/>
+      <c r="AFS84" s="68"/>
+      <c r="AFT84" s="68"/>
+      <c r="AFU84" s="68"/>
+      <c r="AFV84" s="68"/>
+      <c r="AFW84" s="68"/>
+      <c r="AFX84" s="68"/>
+      <c r="AFY84" s="68"/>
+      <c r="AFZ84" s="68"/>
+      <c r="AGA84" s="68"/>
+      <c r="AGB84" s="68"/>
+      <c r="AGC84" s="68"/>
+      <c r="AGD84" s="68"/>
+      <c r="AGE84" s="68"/>
+      <c r="AGF84" s="68"/>
+      <c r="AGG84" s="68"/>
+      <c r="AGH84" s="68"/>
+      <c r="AGI84" s="68"/>
+      <c r="AGJ84" s="68"/>
+      <c r="AGK84" s="68"/>
+      <c r="AGL84" s="68"/>
+      <c r="AGM84" s="68"/>
+      <c r="AGN84" s="68"/>
+      <c r="AGO84" s="68"/>
+      <c r="AGP84" s="68"/>
+      <c r="AGQ84" s="68"/>
+      <c r="AGR84" s="68"/>
+      <c r="AGS84" s="68"/>
+      <c r="AGT84" s="68"/>
+      <c r="AGU84" s="68"/>
+      <c r="AGV84" s="68"/>
+      <c r="AGW84" s="68"/>
+      <c r="AGX84" s="68"/>
+      <c r="AGY84" s="68"/>
+      <c r="AGZ84" s="68"/>
+      <c r="AHA84" s="68"/>
+      <c r="AHB84" s="68"/>
+      <c r="AHC84" s="68"/>
+      <c r="AHD84" s="68"/>
+      <c r="AHE84" s="68"/>
+      <c r="AHF84" s="68"/>
+      <c r="AHG84" s="68"/>
+      <c r="AHH84" s="68"/>
+      <c r="AHI84" s="68"/>
+      <c r="AHJ84" s="68"/>
+      <c r="AHK84" s="68"/>
+      <c r="AHL84" s="68"/>
+      <c r="AHM84" s="68"/>
+      <c r="AHN84" s="68"/>
+      <c r="AHO84" s="68"/>
+      <c r="AHP84" s="68"/>
+      <c r="AHQ84" s="68"/>
+      <c r="AHR84" s="68"/>
+      <c r="AHS84" s="68"/>
+      <c r="AHT84" s="68"/>
+      <c r="AHU84" s="68"/>
+      <c r="AHV84" s="68"/>
+      <c r="AHW84" s="68"/>
+      <c r="AHX84" s="68"/>
+      <c r="AHY84" s="68"/>
+      <c r="AHZ84" s="68"/>
+      <c r="AIA84" s="68"/>
+      <c r="AIB84" s="68"/>
+      <c r="AIC84" s="68"/>
+      <c r="AID84" s="68"/>
+      <c r="AIE84" s="68"/>
+      <c r="AIF84" s="68"/>
+      <c r="AIG84" s="68"/>
+      <c r="AIH84" s="68"/>
+      <c r="AII84" s="68"/>
+      <c r="AIJ84" s="68"/>
+      <c r="AIK84" s="68"/>
+      <c r="AIL84" s="68"/>
+      <c r="AIM84" s="68"/>
+      <c r="AIN84" s="68"/>
+      <c r="AIO84" s="68"/>
+      <c r="AIP84" s="68"/>
+      <c r="AIQ84" s="68"/>
+      <c r="AIR84" s="68"/>
+      <c r="AIS84" s="68"/>
+      <c r="AIT84" s="68"/>
+      <c r="AIU84" s="68"/>
+      <c r="AIV84" s="68"/>
+      <c r="AIW84" s="68"/>
+      <c r="AIX84" s="68"/>
+      <c r="AIY84" s="68"/>
+      <c r="AIZ84" s="68"/>
+      <c r="AJA84" s="68"/>
+      <c r="AJB84" s="68"/>
+      <c r="AJC84" s="68"/>
+      <c r="AJD84" s="68"/>
+      <c r="AJE84" s="68"/>
+      <c r="AJF84" s="68"/>
+      <c r="AJG84" s="68"/>
+      <c r="AJH84" s="68"/>
+      <c r="AJI84" s="68"/>
+      <c r="AJJ84" s="68"/>
+      <c r="AJK84" s="68"/>
+      <c r="AJL84" s="68"/>
+      <c r="AJM84" s="68"/>
+      <c r="AJN84" s="68"/>
+      <c r="AJO84" s="68"/>
+      <c r="AJP84" s="68"/>
+      <c r="AJQ84" s="68"/>
+      <c r="AJR84" s="68"/>
+      <c r="AJS84" s="68"/>
+      <c r="AJT84" s="68"/>
+      <c r="AJU84" s="68"/>
+      <c r="AJV84" s="68"/>
+      <c r="AJW84" s="68"/>
+      <c r="AJX84" s="68"/>
+      <c r="AJY84" s="68"/>
+      <c r="AJZ84" s="68"/>
+      <c r="AKA84" s="68"/>
+      <c r="AKB84" s="68"/>
+      <c r="AKC84" s="68"/>
+      <c r="AKD84" s="68"/>
+      <c r="AKE84" s="68"/>
+      <c r="AKF84" s="68"/>
+      <c r="AKG84" s="68"/>
+      <c r="AKH84" s="68"/>
+      <c r="AKI84" s="68"/>
+      <c r="AKJ84" s="68"/>
+      <c r="AKK84" s="68"/>
+      <c r="AKL84" s="68"/>
+      <c r="AKM84" s="68"/>
+      <c r="AKN84" s="68"/>
+      <c r="AKO84" s="68"/>
+      <c r="AKP84" s="68"/>
+      <c r="AKQ84" s="68"/>
+      <c r="AKR84" s="68"/>
+      <c r="AKS84" s="68"/>
+      <c r="AKT84" s="68"/>
+      <c r="AKU84" s="68"/>
+      <c r="AKV84" s="68"/>
+      <c r="AKW84" s="68"/>
+      <c r="AKX84" s="68"/>
+      <c r="AKY84" s="68"/>
+      <c r="AKZ84" s="68"/>
+      <c r="ALA84" s="68"/>
+      <c r="ALB84" s="68"/>
+      <c r="ALC84" s="68"/>
+      <c r="ALD84" s="68"/>
+      <c r="ALE84" s="68"/>
+      <c r="ALF84" s="68"/>
+      <c r="ALG84" s="68"/>
+      <c r="ALH84" s="68"/>
+      <c r="ALI84" s="68"/>
+      <c r="ALJ84" s="68"/>
+      <c r="ALK84" s="68"/>
+      <c r="ALL84" s="68"/>
+      <c r="ALM84" s="68"/>
+      <c r="ALN84" s="68"/>
+      <c r="ALO84" s="68"/>
+      <c r="ALP84" s="68"/>
+      <c r="ALQ84" s="68"/>
+      <c r="ALR84" s="68"/>
+      <c r="ALS84" s="68"/>
+      <c r="ALT84" s="68"/>
+      <c r="ALU84" s="68"/>
+      <c r="ALV84" s="68"/>
+      <c r="ALW84" s="68"/>
+      <c r="ALX84" s="68"/>
+      <c r="ALY84" s="68"/>
+      <c r="ALZ84" s="68"/>
+      <c r="AMA84" s="68"/>
+      <c r="AMB84" s="68"/>
+      <c r="AMC84" s="68"/>
+      <c r="AMD84" s="68"/>
+      <c r="AME84" s="68"/>
+      <c r="AMF84" s="68"/>
+      <c r="AMG84" s="68"/>
+      <c r="AMH84" s="68"/>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="1" t="s">
@@ -20380,6 +20399,52 @@
       </c>
       <c r="G85" s="12">
         <v>0.9683</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C86" s="10">
+        <v>0.9944397</v>
+      </c>
+      <c r="D86" s="10">
+        <v>0.9636514</v>
+      </c>
+      <c r="E86" s="10">
+        <v>0.9957162</v>
+      </c>
+      <c r="F86" s="11">
+        <v>0.9669696</v>
+      </c>
+      <c r="G86" s="12">
+        <v>0.9686</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" s="61" t="s">
+        <v>147</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C87" s="10">
+        <v>0.9954566</v>
+      </c>
+      <c r="D87" s="10">
+        <v>0.9638042</v>
+      </c>
+      <c r="E87" s="10">
+        <v>0.9965423</v>
+      </c>
+      <c r="F87" s="11">
+        <v>0.967112</v>
+      </c>
+      <c r="G87" s="12">
+        <v>0.9685</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
320 baseline + diff_action_type_time_delta 15 16， 0.96950
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="7860" tabRatio="993"/>
+    <workbookView windowWidth="28695" windowHeight="13305" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="特征选取" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163">
   <si>
     <r>
       <rPr>
@@ -1423,6 +1423,34 @@
   <si>
     <t>344</t>
   </si>
+  <si>
+    <t>diff_action_type_time_delta 25 35</t>
+  </si>
+  <si>
+    <t>348</t>
+  </si>
+  <si>
+    <t>baseline + diff_action_type_time_delta 15</t>
+  </si>
+  <si>
+    <t>320 baseline + diff_action_type_time_delta 15 16</t>
+  </si>
+  <si>
+    <r>
+      <t>添加</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> baseline_features</t>
+    </r>
+  </si>
+  <si>
+    <t>347</t>
+  </si>
 </sst>
 </file>
 
@@ -1436,7 +1464,7 @@
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1462,6 +1490,10 @@
       <sz val="8"/>
       <color rgb="FFFF0000"/>
       <name val="DejaVu Sans Mono"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1998,142 +2030,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2320,10 +2352,13 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2670,8 +2705,8 @@
   <sheetPr/>
   <dimension ref="A1:AMH138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -7986,7 +8021,7 @@
       <c r="AMH13" s="47"/>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:1022">
-      <c r="A14" s="70" t="s">
+      <c r="A14" s="71" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="19" t="s">
@@ -18222,7 +18257,7 @@
       <c r="G72" s="35">
         <v>0.96859</v>
       </c>
-      <c r="H72" s="62" t="s">
+      <c r="H72" s="63" t="s">
         <v>125</v>
       </c>
       <c r="I72" s="46"/>
@@ -19262,7 +19297,7 @@
       <c r="G73" s="12">
         <v>0.9684</v>
       </c>
-      <c r="H73" s="63" t="s">
+      <c r="H73" s="64" t="s">
         <v>127</v>
       </c>
     </row>
@@ -19328,7 +19363,7 @@
       <c r="F76" s="20">
         <v>0.9671155</v>
       </c>
-      <c r="G76" s="64">
+      <c r="G76" s="65">
         <v>0.9682</v>
       </c>
     </row>
@@ -19351,7 +19386,7 @@
       <c r="F78" s="57">
         <v>0.9666471</v>
       </c>
-      <c r="G78" s="65">
+      <c r="G78" s="66">
         <v>0.9678</v>
       </c>
     </row>
@@ -19466,1024 +19501,1024 @@
       <c r="F84" s="60">
         <v>0.9673051</v>
       </c>
-      <c r="G84" s="66">
+      <c r="G84" s="67">
         <v>0.9686</v>
       </c>
-      <c r="H84" s="67"/>
-      <c r="I84" s="69"/>
-      <c r="J84" s="69"/>
-      <c r="K84" s="69"/>
-      <c r="L84" s="69"/>
-      <c r="M84" s="69"/>
-      <c r="N84" s="69"/>
-      <c r="O84" s="69"/>
-      <c r="P84" s="69"/>
-      <c r="Q84" s="69"/>
-      <c r="R84" s="69"/>
-      <c r="S84" s="69"/>
-      <c r="T84" s="69"/>
-      <c r="U84" s="69"/>
-      <c r="V84" s="69"/>
-      <c r="W84" s="69"/>
-      <c r="X84" s="69"/>
-      <c r="Y84" s="69"/>
-      <c r="Z84" s="69"/>
-      <c r="AA84" s="69"/>
-      <c r="AB84" s="69"/>
-      <c r="AC84" s="69"/>
-      <c r="AD84" s="69"/>
-      <c r="AE84" s="69"/>
-      <c r="AF84" s="69"/>
-      <c r="AG84" s="69"/>
-      <c r="AH84" s="69"/>
-      <c r="AI84" s="69"/>
-      <c r="AJ84" s="69"/>
-      <c r="AK84" s="69"/>
-      <c r="AL84" s="69"/>
-      <c r="AM84" s="69"/>
-      <c r="AN84" s="69"/>
-      <c r="AO84" s="69"/>
-      <c r="AP84" s="69"/>
-      <c r="AQ84" s="69"/>
-      <c r="AR84" s="69"/>
-      <c r="AS84" s="69"/>
-      <c r="AT84" s="69"/>
-      <c r="AU84" s="69"/>
-      <c r="AV84" s="69"/>
-      <c r="AW84" s="69"/>
-      <c r="AX84" s="69"/>
-      <c r="AY84" s="69"/>
-      <c r="AZ84" s="69"/>
-      <c r="BA84" s="69"/>
-      <c r="BB84" s="69"/>
-      <c r="BC84" s="69"/>
-      <c r="BD84" s="69"/>
-      <c r="BE84" s="69"/>
-      <c r="BF84" s="69"/>
-      <c r="BG84" s="69"/>
-      <c r="BH84" s="69"/>
-      <c r="BI84" s="69"/>
-      <c r="BJ84" s="69"/>
-      <c r="BK84" s="69"/>
-      <c r="BL84" s="69"/>
-      <c r="BM84" s="69"/>
-      <c r="BN84" s="69"/>
-      <c r="BO84" s="69"/>
-      <c r="BP84" s="69"/>
-      <c r="BQ84" s="69"/>
-      <c r="BR84" s="69"/>
-      <c r="BS84" s="69"/>
-      <c r="BT84" s="69"/>
-      <c r="BU84" s="69"/>
-      <c r="BV84" s="69"/>
-      <c r="BW84" s="69"/>
-      <c r="BX84" s="69"/>
-      <c r="BY84" s="69"/>
-      <c r="BZ84" s="69"/>
-      <c r="CA84" s="69"/>
-      <c r="CB84" s="69"/>
-      <c r="CC84" s="69"/>
-      <c r="CD84" s="69"/>
-      <c r="CE84" s="69"/>
-      <c r="CF84" s="69"/>
-      <c r="CG84" s="69"/>
-      <c r="CH84" s="69"/>
-      <c r="CI84" s="69"/>
-      <c r="CJ84" s="69"/>
-      <c r="CK84" s="69"/>
-      <c r="CL84" s="69"/>
-      <c r="CM84" s="69"/>
-      <c r="CN84" s="69"/>
-      <c r="CO84" s="69"/>
-      <c r="CP84" s="69"/>
-      <c r="CQ84" s="69"/>
-      <c r="CR84" s="69"/>
-      <c r="CS84" s="69"/>
-      <c r="CT84" s="69"/>
-      <c r="CU84" s="69"/>
-      <c r="CV84" s="69"/>
-      <c r="CW84" s="69"/>
-      <c r="CX84" s="69"/>
-      <c r="CY84" s="69"/>
-      <c r="CZ84" s="69"/>
-      <c r="DA84" s="69"/>
-      <c r="DB84" s="69"/>
-      <c r="DC84" s="69"/>
-      <c r="DD84" s="69"/>
-      <c r="DE84" s="69"/>
-      <c r="DF84" s="69"/>
-      <c r="DG84" s="69"/>
-      <c r="DH84" s="69"/>
-      <c r="DI84" s="69"/>
-      <c r="DJ84" s="69"/>
-      <c r="DK84" s="69"/>
-      <c r="DL84" s="69"/>
-      <c r="DM84" s="69"/>
-      <c r="DN84" s="69"/>
-      <c r="DO84" s="69"/>
-      <c r="DP84" s="69"/>
-      <c r="DQ84" s="69"/>
-      <c r="DR84" s="69"/>
-      <c r="DS84" s="69"/>
-      <c r="DT84" s="69"/>
-      <c r="DU84" s="69"/>
-      <c r="DV84" s="69"/>
-      <c r="DW84" s="69"/>
-      <c r="DX84" s="69"/>
-      <c r="DY84" s="69"/>
-      <c r="DZ84" s="69"/>
-      <c r="EA84" s="69"/>
-      <c r="EB84" s="69"/>
-      <c r="EC84" s="69"/>
-      <c r="ED84" s="69"/>
-      <c r="EE84" s="69"/>
-      <c r="EF84" s="69"/>
-      <c r="EG84" s="69"/>
-      <c r="EH84" s="69"/>
-      <c r="EI84" s="69"/>
-      <c r="EJ84" s="69"/>
-      <c r="EK84" s="69"/>
-      <c r="EL84" s="69"/>
-      <c r="EM84" s="69"/>
-      <c r="EN84" s="69"/>
-      <c r="EO84" s="69"/>
-      <c r="EP84" s="69"/>
-      <c r="EQ84" s="69"/>
-      <c r="ER84" s="69"/>
-      <c r="ES84" s="69"/>
-      <c r="ET84" s="69"/>
-      <c r="EU84" s="69"/>
-      <c r="EV84" s="69"/>
-      <c r="EW84" s="69"/>
-      <c r="EX84" s="69"/>
-      <c r="EY84" s="69"/>
-      <c r="EZ84" s="69"/>
-      <c r="FA84" s="69"/>
-      <c r="FB84" s="69"/>
-      <c r="FC84" s="69"/>
-      <c r="FD84" s="69"/>
-      <c r="FE84" s="69"/>
-      <c r="FF84" s="69"/>
-      <c r="FG84" s="69"/>
-      <c r="FH84" s="69"/>
-      <c r="FI84" s="69"/>
-      <c r="FJ84" s="69"/>
-      <c r="FK84" s="69"/>
-      <c r="FL84" s="69"/>
-      <c r="FM84" s="69"/>
-      <c r="FN84" s="69"/>
-      <c r="FO84" s="69"/>
-      <c r="FP84" s="69"/>
-      <c r="FQ84" s="69"/>
-      <c r="FR84" s="69"/>
-      <c r="FS84" s="69"/>
-      <c r="FT84" s="69"/>
-      <c r="FU84" s="69"/>
-      <c r="FV84" s="69"/>
-      <c r="FW84" s="69"/>
-      <c r="FX84" s="69"/>
-      <c r="FY84" s="69"/>
-      <c r="FZ84" s="69"/>
-      <c r="GA84" s="69"/>
-      <c r="GB84" s="69"/>
-      <c r="GC84" s="69"/>
-      <c r="GD84" s="69"/>
-      <c r="GE84" s="69"/>
-      <c r="GF84" s="69"/>
-      <c r="GG84" s="69"/>
-      <c r="GH84" s="69"/>
-      <c r="GI84" s="69"/>
-      <c r="GJ84" s="69"/>
-      <c r="GK84" s="69"/>
-      <c r="GL84" s="69"/>
-      <c r="GM84" s="69"/>
-      <c r="GN84" s="69"/>
-      <c r="GO84" s="69"/>
-      <c r="GP84" s="69"/>
-      <c r="GQ84" s="69"/>
-      <c r="GR84" s="69"/>
-      <c r="GS84" s="69"/>
-      <c r="GT84" s="69"/>
-      <c r="GU84" s="69"/>
-      <c r="GV84" s="69"/>
-      <c r="GW84" s="69"/>
-      <c r="GX84" s="69"/>
-      <c r="GY84" s="69"/>
-      <c r="GZ84" s="69"/>
-      <c r="HA84" s="69"/>
-      <c r="HB84" s="69"/>
-      <c r="HC84" s="69"/>
-      <c r="HD84" s="69"/>
-      <c r="HE84" s="69"/>
-      <c r="HF84" s="69"/>
-      <c r="HG84" s="69"/>
-      <c r="HH84" s="69"/>
-      <c r="HI84" s="69"/>
-      <c r="HJ84" s="69"/>
-      <c r="HK84" s="69"/>
-      <c r="HL84" s="69"/>
-      <c r="HM84" s="69"/>
-      <c r="HN84" s="69"/>
-      <c r="HO84" s="69"/>
-      <c r="HP84" s="69"/>
-      <c r="HQ84" s="69"/>
-      <c r="HR84" s="69"/>
-      <c r="HS84" s="69"/>
-      <c r="HT84" s="69"/>
-      <c r="HU84" s="69"/>
-      <c r="HV84" s="69"/>
-      <c r="HW84" s="69"/>
-      <c r="HX84" s="69"/>
-      <c r="HY84" s="69"/>
-      <c r="HZ84" s="69"/>
-      <c r="IA84" s="69"/>
-      <c r="IB84" s="69"/>
-      <c r="IC84" s="69"/>
-      <c r="ID84" s="69"/>
-      <c r="IE84" s="69"/>
-      <c r="IF84" s="69"/>
-      <c r="IG84" s="69"/>
-      <c r="IH84" s="69"/>
-      <c r="II84" s="69"/>
-      <c r="IJ84" s="69"/>
-      <c r="IK84" s="69"/>
-      <c r="IL84" s="69"/>
-      <c r="IM84" s="69"/>
-      <c r="IN84" s="69"/>
-      <c r="IO84" s="69"/>
-      <c r="IP84" s="69"/>
-      <c r="IQ84" s="69"/>
-      <c r="IR84" s="69"/>
-      <c r="IS84" s="69"/>
-      <c r="IT84" s="69"/>
-      <c r="IU84" s="69"/>
-      <c r="IV84" s="69"/>
-      <c r="IW84" s="69"/>
-      <c r="IX84" s="69"/>
-      <c r="IY84" s="69"/>
-      <c r="IZ84" s="69"/>
-      <c r="JA84" s="69"/>
-      <c r="JB84" s="69"/>
-      <c r="JC84" s="69"/>
-      <c r="JD84" s="69"/>
-      <c r="JE84" s="69"/>
-      <c r="JF84" s="69"/>
-      <c r="JG84" s="69"/>
-      <c r="JH84" s="69"/>
-      <c r="JI84" s="69"/>
-      <c r="JJ84" s="69"/>
-      <c r="JK84" s="69"/>
-      <c r="JL84" s="69"/>
-      <c r="JM84" s="69"/>
-      <c r="JN84" s="69"/>
-      <c r="JO84" s="69"/>
-      <c r="JP84" s="69"/>
-      <c r="JQ84" s="69"/>
-      <c r="JR84" s="69"/>
-      <c r="JS84" s="69"/>
-      <c r="JT84" s="69"/>
-      <c r="JU84" s="69"/>
-      <c r="JV84" s="69"/>
-      <c r="JW84" s="69"/>
-      <c r="JX84" s="69"/>
-      <c r="JY84" s="69"/>
-      <c r="JZ84" s="69"/>
-      <c r="KA84" s="69"/>
-      <c r="KB84" s="69"/>
-      <c r="KC84" s="69"/>
-      <c r="KD84" s="69"/>
-      <c r="KE84" s="69"/>
-      <c r="KF84" s="69"/>
-      <c r="KG84" s="69"/>
-      <c r="KH84" s="69"/>
-      <c r="KI84" s="69"/>
-      <c r="KJ84" s="69"/>
-      <c r="KK84" s="69"/>
-      <c r="KL84" s="69"/>
-      <c r="KM84" s="69"/>
-      <c r="KN84" s="69"/>
-      <c r="KO84" s="69"/>
-      <c r="KP84" s="69"/>
-      <c r="KQ84" s="69"/>
-      <c r="KR84" s="69"/>
-      <c r="KS84" s="69"/>
-      <c r="KT84" s="69"/>
-      <c r="KU84" s="69"/>
-      <c r="KV84" s="69"/>
-      <c r="KW84" s="69"/>
-      <c r="KX84" s="69"/>
-      <c r="KY84" s="69"/>
-      <c r="KZ84" s="69"/>
-      <c r="LA84" s="69"/>
-      <c r="LB84" s="69"/>
-      <c r="LC84" s="69"/>
-      <c r="LD84" s="69"/>
-      <c r="LE84" s="69"/>
-      <c r="LF84" s="69"/>
-      <c r="LG84" s="69"/>
-      <c r="LH84" s="69"/>
-      <c r="LI84" s="69"/>
-      <c r="LJ84" s="69"/>
-      <c r="LK84" s="69"/>
-      <c r="LL84" s="69"/>
-      <c r="LM84" s="69"/>
-      <c r="LN84" s="69"/>
-      <c r="LO84" s="69"/>
-      <c r="LP84" s="69"/>
-      <c r="LQ84" s="69"/>
-      <c r="LR84" s="69"/>
-      <c r="LS84" s="69"/>
-      <c r="LT84" s="69"/>
-      <c r="LU84" s="69"/>
-      <c r="LV84" s="69"/>
-      <c r="LW84" s="69"/>
-      <c r="LX84" s="69"/>
-      <c r="LY84" s="69"/>
-      <c r="LZ84" s="69"/>
-      <c r="MA84" s="69"/>
-      <c r="MB84" s="69"/>
-      <c r="MC84" s="69"/>
-      <c r="MD84" s="69"/>
-      <c r="ME84" s="69"/>
-      <c r="MF84" s="69"/>
-      <c r="MG84" s="69"/>
-      <c r="MH84" s="69"/>
-      <c r="MI84" s="69"/>
-      <c r="MJ84" s="69"/>
-      <c r="MK84" s="69"/>
-      <c r="ML84" s="69"/>
-      <c r="MM84" s="69"/>
-      <c r="MN84" s="69"/>
-      <c r="MO84" s="69"/>
-      <c r="MP84" s="69"/>
-      <c r="MQ84" s="69"/>
-      <c r="MR84" s="69"/>
-      <c r="MS84" s="69"/>
-      <c r="MT84" s="69"/>
-      <c r="MU84" s="69"/>
-      <c r="MV84" s="69"/>
-      <c r="MW84" s="69"/>
-      <c r="MX84" s="69"/>
-      <c r="MY84" s="69"/>
-      <c r="MZ84" s="69"/>
-      <c r="NA84" s="69"/>
-      <c r="NB84" s="69"/>
-      <c r="NC84" s="69"/>
-      <c r="ND84" s="69"/>
-      <c r="NE84" s="69"/>
-      <c r="NF84" s="69"/>
-      <c r="NG84" s="69"/>
-      <c r="NH84" s="69"/>
-      <c r="NI84" s="69"/>
-      <c r="NJ84" s="69"/>
-      <c r="NK84" s="69"/>
-      <c r="NL84" s="69"/>
-      <c r="NM84" s="69"/>
-      <c r="NN84" s="69"/>
-      <c r="NO84" s="69"/>
-      <c r="NP84" s="69"/>
-      <c r="NQ84" s="69"/>
-      <c r="NR84" s="69"/>
-      <c r="NS84" s="69"/>
-      <c r="NT84" s="69"/>
-      <c r="NU84" s="69"/>
-      <c r="NV84" s="69"/>
-      <c r="NW84" s="69"/>
-      <c r="NX84" s="69"/>
-      <c r="NY84" s="69"/>
-      <c r="NZ84" s="69"/>
-      <c r="OA84" s="69"/>
-      <c r="OB84" s="69"/>
-      <c r="OC84" s="69"/>
-      <c r="OD84" s="69"/>
-      <c r="OE84" s="69"/>
-      <c r="OF84" s="69"/>
-      <c r="OG84" s="69"/>
-      <c r="OH84" s="69"/>
-      <c r="OI84" s="69"/>
-      <c r="OJ84" s="69"/>
-      <c r="OK84" s="69"/>
-      <c r="OL84" s="69"/>
-      <c r="OM84" s="69"/>
-      <c r="ON84" s="69"/>
-      <c r="OO84" s="69"/>
-      <c r="OP84" s="69"/>
-      <c r="OQ84" s="69"/>
-      <c r="OR84" s="69"/>
-      <c r="OS84" s="69"/>
-      <c r="OT84" s="69"/>
-      <c r="OU84" s="69"/>
-      <c r="OV84" s="69"/>
-      <c r="OW84" s="69"/>
-      <c r="OX84" s="69"/>
-      <c r="OY84" s="69"/>
-      <c r="OZ84" s="69"/>
-      <c r="PA84" s="69"/>
-      <c r="PB84" s="69"/>
-      <c r="PC84" s="69"/>
-      <c r="PD84" s="69"/>
-      <c r="PE84" s="69"/>
-      <c r="PF84" s="69"/>
-      <c r="PG84" s="69"/>
-      <c r="PH84" s="69"/>
-      <c r="PI84" s="69"/>
-      <c r="PJ84" s="69"/>
-      <c r="PK84" s="69"/>
-      <c r="PL84" s="69"/>
-      <c r="PM84" s="69"/>
-      <c r="PN84" s="69"/>
-      <c r="PO84" s="69"/>
-      <c r="PP84" s="69"/>
-      <c r="PQ84" s="69"/>
-      <c r="PR84" s="69"/>
-      <c r="PS84" s="69"/>
-      <c r="PT84" s="69"/>
-      <c r="PU84" s="69"/>
-      <c r="PV84" s="69"/>
-      <c r="PW84" s="69"/>
-      <c r="PX84" s="69"/>
-      <c r="PY84" s="69"/>
-      <c r="PZ84" s="69"/>
-      <c r="QA84" s="69"/>
-      <c r="QB84" s="69"/>
-      <c r="QC84" s="69"/>
-      <c r="QD84" s="69"/>
-      <c r="QE84" s="69"/>
-      <c r="QF84" s="69"/>
-      <c r="QG84" s="69"/>
-      <c r="QH84" s="69"/>
-      <c r="QI84" s="69"/>
-      <c r="QJ84" s="69"/>
-      <c r="QK84" s="69"/>
-      <c r="QL84" s="69"/>
-      <c r="QM84" s="69"/>
-      <c r="QN84" s="69"/>
-      <c r="QO84" s="69"/>
-      <c r="QP84" s="69"/>
-      <c r="QQ84" s="69"/>
-      <c r="QR84" s="69"/>
-      <c r="QS84" s="69"/>
-      <c r="QT84" s="69"/>
-      <c r="QU84" s="69"/>
-      <c r="QV84" s="69"/>
-      <c r="QW84" s="69"/>
-      <c r="QX84" s="69"/>
-      <c r="QY84" s="69"/>
-      <c r="QZ84" s="69"/>
-      <c r="RA84" s="69"/>
-      <c r="RB84" s="69"/>
-      <c r="RC84" s="69"/>
-      <c r="RD84" s="69"/>
-      <c r="RE84" s="69"/>
-      <c r="RF84" s="69"/>
-      <c r="RG84" s="69"/>
-      <c r="RH84" s="69"/>
-      <c r="RI84" s="69"/>
-      <c r="RJ84" s="69"/>
-      <c r="RK84" s="69"/>
-      <c r="RL84" s="69"/>
-      <c r="RM84" s="69"/>
-      <c r="RN84" s="69"/>
-      <c r="RO84" s="69"/>
-      <c r="RP84" s="69"/>
-      <c r="RQ84" s="69"/>
-      <c r="RR84" s="69"/>
-      <c r="RS84" s="69"/>
-      <c r="RT84" s="69"/>
-      <c r="RU84" s="69"/>
-      <c r="RV84" s="69"/>
-      <c r="RW84" s="69"/>
-      <c r="RX84" s="69"/>
-      <c r="RY84" s="69"/>
-      <c r="RZ84" s="69"/>
-      <c r="SA84" s="69"/>
-      <c r="SB84" s="69"/>
-      <c r="SC84" s="69"/>
-      <c r="SD84" s="69"/>
-      <c r="SE84" s="69"/>
-      <c r="SF84" s="69"/>
-      <c r="SG84" s="69"/>
-      <c r="SH84" s="69"/>
-      <c r="SI84" s="69"/>
-      <c r="SJ84" s="69"/>
-      <c r="SK84" s="69"/>
-      <c r="SL84" s="69"/>
-      <c r="SM84" s="69"/>
-      <c r="SN84" s="69"/>
-      <c r="SO84" s="69"/>
-      <c r="SP84" s="69"/>
-      <c r="SQ84" s="69"/>
-      <c r="SR84" s="69"/>
-      <c r="SS84" s="69"/>
-      <c r="ST84" s="69"/>
-      <c r="SU84" s="69"/>
-      <c r="SV84" s="69"/>
-      <c r="SW84" s="69"/>
-      <c r="SX84" s="69"/>
-      <c r="SY84" s="69"/>
-      <c r="SZ84" s="69"/>
-      <c r="TA84" s="69"/>
-      <c r="TB84" s="69"/>
-      <c r="TC84" s="69"/>
-      <c r="TD84" s="69"/>
-      <c r="TE84" s="69"/>
-      <c r="TF84" s="69"/>
-      <c r="TG84" s="69"/>
-      <c r="TH84" s="69"/>
-      <c r="TI84" s="69"/>
-      <c r="TJ84" s="69"/>
-      <c r="TK84" s="69"/>
-      <c r="TL84" s="69"/>
-      <c r="TM84" s="69"/>
-      <c r="TN84" s="69"/>
-      <c r="TO84" s="69"/>
-      <c r="TP84" s="69"/>
-      <c r="TQ84" s="69"/>
-      <c r="TR84" s="69"/>
-      <c r="TS84" s="69"/>
-      <c r="TT84" s="69"/>
-      <c r="TU84" s="69"/>
-      <c r="TV84" s="69"/>
-      <c r="TW84" s="69"/>
-      <c r="TX84" s="69"/>
-      <c r="TY84" s="69"/>
-      <c r="TZ84" s="69"/>
-      <c r="UA84" s="69"/>
-      <c r="UB84" s="69"/>
-      <c r="UC84" s="69"/>
-      <c r="UD84" s="69"/>
-      <c r="UE84" s="69"/>
-      <c r="UF84" s="69"/>
-      <c r="UG84" s="69"/>
-      <c r="UH84" s="69"/>
-      <c r="UI84" s="69"/>
-      <c r="UJ84" s="69"/>
-      <c r="UK84" s="69"/>
-      <c r="UL84" s="69"/>
-      <c r="UM84" s="69"/>
-      <c r="UN84" s="69"/>
-      <c r="UO84" s="69"/>
-      <c r="UP84" s="69"/>
-      <c r="UQ84" s="69"/>
-      <c r="UR84" s="69"/>
-      <c r="US84" s="69"/>
-      <c r="UT84" s="69"/>
-      <c r="UU84" s="69"/>
-      <c r="UV84" s="69"/>
-      <c r="UW84" s="69"/>
-      <c r="UX84" s="69"/>
-      <c r="UY84" s="69"/>
-      <c r="UZ84" s="69"/>
-      <c r="VA84" s="69"/>
-      <c r="VB84" s="69"/>
-      <c r="VC84" s="69"/>
-      <c r="VD84" s="69"/>
-      <c r="VE84" s="69"/>
-      <c r="VF84" s="69"/>
-      <c r="VG84" s="69"/>
-      <c r="VH84" s="69"/>
-      <c r="VI84" s="69"/>
-      <c r="VJ84" s="69"/>
-      <c r="VK84" s="69"/>
-      <c r="VL84" s="69"/>
-      <c r="VM84" s="69"/>
-      <c r="VN84" s="69"/>
-      <c r="VO84" s="69"/>
-      <c r="VP84" s="69"/>
-      <c r="VQ84" s="69"/>
-      <c r="VR84" s="69"/>
-      <c r="VS84" s="69"/>
-      <c r="VT84" s="69"/>
-      <c r="VU84" s="69"/>
-      <c r="VV84" s="69"/>
-      <c r="VW84" s="69"/>
-      <c r="VX84" s="69"/>
-      <c r="VY84" s="69"/>
-      <c r="VZ84" s="69"/>
-      <c r="WA84" s="69"/>
-      <c r="WB84" s="69"/>
-      <c r="WC84" s="69"/>
-      <c r="WD84" s="69"/>
-      <c r="WE84" s="69"/>
-      <c r="WF84" s="69"/>
-      <c r="WG84" s="69"/>
-      <c r="WH84" s="69"/>
-      <c r="WI84" s="69"/>
-      <c r="WJ84" s="69"/>
-      <c r="WK84" s="69"/>
-      <c r="WL84" s="69"/>
-      <c r="WM84" s="69"/>
-      <c r="WN84" s="69"/>
-      <c r="WO84" s="69"/>
-      <c r="WP84" s="69"/>
-      <c r="WQ84" s="69"/>
-      <c r="WR84" s="69"/>
-      <c r="WS84" s="69"/>
-      <c r="WT84" s="69"/>
-      <c r="WU84" s="69"/>
-      <c r="WV84" s="69"/>
-      <c r="WW84" s="69"/>
-      <c r="WX84" s="69"/>
-      <c r="WY84" s="69"/>
-      <c r="WZ84" s="69"/>
-      <c r="XA84" s="69"/>
-      <c r="XB84" s="69"/>
-      <c r="XC84" s="69"/>
-      <c r="XD84" s="69"/>
-      <c r="XE84" s="69"/>
-      <c r="XF84" s="69"/>
-      <c r="XG84" s="69"/>
-      <c r="XH84" s="69"/>
-      <c r="XI84" s="69"/>
-      <c r="XJ84" s="69"/>
-      <c r="XK84" s="69"/>
-      <c r="XL84" s="69"/>
-      <c r="XM84" s="69"/>
-      <c r="XN84" s="69"/>
-      <c r="XO84" s="69"/>
-      <c r="XP84" s="69"/>
-      <c r="XQ84" s="69"/>
-      <c r="XR84" s="69"/>
-      <c r="XS84" s="69"/>
-      <c r="XT84" s="69"/>
-      <c r="XU84" s="69"/>
-      <c r="XV84" s="69"/>
-      <c r="XW84" s="69"/>
-      <c r="XX84" s="69"/>
-      <c r="XY84" s="69"/>
-      <c r="XZ84" s="69"/>
-      <c r="YA84" s="69"/>
-      <c r="YB84" s="69"/>
-      <c r="YC84" s="69"/>
-      <c r="YD84" s="69"/>
-      <c r="YE84" s="69"/>
-      <c r="YF84" s="69"/>
-      <c r="YG84" s="69"/>
-      <c r="YH84" s="69"/>
-      <c r="YI84" s="69"/>
-      <c r="YJ84" s="69"/>
-      <c r="YK84" s="69"/>
-      <c r="YL84" s="69"/>
-      <c r="YM84" s="69"/>
-      <c r="YN84" s="69"/>
-      <c r="YO84" s="69"/>
-      <c r="YP84" s="69"/>
-      <c r="YQ84" s="69"/>
-      <c r="YR84" s="69"/>
-      <c r="YS84" s="69"/>
-      <c r="YT84" s="69"/>
-      <c r="YU84" s="69"/>
-      <c r="YV84" s="69"/>
-      <c r="YW84" s="69"/>
-      <c r="YX84" s="69"/>
-      <c r="YY84" s="69"/>
-      <c r="YZ84" s="69"/>
-      <c r="ZA84" s="69"/>
-      <c r="ZB84" s="69"/>
-      <c r="ZC84" s="69"/>
-      <c r="ZD84" s="69"/>
-      <c r="ZE84" s="69"/>
-      <c r="ZF84" s="69"/>
-      <c r="ZG84" s="69"/>
-      <c r="ZH84" s="69"/>
-      <c r="ZI84" s="69"/>
-      <c r="ZJ84" s="69"/>
-      <c r="ZK84" s="69"/>
-      <c r="ZL84" s="69"/>
-      <c r="ZM84" s="69"/>
-      <c r="ZN84" s="69"/>
-      <c r="ZO84" s="69"/>
-      <c r="ZP84" s="69"/>
-      <c r="ZQ84" s="69"/>
-      <c r="ZR84" s="69"/>
-      <c r="ZS84" s="69"/>
-      <c r="ZT84" s="69"/>
-      <c r="ZU84" s="69"/>
-      <c r="ZV84" s="69"/>
-      <c r="ZW84" s="69"/>
-      <c r="ZX84" s="69"/>
-      <c r="ZY84" s="69"/>
-      <c r="ZZ84" s="69"/>
-      <c r="AAA84" s="69"/>
-      <c r="AAB84" s="69"/>
-      <c r="AAC84" s="69"/>
-      <c r="AAD84" s="69"/>
-      <c r="AAE84" s="69"/>
-      <c r="AAF84" s="69"/>
-      <c r="AAG84" s="69"/>
-      <c r="AAH84" s="69"/>
-      <c r="AAI84" s="69"/>
-      <c r="AAJ84" s="69"/>
-      <c r="AAK84" s="69"/>
-      <c r="AAL84" s="69"/>
-      <c r="AAM84" s="69"/>
-      <c r="AAN84" s="69"/>
-      <c r="AAO84" s="69"/>
-      <c r="AAP84" s="69"/>
-      <c r="AAQ84" s="69"/>
-      <c r="AAR84" s="69"/>
-      <c r="AAS84" s="69"/>
-      <c r="AAT84" s="69"/>
-      <c r="AAU84" s="69"/>
-      <c r="AAV84" s="69"/>
-      <c r="AAW84" s="69"/>
-      <c r="AAX84" s="69"/>
-      <c r="AAY84" s="69"/>
-      <c r="AAZ84" s="69"/>
-      <c r="ABA84" s="69"/>
-      <c r="ABB84" s="69"/>
-      <c r="ABC84" s="69"/>
-      <c r="ABD84" s="69"/>
-      <c r="ABE84" s="69"/>
-      <c r="ABF84" s="69"/>
-      <c r="ABG84" s="69"/>
-      <c r="ABH84" s="69"/>
-      <c r="ABI84" s="69"/>
-      <c r="ABJ84" s="69"/>
-      <c r="ABK84" s="69"/>
-      <c r="ABL84" s="69"/>
-      <c r="ABM84" s="69"/>
-      <c r="ABN84" s="69"/>
-      <c r="ABO84" s="69"/>
-      <c r="ABP84" s="69"/>
-      <c r="ABQ84" s="69"/>
-      <c r="ABR84" s="69"/>
-      <c r="ABS84" s="69"/>
-      <c r="ABT84" s="69"/>
-      <c r="ABU84" s="69"/>
-      <c r="ABV84" s="69"/>
-      <c r="ABW84" s="69"/>
-      <c r="ABX84" s="69"/>
-      <c r="ABY84" s="69"/>
-      <c r="ABZ84" s="69"/>
-      <c r="ACA84" s="69"/>
-      <c r="ACB84" s="69"/>
-      <c r="ACC84" s="69"/>
-      <c r="ACD84" s="69"/>
-      <c r="ACE84" s="69"/>
-      <c r="ACF84" s="69"/>
-      <c r="ACG84" s="69"/>
-      <c r="ACH84" s="69"/>
-      <c r="ACI84" s="69"/>
-      <c r="ACJ84" s="69"/>
-      <c r="ACK84" s="69"/>
-      <c r="ACL84" s="69"/>
-      <c r="ACM84" s="69"/>
-      <c r="ACN84" s="69"/>
-      <c r="ACO84" s="69"/>
-      <c r="ACP84" s="69"/>
-      <c r="ACQ84" s="69"/>
-      <c r="ACR84" s="69"/>
-      <c r="ACS84" s="69"/>
-      <c r="ACT84" s="69"/>
-      <c r="ACU84" s="69"/>
-      <c r="ACV84" s="69"/>
-      <c r="ACW84" s="69"/>
-      <c r="ACX84" s="69"/>
-      <c r="ACY84" s="69"/>
-      <c r="ACZ84" s="69"/>
-      <c r="ADA84" s="69"/>
-      <c r="ADB84" s="69"/>
-      <c r="ADC84" s="69"/>
-      <c r="ADD84" s="69"/>
-      <c r="ADE84" s="69"/>
-      <c r="ADF84" s="69"/>
-      <c r="ADG84" s="69"/>
-      <c r="ADH84" s="69"/>
-      <c r="ADI84" s="69"/>
-      <c r="ADJ84" s="69"/>
-      <c r="ADK84" s="69"/>
-      <c r="ADL84" s="69"/>
-      <c r="ADM84" s="69"/>
-      <c r="ADN84" s="69"/>
-      <c r="ADO84" s="69"/>
-      <c r="ADP84" s="69"/>
-      <c r="ADQ84" s="69"/>
-      <c r="ADR84" s="69"/>
-      <c r="ADS84" s="69"/>
-      <c r="ADT84" s="69"/>
-      <c r="ADU84" s="69"/>
-      <c r="ADV84" s="69"/>
-      <c r="ADW84" s="69"/>
-      <c r="ADX84" s="69"/>
-      <c r="ADY84" s="69"/>
-      <c r="ADZ84" s="69"/>
-      <c r="AEA84" s="69"/>
-      <c r="AEB84" s="69"/>
-      <c r="AEC84" s="69"/>
-      <c r="AED84" s="69"/>
-      <c r="AEE84" s="69"/>
-      <c r="AEF84" s="69"/>
-      <c r="AEG84" s="69"/>
-      <c r="AEH84" s="69"/>
-      <c r="AEI84" s="69"/>
-      <c r="AEJ84" s="69"/>
-      <c r="AEK84" s="69"/>
-      <c r="AEL84" s="69"/>
-      <c r="AEM84" s="69"/>
-      <c r="AEN84" s="69"/>
-      <c r="AEO84" s="69"/>
-      <c r="AEP84" s="69"/>
-      <c r="AEQ84" s="69"/>
-      <c r="AER84" s="69"/>
-      <c r="AES84" s="69"/>
-      <c r="AET84" s="69"/>
-      <c r="AEU84" s="69"/>
-      <c r="AEV84" s="69"/>
-      <c r="AEW84" s="69"/>
-      <c r="AEX84" s="69"/>
-      <c r="AEY84" s="69"/>
-      <c r="AEZ84" s="69"/>
-      <c r="AFA84" s="69"/>
-      <c r="AFB84" s="69"/>
-      <c r="AFC84" s="69"/>
-      <c r="AFD84" s="69"/>
-      <c r="AFE84" s="69"/>
-      <c r="AFF84" s="69"/>
-      <c r="AFG84" s="69"/>
-      <c r="AFH84" s="69"/>
-      <c r="AFI84" s="69"/>
-      <c r="AFJ84" s="69"/>
-      <c r="AFK84" s="69"/>
-      <c r="AFL84" s="69"/>
-      <c r="AFM84" s="69"/>
-      <c r="AFN84" s="69"/>
-      <c r="AFO84" s="69"/>
-      <c r="AFP84" s="69"/>
-      <c r="AFQ84" s="69"/>
-      <c r="AFR84" s="69"/>
-      <c r="AFS84" s="69"/>
-      <c r="AFT84" s="69"/>
-      <c r="AFU84" s="69"/>
-      <c r="AFV84" s="69"/>
-      <c r="AFW84" s="69"/>
-      <c r="AFX84" s="69"/>
-      <c r="AFY84" s="69"/>
-      <c r="AFZ84" s="69"/>
-      <c r="AGA84" s="69"/>
-      <c r="AGB84" s="69"/>
-      <c r="AGC84" s="69"/>
-      <c r="AGD84" s="69"/>
-      <c r="AGE84" s="69"/>
-      <c r="AGF84" s="69"/>
-      <c r="AGG84" s="69"/>
-      <c r="AGH84" s="69"/>
-      <c r="AGI84" s="69"/>
-      <c r="AGJ84" s="69"/>
-      <c r="AGK84" s="69"/>
-      <c r="AGL84" s="69"/>
-      <c r="AGM84" s="69"/>
-      <c r="AGN84" s="69"/>
-      <c r="AGO84" s="69"/>
-      <c r="AGP84" s="69"/>
-      <c r="AGQ84" s="69"/>
-      <c r="AGR84" s="69"/>
-      <c r="AGS84" s="69"/>
-      <c r="AGT84" s="69"/>
-      <c r="AGU84" s="69"/>
-      <c r="AGV84" s="69"/>
-      <c r="AGW84" s="69"/>
-      <c r="AGX84" s="69"/>
-      <c r="AGY84" s="69"/>
-      <c r="AGZ84" s="69"/>
-      <c r="AHA84" s="69"/>
-      <c r="AHB84" s="69"/>
-      <c r="AHC84" s="69"/>
-      <c r="AHD84" s="69"/>
-      <c r="AHE84" s="69"/>
-      <c r="AHF84" s="69"/>
-      <c r="AHG84" s="69"/>
-      <c r="AHH84" s="69"/>
-      <c r="AHI84" s="69"/>
-      <c r="AHJ84" s="69"/>
-      <c r="AHK84" s="69"/>
-      <c r="AHL84" s="69"/>
-      <c r="AHM84" s="69"/>
-      <c r="AHN84" s="69"/>
-      <c r="AHO84" s="69"/>
-      <c r="AHP84" s="69"/>
-      <c r="AHQ84" s="69"/>
-      <c r="AHR84" s="69"/>
-      <c r="AHS84" s="69"/>
-      <c r="AHT84" s="69"/>
-      <c r="AHU84" s="69"/>
-      <c r="AHV84" s="69"/>
-      <c r="AHW84" s="69"/>
-      <c r="AHX84" s="69"/>
-      <c r="AHY84" s="69"/>
-      <c r="AHZ84" s="69"/>
-      <c r="AIA84" s="69"/>
-      <c r="AIB84" s="69"/>
-      <c r="AIC84" s="69"/>
-      <c r="AID84" s="69"/>
-      <c r="AIE84" s="69"/>
-      <c r="AIF84" s="69"/>
-      <c r="AIG84" s="69"/>
-      <c r="AIH84" s="69"/>
-      <c r="AII84" s="69"/>
-      <c r="AIJ84" s="69"/>
-      <c r="AIK84" s="69"/>
-      <c r="AIL84" s="69"/>
-      <c r="AIM84" s="69"/>
-      <c r="AIN84" s="69"/>
-      <c r="AIO84" s="69"/>
-      <c r="AIP84" s="69"/>
-      <c r="AIQ84" s="69"/>
-      <c r="AIR84" s="69"/>
-      <c r="AIS84" s="69"/>
-      <c r="AIT84" s="69"/>
-      <c r="AIU84" s="69"/>
-      <c r="AIV84" s="69"/>
-      <c r="AIW84" s="69"/>
-      <c r="AIX84" s="69"/>
-      <c r="AIY84" s="69"/>
-      <c r="AIZ84" s="69"/>
-      <c r="AJA84" s="69"/>
-      <c r="AJB84" s="69"/>
-      <c r="AJC84" s="69"/>
-      <c r="AJD84" s="69"/>
-      <c r="AJE84" s="69"/>
-      <c r="AJF84" s="69"/>
-      <c r="AJG84" s="69"/>
-      <c r="AJH84" s="69"/>
-      <c r="AJI84" s="69"/>
-      <c r="AJJ84" s="69"/>
-      <c r="AJK84" s="69"/>
-      <c r="AJL84" s="69"/>
-      <c r="AJM84" s="69"/>
-      <c r="AJN84" s="69"/>
-      <c r="AJO84" s="69"/>
-      <c r="AJP84" s="69"/>
-      <c r="AJQ84" s="69"/>
-      <c r="AJR84" s="69"/>
-      <c r="AJS84" s="69"/>
-      <c r="AJT84" s="69"/>
-      <c r="AJU84" s="69"/>
-      <c r="AJV84" s="69"/>
-      <c r="AJW84" s="69"/>
-      <c r="AJX84" s="69"/>
-      <c r="AJY84" s="69"/>
-      <c r="AJZ84" s="69"/>
-      <c r="AKA84" s="69"/>
-      <c r="AKB84" s="69"/>
-      <c r="AKC84" s="69"/>
-      <c r="AKD84" s="69"/>
-      <c r="AKE84" s="69"/>
-      <c r="AKF84" s="69"/>
-      <c r="AKG84" s="69"/>
-      <c r="AKH84" s="69"/>
-      <c r="AKI84" s="69"/>
-      <c r="AKJ84" s="69"/>
-      <c r="AKK84" s="69"/>
-      <c r="AKL84" s="69"/>
-      <c r="AKM84" s="69"/>
-      <c r="AKN84" s="69"/>
-      <c r="AKO84" s="69"/>
-      <c r="AKP84" s="69"/>
-      <c r="AKQ84" s="69"/>
-      <c r="AKR84" s="69"/>
-      <c r="AKS84" s="69"/>
-      <c r="AKT84" s="69"/>
-      <c r="AKU84" s="69"/>
-      <c r="AKV84" s="69"/>
-      <c r="AKW84" s="69"/>
-      <c r="AKX84" s="69"/>
-      <c r="AKY84" s="69"/>
-      <c r="AKZ84" s="69"/>
-      <c r="ALA84" s="69"/>
-      <c r="ALB84" s="69"/>
-      <c r="ALC84" s="69"/>
-      <c r="ALD84" s="69"/>
-      <c r="ALE84" s="69"/>
-      <c r="ALF84" s="69"/>
-      <c r="ALG84" s="69"/>
-      <c r="ALH84" s="69"/>
-      <c r="ALI84" s="69"/>
-      <c r="ALJ84" s="69"/>
-      <c r="ALK84" s="69"/>
-      <c r="ALL84" s="69"/>
-      <c r="ALM84" s="69"/>
-      <c r="ALN84" s="69"/>
-      <c r="ALO84" s="69"/>
-      <c r="ALP84" s="69"/>
-      <c r="ALQ84" s="69"/>
-      <c r="ALR84" s="69"/>
-      <c r="ALS84" s="69"/>
-      <c r="ALT84" s="69"/>
-      <c r="ALU84" s="69"/>
-      <c r="ALV84" s="69"/>
-      <c r="ALW84" s="69"/>
-      <c r="ALX84" s="69"/>
-      <c r="ALY84" s="69"/>
-      <c r="ALZ84" s="69"/>
-      <c r="AMA84" s="69"/>
-      <c r="AMB84" s="69"/>
-      <c r="AMC84" s="69"/>
-      <c r="AMD84" s="69"/>
-      <c r="AME84" s="69"/>
-      <c r="AMF84" s="69"/>
-      <c r="AMG84" s="69"/>
-      <c r="AMH84" s="69"/>
+      <c r="H84" s="68"/>
+      <c r="I84" s="70"/>
+      <c r="J84" s="70"/>
+      <c r="K84" s="70"/>
+      <c r="L84" s="70"/>
+      <c r="M84" s="70"/>
+      <c r="N84" s="70"/>
+      <c r="O84" s="70"/>
+      <c r="P84" s="70"/>
+      <c r="Q84" s="70"/>
+      <c r="R84" s="70"/>
+      <c r="S84" s="70"/>
+      <c r="T84" s="70"/>
+      <c r="U84" s="70"/>
+      <c r="V84" s="70"/>
+      <c r="W84" s="70"/>
+      <c r="X84" s="70"/>
+      <c r="Y84" s="70"/>
+      <c r="Z84" s="70"/>
+      <c r="AA84" s="70"/>
+      <c r="AB84" s="70"/>
+      <c r="AC84" s="70"/>
+      <c r="AD84" s="70"/>
+      <c r="AE84" s="70"/>
+      <c r="AF84" s="70"/>
+      <c r="AG84" s="70"/>
+      <c r="AH84" s="70"/>
+      <c r="AI84" s="70"/>
+      <c r="AJ84" s="70"/>
+      <c r="AK84" s="70"/>
+      <c r="AL84" s="70"/>
+      <c r="AM84" s="70"/>
+      <c r="AN84" s="70"/>
+      <c r="AO84" s="70"/>
+      <c r="AP84" s="70"/>
+      <c r="AQ84" s="70"/>
+      <c r="AR84" s="70"/>
+      <c r="AS84" s="70"/>
+      <c r="AT84" s="70"/>
+      <c r="AU84" s="70"/>
+      <c r="AV84" s="70"/>
+      <c r="AW84" s="70"/>
+      <c r="AX84" s="70"/>
+      <c r="AY84" s="70"/>
+      <c r="AZ84" s="70"/>
+      <c r="BA84" s="70"/>
+      <c r="BB84" s="70"/>
+      <c r="BC84" s="70"/>
+      <c r="BD84" s="70"/>
+      <c r="BE84" s="70"/>
+      <c r="BF84" s="70"/>
+      <c r="BG84" s="70"/>
+      <c r="BH84" s="70"/>
+      <c r="BI84" s="70"/>
+      <c r="BJ84" s="70"/>
+      <c r="BK84" s="70"/>
+      <c r="BL84" s="70"/>
+      <c r="BM84" s="70"/>
+      <c r="BN84" s="70"/>
+      <c r="BO84" s="70"/>
+      <c r="BP84" s="70"/>
+      <c r="BQ84" s="70"/>
+      <c r="BR84" s="70"/>
+      <c r="BS84" s="70"/>
+      <c r="BT84" s="70"/>
+      <c r="BU84" s="70"/>
+      <c r="BV84" s="70"/>
+      <c r="BW84" s="70"/>
+      <c r="BX84" s="70"/>
+      <c r="BY84" s="70"/>
+      <c r="BZ84" s="70"/>
+      <c r="CA84" s="70"/>
+      <c r="CB84" s="70"/>
+      <c r="CC84" s="70"/>
+      <c r="CD84" s="70"/>
+      <c r="CE84" s="70"/>
+      <c r="CF84" s="70"/>
+      <c r="CG84" s="70"/>
+      <c r="CH84" s="70"/>
+      <c r="CI84" s="70"/>
+      <c r="CJ84" s="70"/>
+      <c r="CK84" s="70"/>
+      <c r="CL84" s="70"/>
+      <c r="CM84" s="70"/>
+      <c r="CN84" s="70"/>
+      <c r="CO84" s="70"/>
+      <c r="CP84" s="70"/>
+      <c r="CQ84" s="70"/>
+      <c r="CR84" s="70"/>
+      <c r="CS84" s="70"/>
+      <c r="CT84" s="70"/>
+      <c r="CU84" s="70"/>
+      <c r="CV84" s="70"/>
+      <c r="CW84" s="70"/>
+      <c r="CX84" s="70"/>
+      <c r="CY84" s="70"/>
+      <c r="CZ84" s="70"/>
+      <c r="DA84" s="70"/>
+      <c r="DB84" s="70"/>
+      <c r="DC84" s="70"/>
+      <c r="DD84" s="70"/>
+      <c r="DE84" s="70"/>
+      <c r="DF84" s="70"/>
+      <c r="DG84" s="70"/>
+      <c r="DH84" s="70"/>
+      <c r="DI84" s="70"/>
+      <c r="DJ84" s="70"/>
+      <c r="DK84" s="70"/>
+      <c r="DL84" s="70"/>
+      <c r="DM84" s="70"/>
+      <c r="DN84" s="70"/>
+      <c r="DO84" s="70"/>
+      <c r="DP84" s="70"/>
+      <c r="DQ84" s="70"/>
+      <c r="DR84" s="70"/>
+      <c r="DS84" s="70"/>
+      <c r="DT84" s="70"/>
+      <c r="DU84" s="70"/>
+      <c r="DV84" s="70"/>
+      <c r="DW84" s="70"/>
+      <c r="DX84" s="70"/>
+      <c r="DY84" s="70"/>
+      <c r="DZ84" s="70"/>
+      <c r="EA84" s="70"/>
+      <c r="EB84" s="70"/>
+      <c r="EC84" s="70"/>
+      <c r="ED84" s="70"/>
+      <c r="EE84" s="70"/>
+      <c r="EF84" s="70"/>
+      <c r="EG84" s="70"/>
+      <c r="EH84" s="70"/>
+      <c r="EI84" s="70"/>
+      <c r="EJ84" s="70"/>
+      <c r="EK84" s="70"/>
+      <c r="EL84" s="70"/>
+      <c r="EM84" s="70"/>
+      <c r="EN84" s="70"/>
+      <c r="EO84" s="70"/>
+      <c r="EP84" s="70"/>
+      <c r="EQ84" s="70"/>
+      <c r="ER84" s="70"/>
+      <c r="ES84" s="70"/>
+      <c r="ET84" s="70"/>
+      <c r="EU84" s="70"/>
+      <c r="EV84" s="70"/>
+      <c r="EW84" s="70"/>
+      <c r="EX84" s="70"/>
+      <c r="EY84" s="70"/>
+      <c r="EZ84" s="70"/>
+      <c r="FA84" s="70"/>
+      <c r="FB84" s="70"/>
+      <c r="FC84" s="70"/>
+      <c r="FD84" s="70"/>
+      <c r="FE84" s="70"/>
+      <c r="FF84" s="70"/>
+      <c r="FG84" s="70"/>
+      <c r="FH84" s="70"/>
+      <c r="FI84" s="70"/>
+      <c r="FJ84" s="70"/>
+      <c r="FK84" s="70"/>
+      <c r="FL84" s="70"/>
+      <c r="FM84" s="70"/>
+      <c r="FN84" s="70"/>
+      <c r="FO84" s="70"/>
+      <c r="FP84" s="70"/>
+      <c r="FQ84" s="70"/>
+      <c r="FR84" s="70"/>
+      <c r="FS84" s="70"/>
+      <c r="FT84" s="70"/>
+      <c r="FU84" s="70"/>
+      <c r="FV84" s="70"/>
+      <c r="FW84" s="70"/>
+      <c r="FX84" s="70"/>
+      <c r="FY84" s="70"/>
+      <c r="FZ84" s="70"/>
+      <c r="GA84" s="70"/>
+      <c r="GB84" s="70"/>
+      <c r="GC84" s="70"/>
+      <c r="GD84" s="70"/>
+      <c r="GE84" s="70"/>
+      <c r="GF84" s="70"/>
+      <c r="GG84" s="70"/>
+      <c r="GH84" s="70"/>
+      <c r="GI84" s="70"/>
+      <c r="GJ84" s="70"/>
+      <c r="GK84" s="70"/>
+      <c r="GL84" s="70"/>
+      <c r="GM84" s="70"/>
+      <c r="GN84" s="70"/>
+      <c r="GO84" s="70"/>
+      <c r="GP84" s="70"/>
+      <c r="GQ84" s="70"/>
+      <c r="GR84" s="70"/>
+      <c r="GS84" s="70"/>
+      <c r="GT84" s="70"/>
+      <c r="GU84" s="70"/>
+      <c r="GV84" s="70"/>
+      <c r="GW84" s="70"/>
+      <c r="GX84" s="70"/>
+      <c r="GY84" s="70"/>
+      <c r="GZ84" s="70"/>
+      <c r="HA84" s="70"/>
+      <c r="HB84" s="70"/>
+      <c r="HC84" s="70"/>
+      <c r="HD84" s="70"/>
+      <c r="HE84" s="70"/>
+      <c r="HF84" s="70"/>
+      <c r="HG84" s="70"/>
+      <c r="HH84" s="70"/>
+      <c r="HI84" s="70"/>
+      <c r="HJ84" s="70"/>
+      <c r="HK84" s="70"/>
+      <c r="HL84" s="70"/>
+      <c r="HM84" s="70"/>
+      <c r="HN84" s="70"/>
+      <c r="HO84" s="70"/>
+      <c r="HP84" s="70"/>
+      <c r="HQ84" s="70"/>
+      <c r="HR84" s="70"/>
+      <c r="HS84" s="70"/>
+      <c r="HT84" s="70"/>
+      <c r="HU84" s="70"/>
+      <c r="HV84" s="70"/>
+      <c r="HW84" s="70"/>
+      <c r="HX84" s="70"/>
+      <c r="HY84" s="70"/>
+      <c r="HZ84" s="70"/>
+      <c r="IA84" s="70"/>
+      <c r="IB84" s="70"/>
+      <c r="IC84" s="70"/>
+      <c r="ID84" s="70"/>
+      <c r="IE84" s="70"/>
+      <c r="IF84" s="70"/>
+      <c r="IG84" s="70"/>
+      <c r="IH84" s="70"/>
+      <c r="II84" s="70"/>
+      <c r="IJ84" s="70"/>
+      <c r="IK84" s="70"/>
+      <c r="IL84" s="70"/>
+      <c r="IM84" s="70"/>
+      <c r="IN84" s="70"/>
+      <c r="IO84" s="70"/>
+      <c r="IP84" s="70"/>
+      <c r="IQ84" s="70"/>
+      <c r="IR84" s="70"/>
+      <c r="IS84" s="70"/>
+      <c r="IT84" s="70"/>
+      <c r="IU84" s="70"/>
+      <c r="IV84" s="70"/>
+      <c r="IW84" s="70"/>
+      <c r="IX84" s="70"/>
+      <c r="IY84" s="70"/>
+      <c r="IZ84" s="70"/>
+      <c r="JA84" s="70"/>
+      <c r="JB84" s="70"/>
+      <c r="JC84" s="70"/>
+      <c r="JD84" s="70"/>
+      <c r="JE84" s="70"/>
+      <c r="JF84" s="70"/>
+      <c r="JG84" s="70"/>
+      <c r="JH84" s="70"/>
+      <c r="JI84" s="70"/>
+      <c r="JJ84" s="70"/>
+      <c r="JK84" s="70"/>
+      <c r="JL84" s="70"/>
+      <c r="JM84" s="70"/>
+      <c r="JN84" s="70"/>
+      <c r="JO84" s="70"/>
+      <c r="JP84" s="70"/>
+      <c r="JQ84" s="70"/>
+      <c r="JR84" s="70"/>
+      <c r="JS84" s="70"/>
+      <c r="JT84" s="70"/>
+      <c r="JU84" s="70"/>
+      <c r="JV84" s="70"/>
+      <c r="JW84" s="70"/>
+      <c r="JX84" s="70"/>
+      <c r="JY84" s="70"/>
+      <c r="JZ84" s="70"/>
+      <c r="KA84" s="70"/>
+      <c r="KB84" s="70"/>
+      <c r="KC84" s="70"/>
+      <c r="KD84" s="70"/>
+      <c r="KE84" s="70"/>
+      <c r="KF84" s="70"/>
+      <c r="KG84" s="70"/>
+      <c r="KH84" s="70"/>
+      <c r="KI84" s="70"/>
+      <c r="KJ84" s="70"/>
+      <c r="KK84" s="70"/>
+      <c r="KL84" s="70"/>
+      <c r="KM84" s="70"/>
+      <c r="KN84" s="70"/>
+      <c r="KO84" s="70"/>
+      <c r="KP84" s="70"/>
+      <c r="KQ84" s="70"/>
+      <c r="KR84" s="70"/>
+      <c r="KS84" s="70"/>
+      <c r="KT84" s="70"/>
+      <c r="KU84" s="70"/>
+      <c r="KV84" s="70"/>
+      <c r="KW84" s="70"/>
+      <c r="KX84" s="70"/>
+      <c r="KY84" s="70"/>
+      <c r="KZ84" s="70"/>
+      <c r="LA84" s="70"/>
+      <c r="LB84" s="70"/>
+      <c r="LC84" s="70"/>
+      <c r="LD84" s="70"/>
+      <c r="LE84" s="70"/>
+      <c r="LF84" s="70"/>
+      <c r="LG84" s="70"/>
+      <c r="LH84" s="70"/>
+      <c r="LI84" s="70"/>
+      <c r="LJ84" s="70"/>
+      <c r="LK84" s="70"/>
+      <c r="LL84" s="70"/>
+      <c r="LM84" s="70"/>
+      <c r="LN84" s="70"/>
+      <c r="LO84" s="70"/>
+      <c r="LP84" s="70"/>
+      <c r="LQ84" s="70"/>
+      <c r="LR84" s="70"/>
+      <c r="LS84" s="70"/>
+      <c r="LT84" s="70"/>
+      <c r="LU84" s="70"/>
+      <c r="LV84" s="70"/>
+      <c r="LW84" s="70"/>
+      <c r="LX84" s="70"/>
+      <c r="LY84" s="70"/>
+      <c r="LZ84" s="70"/>
+      <c r="MA84" s="70"/>
+      <c r="MB84" s="70"/>
+      <c r="MC84" s="70"/>
+      <c r="MD84" s="70"/>
+      <c r="ME84" s="70"/>
+      <c r="MF84" s="70"/>
+      <c r="MG84" s="70"/>
+      <c r="MH84" s="70"/>
+      <c r="MI84" s="70"/>
+      <c r="MJ84" s="70"/>
+      <c r="MK84" s="70"/>
+      <c r="ML84" s="70"/>
+      <c r="MM84" s="70"/>
+      <c r="MN84" s="70"/>
+      <c r="MO84" s="70"/>
+      <c r="MP84" s="70"/>
+      <c r="MQ84" s="70"/>
+      <c r="MR84" s="70"/>
+      <c r="MS84" s="70"/>
+      <c r="MT84" s="70"/>
+      <c r="MU84" s="70"/>
+      <c r="MV84" s="70"/>
+      <c r="MW84" s="70"/>
+      <c r="MX84" s="70"/>
+      <c r="MY84" s="70"/>
+      <c r="MZ84" s="70"/>
+      <c r="NA84" s="70"/>
+      <c r="NB84" s="70"/>
+      <c r="NC84" s="70"/>
+      <c r="ND84" s="70"/>
+      <c r="NE84" s="70"/>
+      <c r="NF84" s="70"/>
+      <c r="NG84" s="70"/>
+      <c r="NH84" s="70"/>
+      <c r="NI84" s="70"/>
+      <c r="NJ84" s="70"/>
+      <c r="NK84" s="70"/>
+      <c r="NL84" s="70"/>
+      <c r="NM84" s="70"/>
+      <c r="NN84" s="70"/>
+      <c r="NO84" s="70"/>
+      <c r="NP84" s="70"/>
+      <c r="NQ84" s="70"/>
+      <c r="NR84" s="70"/>
+      <c r="NS84" s="70"/>
+      <c r="NT84" s="70"/>
+      <c r="NU84" s="70"/>
+      <c r="NV84" s="70"/>
+      <c r="NW84" s="70"/>
+      <c r="NX84" s="70"/>
+      <c r="NY84" s="70"/>
+      <c r="NZ84" s="70"/>
+      <c r="OA84" s="70"/>
+      <c r="OB84" s="70"/>
+      <c r="OC84" s="70"/>
+      <c r="OD84" s="70"/>
+      <c r="OE84" s="70"/>
+      <c r="OF84" s="70"/>
+      <c r="OG84" s="70"/>
+      <c r="OH84" s="70"/>
+      <c r="OI84" s="70"/>
+      <c r="OJ84" s="70"/>
+      <c r="OK84" s="70"/>
+      <c r="OL84" s="70"/>
+      <c r="OM84" s="70"/>
+      <c r="ON84" s="70"/>
+      <c r="OO84" s="70"/>
+      <c r="OP84" s="70"/>
+      <c r="OQ84" s="70"/>
+      <c r="OR84" s="70"/>
+      <c r="OS84" s="70"/>
+      <c r="OT84" s="70"/>
+      <c r="OU84" s="70"/>
+      <c r="OV84" s="70"/>
+      <c r="OW84" s="70"/>
+      <c r="OX84" s="70"/>
+      <c r="OY84" s="70"/>
+      <c r="OZ84" s="70"/>
+      <c r="PA84" s="70"/>
+      <c r="PB84" s="70"/>
+      <c r="PC84" s="70"/>
+      <c r="PD84" s="70"/>
+      <c r="PE84" s="70"/>
+      <c r="PF84" s="70"/>
+      <c r="PG84" s="70"/>
+      <c r="PH84" s="70"/>
+      <c r="PI84" s="70"/>
+      <c r="PJ84" s="70"/>
+      <c r="PK84" s="70"/>
+      <c r="PL84" s="70"/>
+      <c r="PM84" s="70"/>
+      <c r="PN84" s="70"/>
+      <c r="PO84" s="70"/>
+      <c r="PP84" s="70"/>
+      <c r="PQ84" s="70"/>
+      <c r="PR84" s="70"/>
+      <c r="PS84" s="70"/>
+      <c r="PT84" s="70"/>
+      <c r="PU84" s="70"/>
+      <c r="PV84" s="70"/>
+      <c r="PW84" s="70"/>
+      <c r="PX84" s="70"/>
+      <c r="PY84" s="70"/>
+      <c r="PZ84" s="70"/>
+      <c r="QA84" s="70"/>
+      <c r="QB84" s="70"/>
+      <c r="QC84" s="70"/>
+      <c r="QD84" s="70"/>
+      <c r="QE84" s="70"/>
+      <c r="QF84" s="70"/>
+      <c r="QG84" s="70"/>
+      <c r="QH84" s="70"/>
+      <c r="QI84" s="70"/>
+      <c r="QJ84" s="70"/>
+      <c r="QK84" s="70"/>
+      <c r="QL84" s="70"/>
+      <c r="QM84" s="70"/>
+      <c r="QN84" s="70"/>
+      <c r="QO84" s="70"/>
+      <c r="QP84" s="70"/>
+      <c r="QQ84" s="70"/>
+      <c r="QR84" s="70"/>
+      <c r="QS84" s="70"/>
+      <c r="QT84" s="70"/>
+      <c r="QU84" s="70"/>
+      <c r="QV84" s="70"/>
+      <c r="QW84" s="70"/>
+      <c r="QX84" s="70"/>
+      <c r="QY84" s="70"/>
+      <c r="QZ84" s="70"/>
+      <c r="RA84" s="70"/>
+      <c r="RB84" s="70"/>
+      <c r="RC84" s="70"/>
+      <c r="RD84" s="70"/>
+      <c r="RE84" s="70"/>
+      <c r="RF84" s="70"/>
+      <c r="RG84" s="70"/>
+      <c r="RH84" s="70"/>
+      <c r="RI84" s="70"/>
+      <c r="RJ84" s="70"/>
+      <c r="RK84" s="70"/>
+      <c r="RL84" s="70"/>
+      <c r="RM84" s="70"/>
+      <c r="RN84" s="70"/>
+      <c r="RO84" s="70"/>
+      <c r="RP84" s="70"/>
+      <c r="RQ84" s="70"/>
+      <c r="RR84" s="70"/>
+      <c r="RS84" s="70"/>
+      <c r="RT84" s="70"/>
+      <c r="RU84" s="70"/>
+      <c r="RV84" s="70"/>
+      <c r="RW84" s="70"/>
+      <c r="RX84" s="70"/>
+      <c r="RY84" s="70"/>
+      <c r="RZ84" s="70"/>
+      <c r="SA84" s="70"/>
+      <c r="SB84" s="70"/>
+      <c r="SC84" s="70"/>
+      <c r="SD84" s="70"/>
+      <c r="SE84" s="70"/>
+      <c r="SF84" s="70"/>
+      <c r="SG84" s="70"/>
+      <c r="SH84" s="70"/>
+      <c r="SI84" s="70"/>
+      <c r="SJ84" s="70"/>
+      <c r="SK84" s="70"/>
+      <c r="SL84" s="70"/>
+      <c r="SM84" s="70"/>
+      <c r="SN84" s="70"/>
+      <c r="SO84" s="70"/>
+      <c r="SP84" s="70"/>
+      <c r="SQ84" s="70"/>
+      <c r="SR84" s="70"/>
+      <c r="SS84" s="70"/>
+      <c r="ST84" s="70"/>
+      <c r="SU84" s="70"/>
+      <c r="SV84" s="70"/>
+      <c r="SW84" s="70"/>
+      <c r="SX84" s="70"/>
+      <c r="SY84" s="70"/>
+      <c r="SZ84" s="70"/>
+      <c r="TA84" s="70"/>
+      <c r="TB84" s="70"/>
+      <c r="TC84" s="70"/>
+      <c r="TD84" s="70"/>
+      <c r="TE84" s="70"/>
+      <c r="TF84" s="70"/>
+      <c r="TG84" s="70"/>
+      <c r="TH84" s="70"/>
+      <c r="TI84" s="70"/>
+      <c r="TJ84" s="70"/>
+      <c r="TK84" s="70"/>
+      <c r="TL84" s="70"/>
+      <c r="TM84" s="70"/>
+      <c r="TN84" s="70"/>
+      <c r="TO84" s="70"/>
+      <c r="TP84" s="70"/>
+      <c r="TQ84" s="70"/>
+      <c r="TR84" s="70"/>
+      <c r="TS84" s="70"/>
+      <c r="TT84" s="70"/>
+      <c r="TU84" s="70"/>
+      <c r="TV84" s="70"/>
+      <c r="TW84" s="70"/>
+      <c r="TX84" s="70"/>
+      <c r="TY84" s="70"/>
+      <c r="TZ84" s="70"/>
+      <c r="UA84" s="70"/>
+      <c r="UB84" s="70"/>
+      <c r="UC84" s="70"/>
+      <c r="UD84" s="70"/>
+      <c r="UE84" s="70"/>
+      <c r="UF84" s="70"/>
+      <c r="UG84" s="70"/>
+      <c r="UH84" s="70"/>
+      <c r="UI84" s="70"/>
+      <c r="UJ84" s="70"/>
+      <c r="UK84" s="70"/>
+      <c r="UL84" s="70"/>
+      <c r="UM84" s="70"/>
+      <c r="UN84" s="70"/>
+      <c r="UO84" s="70"/>
+      <c r="UP84" s="70"/>
+      <c r="UQ84" s="70"/>
+      <c r="UR84" s="70"/>
+      <c r="US84" s="70"/>
+      <c r="UT84" s="70"/>
+      <c r="UU84" s="70"/>
+      <c r="UV84" s="70"/>
+      <c r="UW84" s="70"/>
+      <c r="UX84" s="70"/>
+      <c r="UY84" s="70"/>
+      <c r="UZ84" s="70"/>
+      <c r="VA84" s="70"/>
+      <c r="VB84" s="70"/>
+      <c r="VC84" s="70"/>
+      <c r="VD84" s="70"/>
+      <c r="VE84" s="70"/>
+      <c r="VF84" s="70"/>
+      <c r="VG84" s="70"/>
+      <c r="VH84" s="70"/>
+      <c r="VI84" s="70"/>
+      <c r="VJ84" s="70"/>
+      <c r="VK84" s="70"/>
+      <c r="VL84" s="70"/>
+      <c r="VM84" s="70"/>
+      <c r="VN84" s="70"/>
+      <c r="VO84" s="70"/>
+      <c r="VP84" s="70"/>
+      <c r="VQ84" s="70"/>
+      <c r="VR84" s="70"/>
+      <c r="VS84" s="70"/>
+      <c r="VT84" s="70"/>
+      <c r="VU84" s="70"/>
+      <c r="VV84" s="70"/>
+      <c r="VW84" s="70"/>
+      <c r="VX84" s="70"/>
+      <c r="VY84" s="70"/>
+      <c r="VZ84" s="70"/>
+      <c r="WA84" s="70"/>
+      <c r="WB84" s="70"/>
+      <c r="WC84" s="70"/>
+      <c r="WD84" s="70"/>
+      <c r="WE84" s="70"/>
+      <c r="WF84" s="70"/>
+      <c r="WG84" s="70"/>
+      <c r="WH84" s="70"/>
+      <c r="WI84" s="70"/>
+      <c r="WJ84" s="70"/>
+      <c r="WK84" s="70"/>
+      <c r="WL84" s="70"/>
+      <c r="WM84" s="70"/>
+      <c r="WN84" s="70"/>
+      <c r="WO84" s="70"/>
+      <c r="WP84" s="70"/>
+      <c r="WQ84" s="70"/>
+      <c r="WR84" s="70"/>
+      <c r="WS84" s="70"/>
+      <c r="WT84" s="70"/>
+      <c r="WU84" s="70"/>
+      <c r="WV84" s="70"/>
+      <c r="WW84" s="70"/>
+      <c r="WX84" s="70"/>
+      <c r="WY84" s="70"/>
+      <c r="WZ84" s="70"/>
+      <c r="XA84" s="70"/>
+      <c r="XB84" s="70"/>
+      <c r="XC84" s="70"/>
+      <c r="XD84" s="70"/>
+      <c r="XE84" s="70"/>
+      <c r="XF84" s="70"/>
+      <c r="XG84" s="70"/>
+      <c r="XH84" s="70"/>
+      <c r="XI84" s="70"/>
+      <c r="XJ84" s="70"/>
+      <c r="XK84" s="70"/>
+      <c r="XL84" s="70"/>
+      <c r="XM84" s="70"/>
+      <c r="XN84" s="70"/>
+      <c r="XO84" s="70"/>
+      <c r="XP84" s="70"/>
+      <c r="XQ84" s="70"/>
+      <c r="XR84" s="70"/>
+      <c r="XS84" s="70"/>
+      <c r="XT84" s="70"/>
+      <c r="XU84" s="70"/>
+      <c r="XV84" s="70"/>
+      <c r="XW84" s="70"/>
+      <c r="XX84" s="70"/>
+      <c r="XY84" s="70"/>
+      <c r="XZ84" s="70"/>
+      <c r="YA84" s="70"/>
+      <c r="YB84" s="70"/>
+      <c r="YC84" s="70"/>
+      <c r="YD84" s="70"/>
+      <c r="YE84" s="70"/>
+      <c r="YF84" s="70"/>
+      <c r="YG84" s="70"/>
+      <c r="YH84" s="70"/>
+      <c r="YI84" s="70"/>
+      <c r="YJ84" s="70"/>
+      <c r="YK84" s="70"/>
+      <c r="YL84" s="70"/>
+      <c r="YM84" s="70"/>
+      <c r="YN84" s="70"/>
+      <c r="YO84" s="70"/>
+      <c r="YP84" s="70"/>
+      <c r="YQ84" s="70"/>
+      <c r="YR84" s="70"/>
+      <c r="YS84" s="70"/>
+      <c r="YT84" s="70"/>
+      <c r="YU84" s="70"/>
+      <c r="YV84" s="70"/>
+      <c r="YW84" s="70"/>
+      <c r="YX84" s="70"/>
+      <c r="YY84" s="70"/>
+      <c r="YZ84" s="70"/>
+      <c r="ZA84" s="70"/>
+      <c r="ZB84" s="70"/>
+      <c r="ZC84" s="70"/>
+      <c r="ZD84" s="70"/>
+      <c r="ZE84" s="70"/>
+      <c r="ZF84" s="70"/>
+      <c r="ZG84" s="70"/>
+      <c r="ZH84" s="70"/>
+      <c r="ZI84" s="70"/>
+      <c r="ZJ84" s="70"/>
+      <c r="ZK84" s="70"/>
+      <c r="ZL84" s="70"/>
+      <c r="ZM84" s="70"/>
+      <c r="ZN84" s="70"/>
+      <c r="ZO84" s="70"/>
+      <c r="ZP84" s="70"/>
+      <c r="ZQ84" s="70"/>
+      <c r="ZR84" s="70"/>
+      <c r="ZS84" s="70"/>
+      <c r="ZT84" s="70"/>
+      <c r="ZU84" s="70"/>
+      <c r="ZV84" s="70"/>
+      <c r="ZW84" s="70"/>
+      <c r="ZX84" s="70"/>
+      <c r="ZY84" s="70"/>
+      <c r="ZZ84" s="70"/>
+      <c r="AAA84" s="70"/>
+      <c r="AAB84" s="70"/>
+      <c r="AAC84" s="70"/>
+      <c r="AAD84" s="70"/>
+      <c r="AAE84" s="70"/>
+      <c r="AAF84" s="70"/>
+      <c r="AAG84" s="70"/>
+      <c r="AAH84" s="70"/>
+      <c r="AAI84" s="70"/>
+      <c r="AAJ84" s="70"/>
+      <c r="AAK84" s="70"/>
+      <c r="AAL84" s="70"/>
+      <c r="AAM84" s="70"/>
+      <c r="AAN84" s="70"/>
+      <c r="AAO84" s="70"/>
+      <c r="AAP84" s="70"/>
+      <c r="AAQ84" s="70"/>
+      <c r="AAR84" s="70"/>
+      <c r="AAS84" s="70"/>
+      <c r="AAT84" s="70"/>
+      <c r="AAU84" s="70"/>
+      <c r="AAV84" s="70"/>
+      <c r="AAW84" s="70"/>
+      <c r="AAX84" s="70"/>
+      <c r="AAY84" s="70"/>
+      <c r="AAZ84" s="70"/>
+      <c r="ABA84" s="70"/>
+      <c r="ABB84" s="70"/>
+      <c r="ABC84" s="70"/>
+      <c r="ABD84" s="70"/>
+      <c r="ABE84" s="70"/>
+      <c r="ABF84" s="70"/>
+      <c r="ABG84" s="70"/>
+      <c r="ABH84" s="70"/>
+      <c r="ABI84" s="70"/>
+      <c r="ABJ84" s="70"/>
+      <c r="ABK84" s="70"/>
+      <c r="ABL84" s="70"/>
+      <c r="ABM84" s="70"/>
+      <c r="ABN84" s="70"/>
+      <c r="ABO84" s="70"/>
+      <c r="ABP84" s="70"/>
+      <c r="ABQ84" s="70"/>
+      <c r="ABR84" s="70"/>
+      <c r="ABS84" s="70"/>
+      <c r="ABT84" s="70"/>
+      <c r="ABU84" s="70"/>
+      <c r="ABV84" s="70"/>
+      <c r="ABW84" s="70"/>
+      <c r="ABX84" s="70"/>
+      <c r="ABY84" s="70"/>
+      <c r="ABZ84" s="70"/>
+      <c r="ACA84" s="70"/>
+      <c r="ACB84" s="70"/>
+      <c r="ACC84" s="70"/>
+      <c r="ACD84" s="70"/>
+      <c r="ACE84" s="70"/>
+      <c r="ACF84" s="70"/>
+      <c r="ACG84" s="70"/>
+      <c r="ACH84" s="70"/>
+      <c r="ACI84" s="70"/>
+      <c r="ACJ84" s="70"/>
+      <c r="ACK84" s="70"/>
+      <c r="ACL84" s="70"/>
+      <c r="ACM84" s="70"/>
+      <c r="ACN84" s="70"/>
+      <c r="ACO84" s="70"/>
+      <c r="ACP84" s="70"/>
+      <c r="ACQ84" s="70"/>
+      <c r="ACR84" s="70"/>
+      <c r="ACS84" s="70"/>
+      <c r="ACT84" s="70"/>
+      <c r="ACU84" s="70"/>
+      <c r="ACV84" s="70"/>
+      <c r="ACW84" s="70"/>
+      <c r="ACX84" s="70"/>
+      <c r="ACY84" s="70"/>
+      <c r="ACZ84" s="70"/>
+      <c r="ADA84" s="70"/>
+      <c r="ADB84" s="70"/>
+      <c r="ADC84" s="70"/>
+      <c r="ADD84" s="70"/>
+      <c r="ADE84" s="70"/>
+      <c r="ADF84" s="70"/>
+      <c r="ADG84" s="70"/>
+      <c r="ADH84" s="70"/>
+      <c r="ADI84" s="70"/>
+      <c r="ADJ84" s="70"/>
+      <c r="ADK84" s="70"/>
+      <c r="ADL84" s="70"/>
+      <c r="ADM84" s="70"/>
+      <c r="ADN84" s="70"/>
+      <c r="ADO84" s="70"/>
+      <c r="ADP84" s="70"/>
+      <c r="ADQ84" s="70"/>
+      <c r="ADR84" s="70"/>
+      <c r="ADS84" s="70"/>
+      <c r="ADT84" s="70"/>
+      <c r="ADU84" s="70"/>
+      <c r="ADV84" s="70"/>
+      <c r="ADW84" s="70"/>
+      <c r="ADX84" s="70"/>
+      <c r="ADY84" s="70"/>
+      <c r="ADZ84" s="70"/>
+      <c r="AEA84" s="70"/>
+      <c r="AEB84" s="70"/>
+      <c r="AEC84" s="70"/>
+      <c r="AED84" s="70"/>
+      <c r="AEE84" s="70"/>
+      <c r="AEF84" s="70"/>
+      <c r="AEG84" s="70"/>
+      <c r="AEH84" s="70"/>
+      <c r="AEI84" s="70"/>
+      <c r="AEJ84" s="70"/>
+      <c r="AEK84" s="70"/>
+      <c r="AEL84" s="70"/>
+      <c r="AEM84" s="70"/>
+      <c r="AEN84" s="70"/>
+      <c r="AEO84" s="70"/>
+      <c r="AEP84" s="70"/>
+      <c r="AEQ84" s="70"/>
+      <c r="AER84" s="70"/>
+      <c r="AES84" s="70"/>
+      <c r="AET84" s="70"/>
+      <c r="AEU84" s="70"/>
+      <c r="AEV84" s="70"/>
+      <c r="AEW84" s="70"/>
+      <c r="AEX84" s="70"/>
+      <c r="AEY84" s="70"/>
+      <c r="AEZ84" s="70"/>
+      <c r="AFA84" s="70"/>
+      <c r="AFB84" s="70"/>
+      <c r="AFC84" s="70"/>
+      <c r="AFD84" s="70"/>
+      <c r="AFE84" s="70"/>
+      <c r="AFF84" s="70"/>
+      <c r="AFG84" s="70"/>
+      <c r="AFH84" s="70"/>
+      <c r="AFI84" s="70"/>
+      <c r="AFJ84" s="70"/>
+      <c r="AFK84" s="70"/>
+      <c r="AFL84" s="70"/>
+      <c r="AFM84" s="70"/>
+      <c r="AFN84" s="70"/>
+      <c r="AFO84" s="70"/>
+      <c r="AFP84" s="70"/>
+      <c r="AFQ84" s="70"/>
+      <c r="AFR84" s="70"/>
+      <c r="AFS84" s="70"/>
+      <c r="AFT84" s="70"/>
+      <c r="AFU84" s="70"/>
+      <c r="AFV84" s="70"/>
+      <c r="AFW84" s="70"/>
+      <c r="AFX84" s="70"/>
+      <c r="AFY84" s="70"/>
+      <c r="AFZ84" s="70"/>
+      <c r="AGA84" s="70"/>
+      <c r="AGB84" s="70"/>
+      <c r="AGC84" s="70"/>
+      <c r="AGD84" s="70"/>
+      <c r="AGE84" s="70"/>
+      <c r="AGF84" s="70"/>
+      <c r="AGG84" s="70"/>
+      <c r="AGH84" s="70"/>
+      <c r="AGI84" s="70"/>
+      <c r="AGJ84" s="70"/>
+      <c r="AGK84" s="70"/>
+      <c r="AGL84" s="70"/>
+      <c r="AGM84" s="70"/>
+      <c r="AGN84" s="70"/>
+      <c r="AGO84" s="70"/>
+      <c r="AGP84" s="70"/>
+      <c r="AGQ84" s="70"/>
+      <c r="AGR84" s="70"/>
+      <c r="AGS84" s="70"/>
+      <c r="AGT84" s="70"/>
+      <c r="AGU84" s="70"/>
+      <c r="AGV84" s="70"/>
+      <c r="AGW84" s="70"/>
+      <c r="AGX84" s="70"/>
+      <c r="AGY84" s="70"/>
+      <c r="AGZ84" s="70"/>
+      <c r="AHA84" s="70"/>
+      <c r="AHB84" s="70"/>
+      <c r="AHC84" s="70"/>
+      <c r="AHD84" s="70"/>
+      <c r="AHE84" s="70"/>
+      <c r="AHF84" s="70"/>
+      <c r="AHG84" s="70"/>
+      <c r="AHH84" s="70"/>
+      <c r="AHI84" s="70"/>
+      <c r="AHJ84" s="70"/>
+      <c r="AHK84" s="70"/>
+      <c r="AHL84" s="70"/>
+      <c r="AHM84" s="70"/>
+      <c r="AHN84" s="70"/>
+      <c r="AHO84" s="70"/>
+      <c r="AHP84" s="70"/>
+      <c r="AHQ84" s="70"/>
+      <c r="AHR84" s="70"/>
+      <c r="AHS84" s="70"/>
+      <c r="AHT84" s="70"/>
+      <c r="AHU84" s="70"/>
+      <c r="AHV84" s="70"/>
+      <c r="AHW84" s="70"/>
+      <c r="AHX84" s="70"/>
+      <c r="AHY84" s="70"/>
+      <c r="AHZ84" s="70"/>
+      <c r="AIA84" s="70"/>
+      <c r="AIB84" s="70"/>
+      <c r="AIC84" s="70"/>
+      <c r="AID84" s="70"/>
+      <c r="AIE84" s="70"/>
+      <c r="AIF84" s="70"/>
+      <c r="AIG84" s="70"/>
+      <c r="AIH84" s="70"/>
+      <c r="AII84" s="70"/>
+      <c r="AIJ84" s="70"/>
+      <c r="AIK84" s="70"/>
+      <c r="AIL84" s="70"/>
+      <c r="AIM84" s="70"/>
+      <c r="AIN84" s="70"/>
+      <c r="AIO84" s="70"/>
+      <c r="AIP84" s="70"/>
+      <c r="AIQ84" s="70"/>
+      <c r="AIR84" s="70"/>
+      <c r="AIS84" s="70"/>
+      <c r="AIT84" s="70"/>
+      <c r="AIU84" s="70"/>
+      <c r="AIV84" s="70"/>
+      <c r="AIW84" s="70"/>
+      <c r="AIX84" s="70"/>
+      <c r="AIY84" s="70"/>
+      <c r="AIZ84" s="70"/>
+      <c r="AJA84" s="70"/>
+      <c r="AJB84" s="70"/>
+      <c r="AJC84" s="70"/>
+      <c r="AJD84" s="70"/>
+      <c r="AJE84" s="70"/>
+      <c r="AJF84" s="70"/>
+      <c r="AJG84" s="70"/>
+      <c r="AJH84" s="70"/>
+      <c r="AJI84" s="70"/>
+      <c r="AJJ84" s="70"/>
+      <c r="AJK84" s="70"/>
+      <c r="AJL84" s="70"/>
+      <c r="AJM84" s="70"/>
+      <c r="AJN84" s="70"/>
+      <c r="AJO84" s="70"/>
+      <c r="AJP84" s="70"/>
+      <c r="AJQ84" s="70"/>
+      <c r="AJR84" s="70"/>
+      <c r="AJS84" s="70"/>
+      <c r="AJT84" s="70"/>
+      <c r="AJU84" s="70"/>
+      <c r="AJV84" s="70"/>
+      <c r="AJW84" s="70"/>
+      <c r="AJX84" s="70"/>
+      <c r="AJY84" s="70"/>
+      <c r="AJZ84" s="70"/>
+      <c r="AKA84" s="70"/>
+      <c r="AKB84" s="70"/>
+      <c r="AKC84" s="70"/>
+      <c r="AKD84" s="70"/>
+      <c r="AKE84" s="70"/>
+      <c r="AKF84" s="70"/>
+      <c r="AKG84" s="70"/>
+      <c r="AKH84" s="70"/>
+      <c r="AKI84" s="70"/>
+      <c r="AKJ84" s="70"/>
+      <c r="AKK84" s="70"/>
+      <c r="AKL84" s="70"/>
+      <c r="AKM84" s="70"/>
+      <c r="AKN84" s="70"/>
+      <c r="AKO84" s="70"/>
+      <c r="AKP84" s="70"/>
+      <c r="AKQ84" s="70"/>
+      <c r="AKR84" s="70"/>
+      <c r="AKS84" s="70"/>
+      <c r="AKT84" s="70"/>
+      <c r="AKU84" s="70"/>
+      <c r="AKV84" s="70"/>
+      <c r="AKW84" s="70"/>
+      <c r="AKX84" s="70"/>
+      <c r="AKY84" s="70"/>
+      <c r="AKZ84" s="70"/>
+      <c r="ALA84" s="70"/>
+      <c r="ALB84" s="70"/>
+      <c r="ALC84" s="70"/>
+      <c r="ALD84" s="70"/>
+      <c r="ALE84" s="70"/>
+      <c r="ALF84" s="70"/>
+      <c r="ALG84" s="70"/>
+      <c r="ALH84" s="70"/>
+      <c r="ALI84" s="70"/>
+      <c r="ALJ84" s="70"/>
+      <c r="ALK84" s="70"/>
+      <c r="ALL84" s="70"/>
+      <c r="ALM84" s="70"/>
+      <c r="ALN84" s="70"/>
+      <c r="ALO84" s="70"/>
+      <c r="ALP84" s="70"/>
+      <c r="ALQ84" s="70"/>
+      <c r="ALR84" s="70"/>
+      <c r="ALS84" s="70"/>
+      <c r="ALT84" s="70"/>
+      <c r="ALU84" s="70"/>
+      <c r="ALV84" s="70"/>
+      <c r="ALW84" s="70"/>
+      <c r="ALX84" s="70"/>
+      <c r="ALY84" s="70"/>
+      <c r="ALZ84" s="70"/>
+      <c r="AMA84" s="70"/>
+      <c r="AMB84" s="70"/>
+      <c r="AMC84" s="70"/>
+      <c r="AMD84" s="70"/>
+      <c r="AME84" s="70"/>
+      <c r="AMF84" s="70"/>
+      <c r="AMG84" s="70"/>
+      <c r="AMH84" s="70"/>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="1" t="s">
@@ -20546,7 +20581,7 @@
       </c>
     </row>
     <row r="88" s="6" customFormat="1" spans="1:1022">
-      <c r="A88" s="71" t="s">
+      <c r="A88" s="72" t="s">
         <v>149</v>
       </c>
       <c r="B88" s="27" t="s">
@@ -23711,10 +23746,10 @@
       </c>
     </row>
     <row r="97" spans="5:5">
-      <c r="E97" s="68"/>
+      <c r="E97" s="69"/>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="72" t="s">
+      <c r="A98" s="73" t="s">
         <v>153</v>
       </c>
       <c r="B98" s="59" t="s">
@@ -23726,7 +23761,7 @@
       <c r="D98" s="60">
         <v>0.9673051</v>
       </c>
-      <c r="E98" s="66">
+      <c r="E98" s="67">
         <v>0.9686</v>
       </c>
     </row>
@@ -23743,7 +23778,7 @@
       <c r="D99" s="10">
         <v>0.9671612</v>
       </c>
-      <c r="E99" s="68">
+      <c r="E99" s="69">
         <v>0.9687</v>
       </c>
     </row>
@@ -23760,7 +23795,7 @@
       <c r="D100" s="10">
         <v>0.9673732</v>
       </c>
-      <c r="E100" s="68">
+      <c r="E100" s="69">
         <v>0.9686</v>
       </c>
     </row>
@@ -23777,120 +23812,172 @@
       <c r="D101" s="10">
         <v>0.9674291</v>
       </c>
-      <c r="E101" s="68">
+      <c r="E101" s="69">
         <v>0.96939</v>
       </c>
     </row>
-    <row r="102" spans="5:5">
-      <c r="E102" s="68"/>
+    <row r="102" spans="1:5">
+      <c r="A102" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C102" s="10">
+        <v>0.994993</v>
+      </c>
+      <c r="D102" s="10">
+        <v>0.967249</v>
+      </c>
+      <c r="E102" s="69"/>
     </row>
-    <row r="103" spans="5:5">
-      <c r="E103" s="68"/>
+    <row r="103" spans="1:5">
+      <c r="A103" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C103" s="10">
+        <v>0.9975126</v>
+      </c>
+      <c r="D103" s="10">
+        <v>0.9673428</v>
+      </c>
+      <c r="E103" s="69"/>
     </row>
-    <row r="104" spans="5:5">
-      <c r="E104" s="68"/>
+    <row r="104" spans="1:5">
+      <c r="A104" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B104" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C104" s="20">
+        <v>0.9965554</v>
+      </c>
+      <c r="D104" s="20">
+        <v>0.9675682</v>
+      </c>
+      <c r="E104" s="35">
+        <v>0.9695</v>
+      </c>
     </row>
-    <row r="105" spans="5:5">
-      <c r="E105" s="68"/>
+    <row r="105" spans="1:5">
+      <c r="A105" s="62" t="s">
+        <v>161</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C105" s="10">
+        <v>0.9961418</v>
+      </c>
+      <c r="D105" s="28">
+        <v>0.967788</v>
+      </c>
+      <c r="E105" s="69">
+        <v>0.9683</v>
+      </c>
     </row>
     <row r="106" spans="5:5">
-      <c r="E106" s="68"/>
+      <c r="E106" s="69"/>
     </row>
     <row r="107" spans="5:5">
-      <c r="E107" s="68"/>
+      <c r="E107" s="69"/>
     </row>
     <row r="108" spans="5:5">
-      <c r="E108" s="68"/>
+      <c r="E108" s="69"/>
     </row>
     <row r="109" spans="5:5">
-      <c r="E109" s="68"/>
+      <c r="E109" s="69"/>
     </row>
     <row r="110" spans="5:5">
-      <c r="E110" s="68"/>
+      <c r="E110" s="69"/>
     </row>
     <row r="111" spans="5:5">
-      <c r="E111" s="68"/>
+      <c r="E111" s="69"/>
     </row>
     <row r="112" spans="5:5">
-      <c r="E112" s="68"/>
+      <c r="E112" s="69"/>
     </row>
     <row r="113" spans="5:5">
-      <c r="E113" s="68"/>
+      <c r="E113" s="69"/>
     </row>
     <row r="114" spans="5:5">
-      <c r="E114" s="68"/>
+      <c r="E114" s="69"/>
     </row>
     <row r="115" spans="5:5">
-      <c r="E115" s="68"/>
+      <c r="E115" s="69"/>
     </row>
     <row r="116" spans="5:5">
-      <c r="E116" s="68"/>
+      <c r="E116" s="69"/>
     </row>
     <row r="117" spans="5:5">
-      <c r="E117" s="68"/>
+      <c r="E117" s="69"/>
     </row>
     <row r="118" spans="5:5">
-      <c r="E118" s="68"/>
+      <c r="E118" s="69"/>
     </row>
     <row r="119" spans="5:5">
-      <c r="E119" s="68"/>
+      <c r="E119" s="69"/>
     </row>
     <row r="120" spans="5:5">
-      <c r="E120" s="68"/>
+      <c r="E120" s="69"/>
     </row>
     <row r="121" spans="5:5">
-      <c r="E121" s="68"/>
+      <c r="E121" s="69"/>
     </row>
     <row r="122" spans="5:5">
-      <c r="E122" s="68"/>
+      <c r="E122" s="69"/>
     </row>
     <row r="123" spans="5:5">
-      <c r="E123" s="68"/>
+      <c r="E123" s="69"/>
     </row>
     <row r="124" spans="5:5">
-      <c r="E124" s="68"/>
+      <c r="E124" s="69"/>
     </row>
     <row r="125" spans="5:5">
-      <c r="E125" s="68"/>
+      <c r="E125" s="69"/>
     </row>
     <row r="126" spans="5:5">
-      <c r="E126" s="68"/>
+      <c r="E126" s="69"/>
     </row>
     <row r="127" spans="5:5">
-      <c r="E127" s="68"/>
+      <c r="E127" s="69"/>
     </row>
     <row r="128" spans="5:5">
-      <c r="E128" s="68"/>
+      <c r="E128" s="69"/>
     </row>
     <row r="129" spans="5:5">
-      <c r="E129" s="68"/>
+      <c r="E129" s="69"/>
     </row>
     <row r="130" spans="5:5">
-      <c r="E130" s="68"/>
+      <c r="E130" s="69"/>
     </row>
     <row r="131" spans="5:5">
-      <c r="E131" s="68"/>
+      <c r="E131" s="69"/>
     </row>
     <row r="132" spans="5:5">
-      <c r="E132" s="68"/>
+      <c r="E132" s="69"/>
     </row>
     <row r="133" spans="5:5">
-      <c r="E133" s="68"/>
+      <c r="E133" s="69"/>
     </row>
     <row r="134" spans="5:5">
-      <c r="E134" s="68"/>
+      <c r="E134" s="69"/>
     </row>
     <row r="135" spans="5:5">
-      <c r="E135" s="68"/>
+      <c r="E135" s="69"/>
     </row>
     <row r="136" spans="5:5">
-      <c r="E136" s="68"/>
+      <c r="E136" s="69"/>
     </row>
     <row r="137" spans="5:5">
-      <c r="E137" s="68"/>
+      <c r="E137" s="69"/>
     </row>
     <row r="138" spans="5:5">
-      <c r="E138" s="68"/>
+      <c r="E138" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
'min_child_weight': 10，feature_percentile = 0.95，0.97000
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13305" tabRatio="993"/>
+    <workbookView windowWidth="20385" windowHeight="8625" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="特征选取" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176">
   <si>
     <r>
       <rPr>
@@ -1508,6 +1508,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>去掉冗余的</t>
     </r>
     <r>
@@ -1519,20 +1524,30 @@
       <t xml:space="preserve"> last_time_orderType</t>
     </r>
   </si>
+  <si>
+    <t>min_child_weight': 10</t>
+  </si>
+  <si>
+    <t>后期调参</t>
+  </si>
+  <si>
+    <t>min_child_weight': 10
+feature_percentile = 0.95</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.0000000_ "/>
-    <numFmt numFmtId="177" formatCode="0.00000_ "/>
+    <numFmt numFmtId="176" formatCode="0.00000_ "/>
+    <numFmt numFmtId="177" formatCode="0.0000000_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="30">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1551,16 +1566,13 @@
     <font>
       <sz val="8"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFFF0000"/>
       <name val="DejaVu Sans Mono"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1571,9 +1583,24 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1586,9 +1613,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1596,7 +1637,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1616,6 +1672,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1623,8 +1680,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1639,15 +1711,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1663,60 +1729,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1801,7 +1813,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1813,7 +1831,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1831,7 +1855,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1843,13 +1927,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1861,19 +1951,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1885,13 +1963,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1903,73 +1975,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1981,7 +1987,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1992,6 +2004,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -2027,9 +2063,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2066,168 +2104,142 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2263,16 +2275,16 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -2293,7 +2305,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2308,7 +2320,7 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2317,13 +2329,13 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2335,40 +2347,40 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -2392,10 +2404,10 @@
     <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2404,7 +2416,7 @@
     <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2413,7 +2425,7 @@
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2422,31 +2434,31 @@
     <xf numFmtId="49" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -2460,6 +2472,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2778,8 +2793,8 @@
   <sheetPr/>
   <dimension ref="A1:AMH137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -18330,7 +18345,7 @@
       <c r="G72" s="35">
         <v>0.96859</v>
       </c>
-      <c r="H72" s="64" t="s">
+      <c r="H72" s="63" t="s">
         <v>125</v>
       </c>
       <c r="I72" s="46"/>
@@ -19370,7 +19385,7 @@
       <c r="G73" s="12">
         <v>0.9684</v>
       </c>
-      <c r="H73" s="65" t="s">
+      <c r="H73" s="64" t="s">
         <v>127</v>
       </c>
     </row>
@@ -19436,7 +19451,7 @@
       <c r="F76" s="20">
         <v>0.9671155</v>
       </c>
-      <c r="G76" s="66">
+      <c r="G76" s="65">
         <v>0.9682</v>
       </c>
     </row>
@@ -19459,7 +19474,7 @@
       <c r="F78" s="57">
         <v>0.9666471</v>
       </c>
-      <c r="G78" s="67">
+      <c r="G78" s="66">
         <v>0.9678</v>
       </c>
     </row>
@@ -19574,10 +19589,10 @@
       <c r="F84" s="60">
         <v>0.9673051</v>
       </c>
-      <c r="G84" s="68">
+      <c r="G84" s="67">
         <v>0.9686</v>
       </c>
-      <c r="H84" s="69"/>
+      <c r="H84" s="68"/>
       <c r="I84" s="72"/>
       <c r="J84" s="72"/>
       <c r="K84" s="72"/>
@@ -23819,7 +23834,7 @@
       </c>
     </row>
     <row r="97" spans="5:5">
-      <c r="E97" s="70"/>
+      <c r="E97" s="69"/>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="75" t="s">
@@ -23834,7 +23849,7 @@
       <c r="D98" s="60">
         <v>0.9673051</v>
       </c>
-      <c r="E98" s="68">
+      <c r="E98" s="67">
         <v>0.9686</v>
       </c>
     </row>
@@ -23851,7 +23866,7 @@
       <c r="D99" s="10">
         <v>0.9671612</v>
       </c>
-      <c r="E99" s="70">
+      <c r="E99" s="69">
         <v>0.9687</v>
       </c>
     </row>
@@ -23868,7 +23883,7 @@
       <c r="D100" s="10">
         <v>0.9673732</v>
       </c>
-      <c r="E100" s="70">
+      <c r="E100" s="69">
         <v>0.9686</v>
       </c>
     </row>
@@ -23885,7 +23900,7 @@
       <c r="D101" s="10">
         <v>0.9674291</v>
       </c>
-      <c r="E101" s="70">
+      <c r="E101" s="69">
         <v>0.96939</v>
       </c>
     </row>
@@ -23902,7 +23917,7 @@
       <c r="D102" s="10">
         <v>0.967249</v>
       </c>
-      <c r="E102" s="70"/>
+      <c r="E102" s="69"/>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="1" t="s">
@@ -23917,7 +23932,7 @@
       <c r="D103" s="10">
         <v>0.9673428</v>
       </c>
-      <c r="E103" s="70"/>
+      <c r="E103" s="69"/>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="19" t="s">
@@ -23952,7 +23967,7 @@
       <c r="D105" s="28">
         <v>0.967788</v>
       </c>
-      <c r="E105" s="70">
+      <c r="E105" s="69">
         <v>0.9683</v>
       </c>
     </row>
@@ -23986,7 +24001,7 @@
       <c r="D107" s="20">
         <v>0.9676965</v>
       </c>
-      <c r="E107" s="67">
+      <c r="E107" s="66">
         <v>0.9689</v>
       </c>
     </row>
@@ -24003,12 +24018,12 @@
       <c r="D108" s="10">
         <v>0.9675807</v>
       </c>
-      <c r="E108" s="67">
+      <c r="E108" s="66">
         <v>0.96939</v>
       </c>
     </row>
     <row r="109" spans="5:5">
-      <c r="E109" s="70"/>
+      <c r="E109" s="69"/>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="1" t="s">
@@ -24023,10 +24038,10 @@
       <c r="D110" s="10">
         <v>0.9673982</v>
       </c>
-      <c r="E110" s="70">
+      <c r="E110" s="69">
         <v>0.9695</v>
       </c>
-      <c r="F110" s="71" t="s">
+      <c r="F110" s="70" t="s">
         <v>170</v>
       </c>
     </row>
@@ -24043,12 +24058,12 @@
       <c r="D111" s="10">
         <v>0.967503</v>
       </c>
-      <c r="E111" s="70">
+      <c r="E111" s="69">
         <v>0.9695</v>
       </c>
     </row>
     <row r="112" spans="1:5">
-      <c r="A112" s="63" t="s">
+      <c r="A112" s="31" t="s">
         <v>172</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -24060,84 +24075,115 @@
       <c r="D112" s="10">
         <v>0.9675222</v>
       </c>
-      <c r="E112" s="70">
+      <c r="E112" s="69">
         <v>0.9697</v>
       </c>
     </row>
-    <row r="113" spans="5:5">
-      <c r="E113" s="70"/>
+    <row r="113" spans="1:6">
+      <c r="A113" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C113" s="10">
+        <v>0.9978254</v>
+      </c>
+      <c r="D113" s="10">
+        <v>0.9678351</v>
+      </c>
+      <c r="E113" s="69">
+        <v>0.9699</v>
+      </c>
+      <c r="F113" s="71" t="s">
+        <v>174</v>
+      </c>
     </row>
-    <row r="114" spans="5:5">
-      <c r="E114" s="70"/>
+    <row r="114" ht="21" spans="1:5">
+      <c r="A114" s="76" t="s">
+        <v>175</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C114" s="10">
+        <v>0.9984165</v>
+      </c>
+      <c r="D114" s="10">
+        <v>0.9678722</v>
+      </c>
+      <c r="E114" s="69">
+        <v>0.97</v>
+      </c>
     </row>
     <row r="115" spans="5:5">
-      <c r="E115" s="70"/>
+      <c r="E115" s="69"/>
     </row>
     <row r="116" spans="5:5">
-      <c r="E116" s="70"/>
+      <c r="E116" s="69"/>
     </row>
     <row r="117" spans="5:5">
-      <c r="E117" s="70"/>
+      <c r="E117" s="69"/>
     </row>
     <row r="118" spans="5:5">
-      <c r="E118" s="70"/>
+      <c r="E118" s="69"/>
     </row>
     <row r="119" spans="5:5">
-      <c r="E119" s="70"/>
+      <c r="E119" s="69"/>
     </row>
     <row r="120" spans="5:5">
-      <c r="E120" s="70"/>
+      <c r="E120" s="69"/>
     </row>
     <row r="121" spans="5:5">
-      <c r="E121" s="70"/>
+      <c r="E121" s="69"/>
     </row>
     <row r="122" spans="5:5">
-      <c r="E122" s="70"/>
+      <c r="E122" s="69"/>
     </row>
     <row r="123" spans="5:5">
-      <c r="E123" s="70"/>
+      <c r="E123" s="69"/>
     </row>
     <row r="124" spans="5:5">
-      <c r="E124" s="70"/>
+      <c r="E124" s="69"/>
     </row>
     <row r="125" spans="5:5">
-      <c r="E125" s="70"/>
+      <c r="E125" s="69"/>
     </row>
     <row r="126" spans="5:5">
-      <c r="E126" s="70"/>
+      <c r="E126" s="69"/>
     </row>
     <row r="127" spans="5:5">
-      <c r="E127" s="70"/>
+      <c r="E127" s="69"/>
     </row>
     <row r="128" spans="5:5">
-      <c r="E128" s="70"/>
+      <c r="E128" s="69"/>
     </row>
     <row r="129" spans="5:5">
-      <c r="E129" s="70"/>
+      <c r="E129" s="69"/>
     </row>
     <row r="130" spans="5:5">
-      <c r="E130" s="70"/>
+      <c r="E130" s="69"/>
     </row>
     <row r="131" spans="5:5">
-      <c r="E131" s="70"/>
+      <c r="E131" s="69"/>
     </row>
     <row r="132" spans="5:5">
-      <c r="E132" s="70"/>
+      <c r="E132" s="69"/>
     </row>
     <row r="133" spans="5:5">
-      <c r="E133" s="70"/>
+      <c r="E133" s="69"/>
     </row>
     <row r="134" spans="5:5">
-      <c r="E134" s="70"/>
+      <c r="E134" s="69"/>
     </row>
     <row r="135" spans="5:5">
-      <c r="E135" s="70"/>
+      <c r="E135" s="69"/>
     </row>
     <row r="136" spans="5:5">
-      <c r="E136" s="70"/>
+      <c r="E136" s="69"/>
     </row>
     <row r="137" spans="5:5">
-      <c r="E137" s="70"/>
+      <c r="E137" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
back to baseline to feature engineering
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -2473,7 +2473,7 @@
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2793,8 +2793,8 @@
   <sheetPr/>
   <dimension ref="A1:AMH137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -24119,8 +24119,22 @@
     <row r="115" spans="5:5">
       <c r="E115" s="69"/>
     </row>
-    <row r="116" spans="5:5">
-      <c r="E116" s="69"/>
+    <row r="116" spans="1:5">
+      <c r="A116" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C116" s="10">
+        <v>0.9972809</v>
+      </c>
+      <c r="D116" s="10">
+        <v>0.9675222</v>
+      </c>
+      <c r="E116" s="69">
+        <v>0.9697</v>
+      </c>
     </row>
     <row r="117" spans="5:5">
       <c r="E117" s="69"/>

</xml_diff>

<commit_message>
设置 2016_2017_first_last_ordertype 为1 的预测概率为1，0.96990
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182">
   <si>
     <r>
       <rPr>
@@ -1601,6 +1601,83 @@
   <si>
     <t>228</t>
   </si>
+  <si>
+    <r>
+      <t>设置</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="9" tint="-0.25"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> 2016_2017_first_last_ordertype </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="9" tint="-0.25"/>
+        <charset val="134"/>
+      </rPr>
+      <t>为</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="9" tint="-0.25"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="9" tint="-0.25"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的预测概率为</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="9" tint="-0.25"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>规则</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="9" tint="-0.25"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> trick</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="9" tint="-0.25"/>
+        <charset val="134"/>
+      </rPr>
+      <t>！</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1614,7 +1691,7 @@
     <numFmt numFmtId="177" formatCode="0.00000_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="33">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1644,6 +1721,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="9" tint="-0.25"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1824,6 +1907,13 @@
       <sz val="8"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="9" tint="-0.25"/>
+      <name val="DejaVu Sans Mono"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -2180,142 +2270,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2514,10 +2604,13 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2539,6 +2632,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -2874,12 +2970,12 @@
   <dimension ref="A1:AMH137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="E119" sqref="E119"/>
+      <selection activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
   <cols>
-    <col min="1" max="1" width="39.5666666666667" style="1" customWidth="1"/>
+    <col min="1" max="1" width="39.65" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.775" style="1"/>
     <col min="3" max="3" width="10.3" style="10" customWidth="1"/>
     <col min="4" max="4" width="9.325" style="10" customWidth="1"/>
@@ -8189,7 +8285,7 @@
       <c r="AMH13" s="47"/>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:1022">
-      <c r="A14" s="76" t="s">
+      <c r="A14" s="78" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="19" t="s">
@@ -18425,7 +18521,7 @@
       <c r="G72" s="35">
         <v>0.96859</v>
       </c>
-      <c r="H72" s="66" t="s">
+      <c r="H72" s="67" t="s">
         <v>125</v>
       </c>
       <c r="I72" s="46"/>
@@ -19465,7 +19561,7 @@
       <c r="G73" s="12">
         <v>0.9684</v>
       </c>
-      <c r="H73" s="67" t="s">
+      <c r="H73" s="68" t="s">
         <v>127</v>
       </c>
     </row>
@@ -19531,7 +19627,7 @@
       <c r="F76" s="20">
         <v>0.9671155</v>
       </c>
-      <c r="G76" s="68">
+      <c r="G76" s="69">
         <v>0.9682</v>
       </c>
     </row>
@@ -19554,7 +19650,7 @@
       <c r="F78" s="57">
         <v>0.9666471</v>
       </c>
-      <c r="G78" s="69">
+      <c r="G78" s="70">
         <v>0.9678</v>
       </c>
     </row>
@@ -19669,1024 +19765,1024 @@
       <c r="F84" s="60">
         <v>0.9673051</v>
       </c>
-      <c r="G84" s="70">
+      <c r="G84" s="71">
         <v>0.9686</v>
       </c>
-      <c r="H84" s="71"/>
-      <c r="I84" s="75"/>
-      <c r="J84" s="75"/>
-      <c r="K84" s="75"/>
-      <c r="L84" s="75"/>
-      <c r="M84" s="75"/>
-      <c r="N84" s="75"/>
-      <c r="O84" s="75"/>
-      <c r="P84" s="75"/>
-      <c r="Q84" s="75"/>
-      <c r="R84" s="75"/>
-      <c r="S84" s="75"/>
-      <c r="T84" s="75"/>
-      <c r="U84" s="75"/>
-      <c r="V84" s="75"/>
-      <c r="W84" s="75"/>
-      <c r="X84" s="75"/>
-      <c r="Y84" s="75"/>
-      <c r="Z84" s="75"/>
-      <c r="AA84" s="75"/>
-      <c r="AB84" s="75"/>
-      <c r="AC84" s="75"/>
-      <c r="AD84" s="75"/>
-      <c r="AE84" s="75"/>
-      <c r="AF84" s="75"/>
-      <c r="AG84" s="75"/>
-      <c r="AH84" s="75"/>
-      <c r="AI84" s="75"/>
-      <c r="AJ84" s="75"/>
-      <c r="AK84" s="75"/>
-      <c r="AL84" s="75"/>
-      <c r="AM84" s="75"/>
-      <c r="AN84" s="75"/>
-      <c r="AO84" s="75"/>
-      <c r="AP84" s="75"/>
-      <c r="AQ84" s="75"/>
-      <c r="AR84" s="75"/>
-      <c r="AS84" s="75"/>
-      <c r="AT84" s="75"/>
-      <c r="AU84" s="75"/>
-      <c r="AV84" s="75"/>
-      <c r="AW84" s="75"/>
-      <c r="AX84" s="75"/>
-      <c r="AY84" s="75"/>
-      <c r="AZ84" s="75"/>
-      <c r="BA84" s="75"/>
-      <c r="BB84" s="75"/>
-      <c r="BC84" s="75"/>
-      <c r="BD84" s="75"/>
-      <c r="BE84" s="75"/>
-      <c r="BF84" s="75"/>
-      <c r="BG84" s="75"/>
-      <c r="BH84" s="75"/>
-      <c r="BI84" s="75"/>
-      <c r="BJ84" s="75"/>
-      <c r="BK84" s="75"/>
-      <c r="BL84" s="75"/>
-      <c r="BM84" s="75"/>
-      <c r="BN84" s="75"/>
-      <c r="BO84" s="75"/>
-      <c r="BP84" s="75"/>
-      <c r="BQ84" s="75"/>
-      <c r="BR84" s="75"/>
-      <c r="BS84" s="75"/>
-      <c r="BT84" s="75"/>
-      <c r="BU84" s="75"/>
-      <c r="BV84" s="75"/>
-      <c r="BW84" s="75"/>
-      <c r="BX84" s="75"/>
-      <c r="BY84" s="75"/>
-      <c r="BZ84" s="75"/>
-      <c r="CA84" s="75"/>
-      <c r="CB84" s="75"/>
-      <c r="CC84" s="75"/>
-      <c r="CD84" s="75"/>
-      <c r="CE84" s="75"/>
-      <c r="CF84" s="75"/>
-      <c r="CG84" s="75"/>
-      <c r="CH84" s="75"/>
-      <c r="CI84" s="75"/>
-      <c r="CJ84" s="75"/>
-      <c r="CK84" s="75"/>
-      <c r="CL84" s="75"/>
-      <c r="CM84" s="75"/>
-      <c r="CN84" s="75"/>
-      <c r="CO84" s="75"/>
-      <c r="CP84" s="75"/>
-      <c r="CQ84" s="75"/>
-      <c r="CR84" s="75"/>
-      <c r="CS84" s="75"/>
-      <c r="CT84" s="75"/>
-      <c r="CU84" s="75"/>
-      <c r="CV84" s="75"/>
-      <c r="CW84" s="75"/>
-      <c r="CX84" s="75"/>
-      <c r="CY84" s="75"/>
-      <c r="CZ84" s="75"/>
-      <c r="DA84" s="75"/>
-      <c r="DB84" s="75"/>
-      <c r="DC84" s="75"/>
-      <c r="DD84" s="75"/>
-      <c r="DE84" s="75"/>
-      <c r="DF84" s="75"/>
-      <c r="DG84" s="75"/>
-      <c r="DH84" s="75"/>
-      <c r="DI84" s="75"/>
-      <c r="DJ84" s="75"/>
-      <c r="DK84" s="75"/>
-      <c r="DL84" s="75"/>
-      <c r="DM84" s="75"/>
-      <c r="DN84" s="75"/>
-      <c r="DO84" s="75"/>
-      <c r="DP84" s="75"/>
-      <c r="DQ84" s="75"/>
-      <c r="DR84" s="75"/>
-      <c r="DS84" s="75"/>
-      <c r="DT84" s="75"/>
-      <c r="DU84" s="75"/>
-      <c r="DV84" s="75"/>
-      <c r="DW84" s="75"/>
-      <c r="DX84" s="75"/>
-      <c r="DY84" s="75"/>
-      <c r="DZ84" s="75"/>
-      <c r="EA84" s="75"/>
-      <c r="EB84" s="75"/>
-      <c r="EC84" s="75"/>
-      <c r="ED84" s="75"/>
-      <c r="EE84" s="75"/>
-      <c r="EF84" s="75"/>
-      <c r="EG84" s="75"/>
-      <c r="EH84" s="75"/>
-      <c r="EI84" s="75"/>
-      <c r="EJ84" s="75"/>
-      <c r="EK84" s="75"/>
-      <c r="EL84" s="75"/>
-      <c r="EM84" s="75"/>
-      <c r="EN84" s="75"/>
-      <c r="EO84" s="75"/>
-      <c r="EP84" s="75"/>
-      <c r="EQ84" s="75"/>
-      <c r="ER84" s="75"/>
-      <c r="ES84" s="75"/>
-      <c r="ET84" s="75"/>
-      <c r="EU84" s="75"/>
-      <c r="EV84" s="75"/>
-      <c r="EW84" s="75"/>
-      <c r="EX84" s="75"/>
-      <c r="EY84" s="75"/>
-      <c r="EZ84" s="75"/>
-      <c r="FA84" s="75"/>
-      <c r="FB84" s="75"/>
-      <c r="FC84" s="75"/>
-      <c r="FD84" s="75"/>
-      <c r="FE84" s="75"/>
-      <c r="FF84" s="75"/>
-      <c r="FG84" s="75"/>
-      <c r="FH84" s="75"/>
-      <c r="FI84" s="75"/>
-      <c r="FJ84" s="75"/>
-      <c r="FK84" s="75"/>
-      <c r="FL84" s="75"/>
-      <c r="FM84" s="75"/>
-      <c r="FN84" s="75"/>
-      <c r="FO84" s="75"/>
-      <c r="FP84" s="75"/>
-      <c r="FQ84" s="75"/>
-      <c r="FR84" s="75"/>
-      <c r="FS84" s="75"/>
-      <c r="FT84" s="75"/>
-      <c r="FU84" s="75"/>
-      <c r="FV84" s="75"/>
-      <c r="FW84" s="75"/>
-      <c r="FX84" s="75"/>
-      <c r="FY84" s="75"/>
-      <c r="FZ84" s="75"/>
-      <c r="GA84" s="75"/>
-      <c r="GB84" s="75"/>
-      <c r="GC84" s="75"/>
-      <c r="GD84" s="75"/>
-      <c r="GE84" s="75"/>
-      <c r="GF84" s="75"/>
-      <c r="GG84" s="75"/>
-      <c r="GH84" s="75"/>
-      <c r="GI84" s="75"/>
-      <c r="GJ84" s="75"/>
-      <c r="GK84" s="75"/>
-      <c r="GL84" s="75"/>
-      <c r="GM84" s="75"/>
-      <c r="GN84" s="75"/>
-      <c r="GO84" s="75"/>
-      <c r="GP84" s="75"/>
-      <c r="GQ84" s="75"/>
-      <c r="GR84" s="75"/>
-      <c r="GS84" s="75"/>
-      <c r="GT84" s="75"/>
-      <c r="GU84" s="75"/>
-      <c r="GV84" s="75"/>
-      <c r="GW84" s="75"/>
-      <c r="GX84" s="75"/>
-      <c r="GY84" s="75"/>
-      <c r="GZ84" s="75"/>
-      <c r="HA84" s="75"/>
-      <c r="HB84" s="75"/>
-      <c r="HC84" s="75"/>
-      <c r="HD84" s="75"/>
-      <c r="HE84" s="75"/>
-      <c r="HF84" s="75"/>
-      <c r="HG84" s="75"/>
-      <c r="HH84" s="75"/>
-      <c r="HI84" s="75"/>
-      <c r="HJ84" s="75"/>
-      <c r="HK84" s="75"/>
-      <c r="HL84" s="75"/>
-      <c r="HM84" s="75"/>
-      <c r="HN84" s="75"/>
-      <c r="HO84" s="75"/>
-      <c r="HP84" s="75"/>
-      <c r="HQ84" s="75"/>
-      <c r="HR84" s="75"/>
-      <c r="HS84" s="75"/>
-      <c r="HT84" s="75"/>
-      <c r="HU84" s="75"/>
-      <c r="HV84" s="75"/>
-      <c r="HW84" s="75"/>
-      <c r="HX84" s="75"/>
-      <c r="HY84" s="75"/>
-      <c r="HZ84" s="75"/>
-      <c r="IA84" s="75"/>
-      <c r="IB84" s="75"/>
-      <c r="IC84" s="75"/>
-      <c r="ID84" s="75"/>
-      <c r="IE84" s="75"/>
-      <c r="IF84" s="75"/>
-      <c r="IG84" s="75"/>
-      <c r="IH84" s="75"/>
-      <c r="II84" s="75"/>
-      <c r="IJ84" s="75"/>
-      <c r="IK84" s="75"/>
-      <c r="IL84" s="75"/>
-      <c r="IM84" s="75"/>
-      <c r="IN84" s="75"/>
-      <c r="IO84" s="75"/>
-      <c r="IP84" s="75"/>
-      <c r="IQ84" s="75"/>
-      <c r="IR84" s="75"/>
-      <c r="IS84" s="75"/>
-      <c r="IT84" s="75"/>
-      <c r="IU84" s="75"/>
-      <c r="IV84" s="75"/>
-      <c r="IW84" s="75"/>
-      <c r="IX84" s="75"/>
-      <c r="IY84" s="75"/>
-      <c r="IZ84" s="75"/>
-      <c r="JA84" s="75"/>
-      <c r="JB84" s="75"/>
-      <c r="JC84" s="75"/>
-      <c r="JD84" s="75"/>
-      <c r="JE84" s="75"/>
-      <c r="JF84" s="75"/>
-      <c r="JG84" s="75"/>
-      <c r="JH84" s="75"/>
-      <c r="JI84" s="75"/>
-      <c r="JJ84" s="75"/>
-      <c r="JK84" s="75"/>
-      <c r="JL84" s="75"/>
-      <c r="JM84" s="75"/>
-      <c r="JN84" s="75"/>
-      <c r="JO84" s="75"/>
-      <c r="JP84" s="75"/>
-      <c r="JQ84" s="75"/>
-      <c r="JR84" s="75"/>
-      <c r="JS84" s="75"/>
-      <c r="JT84" s="75"/>
-      <c r="JU84" s="75"/>
-      <c r="JV84" s="75"/>
-      <c r="JW84" s="75"/>
-      <c r="JX84" s="75"/>
-      <c r="JY84" s="75"/>
-      <c r="JZ84" s="75"/>
-      <c r="KA84" s="75"/>
-      <c r="KB84" s="75"/>
-      <c r="KC84" s="75"/>
-      <c r="KD84" s="75"/>
-      <c r="KE84" s="75"/>
-      <c r="KF84" s="75"/>
-      <c r="KG84" s="75"/>
-      <c r="KH84" s="75"/>
-      <c r="KI84" s="75"/>
-      <c r="KJ84" s="75"/>
-      <c r="KK84" s="75"/>
-      <c r="KL84" s="75"/>
-      <c r="KM84" s="75"/>
-      <c r="KN84" s="75"/>
-      <c r="KO84" s="75"/>
-      <c r="KP84" s="75"/>
-      <c r="KQ84" s="75"/>
-      <c r="KR84" s="75"/>
-      <c r="KS84" s="75"/>
-      <c r="KT84" s="75"/>
-      <c r="KU84" s="75"/>
-      <c r="KV84" s="75"/>
-      <c r="KW84" s="75"/>
-      <c r="KX84" s="75"/>
-      <c r="KY84" s="75"/>
-      <c r="KZ84" s="75"/>
-      <c r="LA84" s="75"/>
-      <c r="LB84" s="75"/>
-      <c r="LC84" s="75"/>
-      <c r="LD84" s="75"/>
-      <c r="LE84" s="75"/>
-      <c r="LF84" s="75"/>
-      <c r="LG84" s="75"/>
-      <c r="LH84" s="75"/>
-      <c r="LI84" s="75"/>
-      <c r="LJ84" s="75"/>
-      <c r="LK84" s="75"/>
-      <c r="LL84" s="75"/>
-      <c r="LM84" s="75"/>
-      <c r="LN84" s="75"/>
-      <c r="LO84" s="75"/>
-      <c r="LP84" s="75"/>
-      <c r="LQ84" s="75"/>
-      <c r="LR84" s="75"/>
-      <c r="LS84" s="75"/>
-      <c r="LT84" s="75"/>
-      <c r="LU84" s="75"/>
-      <c r="LV84" s="75"/>
-      <c r="LW84" s="75"/>
-      <c r="LX84" s="75"/>
-      <c r="LY84" s="75"/>
-      <c r="LZ84" s="75"/>
-      <c r="MA84" s="75"/>
-      <c r="MB84" s="75"/>
-      <c r="MC84" s="75"/>
-      <c r="MD84" s="75"/>
-      <c r="ME84" s="75"/>
-      <c r="MF84" s="75"/>
-      <c r="MG84" s="75"/>
-      <c r="MH84" s="75"/>
-      <c r="MI84" s="75"/>
-      <c r="MJ84" s="75"/>
-      <c r="MK84" s="75"/>
-      <c r="ML84" s="75"/>
-      <c r="MM84" s="75"/>
-      <c r="MN84" s="75"/>
-      <c r="MO84" s="75"/>
-      <c r="MP84" s="75"/>
-      <c r="MQ84" s="75"/>
-      <c r="MR84" s="75"/>
-      <c r="MS84" s="75"/>
-      <c r="MT84" s="75"/>
-      <c r="MU84" s="75"/>
-      <c r="MV84" s="75"/>
-      <c r="MW84" s="75"/>
-      <c r="MX84" s="75"/>
-      <c r="MY84" s="75"/>
-      <c r="MZ84" s="75"/>
-      <c r="NA84" s="75"/>
-      <c r="NB84" s="75"/>
-      <c r="NC84" s="75"/>
-      <c r="ND84" s="75"/>
-      <c r="NE84" s="75"/>
-      <c r="NF84" s="75"/>
-      <c r="NG84" s="75"/>
-      <c r="NH84" s="75"/>
-      <c r="NI84" s="75"/>
-      <c r="NJ84" s="75"/>
-      <c r="NK84" s="75"/>
-      <c r="NL84" s="75"/>
-      <c r="NM84" s="75"/>
-      <c r="NN84" s="75"/>
-      <c r="NO84" s="75"/>
-      <c r="NP84" s="75"/>
-      <c r="NQ84" s="75"/>
-      <c r="NR84" s="75"/>
-      <c r="NS84" s="75"/>
-      <c r="NT84" s="75"/>
-      <c r="NU84" s="75"/>
-      <c r="NV84" s="75"/>
-      <c r="NW84" s="75"/>
-      <c r="NX84" s="75"/>
-      <c r="NY84" s="75"/>
-      <c r="NZ84" s="75"/>
-      <c r="OA84" s="75"/>
-      <c r="OB84" s="75"/>
-      <c r="OC84" s="75"/>
-      <c r="OD84" s="75"/>
-      <c r="OE84" s="75"/>
-      <c r="OF84" s="75"/>
-      <c r="OG84" s="75"/>
-      <c r="OH84" s="75"/>
-      <c r="OI84" s="75"/>
-      <c r="OJ84" s="75"/>
-      <c r="OK84" s="75"/>
-      <c r="OL84" s="75"/>
-      <c r="OM84" s="75"/>
-      <c r="ON84" s="75"/>
-      <c r="OO84" s="75"/>
-      <c r="OP84" s="75"/>
-      <c r="OQ84" s="75"/>
-      <c r="OR84" s="75"/>
-      <c r="OS84" s="75"/>
-      <c r="OT84" s="75"/>
-      <c r="OU84" s="75"/>
-      <c r="OV84" s="75"/>
-      <c r="OW84" s="75"/>
-      <c r="OX84" s="75"/>
-      <c r="OY84" s="75"/>
-      <c r="OZ84" s="75"/>
-      <c r="PA84" s="75"/>
-      <c r="PB84" s="75"/>
-      <c r="PC84" s="75"/>
-      <c r="PD84" s="75"/>
-      <c r="PE84" s="75"/>
-      <c r="PF84" s="75"/>
-      <c r="PG84" s="75"/>
-      <c r="PH84" s="75"/>
-      <c r="PI84" s="75"/>
-      <c r="PJ84" s="75"/>
-      <c r="PK84" s="75"/>
-      <c r="PL84" s="75"/>
-      <c r="PM84" s="75"/>
-      <c r="PN84" s="75"/>
-      <c r="PO84" s="75"/>
-      <c r="PP84" s="75"/>
-      <c r="PQ84" s="75"/>
-      <c r="PR84" s="75"/>
-      <c r="PS84" s="75"/>
-      <c r="PT84" s="75"/>
-      <c r="PU84" s="75"/>
-      <c r="PV84" s="75"/>
-      <c r="PW84" s="75"/>
-      <c r="PX84" s="75"/>
-      <c r="PY84" s="75"/>
-      <c r="PZ84" s="75"/>
-      <c r="QA84" s="75"/>
-      <c r="QB84" s="75"/>
-      <c r="QC84" s="75"/>
-      <c r="QD84" s="75"/>
-      <c r="QE84" s="75"/>
-      <c r="QF84" s="75"/>
-      <c r="QG84" s="75"/>
-      <c r="QH84" s="75"/>
-      <c r="QI84" s="75"/>
-      <c r="QJ84" s="75"/>
-      <c r="QK84" s="75"/>
-      <c r="QL84" s="75"/>
-      <c r="QM84" s="75"/>
-      <c r="QN84" s="75"/>
-      <c r="QO84" s="75"/>
-      <c r="QP84" s="75"/>
-      <c r="QQ84" s="75"/>
-      <c r="QR84" s="75"/>
-      <c r="QS84" s="75"/>
-      <c r="QT84" s="75"/>
-      <c r="QU84" s="75"/>
-      <c r="QV84" s="75"/>
-      <c r="QW84" s="75"/>
-      <c r="QX84" s="75"/>
-      <c r="QY84" s="75"/>
-      <c r="QZ84" s="75"/>
-      <c r="RA84" s="75"/>
-      <c r="RB84" s="75"/>
-      <c r="RC84" s="75"/>
-      <c r="RD84" s="75"/>
-      <c r="RE84" s="75"/>
-      <c r="RF84" s="75"/>
-      <c r="RG84" s="75"/>
-      <c r="RH84" s="75"/>
-      <c r="RI84" s="75"/>
-      <c r="RJ84" s="75"/>
-      <c r="RK84" s="75"/>
-      <c r="RL84" s="75"/>
-      <c r="RM84" s="75"/>
-      <c r="RN84" s="75"/>
-      <c r="RO84" s="75"/>
-      <c r="RP84" s="75"/>
-      <c r="RQ84" s="75"/>
-      <c r="RR84" s="75"/>
-      <c r="RS84" s="75"/>
-      <c r="RT84" s="75"/>
-      <c r="RU84" s="75"/>
-      <c r="RV84" s="75"/>
-      <c r="RW84" s="75"/>
-      <c r="RX84" s="75"/>
-      <c r="RY84" s="75"/>
-      <c r="RZ84" s="75"/>
-      <c r="SA84" s="75"/>
-      <c r="SB84" s="75"/>
-      <c r="SC84" s="75"/>
-      <c r="SD84" s="75"/>
-      <c r="SE84" s="75"/>
-      <c r="SF84" s="75"/>
-      <c r="SG84" s="75"/>
-      <c r="SH84" s="75"/>
-      <c r="SI84" s="75"/>
-      <c r="SJ84" s="75"/>
-      <c r="SK84" s="75"/>
-      <c r="SL84" s="75"/>
-      <c r="SM84" s="75"/>
-      <c r="SN84" s="75"/>
-      <c r="SO84" s="75"/>
-      <c r="SP84" s="75"/>
-      <c r="SQ84" s="75"/>
-      <c r="SR84" s="75"/>
-      <c r="SS84" s="75"/>
-      <c r="ST84" s="75"/>
-      <c r="SU84" s="75"/>
-      <c r="SV84" s="75"/>
-      <c r="SW84" s="75"/>
-      <c r="SX84" s="75"/>
-      <c r="SY84" s="75"/>
-      <c r="SZ84" s="75"/>
-      <c r="TA84" s="75"/>
-      <c r="TB84" s="75"/>
-      <c r="TC84" s="75"/>
-      <c r="TD84" s="75"/>
-      <c r="TE84" s="75"/>
-      <c r="TF84" s="75"/>
-      <c r="TG84" s="75"/>
-      <c r="TH84" s="75"/>
-      <c r="TI84" s="75"/>
-      <c r="TJ84" s="75"/>
-      <c r="TK84" s="75"/>
-      <c r="TL84" s="75"/>
-      <c r="TM84" s="75"/>
-      <c r="TN84" s="75"/>
-      <c r="TO84" s="75"/>
-      <c r="TP84" s="75"/>
-      <c r="TQ84" s="75"/>
-      <c r="TR84" s="75"/>
-      <c r="TS84" s="75"/>
-      <c r="TT84" s="75"/>
-      <c r="TU84" s="75"/>
-      <c r="TV84" s="75"/>
-      <c r="TW84" s="75"/>
-      <c r="TX84" s="75"/>
-      <c r="TY84" s="75"/>
-      <c r="TZ84" s="75"/>
-      <c r="UA84" s="75"/>
-      <c r="UB84" s="75"/>
-      <c r="UC84" s="75"/>
-      <c r="UD84" s="75"/>
-      <c r="UE84" s="75"/>
-      <c r="UF84" s="75"/>
-      <c r="UG84" s="75"/>
-      <c r="UH84" s="75"/>
-      <c r="UI84" s="75"/>
-      <c r="UJ84" s="75"/>
-      <c r="UK84" s="75"/>
-      <c r="UL84" s="75"/>
-      <c r="UM84" s="75"/>
-      <c r="UN84" s="75"/>
-      <c r="UO84" s="75"/>
-      <c r="UP84" s="75"/>
-      <c r="UQ84" s="75"/>
-      <c r="UR84" s="75"/>
-      <c r="US84" s="75"/>
-      <c r="UT84" s="75"/>
-      <c r="UU84" s="75"/>
-      <c r="UV84" s="75"/>
-      <c r="UW84" s="75"/>
-      <c r="UX84" s="75"/>
-      <c r="UY84" s="75"/>
-      <c r="UZ84" s="75"/>
-      <c r="VA84" s="75"/>
-      <c r="VB84" s="75"/>
-      <c r="VC84" s="75"/>
-      <c r="VD84" s="75"/>
-      <c r="VE84" s="75"/>
-      <c r="VF84" s="75"/>
-      <c r="VG84" s="75"/>
-      <c r="VH84" s="75"/>
-      <c r="VI84" s="75"/>
-      <c r="VJ84" s="75"/>
-      <c r="VK84" s="75"/>
-      <c r="VL84" s="75"/>
-      <c r="VM84" s="75"/>
-      <c r="VN84" s="75"/>
-      <c r="VO84" s="75"/>
-      <c r="VP84" s="75"/>
-      <c r="VQ84" s="75"/>
-      <c r="VR84" s="75"/>
-      <c r="VS84" s="75"/>
-      <c r="VT84" s="75"/>
-      <c r="VU84" s="75"/>
-      <c r="VV84" s="75"/>
-      <c r="VW84" s="75"/>
-      <c r="VX84" s="75"/>
-      <c r="VY84" s="75"/>
-      <c r="VZ84" s="75"/>
-      <c r="WA84" s="75"/>
-      <c r="WB84" s="75"/>
-      <c r="WC84" s="75"/>
-      <c r="WD84" s="75"/>
-      <c r="WE84" s="75"/>
-      <c r="WF84" s="75"/>
-      <c r="WG84" s="75"/>
-      <c r="WH84" s="75"/>
-      <c r="WI84" s="75"/>
-      <c r="WJ84" s="75"/>
-      <c r="WK84" s="75"/>
-      <c r="WL84" s="75"/>
-      <c r="WM84" s="75"/>
-      <c r="WN84" s="75"/>
-      <c r="WO84" s="75"/>
-      <c r="WP84" s="75"/>
-      <c r="WQ84" s="75"/>
-      <c r="WR84" s="75"/>
-      <c r="WS84" s="75"/>
-      <c r="WT84" s="75"/>
-      <c r="WU84" s="75"/>
-      <c r="WV84" s="75"/>
-      <c r="WW84" s="75"/>
-      <c r="WX84" s="75"/>
-      <c r="WY84" s="75"/>
-      <c r="WZ84" s="75"/>
-      <c r="XA84" s="75"/>
-      <c r="XB84" s="75"/>
-      <c r="XC84" s="75"/>
-      <c r="XD84" s="75"/>
-      <c r="XE84" s="75"/>
-      <c r="XF84" s="75"/>
-      <c r="XG84" s="75"/>
-      <c r="XH84" s="75"/>
-      <c r="XI84" s="75"/>
-      <c r="XJ84" s="75"/>
-      <c r="XK84" s="75"/>
-      <c r="XL84" s="75"/>
-      <c r="XM84" s="75"/>
-      <c r="XN84" s="75"/>
-      <c r="XO84" s="75"/>
-      <c r="XP84" s="75"/>
-      <c r="XQ84" s="75"/>
-      <c r="XR84" s="75"/>
-      <c r="XS84" s="75"/>
-      <c r="XT84" s="75"/>
-      <c r="XU84" s="75"/>
-      <c r="XV84" s="75"/>
-      <c r="XW84" s="75"/>
-      <c r="XX84" s="75"/>
-      <c r="XY84" s="75"/>
-      <c r="XZ84" s="75"/>
-      <c r="YA84" s="75"/>
-      <c r="YB84" s="75"/>
-      <c r="YC84" s="75"/>
-      <c r="YD84" s="75"/>
-      <c r="YE84" s="75"/>
-      <c r="YF84" s="75"/>
-      <c r="YG84" s="75"/>
-      <c r="YH84" s="75"/>
-      <c r="YI84" s="75"/>
-      <c r="YJ84" s="75"/>
-      <c r="YK84" s="75"/>
-      <c r="YL84" s="75"/>
-      <c r="YM84" s="75"/>
-      <c r="YN84" s="75"/>
-      <c r="YO84" s="75"/>
-      <c r="YP84" s="75"/>
-      <c r="YQ84" s="75"/>
-      <c r="YR84" s="75"/>
-      <c r="YS84" s="75"/>
-      <c r="YT84" s="75"/>
-      <c r="YU84" s="75"/>
-      <c r="YV84" s="75"/>
-      <c r="YW84" s="75"/>
-      <c r="YX84" s="75"/>
-      <c r="YY84" s="75"/>
-      <c r="YZ84" s="75"/>
-      <c r="ZA84" s="75"/>
-      <c r="ZB84" s="75"/>
-      <c r="ZC84" s="75"/>
-      <c r="ZD84" s="75"/>
-      <c r="ZE84" s="75"/>
-      <c r="ZF84" s="75"/>
-      <c r="ZG84" s="75"/>
-      <c r="ZH84" s="75"/>
-      <c r="ZI84" s="75"/>
-      <c r="ZJ84" s="75"/>
-      <c r="ZK84" s="75"/>
-      <c r="ZL84" s="75"/>
-      <c r="ZM84" s="75"/>
-      <c r="ZN84" s="75"/>
-      <c r="ZO84" s="75"/>
-      <c r="ZP84" s="75"/>
-      <c r="ZQ84" s="75"/>
-      <c r="ZR84" s="75"/>
-      <c r="ZS84" s="75"/>
-      <c r="ZT84" s="75"/>
-      <c r="ZU84" s="75"/>
-      <c r="ZV84" s="75"/>
-      <c r="ZW84" s="75"/>
-      <c r="ZX84" s="75"/>
-      <c r="ZY84" s="75"/>
-      <c r="ZZ84" s="75"/>
-      <c r="AAA84" s="75"/>
-      <c r="AAB84" s="75"/>
-      <c r="AAC84" s="75"/>
-      <c r="AAD84" s="75"/>
-      <c r="AAE84" s="75"/>
-      <c r="AAF84" s="75"/>
-      <c r="AAG84" s="75"/>
-      <c r="AAH84" s="75"/>
-      <c r="AAI84" s="75"/>
-      <c r="AAJ84" s="75"/>
-      <c r="AAK84" s="75"/>
-      <c r="AAL84" s="75"/>
-      <c r="AAM84" s="75"/>
-      <c r="AAN84" s="75"/>
-      <c r="AAO84" s="75"/>
-      <c r="AAP84" s="75"/>
-      <c r="AAQ84" s="75"/>
-      <c r="AAR84" s="75"/>
-      <c r="AAS84" s="75"/>
-      <c r="AAT84" s="75"/>
-      <c r="AAU84" s="75"/>
-      <c r="AAV84" s="75"/>
-      <c r="AAW84" s="75"/>
-      <c r="AAX84" s="75"/>
-      <c r="AAY84" s="75"/>
-      <c r="AAZ84" s="75"/>
-      <c r="ABA84" s="75"/>
-      <c r="ABB84" s="75"/>
-      <c r="ABC84" s="75"/>
-      <c r="ABD84" s="75"/>
-      <c r="ABE84" s="75"/>
-      <c r="ABF84" s="75"/>
-      <c r="ABG84" s="75"/>
-      <c r="ABH84" s="75"/>
-      <c r="ABI84" s="75"/>
-      <c r="ABJ84" s="75"/>
-      <c r="ABK84" s="75"/>
-      <c r="ABL84" s="75"/>
-      <c r="ABM84" s="75"/>
-      <c r="ABN84" s="75"/>
-      <c r="ABO84" s="75"/>
-      <c r="ABP84" s="75"/>
-      <c r="ABQ84" s="75"/>
-      <c r="ABR84" s="75"/>
-      <c r="ABS84" s="75"/>
-      <c r="ABT84" s="75"/>
-      <c r="ABU84" s="75"/>
-      <c r="ABV84" s="75"/>
-      <c r="ABW84" s="75"/>
-      <c r="ABX84" s="75"/>
-      <c r="ABY84" s="75"/>
-      <c r="ABZ84" s="75"/>
-      <c r="ACA84" s="75"/>
-      <c r="ACB84" s="75"/>
-      <c r="ACC84" s="75"/>
-      <c r="ACD84" s="75"/>
-      <c r="ACE84" s="75"/>
-      <c r="ACF84" s="75"/>
-      <c r="ACG84" s="75"/>
-      <c r="ACH84" s="75"/>
-      <c r="ACI84" s="75"/>
-      <c r="ACJ84" s="75"/>
-      <c r="ACK84" s="75"/>
-      <c r="ACL84" s="75"/>
-      <c r="ACM84" s="75"/>
-      <c r="ACN84" s="75"/>
-      <c r="ACO84" s="75"/>
-      <c r="ACP84" s="75"/>
-      <c r="ACQ84" s="75"/>
-      <c r="ACR84" s="75"/>
-      <c r="ACS84" s="75"/>
-      <c r="ACT84" s="75"/>
-      <c r="ACU84" s="75"/>
-      <c r="ACV84" s="75"/>
-      <c r="ACW84" s="75"/>
-      <c r="ACX84" s="75"/>
-      <c r="ACY84" s="75"/>
-      <c r="ACZ84" s="75"/>
-      <c r="ADA84" s="75"/>
-      <c r="ADB84" s="75"/>
-      <c r="ADC84" s="75"/>
-      <c r="ADD84" s="75"/>
-      <c r="ADE84" s="75"/>
-      <c r="ADF84" s="75"/>
-      <c r="ADG84" s="75"/>
-      <c r="ADH84" s="75"/>
-      <c r="ADI84" s="75"/>
-      <c r="ADJ84" s="75"/>
-      <c r="ADK84" s="75"/>
-      <c r="ADL84" s="75"/>
-      <c r="ADM84" s="75"/>
-      <c r="ADN84" s="75"/>
-      <c r="ADO84" s="75"/>
-      <c r="ADP84" s="75"/>
-      <c r="ADQ84" s="75"/>
-      <c r="ADR84" s="75"/>
-      <c r="ADS84" s="75"/>
-      <c r="ADT84" s="75"/>
-      <c r="ADU84" s="75"/>
-      <c r="ADV84" s="75"/>
-      <c r="ADW84" s="75"/>
-      <c r="ADX84" s="75"/>
-      <c r="ADY84" s="75"/>
-      <c r="ADZ84" s="75"/>
-      <c r="AEA84" s="75"/>
-      <c r="AEB84" s="75"/>
-      <c r="AEC84" s="75"/>
-      <c r="AED84" s="75"/>
-      <c r="AEE84" s="75"/>
-      <c r="AEF84" s="75"/>
-      <c r="AEG84" s="75"/>
-      <c r="AEH84" s="75"/>
-      <c r="AEI84" s="75"/>
-      <c r="AEJ84" s="75"/>
-      <c r="AEK84" s="75"/>
-      <c r="AEL84" s="75"/>
-      <c r="AEM84" s="75"/>
-      <c r="AEN84" s="75"/>
-      <c r="AEO84" s="75"/>
-      <c r="AEP84" s="75"/>
-      <c r="AEQ84" s="75"/>
-      <c r="AER84" s="75"/>
-      <c r="AES84" s="75"/>
-      <c r="AET84" s="75"/>
-      <c r="AEU84" s="75"/>
-      <c r="AEV84" s="75"/>
-      <c r="AEW84" s="75"/>
-      <c r="AEX84" s="75"/>
-      <c r="AEY84" s="75"/>
-      <c r="AEZ84" s="75"/>
-      <c r="AFA84" s="75"/>
-      <c r="AFB84" s="75"/>
-      <c r="AFC84" s="75"/>
-      <c r="AFD84" s="75"/>
-      <c r="AFE84" s="75"/>
-      <c r="AFF84" s="75"/>
-      <c r="AFG84" s="75"/>
-      <c r="AFH84" s="75"/>
-      <c r="AFI84" s="75"/>
-      <c r="AFJ84" s="75"/>
-      <c r="AFK84" s="75"/>
-      <c r="AFL84" s="75"/>
-      <c r="AFM84" s="75"/>
-      <c r="AFN84" s="75"/>
-      <c r="AFO84" s="75"/>
-      <c r="AFP84" s="75"/>
-      <c r="AFQ84" s="75"/>
-      <c r="AFR84" s="75"/>
-      <c r="AFS84" s="75"/>
-      <c r="AFT84" s="75"/>
-      <c r="AFU84" s="75"/>
-      <c r="AFV84" s="75"/>
-      <c r="AFW84" s="75"/>
-      <c r="AFX84" s="75"/>
-      <c r="AFY84" s="75"/>
-      <c r="AFZ84" s="75"/>
-      <c r="AGA84" s="75"/>
-      <c r="AGB84" s="75"/>
-      <c r="AGC84" s="75"/>
-      <c r="AGD84" s="75"/>
-      <c r="AGE84" s="75"/>
-      <c r="AGF84" s="75"/>
-      <c r="AGG84" s="75"/>
-      <c r="AGH84" s="75"/>
-      <c r="AGI84" s="75"/>
-      <c r="AGJ84" s="75"/>
-      <c r="AGK84" s="75"/>
-      <c r="AGL84" s="75"/>
-      <c r="AGM84" s="75"/>
-      <c r="AGN84" s="75"/>
-      <c r="AGO84" s="75"/>
-      <c r="AGP84" s="75"/>
-      <c r="AGQ84" s="75"/>
-      <c r="AGR84" s="75"/>
-      <c r="AGS84" s="75"/>
-      <c r="AGT84" s="75"/>
-      <c r="AGU84" s="75"/>
-      <c r="AGV84" s="75"/>
-      <c r="AGW84" s="75"/>
-      <c r="AGX84" s="75"/>
-      <c r="AGY84" s="75"/>
-      <c r="AGZ84" s="75"/>
-      <c r="AHA84" s="75"/>
-      <c r="AHB84" s="75"/>
-      <c r="AHC84" s="75"/>
-      <c r="AHD84" s="75"/>
-      <c r="AHE84" s="75"/>
-      <c r="AHF84" s="75"/>
-      <c r="AHG84" s="75"/>
-      <c r="AHH84" s="75"/>
-      <c r="AHI84" s="75"/>
-      <c r="AHJ84" s="75"/>
-      <c r="AHK84" s="75"/>
-      <c r="AHL84" s="75"/>
-      <c r="AHM84" s="75"/>
-      <c r="AHN84" s="75"/>
-      <c r="AHO84" s="75"/>
-      <c r="AHP84" s="75"/>
-      <c r="AHQ84" s="75"/>
-      <c r="AHR84" s="75"/>
-      <c r="AHS84" s="75"/>
-      <c r="AHT84" s="75"/>
-      <c r="AHU84" s="75"/>
-      <c r="AHV84" s="75"/>
-      <c r="AHW84" s="75"/>
-      <c r="AHX84" s="75"/>
-      <c r="AHY84" s="75"/>
-      <c r="AHZ84" s="75"/>
-      <c r="AIA84" s="75"/>
-      <c r="AIB84" s="75"/>
-      <c r="AIC84" s="75"/>
-      <c r="AID84" s="75"/>
-      <c r="AIE84" s="75"/>
-      <c r="AIF84" s="75"/>
-      <c r="AIG84" s="75"/>
-      <c r="AIH84" s="75"/>
-      <c r="AII84" s="75"/>
-      <c r="AIJ84" s="75"/>
-      <c r="AIK84" s="75"/>
-      <c r="AIL84" s="75"/>
-      <c r="AIM84" s="75"/>
-      <c r="AIN84" s="75"/>
-      <c r="AIO84" s="75"/>
-      <c r="AIP84" s="75"/>
-      <c r="AIQ84" s="75"/>
-      <c r="AIR84" s="75"/>
-      <c r="AIS84" s="75"/>
-      <c r="AIT84" s="75"/>
-      <c r="AIU84" s="75"/>
-      <c r="AIV84" s="75"/>
-      <c r="AIW84" s="75"/>
-      <c r="AIX84" s="75"/>
-      <c r="AIY84" s="75"/>
-      <c r="AIZ84" s="75"/>
-      <c r="AJA84" s="75"/>
-      <c r="AJB84" s="75"/>
-      <c r="AJC84" s="75"/>
-      <c r="AJD84" s="75"/>
-      <c r="AJE84" s="75"/>
-      <c r="AJF84" s="75"/>
-      <c r="AJG84" s="75"/>
-      <c r="AJH84" s="75"/>
-      <c r="AJI84" s="75"/>
-      <c r="AJJ84" s="75"/>
-      <c r="AJK84" s="75"/>
-      <c r="AJL84" s="75"/>
-      <c r="AJM84" s="75"/>
-      <c r="AJN84" s="75"/>
-      <c r="AJO84" s="75"/>
-      <c r="AJP84" s="75"/>
-      <c r="AJQ84" s="75"/>
-      <c r="AJR84" s="75"/>
-      <c r="AJS84" s="75"/>
-      <c r="AJT84" s="75"/>
-      <c r="AJU84" s="75"/>
-      <c r="AJV84" s="75"/>
-      <c r="AJW84" s="75"/>
-      <c r="AJX84" s="75"/>
-      <c r="AJY84" s="75"/>
-      <c r="AJZ84" s="75"/>
-      <c r="AKA84" s="75"/>
-      <c r="AKB84" s="75"/>
-      <c r="AKC84" s="75"/>
-      <c r="AKD84" s="75"/>
-      <c r="AKE84" s="75"/>
-      <c r="AKF84" s="75"/>
-      <c r="AKG84" s="75"/>
-      <c r="AKH84" s="75"/>
-      <c r="AKI84" s="75"/>
-      <c r="AKJ84" s="75"/>
-      <c r="AKK84" s="75"/>
-      <c r="AKL84" s="75"/>
-      <c r="AKM84" s="75"/>
-      <c r="AKN84" s="75"/>
-      <c r="AKO84" s="75"/>
-      <c r="AKP84" s="75"/>
-      <c r="AKQ84" s="75"/>
-      <c r="AKR84" s="75"/>
-      <c r="AKS84" s="75"/>
-      <c r="AKT84" s="75"/>
-      <c r="AKU84" s="75"/>
-      <c r="AKV84" s="75"/>
-      <c r="AKW84" s="75"/>
-      <c r="AKX84" s="75"/>
-      <c r="AKY84" s="75"/>
-      <c r="AKZ84" s="75"/>
-      <c r="ALA84" s="75"/>
-      <c r="ALB84" s="75"/>
-      <c r="ALC84" s="75"/>
-      <c r="ALD84" s="75"/>
-      <c r="ALE84" s="75"/>
-      <c r="ALF84" s="75"/>
-      <c r="ALG84" s="75"/>
-      <c r="ALH84" s="75"/>
-      <c r="ALI84" s="75"/>
-      <c r="ALJ84" s="75"/>
-      <c r="ALK84" s="75"/>
-      <c r="ALL84" s="75"/>
-      <c r="ALM84" s="75"/>
-      <c r="ALN84" s="75"/>
-      <c r="ALO84" s="75"/>
-      <c r="ALP84" s="75"/>
-      <c r="ALQ84" s="75"/>
-      <c r="ALR84" s="75"/>
-      <c r="ALS84" s="75"/>
-      <c r="ALT84" s="75"/>
-      <c r="ALU84" s="75"/>
-      <c r="ALV84" s="75"/>
-      <c r="ALW84" s="75"/>
-      <c r="ALX84" s="75"/>
-      <c r="ALY84" s="75"/>
-      <c r="ALZ84" s="75"/>
-      <c r="AMA84" s="75"/>
-      <c r="AMB84" s="75"/>
-      <c r="AMC84" s="75"/>
-      <c r="AMD84" s="75"/>
-      <c r="AME84" s="75"/>
-      <c r="AMF84" s="75"/>
-      <c r="AMG84" s="75"/>
-      <c r="AMH84" s="75"/>
+      <c r="H84" s="72"/>
+      <c r="I84" s="77"/>
+      <c r="J84" s="77"/>
+      <c r="K84" s="77"/>
+      <c r="L84" s="77"/>
+      <c r="M84" s="77"/>
+      <c r="N84" s="77"/>
+      <c r="O84" s="77"/>
+      <c r="P84" s="77"/>
+      <c r="Q84" s="77"/>
+      <c r="R84" s="77"/>
+      <c r="S84" s="77"/>
+      <c r="T84" s="77"/>
+      <c r="U84" s="77"/>
+      <c r="V84" s="77"/>
+      <c r="W84" s="77"/>
+      <c r="X84" s="77"/>
+      <c r="Y84" s="77"/>
+      <c r="Z84" s="77"/>
+      <c r="AA84" s="77"/>
+      <c r="AB84" s="77"/>
+      <c r="AC84" s="77"/>
+      <c r="AD84" s="77"/>
+      <c r="AE84" s="77"/>
+      <c r="AF84" s="77"/>
+      <c r="AG84" s="77"/>
+      <c r="AH84" s="77"/>
+      <c r="AI84" s="77"/>
+      <c r="AJ84" s="77"/>
+      <c r="AK84" s="77"/>
+      <c r="AL84" s="77"/>
+      <c r="AM84" s="77"/>
+      <c r="AN84" s="77"/>
+      <c r="AO84" s="77"/>
+      <c r="AP84" s="77"/>
+      <c r="AQ84" s="77"/>
+      <c r="AR84" s="77"/>
+      <c r="AS84" s="77"/>
+      <c r="AT84" s="77"/>
+      <c r="AU84" s="77"/>
+      <c r="AV84" s="77"/>
+      <c r="AW84" s="77"/>
+      <c r="AX84" s="77"/>
+      <c r="AY84" s="77"/>
+      <c r="AZ84" s="77"/>
+      <c r="BA84" s="77"/>
+      <c r="BB84" s="77"/>
+      <c r="BC84" s="77"/>
+      <c r="BD84" s="77"/>
+      <c r="BE84" s="77"/>
+      <c r="BF84" s="77"/>
+      <c r="BG84" s="77"/>
+      <c r="BH84" s="77"/>
+      <c r="BI84" s="77"/>
+      <c r="BJ84" s="77"/>
+      <c r="BK84" s="77"/>
+      <c r="BL84" s="77"/>
+      <c r="BM84" s="77"/>
+      <c r="BN84" s="77"/>
+      <c r="BO84" s="77"/>
+      <c r="BP84" s="77"/>
+      <c r="BQ84" s="77"/>
+      <c r="BR84" s="77"/>
+      <c r="BS84" s="77"/>
+      <c r="BT84" s="77"/>
+      <c r="BU84" s="77"/>
+      <c r="BV84" s="77"/>
+      <c r="BW84" s="77"/>
+      <c r="BX84" s="77"/>
+      <c r="BY84" s="77"/>
+      <c r="BZ84" s="77"/>
+      <c r="CA84" s="77"/>
+      <c r="CB84" s="77"/>
+      <c r="CC84" s="77"/>
+      <c r="CD84" s="77"/>
+      <c r="CE84" s="77"/>
+      <c r="CF84" s="77"/>
+      <c r="CG84" s="77"/>
+      <c r="CH84" s="77"/>
+      <c r="CI84" s="77"/>
+      <c r="CJ84" s="77"/>
+      <c r="CK84" s="77"/>
+      <c r="CL84" s="77"/>
+      <c r="CM84" s="77"/>
+      <c r="CN84" s="77"/>
+      <c r="CO84" s="77"/>
+      <c r="CP84" s="77"/>
+      <c r="CQ84" s="77"/>
+      <c r="CR84" s="77"/>
+      <c r="CS84" s="77"/>
+      <c r="CT84" s="77"/>
+      <c r="CU84" s="77"/>
+      <c r="CV84" s="77"/>
+      <c r="CW84" s="77"/>
+      <c r="CX84" s="77"/>
+      <c r="CY84" s="77"/>
+      <c r="CZ84" s="77"/>
+      <c r="DA84" s="77"/>
+      <c r="DB84" s="77"/>
+      <c r="DC84" s="77"/>
+      <c r="DD84" s="77"/>
+      <c r="DE84" s="77"/>
+      <c r="DF84" s="77"/>
+      <c r="DG84" s="77"/>
+      <c r="DH84" s="77"/>
+      <c r="DI84" s="77"/>
+      <c r="DJ84" s="77"/>
+      <c r="DK84" s="77"/>
+      <c r="DL84" s="77"/>
+      <c r="DM84" s="77"/>
+      <c r="DN84" s="77"/>
+      <c r="DO84" s="77"/>
+      <c r="DP84" s="77"/>
+      <c r="DQ84" s="77"/>
+      <c r="DR84" s="77"/>
+      <c r="DS84" s="77"/>
+      <c r="DT84" s="77"/>
+      <c r="DU84" s="77"/>
+      <c r="DV84" s="77"/>
+      <c r="DW84" s="77"/>
+      <c r="DX84" s="77"/>
+      <c r="DY84" s="77"/>
+      <c r="DZ84" s="77"/>
+      <c r="EA84" s="77"/>
+      <c r="EB84" s="77"/>
+      <c r="EC84" s="77"/>
+      <c r="ED84" s="77"/>
+      <c r="EE84" s="77"/>
+      <c r="EF84" s="77"/>
+      <c r="EG84" s="77"/>
+      <c r="EH84" s="77"/>
+      <c r="EI84" s="77"/>
+      <c r="EJ84" s="77"/>
+      <c r="EK84" s="77"/>
+      <c r="EL84" s="77"/>
+      <c r="EM84" s="77"/>
+      <c r="EN84" s="77"/>
+      <c r="EO84" s="77"/>
+      <c r="EP84" s="77"/>
+      <c r="EQ84" s="77"/>
+      <c r="ER84" s="77"/>
+      <c r="ES84" s="77"/>
+      <c r="ET84" s="77"/>
+      <c r="EU84" s="77"/>
+      <c r="EV84" s="77"/>
+      <c r="EW84" s="77"/>
+      <c r="EX84" s="77"/>
+      <c r="EY84" s="77"/>
+      <c r="EZ84" s="77"/>
+      <c r="FA84" s="77"/>
+      <c r="FB84" s="77"/>
+      <c r="FC84" s="77"/>
+      <c r="FD84" s="77"/>
+      <c r="FE84" s="77"/>
+      <c r="FF84" s="77"/>
+      <c r="FG84" s="77"/>
+      <c r="FH84" s="77"/>
+      <c r="FI84" s="77"/>
+      <c r="FJ84" s="77"/>
+      <c r="FK84" s="77"/>
+      <c r="FL84" s="77"/>
+      <c r="FM84" s="77"/>
+      <c r="FN84" s="77"/>
+      <c r="FO84" s="77"/>
+      <c r="FP84" s="77"/>
+      <c r="FQ84" s="77"/>
+      <c r="FR84" s="77"/>
+      <c r="FS84" s="77"/>
+      <c r="FT84" s="77"/>
+      <c r="FU84" s="77"/>
+      <c r="FV84" s="77"/>
+      <c r="FW84" s="77"/>
+      <c r="FX84" s="77"/>
+      <c r="FY84" s="77"/>
+      <c r="FZ84" s="77"/>
+      <c r="GA84" s="77"/>
+      <c r="GB84" s="77"/>
+      <c r="GC84" s="77"/>
+      <c r="GD84" s="77"/>
+      <c r="GE84" s="77"/>
+      <c r="GF84" s="77"/>
+      <c r="GG84" s="77"/>
+      <c r="GH84" s="77"/>
+      <c r="GI84" s="77"/>
+      <c r="GJ84" s="77"/>
+      <c r="GK84" s="77"/>
+      <c r="GL84" s="77"/>
+      <c r="GM84" s="77"/>
+      <c r="GN84" s="77"/>
+      <c r="GO84" s="77"/>
+      <c r="GP84" s="77"/>
+      <c r="GQ84" s="77"/>
+      <c r="GR84" s="77"/>
+      <c r="GS84" s="77"/>
+      <c r="GT84" s="77"/>
+      <c r="GU84" s="77"/>
+      <c r="GV84" s="77"/>
+      <c r="GW84" s="77"/>
+      <c r="GX84" s="77"/>
+      <c r="GY84" s="77"/>
+      <c r="GZ84" s="77"/>
+      <c r="HA84" s="77"/>
+      <c r="HB84" s="77"/>
+      <c r="HC84" s="77"/>
+      <c r="HD84" s="77"/>
+      <c r="HE84" s="77"/>
+      <c r="HF84" s="77"/>
+      <c r="HG84" s="77"/>
+      <c r="HH84" s="77"/>
+      <c r="HI84" s="77"/>
+      <c r="HJ84" s="77"/>
+      <c r="HK84" s="77"/>
+      <c r="HL84" s="77"/>
+      <c r="HM84" s="77"/>
+      <c r="HN84" s="77"/>
+      <c r="HO84" s="77"/>
+      <c r="HP84" s="77"/>
+      <c r="HQ84" s="77"/>
+      <c r="HR84" s="77"/>
+      <c r="HS84" s="77"/>
+      <c r="HT84" s="77"/>
+      <c r="HU84" s="77"/>
+      <c r="HV84" s="77"/>
+      <c r="HW84" s="77"/>
+      <c r="HX84" s="77"/>
+      <c r="HY84" s="77"/>
+      <c r="HZ84" s="77"/>
+      <c r="IA84" s="77"/>
+      <c r="IB84" s="77"/>
+      <c r="IC84" s="77"/>
+      <c r="ID84" s="77"/>
+      <c r="IE84" s="77"/>
+      <c r="IF84" s="77"/>
+      <c r="IG84" s="77"/>
+      <c r="IH84" s="77"/>
+      <c r="II84" s="77"/>
+      <c r="IJ84" s="77"/>
+      <c r="IK84" s="77"/>
+      <c r="IL84" s="77"/>
+      <c r="IM84" s="77"/>
+      <c r="IN84" s="77"/>
+      <c r="IO84" s="77"/>
+      <c r="IP84" s="77"/>
+      <c r="IQ84" s="77"/>
+      <c r="IR84" s="77"/>
+      <c r="IS84" s="77"/>
+      <c r="IT84" s="77"/>
+      <c r="IU84" s="77"/>
+      <c r="IV84" s="77"/>
+      <c r="IW84" s="77"/>
+      <c r="IX84" s="77"/>
+      <c r="IY84" s="77"/>
+      <c r="IZ84" s="77"/>
+      <c r="JA84" s="77"/>
+      <c r="JB84" s="77"/>
+      <c r="JC84" s="77"/>
+      <c r="JD84" s="77"/>
+      <c r="JE84" s="77"/>
+      <c r="JF84" s="77"/>
+      <c r="JG84" s="77"/>
+      <c r="JH84" s="77"/>
+      <c r="JI84" s="77"/>
+      <c r="JJ84" s="77"/>
+      <c r="JK84" s="77"/>
+      <c r="JL84" s="77"/>
+      <c r="JM84" s="77"/>
+      <c r="JN84" s="77"/>
+      <c r="JO84" s="77"/>
+      <c r="JP84" s="77"/>
+      <c r="JQ84" s="77"/>
+      <c r="JR84" s="77"/>
+      <c r="JS84" s="77"/>
+      <c r="JT84" s="77"/>
+      <c r="JU84" s="77"/>
+      <c r="JV84" s="77"/>
+      <c r="JW84" s="77"/>
+      <c r="JX84" s="77"/>
+      <c r="JY84" s="77"/>
+      <c r="JZ84" s="77"/>
+      <c r="KA84" s="77"/>
+      <c r="KB84" s="77"/>
+      <c r="KC84" s="77"/>
+      <c r="KD84" s="77"/>
+      <c r="KE84" s="77"/>
+      <c r="KF84" s="77"/>
+      <c r="KG84" s="77"/>
+      <c r="KH84" s="77"/>
+      <c r="KI84" s="77"/>
+      <c r="KJ84" s="77"/>
+      <c r="KK84" s="77"/>
+      <c r="KL84" s="77"/>
+      <c r="KM84" s="77"/>
+      <c r="KN84" s="77"/>
+      <c r="KO84" s="77"/>
+      <c r="KP84" s="77"/>
+      <c r="KQ84" s="77"/>
+      <c r="KR84" s="77"/>
+      <c r="KS84" s="77"/>
+      <c r="KT84" s="77"/>
+      <c r="KU84" s="77"/>
+      <c r="KV84" s="77"/>
+      <c r="KW84" s="77"/>
+      <c r="KX84" s="77"/>
+      <c r="KY84" s="77"/>
+      <c r="KZ84" s="77"/>
+      <c r="LA84" s="77"/>
+      <c r="LB84" s="77"/>
+      <c r="LC84" s="77"/>
+      <c r="LD84" s="77"/>
+      <c r="LE84" s="77"/>
+      <c r="LF84" s="77"/>
+      <c r="LG84" s="77"/>
+      <c r="LH84" s="77"/>
+      <c r="LI84" s="77"/>
+      <c r="LJ84" s="77"/>
+      <c r="LK84" s="77"/>
+      <c r="LL84" s="77"/>
+      <c r="LM84" s="77"/>
+      <c r="LN84" s="77"/>
+      <c r="LO84" s="77"/>
+      <c r="LP84" s="77"/>
+      <c r="LQ84" s="77"/>
+      <c r="LR84" s="77"/>
+      <c r="LS84" s="77"/>
+      <c r="LT84" s="77"/>
+      <c r="LU84" s="77"/>
+      <c r="LV84" s="77"/>
+      <c r="LW84" s="77"/>
+      <c r="LX84" s="77"/>
+      <c r="LY84" s="77"/>
+      <c r="LZ84" s="77"/>
+      <c r="MA84" s="77"/>
+      <c r="MB84" s="77"/>
+      <c r="MC84" s="77"/>
+      <c r="MD84" s="77"/>
+      <c r="ME84" s="77"/>
+      <c r="MF84" s="77"/>
+      <c r="MG84" s="77"/>
+      <c r="MH84" s="77"/>
+      <c r="MI84" s="77"/>
+      <c r="MJ84" s="77"/>
+      <c r="MK84" s="77"/>
+      <c r="ML84" s="77"/>
+      <c r="MM84" s="77"/>
+      <c r="MN84" s="77"/>
+      <c r="MO84" s="77"/>
+      <c r="MP84" s="77"/>
+      <c r="MQ84" s="77"/>
+      <c r="MR84" s="77"/>
+      <c r="MS84" s="77"/>
+      <c r="MT84" s="77"/>
+      <c r="MU84" s="77"/>
+      <c r="MV84" s="77"/>
+      <c r="MW84" s="77"/>
+      <c r="MX84" s="77"/>
+      <c r="MY84" s="77"/>
+      <c r="MZ84" s="77"/>
+      <c r="NA84" s="77"/>
+      <c r="NB84" s="77"/>
+      <c r="NC84" s="77"/>
+      <c r="ND84" s="77"/>
+      <c r="NE84" s="77"/>
+      <c r="NF84" s="77"/>
+      <c r="NG84" s="77"/>
+      <c r="NH84" s="77"/>
+      <c r="NI84" s="77"/>
+      <c r="NJ84" s="77"/>
+      <c r="NK84" s="77"/>
+      <c r="NL84" s="77"/>
+      <c r="NM84" s="77"/>
+      <c r="NN84" s="77"/>
+      <c r="NO84" s="77"/>
+      <c r="NP84" s="77"/>
+      <c r="NQ84" s="77"/>
+      <c r="NR84" s="77"/>
+      <c r="NS84" s="77"/>
+      <c r="NT84" s="77"/>
+      <c r="NU84" s="77"/>
+      <c r="NV84" s="77"/>
+      <c r="NW84" s="77"/>
+      <c r="NX84" s="77"/>
+      <c r="NY84" s="77"/>
+      <c r="NZ84" s="77"/>
+      <c r="OA84" s="77"/>
+      <c r="OB84" s="77"/>
+      <c r="OC84" s="77"/>
+      <c r="OD84" s="77"/>
+      <c r="OE84" s="77"/>
+      <c r="OF84" s="77"/>
+      <c r="OG84" s="77"/>
+      <c r="OH84" s="77"/>
+      <c r="OI84" s="77"/>
+      <c r="OJ84" s="77"/>
+      <c r="OK84" s="77"/>
+      <c r="OL84" s="77"/>
+      <c r="OM84" s="77"/>
+      <c r="ON84" s="77"/>
+      <c r="OO84" s="77"/>
+      <c r="OP84" s="77"/>
+      <c r="OQ84" s="77"/>
+      <c r="OR84" s="77"/>
+      <c r="OS84" s="77"/>
+      <c r="OT84" s="77"/>
+      <c r="OU84" s="77"/>
+      <c r="OV84" s="77"/>
+      <c r="OW84" s="77"/>
+      <c r="OX84" s="77"/>
+      <c r="OY84" s="77"/>
+      <c r="OZ84" s="77"/>
+      <c r="PA84" s="77"/>
+      <c r="PB84" s="77"/>
+      <c r="PC84" s="77"/>
+      <c r="PD84" s="77"/>
+      <c r="PE84" s="77"/>
+      <c r="PF84" s="77"/>
+      <c r="PG84" s="77"/>
+      <c r="PH84" s="77"/>
+      <c r="PI84" s="77"/>
+      <c r="PJ84" s="77"/>
+      <c r="PK84" s="77"/>
+      <c r="PL84" s="77"/>
+      <c r="PM84" s="77"/>
+      <c r="PN84" s="77"/>
+      <c r="PO84" s="77"/>
+      <c r="PP84" s="77"/>
+      <c r="PQ84" s="77"/>
+      <c r="PR84" s="77"/>
+      <c r="PS84" s="77"/>
+      <c r="PT84" s="77"/>
+      <c r="PU84" s="77"/>
+      <c r="PV84" s="77"/>
+      <c r="PW84" s="77"/>
+      <c r="PX84" s="77"/>
+      <c r="PY84" s="77"/>
+      <c r="PZ84" s="77"/>
+      <c r="QA84" s="77"/>
+      <c r="QB84" s="77"/>
+      <c r="QC84" s="77"/>
+      <c r="QD84" s="77"/>
+      <c r="QE84" s="77"/>
+      <c r="QF84" s="77"/>
+      <c r="QG84" s="77"/>
+      <c r="QH84" s="77"/>
+      <c r="QI84" s="77"/>
+      <c r="QJ84" s="77"/>
+      <c r="QK84" s="77"/>
+      <c r="QL84" s="77"/>
+      <c r="QM84" s="77"/>
+      <c r="QN84" s="77"/>
+      <c r="QO84" s="77"/>
+      <c r="QP84" s="77"/>
+      <c r="QQ84" s="77"/>
+      <c r="QR84" s="77"/>
+      <c r="QS84" s="77"/>
+      <c r="QT84" s="77"/>
+      <c r="QU84" s="77"/>
+      <c r="QV84" s="77"/>
+      <c r="QW84" s="77"/>
+      <c r="QX84" s="77"/>
+      <c r="QY84" s="77"/>
+      <c r="QZ84" s="77"/>
+      <c r="RA84" s="77"/>
+      <c r="RB84" s="77"/>
+      <c r="RC84" s="77"/>
+      <c r="RD84" s="77"/>
+      <c r="RE84" s="77"/>
+      <c r="RF84" s="77"/>
+      <c r="RG84" s="77"/>
+      <c r="RH84" s="77"/>
+      <c r="RI84" s="77"/>
+      <c r="RJ84" s="77"/>
+      <c r="RK84" s="77"/>
+      <c r="RL84" s="77"/>
+      <c r="RM84" s="77"/>
+      <c r="RN84" s="77"/>
+      <c r="RO84" s="77"/>
+      <c r="RP84" s="77"/>
+      <c r="RQ84" s="77"/>
+      <c r="RR84" s="77"/>
+      <c r="RS84" s="77"/>
+      <c r="RT84" s="77"/>
+      <c r="RU84" s="77"/>
+      <c r="RV84" s="77"/>
+      <c r="RW84" s="77"/>
+      <c r="RX84" s="77"/>
+      <c r="RY84" s="77"/>
+      <c r="RZ84" s="77"/>
+      <c r="SA84" s="77"/>
+      <c r="SB84" s="77"/>
+      <c r="SC84" s="77"/>
+      <c r="SD84" s="77"/>
+      <c r="SE84" s="77"/>
+      <c r="SF84" s="77"/>
+      <c r="SG84" s="77"/>
+      <c r="SH84" s="77"/>
+      <c r="SI84" s="77"/>
+      <c r="SJ84" s="77"/>
+      <c r="SK84" s="77"/>
+      <c r="SL84" s="77"/>
+      <c r="SM84" s="77"/>
+      <c r="SN84" s="77"/>
+      <c r="SO84" s="77"/>
+      <c r="SP84" s="77"/>
+      <c r="SQ84" s="77"/>
+      <c r="SR84" s="77"/>
+      <c r="SS84" s="77"/>
+      <c r="ST84" s="77"/>
+      <c r="SU84" s="77"/>
+      <c r="SV84" s="77"/>
+      <c r="SW84" s="77"/>
+      <c r="SX84" s="77"/>
+      <c r="SY84" s="77"/>
+      <c r="SZ84" s="77"/>
+      <c r="TA84" s="77"/>
+      <c r="TB84" s="77"/>
+      <c r="TC84" s="77"/>
+      <c r="TD84" s="77"/>
+      <c r="TE84" s="77"/>
+      <c r="TF84" s="77"/>
+      <c r="TG84" s="77"/>
+      <c r="TH84" s="77"/>
+      <c r="TI84" s="77"/>
+      <c r="TJ84" s="77"/>
+      <c r="TK84" s="77"/>
+      <c r="TL84" s="77"/>
+      <c r="TM84" s="77"/>
+      <c r="TN84" s="77"/>
+      <c r="TO84" s="77"/>
+      <c r="TP84" s="77"/>
+      <c r="TQ84" s="77"/>
+      <c r="TR84" s="77"/>
+      <c r="TS84" s="77"/>
+      <c r="TT84" s="77"/>
+      <c r="TU84" s="77"/>
+      <c r="TV84" s="77"/>
+      <c r="TW84" s="77"/>
+      <c r="TX84" s="77"/>
+      <c r="TY84" s="77"/>
+      <c r="TZ84" s="77"/>
+      <c r="UA84" s="77"/>
+      <c r="UB84" s="77"/>
+      <c r="UC84" s="77"/>
+      <c r="UD84" s="77"/>
+      <c r="UE84" s="77"/>
+      <c r="UF84" s="77"/>
+      <c r="UG84" s="77"/>
+      <c r="UH84" s="77"/>
+      <c r="UI84" s="77"/>
+      <c r="UJ84" s="77"/>
+      <c r="UK84" s="77"/>
+      <c r="UL84" s="77"/>
+      <c r="UM84" s="77"/>
+      <c r="UN84" s="77"/>
+      <c r="UO84" s="77"/>
+      <c r="UP84" s="77"/>
+      <c r="UQ84" s="77"/>
+      <c r="UR84" s="77"/>
+      <c r="US84" s="77"/>
+      <c r="UT84" s="77"/>
+      <c r="UU84" s="77"/>
+      <c r="UV84" s="77"/>
+      <c r="UW84" s="77"/>
+      <c r="UX84" s="77"/>
+      <c r="UY84" s="77"/>
+      <c r="UZ84" s="77"/>
+      <c r="VA84" s="77"/>
+      <c r="VB84" s="77"/>
+      <c r="VC84" s="77"/>
+      <c r="VD84" s="77"/>
+      <c r="VE84" s="77"/>
+      <c r="VF84" s="77"/>
+      <c r="VG84" s="77"/>
+      <c r="VH84" s="77"/>
+      <c r="VI84" s="77"/>
+      <c r="VJ84" s="77"/>
+      <c r="VK84" s="77"/>
+      <c r="VL84" s="77"/>
+      <c r="VM84" s="77"/>
+      <c r="VN84" s="77"/>
+      <c r="VO84" s="77"/>
+      <c r="VP84" s="77"/>
+      <c r="VQ84" s="77"/>
+      <c r="VR84" s="77"/>
+      <c r="VS84" s="77"/>
+      <c r="VT84" s="77"/>
+      <c r="VU84" s="77"/>
+      <c r="VV84" s="77"/>
+      <c r="VW84" s="77"/>
+      <c r="VX84" s="77"/>
+      <c r="VY84" s="77"/>
+      <c r="VZ84" s="77"/>
+      <c r="WA84" s="77"/>
+      <c r="WB84" s="77"/>
+      <c r="WC84" s="77"/>
+      <c r="WD84" s="77"/>
+      <c r="WE84" s="77"/>
+      <c r="WF84" s="77"/>
+      <c r="WG84" s="77"/>
+      <c r="WH84" s="77"/>
+      <c r="WI84" s="77"/>
+      <c r="WJ84" s="77"/>
+      <c r="WK84" s="77"/>
+      <c r="WL84" s="77"/>
+      <c r="WM84" s="77"/>
+      <c r="WN84" s="77"/>
+      <c r="WO84" s="77"/>
+      <c r="WP84" s="77"/>
+      <c r="WQ84" s="77"/>
+      <c r="WR84" s="77"/>
+      <c r="WS84" s="77"/>
+      <c r="WT84" s="77"/>
+      <c r="WU84" s="77"/>
+      <c r="WV84" s="77"/>
+      <c r="WW84" s="77"/>
+      <c r="WX84" s="77"/>
+      <c r="WY84" s="77"/>
+      <c r="WZ84" s="77"/>
+      <c r="XA84" s="77"/>
+      <c r="XB84" s="77"/>
+      <c r="XC84" s="77"/>
+      <c r="XD84" s="77"/>
+      <c r="XE84" s="77"/>
+      <c r="XF84" s="77"/>
+      <c r="XG84" s="77"/>
+      <c r="XH84" s="77"/>
+      <c r="XI84" s="77"/>
+      <c r="XJ84" s="77"/>
+      <c r="XK84" s="77"/>
+      <c r="XL84" s="77"/>
+      <c r="XM84" s="77"/>
+      <c r="XN84" s="77"/>
+      <c r="XO84" s="77"/>
+      <c r="XP84" s="77"/>
+      <c r="XQ84" s="77"/>
+      <c r="XR84" s="77"/>
+      <c r="XS84" s="77"/>
+      <c r="XT84" s="77"/>
+      <c r="XU84" s="77"/>
+      <c r="XV84" s="77"/>
+      <c r="XW84" s="77"/>
+      <c r="XX84" s="77"/>
+      <c r="XY84" s="77"/>
+      <c r="XZ84" s="77"/>
+      <c r="YA84" s="77"/>
+      <c r="YB84" s="77"/>
+      <c r="YC84" s="77"/>
+      <c r="YD84" s="77"/>
+      <c r="YE84" s="77"/>
+      <c r="YF84" s="77"/>
+      <c r="YG84" s="77"/>
+      <c r="YH84" s="77"/>
+      <c r="YI84" s="77"/>
+      <c r="YJ84" s="77"/>
+      <c r="YK84" s="77"/>
+      <c r="YL84" s="77"/>
+      <c r="YM84" s="77"/>
+      <c r="YN84" s="77"/>
+      <c r="YO84" s="77"/>
+      <c r="YP84" s="77"/>
+      <c r="YQ84" s="77"/>
+      <c r="YR84" s="77"/>
+      <c r="YS84" s="77"/>
+      <c r="YT84" s="77"/>
+      <c r="YU84" s="77"/>
+      <c r="YV84" s="77"/>
+      <c r="YW84" s="77"/>
+      <c r="YX84" s="77"/>
+      <c r="YY84" s="77"/>
+      <c r="YZ84" s="77"/>
+      <c r="ZA84" s="77"/>
+      <c r="ZB84" s="77"/>
+      <c r="ZC84" s="77"/>
+      <c r="ZD84" s="77"/>
+      <c r="ZE84" s="77"/>
+      <c r="ZF84" s="77"/>
+      <c r="ZG84" s="77"/>
+      <c r="ZH84" s="77"/>
+      <c r="ZI84" s="77"/>
+      <c r="ZJ84" s="77"/>
+      <c r="ZK84" s="77"/>
+      <c r="ZL84" s="77"/>
+      <c r="ZM84" s="77"/>
+      <c r="ZN84" s="77"/>
+      <c r="ZO84" s="77"/>
+      <c r="ZP84" s="77"/>
+      <c r="ZQ84" s="77"/>
+      <c r="ZR84" s="77"/>
+      <c r="ZS84" s="77"/>
+      <c r="ZT84" s="77"/>
+      <c r="ZU84" s="77"/>
+      <c r="ZV84" s="77"/>
+      <c r="ZW84" s="77"/>
+      <c r="ZX84" s="77"/>
+      <c r="ZY84" s="77"/>
+      <c r="ZZ84" s="77"/>
+      <c r="AAA84" s="77"/>
+      <c r="AAB84" s="77"/>
+      <c r="AAC84" s="77"/>
+      <c r="AAD84" s="77"/>
+      <c r="AAE84" s="77"/>
+      <c r="AAF84" s="77"/>
+      <c r="AAG84" s="77"/>
+      <c r="AAH84" s="77"/>
+      <c r="AAI84" s="77"/>
+      <c r="AAJ84" s="77"/>
+      <c r="AAK84" s="77"/>
+      <c r="AAL84" s="77"/>
+      <c r="AAM84" s="77"/>
+      <c r="AAN84" s="77"/>
+      <c r="AAO84" s="77"/>
+      <c r="AAP84" s="77"/>
+      <c r="AAQ84" s="77"/>
+      <c r="AAR84" s="77"/>
+      <c r="AAS84" s="77"/>
+      <c r="AAT84" s="77"/>
+      <c r="AAU84" s="77"/>
+      <c r="AAV84" s="77"/>
+      <c r="AAW84" s="77"/>
+      <c r="AAX84" s="77"/>
+      <c r="AAY84" s="77"/>
+      <c r="AAZ84" s="77"/>
+      <c r="ABA84" s="77"/>
+      <c r="ABB84" s="77"/>
+      <c r="ABC84" s="77"/>
+      <c r="ABD84" s="77"/>
+      <c r="ABE84" s="77"/>
+      <c r="ABF84" s="77"/>
+      <c r="ABG84" s="77"/>
+      <c r="ABH84" s="77"/>
+      <c r="ABI84" s="77"/>
+      <c r="ABJ84" s="77"/>
+      <c r="ABK84" s="77"/>
+      <c r="ABL84" s="77"/>
+      <c r="ABM84" s="77"/>
+      <c r="ABN84" s="77"/>
+      <c r="ABO84" s="77"/>
+      <c r="ABP84" s="77"/>
+      <c r="ABQ84" s="77"/>
+      <c r="ABR84" s="77"/>
+      <c r="ABS84" s="77"/>
+      <c r="ABT84" s="77"/>
+      <c r="ABU84" s="77"/>
+      <c r="ABV84" s="77"/>
+      <c r="ABW84" s="77"/>
+      <c r="ABX84" s="77"/>
+      <c r="ABY84" s="77"/>
+      <c r="ABZ84" s="77"/>
+      <c r="ACA84" s="77"/>
+      <c r="ACB84" s="77"/>
+      <c r="ACC84" s="77"/>
+      <c r="ACD84" s="77"/>
+      <c r="ACE84" s="77"/>
+      <c r="ACF84" s="77"/>
+      <c r="ACG84" s="77"/>
+      <c r="ACH84" s="77"/>
+      <c r="ACI84" s="77"/>
+      <c r="ACJ84" s="77"/>
+      <c r="ACK84" s="77"/>
+      <c r="ACL84" s="77"/>
+      <c r="ACM84" s="77"/>
+      <c r="ACN84" s="77"/>
+      <c r="ACO84" s="77"/>
+      <c r="ACP84" s="77"/>
+      <c r="ACQ84" s="77"/>
+      <c r="ACR84" s="77"/>
+      <c r="ACS84" s="77"/>
+      <c r="ACT84" s="77"/>
+      <c r="ACU84" s="77"/>
+      <c r="ACV84" s="77"/>
+      <c r="ACW84" s="77"/>
+      <c r="ACX84" s="77"/>
+      <c r="ACY84" s="77"/>
+      <c r="ACZ84" s="77"/>
+      <c r="ADA84" s="77"/>
+      <c r="ADB84" s="77"/>
+      <c r="ADC84" s="77"/>
+      <c r="ADD84" s="77"/>
+      <c r="ADE84" s="77"/>
+      <c r="ADF84" s="77"/>
+      <c r="ADG84" s="77"/>
+      <c r="ADH84" s="77"/>
+      <c r="ADI84" s="77"/>
+      <c r="ADJ84" s="77"/>
+      <c r="ADK84" s="77"/>
+      <c r="ADL84" s="77"/>
+      <c r="ADM84" s="77"/>
+      <c r="ADN84" s="77"/>
+      <c r="ADO84" s="77"/>
+      <c r="ADP84" s="77"/>
+      <c r="ADQ84" s="77"/>
+      <c r="ADR84" s="77"/>
+      <c r="ADS84" s="77"/>
+      <c r="ADT84" s="77"/>
+      <c r="ADU84" s="77"/>
+      <c r="ADV84" s="77"/>
+      <c r="ADW84" s="77"/>
+      <c r="ADX84" s="77"/>
+      <c r="ADY84" s="77"/>
+      <c r="ADZ84" s="77"/>
+      <c r="AEA84" s="77"/>
+      <c r="AEB84" s="77"/>
+      <c r="AEC84" s="77"/>
+      <c r="AED84" s="77"/>
+      <c r="AEE84" s="77"/>
+      <c r="AEF84" s="77"/>
+      <c r="AEG84" s="77"/>
+      <c r="AEH84" s="77"/>
+      <c r="AEI84" s="77"/>
+      <c r="AEJ84" s="77"/>
+      <c r="AEK84" s="77"/>
+      <c r="AEL84" s="77"/>
+      <c r="AEM84" s="77"/>
+      <c r="AEN84" s="77"/>
+      <c r="AEO84" s="77"/>
+      <c r="AEP84" s="77"/>
+      <c r="AEQ84" s="77"/>
+      <c r="AER84" s="77"/>
+      <c r="AES84" s="77"/>
+      <c r="AET84" s="77"/>
+      <c r="AEU84" s="77"/>
+      <c r="AEV84" s="77"/>
+      <c r="AEW84" s="77"/>
+      <c r="AEX84" s="77"/>
+      <c r="AEY84" s="77"/>
+      <c r="AEZ84" s="77"/>
+      <c r="AFA84" s="77"/>
+      <c r="AFB84" s="77"/>
+      <c r="AFC84" s="77"/>
+      <c r="AFD84" s="77"/>
+      <c r="AFE84" s="77"/>
+      <c r="AFF84" s="77"/>
+      <c r="AFG84" s="77"/>
+      <c r="AFH84" s="77"/>
+      <c r="AFI84" s="77"/>
+      <c r="AFJ84" s="77"/>
+      <c r="AFK84" s="77"/>
+      <c r="AFL84" s="77"/>
+      <c r="AFM84" s="77"/>
+      <c r="AFN84" s="77"/>
+      <c r="AFO84" s="77"/>
+      <c r="AFP84" s="77"/>
+      <c r="AFQ84" s="77"/>
+      <c r="AFR84" s="77"/>
+      <c r="AFS84" s="77"/>
+      <c r="AFT84" s="77"/>
+      <c r="AFU84" s="77"/>
+      <c r="AFV84" s="77"/>
+      <c r="AFW84" s="77"/>
+      <c r="AFX84" s="77"/>
+      <c r="AFY84" s="77"/>
+      <c r="AFZ84" s="77"/>
+      <c r="AGA84" s="77"/>
+      <c r="AGB84" s="77"/>
+      <c r="AGC84" s="77"/>
+      <c r="AGD84" s="77"/>
+      <c r="AGE84" s="77"/>
+      <c r="AGF84" s="77"/>
+      <c r="AGG84" s="77"/>
+      <c r="AGH84" s="77"/>
+      <c r="AGI84" s="77"/>
+      <c r="AGJ84" s="77"/>
+      <c r="AGK84" s="77"/>
+      <c r="AGL84" s="77"/>
+      <c r="AGM84" s="77"/>
+      <c r="AGN84" s="77"/>
+      <c r="AGO84" s="77"/>
+      <c r="AGP84" s="77"/>
+      <c r="AGQ84" s="77"/>
+      <c r="AGR84" s="77"/>
+      <c r="AGS84" s="77"/>
+      <c r="AGT84" s="77"/>
+      <c r="AGU84" s="77"/>
+      <c r="AGV84" s="77"/>
+      <c r="AGW84" s="77"/>
+      <c r="AGX84" s="77"/>
+      <c r="AGY84" s="77"/>
+      <c r="AGZ84" s="77"/>
+      <c r="AHA84" s="77"/>
+      <c r="AHB84" s="77"/>
+      <c r="AHC84" s="77"/>
+      <c r="AHD84" s="77"/>
+      <c r="AHE84" s="77"/>
+      <c r="AHF84" s="77"/>
+      <c r="AHG84" s="77"/>
+      <c r="AHH84" s="77"/>
+      <c r="AHI84" s="77"/>
+      <c r="AHJ84" s="77"/>
+      <c r="AHK84" s="77"/>
+      <c r="AHL84" s="77"/>
+      <c r="AHM84" s="77"/>
+      <c r="AHN84" s="77"/>
+      <c r="AHO84" s="77"/>
+      <c r="AHP84" s="77"/>
+      <c r="AHQ84" s="77"/>
+      <c r="AHR84" s="77"/>
+      <c r="AHS84" s="77"/>
+      <c r="AHT84" s="77"/>
+      <c r="AHU84" s="77"/>
+      <c r="AHV84" s="77"/>
+      <c r="AHW84" s="77"/>
+      <c r="AHX84" s="77"/>
+      <c r="AHY84" s="77"/>
+      <c r="AHZ84" s="77"/>
+      <c r="AIA84" s="77"/>
+      <c r="AIB84" s="77"/>
+      <c r="AIC84" s="77"/>
+      <c r="AID84" s="77"/>
+      <c r="AIE84" s="77"/>
+      <c r="AIF84" s="77"/>
+      <c r="AIG84" s="77"/>
+      <c r="AIH84" s="77"/>
+      <c r="AII84" s="77"/>
+      <c r="AIJ84" s="77"/>
+      <c r="AIK84" s="77"/>
+      <c r="AIL84" s="77"/>
+      <c r="AIM84" s="77"/>
+      <c r="AIN84" s="77"/>
+      <c r="AIO84" s="77"/>
+      <c r="AIP84" s="77"/>
+      <c r="AIQ84" s="77"/>
+      <c r="AIR84" s="77"/>
+      <c r="AIS84" s="77"/>
+      <c r="AIT84" s="77"/>
+      <c r="AIU84" s="77"/>
+      <c r="AIV84" s="77"/>
+      <c r="AIW84" s="77"/>
+      <c r="AIX84" s="77"/>
+      <c r="AIY84" s="77"/>
+      <c r="AIZ84" s="77"/>
+      <c r="AJA84" s="77"/>
+      <c r="AJB84" s="77"/>
+      <c r="AJC84" s="77"/>
+      <c r="AJD84" s="77"/>
+      <c r="AJE84" s="77"/>
+      <c r="AJF84" s="77"/>
+      <c r="AJG84" s="77"/>
+      <c r="AJH84" s="77"/>
+      <c r="AJI84" s="77"/>
+      <c r="AJJ84" s="77"/>
+      <c r="AJK84" s="77"/>
+      <c r="AJL84" s="77"/>
+      <c r="AJM84" s="77"/>
+      <c r="AJN84" s="77"/>
+      <c r="AJO84" s="77"/>
+      <c r="AJP84" s="77"/>
+      <c r="AJQ84" s="77"/>
+      <c r="AJR84" s="77"/>
+      <c r="AJS84" s="77"/>
+      <c r="AJT84" s="77"/>
+      <c r="AJU84" s="77"/>
+      <c r="AJV84" s="77"/>
+      <c r="AJW84" s="77"/>
+      <c r="AJX84" s="77"/>
+      <c r="AJY84" s="77"/>
+      <c r="AJZ84" s="77"/>
+      <c r="AKA84" s="77"/>
+      <c r="AKB84" s="77"/>
+      <c r="AKC84" s="77"/>
+      <c r="AKD84" s="77"/>
+      <c r="AKE84" s="77"/>
+      <c r="AKF84" s="77"/>
+      <c r="AKG84" s="77"/>
+      <c r="AKH84" s="77"/>
+      <c r="AKI84" s="77"/>
+      <c r="AKJ84" s="77"/>
+      <c r="AKK84" s="77"/>
+      <c r="AKL84" s="77"/>
+      <c r="AKM84" s="77"/>
+      <c r="AKN84" s="77"/>
+      <c r="AKO84" s="77"/>
+      <c r="AKP84" s="77"/>
+      <c r="AKQ84" s="77"/>
+      <c r="AKR84" s="77"/>
+      <c r="AKS84" s="77"/>
+      <c r="AKT84" s="77"/>
+      <c r="AKU84" s="77"/>
+      <c r="AKV84" s="77"/>
+      <c r="AKW84" s="77"/>
+      <c r="AKX84" s="77"/>
+      <c r="AKY84" s="77"/>
+      <c r="AKZ84" s="77"/>
+      <c r="ALA84" s="77"/>
+      <c r="ALB84" s="77"/>
+      <c r="ALC84" s="77"/>
+      <c r="ALD84" s="77"/>
+      <c r="ALE84" s="77"/>
+      <c r="ALF84" s="77"/>
+      <c r="ALG84" s="77"/>
+      <c r="ALH84" s="77"/>
+      <c r="ALI84" s="77"/>
+      <c r="ALJ84" s="77"/>
+      <c r="ALK84" s="77"/>
+      <c r="ALL84" s="77"/>
+      <c r="ALM84" s="77"/>
+      <c r="ALN84" s="77"/>
+      <c r="ALO84" s="77"/>
+      <c r="ALP84" s="77"/>
+      <c r="ALQ84" s="77"/>
+      <c r="ALR84" s="77"/>
+      <c r="ALS84" s="77"/>
+      <c r="ALT84" s="77"/>
+      <c r="ALU84" s="77"/>
+      <c r="ALV84" s="77"/>
+      <c r="ALW84" s="77"/>
+      <c r="ALX84" s="77"/>
+      <c r="ALY84" s="77"/>
+      <c r="ALZ84" s="77"/>
+      <c r="AMA84" s="77"/>
+      <c r="AMB84" s="77"/>
+      <c r="AMC84" s="77"/>
+      <c r="AMD84" s="77"/>
+      <c r="AME84" s="77"/>
+      <c r="AMF84" s="77"/>
+      <c r="AMG84" s="77"/>
+      <c r="AMH84" s="77"/>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="1" t="s">
@@ -20749,7 +20845,7 @@
       </c>
     </row>
     <row r="88" s="6" customFormat="1" spans="1:1022">
-      <c r="A88" s="77" t="s">
+      <c r="A88" s="79" t="s">
         <v>149</v>
       </c>
       <c r="B88" s="27" t="s">
@@ -23914,10 +24010,10 @@
       </c>
     </row>
     <row r="97" spans="5:5">
-      <c r="E97" s="72"/>
+      <c r="E97" s="73"/>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="78" t="s">
+      <c r="A98" s="80" t="s">
         <v>153</v>
       </c>
       <c r="B98" s="59" t="s">
@@ -23929,7 +24025,7 @@
       <c r="D98" s="60">
         <v>0.9673051</v>
       </c>
-      <c r="E98" s="70">
+      <c r="E98" s="71">
         <v>0.9686</v>
       </c>
     </row>
@@ -23946,7 +24042,7 @@
       <c r="D99" s="10">
         <v>0.9671612</v>
       </c>
-      <c r="E99" s="72">
+      <c r="E99" s="73">
         <v>0.9687</v>
       </c>
     </row>
@@ -23963,7 +24059,7 @@
       <c r="D100" s="10">
         <v>0.9673732</v>
       </c>
-      <c r="E100" s="72">
+      <c r="E100" s="73">
         <v>0.9686</v>
       </c>
     </row>
@@ -23980,7 +24076,7 @@
       <c r="D101" s="10">
         <v>0.9674291</v>
       </c>
-      <c r="E101" s="72">
+      <c r="E101" s="73">
         <v>0.96939</v>
       </c>
     </row>
@@ -23997,7 +24093,7 @@
       <c r="D102" s="10">
         <v>0.967249</v>
       </c>
-      <c r="E102" s="72"/>
+      <c r="E102" s="73"/>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="1" t="s">
@@ -24012,7 +24108,7 @@
       <c r="D103" s="10">
         <v>0.9673428</v>
       </c>
-      <c r="E103" s="72"/>
+      <c r="E103" s="73"/>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="19" t="s">
@@ -24047,7 +24143,7 @@
       <c r="D105" s="28">
         <v>0.967788</v>
       </c>
-      <c r="E105" s="72">
+      <c r="E105" s="73">
         <v>0.9683</v>
       </c>
     </row>
@@ -24081,7 +24177,7 @@
       <c r="D107" s="20">
         <v>0.9676965</v>
       </c>
-      <c r="E107" s="69">
+      <c r="E107" s="70">
         <v>0.9689</v>
       </c>
     </row>
@@ -24098,12 +24194,12 @@
       <c r="D108" s="10">
         <v>0.9675807</v>
       </c>
-      <c r="E108" s="69">
+      <c r="E108" s="70">
         <v>0.96939</v>
       </c>
     </row>
     <row r="109" spans="5:5">
-      <c r="E109" s="72"/>
+      <c r="E109" s="73"/>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="1" t="s">
@@ -24118,10 +24214,10 @@
       <c r="D110" s="10">
         <v>0.9673982</v>
       </c>
-      <c r="E110" s="72">
+      <c r="E110" s="73">
         <v>0.9695</v>
       </c>
-      <c r="F110" s="73" t="s">
+      <c r="F110" s="74" t="s">
         <v>170</v>
       </c>
     </row>
@@ -24138,7 +24234,7 @@
       <c r="D111" s="10">
         <v>0.967503</v>
       </c>
-      <c r="E111" s="72">
+      <c r="E111" s="73">
         <v>0.9695</v>
       </c>
     </row>
@@ -24155,7 +24251,7 @@
       <c r="D112" s="10">
         <v>0.9675222</v>
       </c>
-      <c r="E112" s="72">
+      <c r="E112" s="73">
         <v>0.9697</v>
       </c>
     </row>
@@ -24172,15 +24268,15 @@
       <c r="D113" s="10">
         <v>0.9678351</v>
       </c>
-      <c r="E113" s="72">
+      <c r="E113" s="73">
         <v>0.9699</v>
       </c>
-      <c r="F113" s="74" t="s">
+      <c r="F113" s="75" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="114" ht="21" spans="1:5">
-      <c r="A114" s="79" t="s">
+      <c r="A114" s="81" t="s">
         <v>175</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -24192,12 +24288,12 @@
       <c r="D114" s="10">
         <v>0.9678722</v>
       </c>
-      <c r="E114" s="72">
+      <c r="E114" s="73">
         <v>0.97</v>
       </c>
     </row>
     <row r="115" spans="5:5">
-      <c r="E115" s="72"/>
+      <c r="E115" s="73"/>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="1" t="s">
@@ -24212,7 +24308,7 @@
       <c r="D116" s="10">
         <v>0.9675222</v>
       </c>
-      <c r="E116" s="72">
+      <c r="E116" s="73">
         <v>0.9697</v>
       </c>
     </row>
@@ -24229,7 +24325,7 @@
       <c r="D117" s="10">
         <v>0.9675741</v>
       </c>
-      <c r="E117" s="72">
+      <c r="E117" s="73">
         <v>0.9691</v>
       </c>
     </row>
@@ -24250,62 +24346,79 @@
         <v>0.96979</v>
       </c>
     </row>
-    <row r="119" spans="5:5">
-      <c r="E119" s="72"/>
+    <row r="119" spans="1:6">
+      <c r="A119" s="66" t="s">
+        <v>180</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C119" s="10">
+        <v>0.9962458</v>
+      </c>
+      <c r="D119" s="10">
+        <v>0.9674325</v>
+      </c>
+      <c r="E119" s="73">
+        <v>0.9699</v>
+      </c>
+      <c r="F119" s="76" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="120" spans="5:5">
-      <c r="E120" s="72"/>
+      <c r="E120" s="73"/>
     </row>
     <row r="121" spans="5:5">
-      <c r="E121" s="72"/>
+      <c r="E121" s="73"/>
     </row>
     <row r="122" spans="5:5">
-      <c r="E122" s="72"/>
+      <c r="E122" s="73"/>
     </row>
     <row r="123" spans="5:5">
-      <c r="E123" s="72"/>
+      <c r="E123" s="73"/>
     </row>
     <row r="124" spans="5:5">
-      <c r="E124" s="72"/>
+      <c r="E124" s="73"/>
     </row>
     <row r="125" spans="5:5">
-      <c r="E125" s="72"/>
+      <c r="E125" s="73"/>
     </row>
     <row r="126" spans="5:5">
-      <c r="E126" s="72"/>
+      <c r="E126" s="73"/>
     </row>
     <row r="127" spans="5:5">
-      <c r="E127" s="72"/>
+      <c r="E127" s="73"/>
     </row>
     <row r="128" spans="5:5">
-      <c r="E128" s="72"/>
+      <c r="E128" s="73"/>
     </row>
     <row r="129" spans="5:5">
-      <c r="E129" s="72"/>
+      <c r="E129" s="73"/>
     </row>
     <row r="130" spans="5:5">
-      <c r="E130" s="72"/>
+      <c r="E130" s="73"/>
     </row>
     <row r="131" spans="5:5">
-      <c r="E131" s="72"/>
+      <c r="E131" s="73"/>
     </row>
     <row r="132" spans="5:5">
-      <c r="E132" s="72"/>
+      <c r="E132" s="73"/>
     </row>
     <row r="133" spans="5:5">
-      <c r="E133" s="72"/>
+      <c r="E133" s="73"/>
     </row>
     <row r="134" spans="5:5">
-      <c r="E134" s="72"/>
+      <c r="E134" s="73"/>
     </row>
     <row r="135" spans="5:5">
-      <c r="E135" s="72"/>
+      <c r="E135" s="73"/>
     </row>
     <row r="136" spans="5:5">
-      <c r="E136" s="72"/>
+      <c r="E136" s="73"/>
     </row>
     <row r="137" spans="5:5">
-      <c r="E137" s="72"/>
+      <c r="E137" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fix some bug，添加 has_good_order 强特，0.96990
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196">
   <si>
     <r>
       <rPr>
@@ -1662,7 +1662,7 @@
       <rPr>
         <b/>
         <sz val="8"/>
-        <color theme="9" tint="-0.25"/>
+        <color rgb="FFFF0000"/>
         <rFont val="DejaVu Sans Mono"/>
         <charset val="134"/>
       </rPr>
@@ -1672,7 +1672,7 @@
       <rPr>
         <b/>
         <sz val="8"/>
-        <color theme="9" tint="-0.25"/>
+        <color rgb="FFFF0000"/>
         <charset val="134"/>
       </rPr>
       <t>！</t>
@@ -1808,6 +1808,26 @@
       <t xml:space="preserve"> has_history_flag</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>fix some bug</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，添加</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> has_good_order</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1821,7 +1841,7 @@
     <numFmt numFmtId="177" formatCode="0.00000_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="35">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1864,6 +1884,12 @@
       <sz val="8"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2043,6 +2069,13 @@
       <b/>
       <sz val="8"/>
       <color theme="9" tint="-0.25"/>
+      <name val="DejaVu Sans Mono"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
       <name val="DejaVu Sans Mono"/>
       <charset val="134"/>
     </font>
@@ -2400,142 +2433,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2758,13 +2791,10 @@
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -3099,8 +3129,8 @@
   <sheetPr/>
   <dimension ref="A1:AMH137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -8415,7 +8445,7 @@
       <c r="AMH13" s="47"/>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:1022">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="77" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="19" t="s">
@@ -19899,1020 +19929,1020 @@
         <v>0.9686</v>
       </c>
       <c r="H84" s="72"/>
-      <c r="I84" s="77"/>
-      <c r="J84" s="77"/>
-      <c r="K84" s="77"/>
-      <c r="L84" s="77"/>
-      <c r="M84" s="77"/>
-      <c r="N84" s="77"/>
-      <c r="O84" s="77"/>
-      <c r="P84" s="77"/>
-      <c r="Q84" s="77"/>
-      <c r="R84" s="77"/>
-      <c r="S84" s="77"/>
-      <c r="T84" s="77"/>
-      <c r="U84" s="77"/>
-      <c r="V84" s="77"/>
-      <c r="W84" s="77"/>
-      <c r="X84" s="77"/>
-      <c r="Y84" s="77"/>
-      <c r="Z84" s="77"/>
-      <c r="AA84" s="77"/>
-      <c r="AB84" s="77"/>
-      <c r="AC84" s="77"/>
-      <c r="AD84" s="77"/>
-      <c r="AE84" s="77"/>
-      <c r="AF84" s="77"/>
-      <c r="AG84" s="77"/>
-      <c r="AH84" s="77"/>
-      <c r="AI84" s="77"/>
-      <c r="AJ84" s="77"/>
-      <c r="AK84" s="77"/>
-      <c r="AL84" s="77"/>
-      <c r="AM84" s="77"/>
-      <c r="AN84" s="77"/>
-      <c r="AO84" s="77"/>
-      <c r="AP84" s="77"/>
-      <c r="AQ84" s="77"/>
-      <c r="AR84" s="77"/>
-      <c r="AS84" s="77"/>
-      <c r="AT84" s="77"/>
-      <c r="AU84" s="77"/>
-      <c r="AV84" s="77"/>
-      <c r="AW84" s="77"/>
-      <c r="AX84" s="77"/>
-      <c r="AY84" s="77"/>
-      <c r="AZ84" s="77"/>
-      <c r="BA84" s="77"/>
-      <c r="BB84" s="77"/>
-      <c r="BC84" s="77"/>
-      <c r="BD84" s="77"/>
-      <c r="BE84" s="77"/>
-      <c r="BF84" s="77"/>
-      <c r="BG84" s="77"/>
-      <c r="BH84" s="77"/>
-      <c r="BI84" s="77"/>
-      <c r="BJ84" s="77"/>
-      <c r="BK84" s="77"/>
-      <c r="BL84" s="77"/>
-      <c r="BM84" s="77"/>
-      <c r="BN84" s="77"/>
-      <c r="BO84" s="77"/>
-      <c r="BP84" s="77"/>
-      <c r="BQ84" s="77"/>
-      <c r="BR84" s="77"/>
-      <c r="BS84" s="77"/>
-      <c r="BT84" s="77"/>
-      <c r="BU84" s="77"/>
-      <c r="BV84" s="77"/>
-      <c r="BW84" s="77"/>
-      <c r="BX84" s="77"/>
-      <c r="BY84" s="77"/>
-      <c r="BZ84" s="77"/>
-      <c r="CA84" s="77"/>
-      <c r="CB84" s="77"/>
-      <c r="CC84" s="77"/>
-      <c r="CD84" s="77"/>
-      <c r="CE84" s="77"/>
-      <c r="CF84" s="77"/>
-      <c r="CG84" s="77"/>
-      <c r="CH84" s="77"/>
-      <c r="CI84" s="77"/>
-      <c r="CJ84" s="77"/>
-      <c r="CK84" s="77"/>
-      <c r="CL84" s="77"/>
-      <c r="CM84" s="77"/>
-      <c r="CN84" s="77"/>
-      <c r="CO84" s="77"/>
-      <c r="CP84" s="77"/>
-      <c r="CQ84" s="77"/>
-      <c r="CR84" s="77"/>
-      <c r="CS84" s="77"/>
-      <c r="CT84" s="77"/>
-      <c r="CU84" s="77"/>
-      <c r="CV84" s="77"/>
-      <c r="CW84" s="77"/>
-      <c r="CX84" s="77"/>
-      <c r="CY84" s="77"/>
-      <c r="CZ84" s="77"/>
-      <c r="DA84" s="77"/>
-      <c r="DB84" s="77"/>
-      <c r="DC84" s="77"/>
-      <c r="DD84" s="77"/>
-      <c r="DE84" s="77"/>
-      <c r="DF84" s="77"/>
-      <c r="DG84" s="77"/>
-      <c r="DH84" s="77"/>
-      <c r="DI84" s="77"/>
-      <c r="DJ84" s="77"/>
-      <c r="DK84" s="77"/>
-      <c r="DL84" s="77"/>
-      <c r="DM84" s="77"/>
-      <c r="DN84" s="77"/>
-      <c r="DO84" s="77"/>
-      <c r="DP84" s="77"/>
-      <c r="DQ84" s="77"/>
-      <c r="DR84" s="77"/>
-      <c r="DS84" s="77"/>
-      <c r="DT84" s="77"/>
-      <c r="DU84" s="77"/>
-      <c r="DV84" s="77"/>
-      <c r="DW84" s="77"/>
-      <c r="DX84" s="77"/>
-      <c r="DY84" s="77"/>
-      <c r="DZ84" s="77"/>
-      <c r="EA84" s="77"/>
-      <c r="EB84" s="77"/>
-      <c r="EC84" s="77"/>
-      <c r="ED84" s="77"/>
-      <c r="EE84" s="77"/>
-      <c r="EF84" s="77"/>
-      <c r="EG84" s="77"/>
-      <c r="EH84" s="77"/>
-      <c r="EI84" s="77"/>
-      <c r="EJ84" s="77"/>
-      <c r="EK84" s="77"/>
-      <c r="EL84" s="77"/>
-      <c r="EM84" s="77"/>
-      <c r="EN84" s="77"/>
-      <c r="EO84" s="77"/>
-      <c r="EP84" s="77"/>
-      <c r="EQ84" s="77"/>
-      <c r="ER84" s="77"/>
-      <c r="ES84" s="77"/>
-      <c r="ET84" s="77"/>
-      <c r="EU84" s="77"/>
-      <c r="EV84" s="77"/>
-      <c r="EW84" s="77"/>
-      <c r="EX84" s="77"/>
-      <c r="EY84" s="77"/>
-      <c r="EZ84" s="77"/>
-      <c r="FA84" s="77"/>
-      <c r="FB84" s="77"/>
-      <c r="FC84" s="77"/>
-      <c r="FD84" s="77"/>
-      <c r="FE84" s="77"/>
-      <c r="FF84" s="77"/>
-      <c r="FG84" s="77"/>
-      <c r="FH84" s="77"/>
-      <c r="FI84" s="77"/>
-      <c r="FJ84" s="77"/>
-      <c r="FK84" s="77"/>
-      <c r="FL84" s="77"/>
-      <c r="FM84" s="77"/>
-      <c r="FN84" s="77"/>
-      <c r="FO84" s="77"/>
-      <c r="FP84" s="77"/>
-      <c r="FQ84" s="77"/>
-      <c r="FR84" s="77"/>
-      <c r="FS84" s="77"/>
-      <c r="FT84" s="77"/>
-      <c r="FU84" s="77"/>
-      <c r="FV84" s="77"/>
-      <c r="FW84" s="77"/>
-      <c r="FX84" s="77"/>
-      <c r="FY84" s="77"/>
-      <c r="FZ84" s="77"/>
-      <c r="GA84" s="77"/>
-      <c r="GB84" s="77"/>
-      <c r="GC84" s="77"/>
-      <c r="GD84" s="77"/>
-      <c r="GE84" s="77"/>
-      <c r="GF84" s="77"/>
-      <c r="GG84" s="77"/>
-      <c r="GH84" s="77"/>
-      <c r="GI84" s="77"/>
-      <c r="GJ84" s="77"/>
-      <c r="GK84" s="77"/>
-      <c r="GL84" s="77"/>
-      <c r="GM84" s="77"/>
-      <c r="GN84" s="77"/>
-      <c r="GO84" s="77"/>
-      <c r="GP84" s="77"/>
-      <c r="GQ84" s="77"/>
-      <c r="GR84" s="77"/>
-      <c r="GS84" s="77"/>
-      <c r="GT84" s="77"/>
-      <c r="GU84" s="77"/>
-      <c r="GV84" s="77"/>
-      <c r="GW84" s="77"/>
-      <c r="GX84" s="77"/>
-      <c r="GY84" s="77"/>
-      <c r="GZ84" s="77"/>
-      <c r="HA84" s="77"/>
-      <c r="HB84" s="77"/>
-      <c r="HC84" s="77"/>
-      <c r="HD84" s="77"/>
-      <c r="HE84" s="77"/>
-      <c r="HF84" s="77"/>
-      <c r="HG84" s="77"/>
-      <c r="HH84" s="77"/>
-      <c r="HI84" s="77"/>
-      <c r="HJ84" s="77"/>
-      <c r="HK84" s="77"/>
-      <c r="HL84" s="77"/>
-      <c r="HM84" s="77"/>
-      <c r="HN84" s="77"/>
-      <c r="HO84" s="77"/>
-      <c r="HP84" s="77"/>
-      <c r="HQ84" s="77"/>
-      <c r="HR84" s="77"/>
-      <c r="HS84" s="77"/>
-      <c r="HT84" s="77"/>
-      <c r="HU84" s="77"/>
-      <c r="HV84" s="77"/>
-      <c r="HW84" s="77"/>
-      <c r="HX84" s="77"/>
-      <c r="HY84" s="77"/>
-      <c r="HZ84" s="77"/>
-      <c r="IA84" s="77"/>
-      <c r="IB84" s="77"/>
-      <c r="IC84" s="77"/>
-      <c r="ID84" s="77"/>
-      <c r="IE84" s="77"/>
-      <c r="IF84" s="77"/>
-      <c r="IG84" s="77"/>
-      <c r="IH84" s="77"/>
-      <c r="II84" s="77"/>
-      <c r="IJ84" s="77"/>
-      <c r="IK84" s="77"/>
-      <c r="IL84" s="77"/>
-      <c r="IM84" s="77"/>
-      <c r="IN84" s="77"/>
-      <c r="IO84" s="77"/>
-      <c r="IP84" s="77"/>
-      <c r="IQ84" s="77"/>
-      <c r="IR84" s="77"/>
-      <c r="IS84" s="77"/>
-      <c r="IT84" s="77"/>
-      <c r="IU84" s="77"/>
-      <c r="IV84" s="77"/>
-      <c r="IW84" s="77"/>
-      <c r="IX84" s="77"/>
-      <c r="IY84" s="77"/>
-      <c r="IZ84" s="77"/>
-      <c r="JA84" s="77"/>
-      <c r="JB84" s="77"/>
-      <c r="JC84" s="77"/>
-      <c r="JD84" s="77"/>
-      <c r="JE84" s="77"/>
-      <c r="JF84" s="77"/>
-      <c r="JG84" s="77"/>
-      <c r="JH84" s="77"/>
-      <c r="JI84" s="77"/>
-      <c r="JJ84" s="77"/>
-      <c r="JK84" s="77"/>
-      <c r="JL84" s="77"/>
-      <c r="JM84" s="77"/>
-      <c r="JN84" s="77"/>
-      <c r="JO84" s="77"/>
-      <c r="JP84" s="77"/>
-      <c r="JQ84" s="77"/>
-      <c r="JR84" s="77"/>
-      <c r="JS84" s="77"/>
-      <c r="JT84" s="77"/>
-      <c r="JU84" s="77"/>
-      <c r="JV84" s="77"/>
-      <c r="JW84" s="77"/>
-      <c r="JX84" s="77"/>
-      <c r="JY84" s="77"/>
-      <c r="JZ84" s="77"/>
-      <c r="KA84" s="77"/>
-      <c r="KB84" s="77"/>
-      <c r="KC84" s="77"/>
-      <c r="KD84" s="77"/>
-      <c r="KE84" s="77"/>
-      <c r="KF84" s="77"/>
-      <c r="KG84" s="77"/>
-      <c r="KH84" s="77"/>
-      <c r="KI84" s="77"/>
-      <c r="KJ84" s="77"/>
-      <c r="KK84" s="77"/>
-      <c r="KL84" s="77"/>
-      <c r="KM84" s="77"/>
-      <c r="KN84" s="77"/>
-      <c r="KO84" s="77"/>
-      <c r="KP84" s="77"/>
-      <c r="KQ84" s="77"/>
-      <c r="KR84" s="77"/>
-      <c r="KS84" s="77"/>
-      <c r="KT84" s="77"/>
-      <c r="KU84" s="77"/>
-      <c r="KV84" s="77"/>
-      <c r="KW84" s="77"/>
-      <c r="KX84" s="77"/>
-      <c r="KY84" s="77"/>
-      <c r="KZ84" s="77"/>
-      <c r="LA84" s="77"/>
-      <c r="LB84" s="77"/>
-      <c r="LC84" s="77"/>
-      <c r="LD84" s="77"/>
-      <c r="LE84" s="77"/>
-      <c r="LF84" s="77"/>
-      <c r="LG84" s="77"/>
-      <c r="LH84" s="77"/>
-      <c r="LI84" s="77"/>
-      <c r="LJ84" s="77"/>
-      <c r="LK84" s="77"/>
-      <c r="LL84" s="77"/>
-      <c r="LM84" s="77"/>
-      <c r="LN84" s="77"/>
-      <c r="LO84" s="77"/>
-      <c r="LP84" s="77"/>
-      <c r="LQ84" s="77"/>
-      <c r="LR84" s="77"/>
-      <c r="LS84" s="77"/>
-      <c r="LT84" s="77"/>
-      <c r="LU84" s="77"/>
-      <c r="LV84" s="77"/>
-      <c r="LW84" s="77"/>
-      <c r="LX84" s="77"/>
-      <c r="LY84" s="77"/>
-      <c r="LZ84" s="77"/>
-      <c r="MA84" s="77"/>
-      <c r="MB84" s="77"/>
-      <c r="MC84" s="77"/>
-      <c r="MD84" s="77"/>
-      <c r="ME84" s="77"/>
-      <c r="MF84" s="77"/>
-      <c r="MG84" s="77"/>
-      <c r="MH84" s="77"/>
-      <c r="MI84" s="77"/>
-      <c r="MJ84" s="77"/>
-      <c r="MK84" s="77"/>
-      <c r="ML84" s="77"/>
-      <c r="MM84" s="77"/>
-      <c r="MN84" s="77"/>
-      <c r="MO84" s="77"/>
-      <c r="MP84" s="77"/>
-      <c r="MQ84" s="77"/>
-      <c r="MR84" s="77"/>
-      <c r="MS84" s="77"/>
-      <c r="MT84" s="77"/>
-      <c r="MU84" s="77"/>
-      <c r="MV84" s="77"/>
-      <c r="MW84" s="77"/>
-      <c r="MX84" s="77"/>
-      <c r="MY84" s="77"/>
-      <c r="MZ84" s="77"/>
-      <c r="NA84" s="77"/>
-      <c r="NB84" s="77"/>
-      <c r="NC84" s="77"/>
-      <c r="ND84" s="77"/>
-      <c r="NE84" s="77"/>
-      <c r="NF84" s="77"/>
-      <c r="NG84" s="77"/>
-      <c r="NH84" s="77"/>
-      <c r="NI84" s="77"/>
-      <c r="NJ84" s="77"/>
-      <c r="NK84" s="77"/>
-      <c r="NL84" s="77"/>
-      <c r="NM84" s="77"/>
-      <c r="NN84" s="77"/>
-      <c r="NO84" s="77"/>
-      <c r="NP84" s="77"/>
-      <c r="NQ84" s="77"/>
-      <c r="NR84" s="77"/>
-      <c r="NS84" s="77"/>
-      <c r="NT84" s="77"/>
-      <c r="NU84" s="77"/>
-      <c r="NV84" s="77"/>
-      <c r="NW84" s="77"/>
-      <c r="NX84" s="77"/>
-      <c r="NY84" s="77"/>
-      <c r="NZ84" s="77"/>
-      <c r="OA84" s="77"/>
-      <c r="OB84" s="77"/>
-      <c r="OC84" s="77"/>
-      <c r="OD84" s="77"/>
-      <c r="OE84" s="77"/>
-      <c r="OF84" s="77"/>
-      <c r="OG84" s="77"/>
-      <c r="OH84" s="77"/>
-      <c r="OI84" s="77"/>
-      <c r="OJ84" s="77"/>
-      <c r="OK84" s="77"/>
-      <c r="OL84" s="77"/>
-      <c r="OM84" s="77"/>
-      <c r="ON84" s="77"/>
-      <c r="OO84" s="77"/>
-      <c r="OP84" s="77"/>
-      <c r="OQ84" s="77"/>
-      <c r="OR84" s="77"/>
-      <c r="OS84" s="77"/>
-      <c r="OT84" s="77"/>
-      <c r="OU84" s="77"/>
-      <c r="OV84" s="77"/>
-      <c r="OW84" s="77"/>
-      <c r="OX84" s="77"/>
-      <c r="OY84" s="77"/>
-      <c r="OZ84" s="77"/>
-      <c r="PA84" s="77"/>
-      <c r="PB84" s="77"/>
-      <c r="PC84" s="77"/>
-      <c r="PD84" s="77"/>
-      <c r="PE84" s="77"/>
-      <c r="PF84" s="77"/>
-      <c r="PG84" s="77"/>
-      <c r="PH84" s="77"/>
-      <c r="PI84" s="77"/>
-      <c r="PJ84" s="77"/>
-      <c r="PK84" s="77"/>
-      <c r="PL84" s="77"/>
-      <c r="PM84" s="77"/>
-      <c r="PN84" s="77"/>
-      <c r="PO84" s="77"/>
-      <c r="PP84" s="77"/>
-      <c r="PQ84" s="77"/>
-      <c r="PR84" s="77"/>
-      <c r="PS84" s="77"/>
-      <c r="PT84" s="77"/>
-      <c r="PU84" s="77"/>
-      <c r="PV84" s="77"/>
-      <c r="PW84" s="77"/>
-      <c r="PX84" s="77"/>
-      <c r="PY84" s="77"/>
-      <c r="PZ84" s="77"/>
-      <c r="QA84" s="77"/>
-      <c r="QB84" s="77"/>
-      <c r="QC84" s="77"/>
-      <c r="QD84" s="77"/>
-      <c r="QE84" s="77"/>
-      <c r="QF84" s="77"/>
-      <c r="QG84" s="77"/>
-      <c r="QH84" s="77"/>
-      <c r="QI84" s="77"/>
-      <c r="QJ84" s="77"/>
-      <c r="QK84" s="77"/>
-      <c r="QL84" s="77"/>
-      <c r="QM84" s="77"/>
-      <c r="QN84" s="77"/>
-      <c r="QO84" s="77"/>
-      <c r="QP84" s="77"/>
-      <c r="QQ84" s="77"/>
-      <c r="QR84" s="77"/>
-      <c r="QS84" s="77"/>
-      <c r="QT84" s="77"/>
-      <c r="QU84" s="77"/>
-      <c r="QV84" s="77"/>
-      <c r="QW84" s="77"/>
-      <c r="QX84" s="77"/>
-      <c r="QY84" s="77"/>
-      <c r="QZ84" s="77"/>
-      <c r="RA84" s="77"/>
-      <c r="RB84" s="77"/>
-      <c r="RC84" s="77"/>
-      <c r="RD84" s="77"/>
-      <c r="RE84" s="77"/>
-      <c r="RF84" s="77"/>
-      <c r="RG84" s="77"/>
-      <c r="RH84" s="77"/>
-      <c r="RI84" s="77"/>
-      <c r="RJ84" s="77"/>
-      <c r="RK84" s="77"/>
-      <c r="RL84" s="77"/>
-      <c r="RM84" s="77"/>
-      <c r="RN84" s="77"/>
-      <c r="RO84" s="77"/>
-      <c r="RP84" s="77"/>
-      <c r="RQ84" s="77"/>
-      <c r="RR84" s="77"/>
-      <c r="RS84" s="77"/>
-      <c r="RT84" s="77"/>
-      <c r="RU84" s="77"/>
-      <c r="RV84" s="77"/>
-      <c r="RW84" s="77"/>
-      <c r="RX84" s="77"/>
-      <c r="RY84" s="77"/>
-      <c r="RZ84" s="77"/>
-      <c r="SA84" s="77"/>
-      <c r="SB84" s="77"/>
-      <c r="SC84" s="77"/>
-      <c r="SD84" s="77"/>
-      <c r="SE84" s="77"/>
-      <c r="SF84" s="77"/>
-      <c r="SG84" s="77"/>
-      <c r="SH84" s="77"/>
-      <c r="SI84" s="77"/>
-      <c r="SJ84" s="77"/>
-      <c r="SK84" s="77"/>
-      <c r="SL84" s="77"/>
-      <c r="SM84" s="77"/>
-      <c r="SN84" s="77"/>
-      <c r="SO84" s="77"/>
-      <c r="SP84" s="77"/>
-      <c r="SQ84" s="77"/>
-      <c r="SR84" s="77"/>
-      <c r="SS84" s="77"/>
-      <c r="ST84" s="77"/>
-      <c r="SU84" s="77"/>
-      <c r="SV84" s="77"/>
-      <c r="SW84" s="77"/>
-      <c r="SX84" s="77"/>
-      <c r="SY84" s="77"/>
-      <c r="SZ84" s="77"/>
-      <c r="TA84" s="77"/>
-      <c r="TB84" s="77"/>
-      <c r="TC84" s="77"/>
-      <c r="TD84" s="77"/>
-      <c r="TE84" s="77"/>
-      <c r="TF84" s="77"/>
-      <c r="TG84" s="77"/>
-      <c r="TH84" s="77"/>
-      <c r="TI84" s="77"/>
-      <c r="TJ84" s="77"/>
-      <c r="TK84" s="77"/>
-      <c r="TL84" s="77"/>
-      <c r="TM84" s="77"/>
-      <c r="TN84" s="77"/>
-      <c r="TO84" s="77"/>
-      <c r="TP84" s="77"/>
-      <c r="TQ84" s="77"/>
-      <c r="TR84" s="77"/>
-      <c r="TS84" s="77"/>
-      <c r="TT84" s="77"/>
-      <c r="TU84" s="77"/>
-      <c r="TV84" s="77"/>
-      <c r="TW84" s="77"/>
-      <c r="TX84" s="77"/>
-      <c r="TY84" s="77"/>
-      <c r="TZ84" s="77"/>
-      <c r="UA84" s="77"/>
-      <c r="UB84" s="77"/>
-      <c r="UC84" s="77"/>
-      <c r="UD84" s="77"/>
-      <c r="UE84" s="77"/>
-      <c r="UF84" s="77"/>
-      <c r="UG84" s="77"/>
-      <c r="UH84" s="77"/>
-      <c r="UI84" s="77"/>
-      <c r="UJ84" s="77"/>
-      <c r="UK84" s="77"/>
-      <c r="UL84" s="77"/>
-      <c r="UM84" s="77"/>
-      <c r="UN84" s="77"/>
-      <c r="UO84" s="77"/>
-      <c r="UP84" s="77"/>
-      <c r="UQ84" s="77"/>
-      <c r="UR84" s="77"/>
-      <c r="US84" s="77"/>
-      <c r="UT84" s="77"/>
-      <c r="UU84" s="77"/>
-      <c r="UV84" s="77"/>
-      <c r="UW84" s="77"/>
-      <c r="UX84" s="77"/>
-      <c r="UY84" s="77"/>
-      <c r="UZ84" s="77"/>
-      <c r="VA84" s="77"/>
-      <c r="VB84" s="77"/>
-      <c r="VC84" s="77"/>
-      <c r="VD84" s="77"/>
-      <c r="VE84" s="77"/>
-      <c r="VF84" s="77"/>
-      <c r="VG84" s="77"/>
-      <c r="VH84" s="77"/>
-      <c r="VI84" s="77"/>
-      <c r="VJ84" s="77"/>
-      <c r="VK84" s="77"/>
-      <c r="VL84" s="77"/>
-      <c r="VM84" s="77"/>
-      <c r="VN84" s="77"/>
-      <c r="VO84" s="77"/>
-      <c r="VP84" s="77"/>
-      <c r="VQ84" s="77"/>
-      <c r="VR84" s="77"/>
-      <c r="VS84" s="77"/>
-      <c r="VT84" s="77"/>
-      <c r="VU84" s="77"/>
-      <c r="VV84" s="77"/>
-      <c r="VW84" s="77"/>
-      <c r="VX84" s="77"/>
-      <c r="VY84" s="77"/>
-      <c r="VZ84" s="77"/>
-      <c r="WA84" s="77"/>
-      <c r="WB84" s="77"/>
-      <c r="WC84" s="77"/>
-      <c r="WD84" s="77"/>
-      <c r="WE84" s="77"/>
-      <c r="WF84" s="77"/>
-      <c r="WG84" s="77"/>
-      <c r="WH84" s="77"/>
-      <c r="WI84" s="77"/>
-      <c r="WJ84" s="77"/>
-      <c r="WK84" s="77"/>
-      <c r="WL84" s="77"/>
-      <c r="WM84" s="77"/>
-      <c r="WN84" s="77"/>
-      <c r="WO84" s="77"/>
-      <c r="WP84" s="77"/>
-      <c r="WQ84" s="77"/>
-      <c r="WR84" s="77"/>
-      <c r="WS84" s="77"/>
-      <c r="WT84" s="77"/>
-      <c r="WU84" s="77"/>
-      <c r="WV84" s="77"/>
-      <c r="WW84" s="77"/>
-      <c r="WX84" s="77"/>
-      <c r="WY84" s="77"/>
-      <c r="WZ84" s="77"/>
-      <c r="XA84" s="77"/>
-      <c r="XB84" s="77"/>
-      <c r="XC84" s="77"/>
-      <c r="XD84" s="77"/>
-      <c r="XE84" s="77"/>
-      <c r="XF84" s="77"/>
-      <c r="XG84" s="77"/>
-      <c r="XH84" s="77"/>
-      <c r="XI84" s="77"/>
-      <c r="XJ84" s="77"/>
-      <c r="XK84" s="77"/>
-      <c r="XL84" s="77"/>
-      <c r="XM84" s="77"/>
-      <c r="XN84" s="77"/>
-      <c r="XO84" s="77"/>
-      <c r="XP84" s="77"/>
-      <c r="XQ84" s="77"/>
-      <c r="XR84" s="77"/>
-      <c r="XS84" s="77"/>
-      <c r="XT84" s="77"/>
-      <c r="XU84" s="77"/>
-      <c r="XV84" s="77"/>
-      <c r="XW84" s="77"/>
-      <c r="XX84" s="77"/>
-      <c r="XY84" s="77"/>
-      <c r="XZ84" s="77"/>
-      <c r="YA84" s="77"/>
-      <c r="YB84" s="77"/>
-      <c r="YC84" s="77"/>
-      <c r="YD84" s="77"/>
-      <c r="YE84" s="77"/>
-      <c r="YF84" s="77"/>
-      <c r="YG84" s="77"/>
-      <c r="YH84" s="77"/>
-      <c r="YI84" s="77"/>
-      <c r="YJ84" s="77"/>
-      <c r="YK84" s="77"/>
-      <c r="YL84" s="77"/>
-      <c r="YM84" s="77"/>
-      <c r="YN84" s="77"/>
-      <c r="YO84" s="77"/>
-      <c r="YP84" s="77"/>
-      <c r="YQ84" s="77"/>
-      <c r="YR84" s="77"/>
-      <c r="YS84" s="77"/>
-      <c r="YT84" s="77"/>
-      <c r="YU84" s="77"/>
-      <c r="YV84" s="77"/>
-      <c r="YW84" s="77"/>
-      <c r="YX84" s="77"/>
-      <c r="YY84" s="77"/>
-      <c r="YZ84" s="77"/>
-      <c r="ZA84" s="77"/>
-      <c r="ZB84" s="77"/>
-      <c r="ZC84" s="77"/>
-      <c r="ZD84" s="77"/>
-      <c r="ZE84" s="77"/>
-      <c r="ZF84" s="77"/>
-      <c r="ZG84" s="77"/>
-      <c r="ZH84" s="77"/>
-      <c r="ZI84" s="77"/>
-      <c r="ZJ84" s="77"/>
-      <c r="ZK84" s="77"/>
-      <c r="ZL84" s="77"/>
-      <c r="ZM84" s="77"/>
-      <c r="ZN84" s="77"/>
-      <c r="ZO84" s="77"/>
-      <c r="ZP84" s="77"/>
-      <c r="ZQ84" s="77"/>
-      <c r="ZR84" s="77"/>
-      <c r="ZS84" s="77"/>
-      <c r="ZT84" s="77"/>
-      <c r="ZU84" s="77"/>
-      <c r="ZV84" s="77"/>
-      <c r="ZW84" s="77"/>
-      <c r="ZX84" s="77"/>
-      <c r="ZY84" s="77"/>
-      <c r="ZZ84" s="77"/>
-      <c r="AAA84" s="77"/>
-      <c r="AAB84" s="77"/>
-      <c r="AAC84" s="77"/>
-      <c r="AAD84" s="77"/>
-      <c r="AAE84" s="77"/>
-      <c r="AAF84" s="77"/>
-      <c r="AAG84" s="77"/>
-      <c r="AAH84" s="77"/>
-      <c r="AAI84" s="77"/>
-      <c r="AAJ84" s="77"/>
-      <c r="AAK84" s="77"/>
-      <c r="AAL84" s="77"/>
-      <c r="AAM84" s="77"/>
-      <c r="AAN84" s="77"/>
-      <c r="AAO84" s="77"/>
-      <c r="AAP84" s="77"/>
-      <c r="AAQ84" s="77"/>
-      <c r="AAR84" s="77"/>
-      <c r="AAS84" s="77"/>
-      <c r="AAT84" s="77"/>
-      <c r="AAU84" s="77"/>
-      <c r="AAV84" s="77"/>
-      <c r="AAW84" s="77"/>
-      <c r="AAX84" s="77"/>
-      <c r="AAY84" s="77"/>
-      <c r="AAZ84" s="77"/>
-      <c r="ABA84" s="77"/>
-      <c r="ABB84" s="77"/>
-      <c r="ABC84" s="77"/>
-      <c r="ABD84" s="77"/>
-      <c r="ABE84" s="77"/>
-      <c r="ABF84" s="77"/>
-      <c r="ABG84" s="77"/>
-      <c r="ABH84" s="77"/>
-      <c r="ABI84" s="77"/>
-      <c r="ABJ84" s="77"/>
-      <c r="ABK84" s="77"/>
-      <c r="ABL84" s="77"/>
-      <c r="ABM84" s="77"/>
-      <c r="ABN84" s="77"/>
-      <c r="ABO84" s="77"/>
-      <c r="ABP84" s="77"/>
-      <c r="ABQ84" s="77"/>
-      <c r="ABR84" s="77"/>
-      <c r="ABS84" s="77"/>
-      <c r="ABT84" s="77"/>
-      <c r="ABU84" s="77"/>
-      <c r="ABV84" s="77"/>
-      <c r="ABW84" s="77"/>
-      <c r="ABX84" s="77"/>
-      <c r="ABY84" s="77"/>
-      <c r="ABZ84" s="77"/>
-      <c r="ACA84" s="77"/>
-      <c r="ACB84" s="77"/>
-      <c r="ACC84" s="77"/>
-      <c r="ACD84" s="77"/>
-      <c r="ACE84" s="77"/>
-      <c r="ACF84" s="77"/>
-      <c r="ACG84" s="77"/>
-      <c r="ACH84" s="77"/>
-      <c r="ACI84" s="77"/>
-      <c r="ACJ84" s="77"/>
-      <c r="ACK84" s="77"/>
-      <c r="ACL84" s="77"/>
-      <c r="ACM84" s="77"/>
-      <c r="ACN84" s="77"/>
-      <c r="ACO84" s="77"/>
-      <c r="ACP84" s="77"/>
-      <c r="ACQ84" s="77"/>
-      <c r="ACR84" s="77"/>
-      <c r="ACS84" s="77"/>
-      <c r="ACT84" s="77"/>
-      <c r="ACU84" s="77"/>
-      <c r="ACV84" s="77"/>
-      <c r="ACW84" s="77"/>
-      <c r="ACX84" s="77"/>
-      <c r="ACY84" s="77"/>
-      <c r="ACZ84" s="77"/>
-      <c r="ADA84" s="77"/>
-      <c r="ADB84" s="77"/>
-      <c r="ADC84" s="77"/>
-      <c r="ADD84" s="77"/>
-      <c r="ADE84" s="77"/>
-      <c r="ADF84" s="77"/>
-      <c r="ADG84" s="77"/>
-      <c r="ADH84" s="77"/>
-      <c r="ADI84" s="77"/>
-      <c r="ADJ84" s="77"/>
-      <c r="ADK84" s="77"/>
-      <c r="ADL84" s="77"/>
-      <c r="ADM84" s="77"/>
-      <c r="ADN84" s="77"/>
-      <c r="ADO84" s="77"/>
-      <c r="ADP84" s="77"/>
-      <c r="ADQ84" s="77"/>
-      <c r="ADR84" s="77"/>
-      <c r="ADS84" s="77"/>
-      <c r="ADT84" s="77"/>
-      <c r="ADU84" s="77"/>
-      <c r="ADV84" s="77"/>
-      <c r="ADW84" s="77"/>
-      <c r="ADX84" s="77"/>
-      <c r="ADY84" s="77"/>
-      <c r="ADZ84" s="77"/>
-      <c r="AEA84" s="77"/>
-      <c r="AEB84" s="77"/>
-      <c r="AEC84" s="77"/>
-      <c r="AED84" s="77"/>
-      <c r="AEE84" s="77"/>
-      <c r="AEF84" s="77"/>
-      <c r="AEG84" s="77"/>
-      <c r="AEH84" s="77"/>
-      <c r="AEI84" s="77"/>
-      <c r="AEJ84" s="77"/>
-      <c r="AEK84" s="77"/>
-      <c r="AEL84" s="77"/>
-      <c r="AEM84" s="77"/>
-      <c r="AEN84" s="77"/>
-      <c r="AEO84" s="77"/>
-      <c r="AEP84" s="77"/>
-      <c r="AEQ84" s="77"/>
-      <c r="AER84" s="77"/>
-      <c r="AES84" s="77"/>
-      <c r="AET84" s="77"/>
-      <c r="AEU84" s="77"/>
-      <c r="AEV84" s="77"/>
-      <c r="AEW84" s="77"/>
-      <c r="AEX84" s="77"/>
-      <c r="AEY84" s="77"/>
-      <c r="AEZ84" s="77"/>
-      <c r="AFA84" s="77"/>
-      <c r="AFB84" s="77"/>
-      <c r="AFC84" s="77"/>
-      <c r="AFD84" s="77"/>
-      <c r="AFE84" s="77"/>
-      <c r="AFF84" s="77"/>
-      <c r="AFG84" s="77"/>
-      <c r="AFH84" s="77"/>
-      <c r="AFI84" s="77"/>
-      <c r="AFJ84" s="77"/>
-      <c r="AFK84" s="77"/>
-      <c r="AFL84" s="77"/>
-      <c r="AFM84" s="77"/>
-      <c r="AFN84" s="77"/>
-      <c r="AFO84" s="77"/>
-      <c r="AFP84" s="77"/>
-      <c r="AFQ84" s="77"/>
-      <c r="AFR84" s="77"/>
-      <c r="AFS84" s="77"/>
-      <c r="AFT84" s="77"/>
-      <c r="AFU84" s="77"/>
-      <c r="AFV84" s="77"/>
-      <c r="AFW84" s="77"/>
-      <c r="AFX84" s="77"/>
-      <c r="AFY84" s="77"/>
-      <c r="AFZ84" s="77"/>
-      <c r="AGA84" s="77"/>
-      <c r="AGB84" s="77"/>
-      <c r="AGC84" s="77"/>
-      <c r="AGD84" s="77"/>
-      <c r="AGE84" s="77"/>
-      <c r="AGF84" s="77"/>
-      <c r="AGG84" s="77"/>
-      <c r="AGH84" s="77"/>
-      <c r="AGI84" s="77"/>
-      <c r="AGJ84" s="77"/>
-      <c r="AGK84" s="77"/>
-      <c r="AGL84" s="77"/>
-      <c r="AGM84" s="77"/>
-      <c r="AGN84" s="77"/>
-      <c r="AGO84" s="77"/>
-      <c r="AGP84" s="77"/>
-      <c r="AGQ84" s="77"/>
-      <c r="AGR84" s="77"/>
-      <c r="AGS84" s="77"/>
-      <c r="AGT84" s="77"/>
-      <c r="AGU84" s="77"/>
-      <c r="AGV84" s="77"/>
-      <c r="AGW84" s="77"/>
-      <c r="AGX84" s="77"/>
-      <c r="AGY84" s="77"/>
-      <c r="AGZ84" s="77"/>
-      <c r="AHA84" s="77"/>
-      <c r="AHB84" s="77"/>
-      <c r="AHC84" s="77"/>
-      <c r="AHD84" s="77"/>
-      <c r="AHE84" s="77"/>
-      <c r="AHF84" s="77"/>
-      <c r="AHG84" s="77"/>
-      <c r="AHH84" s="77"/>
-      <c r="AHI84" s="77"/>
-      <c r="AHJ84" s="77"/>
-      <c r="AHK84" s="77"/>
-      <c r="AHL84" s="77"/>
-      <c r="AHM84" s="77"/>
-      <c r="AHN84" s="77"/>
-      <c r="AHO84" s="77"/>
-      <c r="AHP84" s="77"/>
-      <c r="AHQ84" s="77"/>
-      <c r="AHR84" s="77"/>
-      <c r="AHS84" s="77"/>
-      <c r="AHT84" s="77"/>
-      <c r="AHU84" s="77"/>
-      <c r="AHV84" s="77"/>
-      <c r="AHW84" s="77"/>
-      <c r="AHX84" s="77"/>
-      <c r="AHY84" s="77"/>
-      <c r="AHZ84" s="77"/>
-      <c r="AIA84" s="77"/>
-      <c r="AIB84" s="77"/>
-      <c r="AIC84" s="77"/>
-      <c r="AID84" s="77"/>
-      <c r="AIE84" s="77"/>
-      <c r="AIF84" s="77"/>
-      <c r="AIG84" s="77"/>
-      <c r="AIH84" s="77"/>
-      <c r="AII84" s="77"/>
-      <c r="AIJ84" s="77"/>
-      <c r="AIK84" s="77"/>
-      <c r="AIL84" s="77"/>
-      <c r="AIM84" s="77"/>
-      <c r="AIN84" s="77"/>
-      <c r="AIO84" s="77"/>
-      <c r="AIP84" s="77"/>
-      <c r="AIQ84" s="77"/>
-      <c r="AIR84" s="77"/>
-      <c r="AIS84" s="77"/>
-      <c r="AIT84" s="77"/>
-      <c r="AIU84" s="77"/>
-      <c r="AIV84" s="77"/>
-      <c r="AIW84" s="77"/>
-      <c r="AIX84" s="77"/>
-      <c r="AIY84" s="77"/>
-      <c r="AIZ84" s="77"/>
-      <c r="AJA84" s="77"/>
-      <c r="AJB84" s="77"/>
-      <c r="AJC84" s="77"/>
-      <c r="AJD84" s="77"/>
-      <c r="AJE84" s="77"/>
-      <c r="AJF84" s="77"/>
-      <c r="AJG84" s="77"/>
-      <c r="AJH84" s="77"/>
-      <c r="AJI84" s="77"/>
-      <c r="AJJ84" s="77"/>
-      <c r="AJK84" s="77"/>
-      <c r="AJL84" s="77"/>
-      <c r="AJM84" s="77"/>
-      <c r="AJN84" s="77"/>
-      <c r="AJO84" s="77"/>
-      <c r="AJP84" s="77"/>
-      <c r="AJQ84" s="77"/>
-      <c r="AJR84" s="77"/>
-      <c r="AJS84" s="77"/>
-      <c r="AJT84" s="77"/>
-      <c r="AJU84" s="77"/>
-      <c r="AJV84" s="77"/>
-      <c r="AJW84" s="77"/>
-      <c r="AJX84" s="77"/>
-      <c r="AJY84" s="77"/>
-      <c r="AJZ84" s="77"/>
-      <c r="AKA84" s="77"/>
-      <c r="AKB84" s="77"/>
-      <c r="AKC84" s="77"/>
-      <c r="AKD84" s="77"/>
-      <c r="AKE84" s="77"/>
-      <c r="AKF84" s="77"/>
-      <c r="AKG84" s="77"/>
-      <c r="AKH84" s="77"/>
-      <c r="AKI84" s="77"/>
-      <c r="AKJ84" s="77"/>
-      <c r="AKK84" s="77"/>
-      <c r="AKL84" s="77"/>
-      <c r="AKM84" s="77"/>
-      <c r="AKN84" s="77"/>
-      <c r="AKO84" s="77"/>
-      <c r="AKP84" s="77"/>
-      <c r="AKQ84" s="77"/>
-      <c r="AKR84" s="77"/>
-      <c r="AKS84" s="77"/>
-      <c r="AKT84" s="77"/>
-      <c r="AKU84" s="77"/>
-      <c r="AKV84" s="77"/>
-      <c r="AKW84" s="77"/>
-      <c r="AKX84" s="77"/>
-      <c r="AKY84" s="77"/>
-      <c r="AKZ84" s="77"/>
-      <c r="ALA84" s="77"/>
-      <c r="ALB84" s="77"/>
-      <c r="ALC84" s="77"/>
-      <c r="ALD84" s="77"/>
-      <c r="ALE84" s="77"/>
-      <c r="ALF84" s="77"/>
-      <c r="ALG84" s="77"/>
-      <c r="ALH84" s="77"/>
-      <c r="ALI84" s="77"/>
-      <c r="ALJ84" s="77"/>
-      <c r="ALK84" s="77"/>
-      <c r="ALL84" s="77"/>
-      <c r="ALM84" s="77"/>
-      <c r="ALN84" s="77"/>
-      <c r="ALO84" s="77"/>
-      <c r="ALP84" s="77"/>
-      <c r="ALQ84" s="77"/>
-      <c r="ALR84" s="77"/>
-      <c r="ALS84" s="77"/>
-      <c r="ALT84" s="77"/>
-      <c r="ALU84" s="77"/>
-      <c r="ALV84" s="77"/>
-      <c r="ALW84" s="77"/>
-      <c r="ALX84" s="77"/>
-      <c r="ALY84" s="77"/>
-      <c r="ALZ84" s="77"/>
-      <c r="AMA84" s="77"/>
-      <c r="AMB84" s="77"/>
-      <c r="AMC84" s="77"/>
-      <c r="AMD84" s="77"/>
-      <c r="AME84" s="77"/>
-      <c r="AMF84" s="77"/>
-      <c r="AMG84" s="77"/>
-      <c r="AMH84" s="77"/>
+      <c r="I84" s="76"/>
+      <c r="J84" s="76"/>
+      <c r="K84" s="76"/>
+      <c r="L84" s="76"/>
+      <c r="M84" s="76"/>
+      <c r="N84" s="76"/>
+      <c r="O84" s="76"/>
+      <c r="P84" s="76"/>
+      <c r="Q84" s="76"/>
+      <c r="R84" s="76"/>
+      <c r="S84" s="76"/>
+      <c r="T84" s="76"/>
+      <c r="U84" s="76"/>
+      <c r="V84" s="76"/>
+      <c r="W84" s="76"/>
+      <c r="X84" s="76"/>
+      <c r="Y84" s="76"/>
+      <c r="Z84" s="76"/>
+      <c r="AA84" s="76"/>
+      <c r="AB84" s="76"/>
+      <c r="AC84" s="76"/>
+      <c r="AD84" s="76"/>
+      <c r="AE84" s="76"/>
+      <c r="AF84" s="76"/>
+      <c r="AG84" s="76"/>
+      <c r="AH84" s="76"/>
+      <c r="AI84" s="76"/>
+      <c r="AJ84" s="76"/>
+      <c r="AK84" s="76"/>
+      <c r="AL84" s="76"/>
+      <c r="AM84" s="76"/>
+      <c r="AN84" s="76"/>
+      <c r="AO84" s="76"/>
+      <c r="AP84" s="76"/>
+      <c r="AQ84" s="76"/>
+      <c r="AR84" s="76"/>
+      <c r="AS84" s="76"/>
+      <c r="AT84" s="76"/>
+      <c r="AU84" s="76"/>
+      <c r="AV84" s="76"/>
+      <c r="AW84" s="76"/>
+      <c r="AX84" s="76"/>
+      <c r="AY84" s="76"/>
+      <c r="AZ84" s="76"/>
+      <c r="BA84" s="76"/>
+      <c r="BB84" s="76"/>
+      <c r="BC84" s="76"/>
+      <c r="BD84" s="76"/>
+      <c r="BE84" s="76"/>
+      <c r="BF84" s="76"/>
+      <c r="BG84" s="76"/>
+      <c r="BH84" s="76"/>
+      <c r="BI84" s="76"/>
+      <c r="BJ84" s="76"/>
+      <c r="BK84" s="76"/>
+      <c r="BL84" s="76"/>
+      <c r="BM84" s="76"/>
+      <c r="BN84" s="76"/>
+      <c r="BO84" s="76"/>
+      <c r="BP84" s="76"/>
+      <c r="BQ84" s="76"/>
+      <c r="BR84" s="76"/>
+      <c r="BS84" s="76"/>
+      <c r="BT84" s="76"/>
+      <c r="BU84" s="76"/>
+      <c r="BV84" s="76"/>
+      <c r="BW84" s="76"/>
+      <c r="BX84" s="76"/>
+      <c r="BY84" s="76"/>
+      <c r="BZ84" s="76"/>
+      <c r="CA84" s="76"/>
+      <c r="CB84" s="76"/>
+      <c r="CC84" s="76"/>
+      <c r="CD84" s="76"/>
+      <c r="CE84" s="76"/>
+      <c r="CF84" s="76"/>
+      <c r="CG84" s="76"/>
+      <c r="CH84" s="76"/>
+      <c r="CI84" s="76"/>
+      <c r="CJ84" s="76"/>
+      <c r="CK84" s="76"/>
+      <c r="CL84" s="76"/>
+      <c r="CM84" s="76"/>
+      <c r="CN84" s="76"/>
+      <c r="CO84" s="76"/>
+      <c r="CP84" s="76"/>
+      <c r="CQ84" s="76"/>
+      <c r="CR84" s="76"/>
+      <c r="CS84" s="76"/>
+      <c r="CT84" s="76"/>
+      <c r="CU84" s="76"/>
+      <c r="CV84" s="76"/>
+      <c r="CW84" s="76"/>
+      <c r="CX84" s="76"/>
+      <c r="CY84" s="76"/>
+      <c r="CZ84" s="76"/>
+      <c r="DA84" s="76"/>
+      <c r="DB84" s="76"/>
+      <c r="DC84" s="76"/>
+      <c r="DD84" s="76"/>
+      <c r="DE84" s="76"/>
+      <c r="DF84" s="76"/>
+      <c r="DG84" s="76"/>
+      <c r="DH84" s="76"/>
+      <c r="DI84" s="76"/>
+      <c r="DJ84" s="76"/>
+      <c r="DK84" s="76"/>
+      <c r="DL84" s="76"/>
+      <c r="DM84" s="76"/>
+      <c r="DN84" s="76"/>
+      <c r="DO84" s="76"/>
+      <c r="DP84" s="76"/>
+      <c r="DQ84" s="76"/>
+      <c r="DR84" s="76"/>
+      <c r="DS84" s="76"/>
+      <c r="DT84" s="76"/>
+      <c r="DU84" s="76"/>
+      <c r="DV84" s="76"/>
+      <c r="DW84" s="76"/>
+      <c r="DX84" s="76"/>
+      <c r="DY84" s="76"/>
+      <c r="DZ84" s="76"/>
+      <c r="EA84" s="76"/>
+      <c r="EB84" s="76"/>
+      <c r="EC84" s="76"/>
+      <c r="ED84" s="76"/>
+      <c r="EE84" s="76"/>
+      <c r="EF84" s="76"/>
+      <c r="EG84" s="76"/>
+      <c r="EH84" s="76"/>
+      <c r="EI84" s="76"/>
+      <c r="EJ84" s="76"/>
+      <c r="EK84" s="76"/>
+      <c r="EL84" s="76"/>
+      <c r="EM84" s="76"/>
+      <c r="EN84" s="76"/>
+      <c r="EO84" s="76"/>
+      <c r="EP84" s="76"/>
+      <c r="EQ84" s="76"/>
+      <c r="ER84" s="76"/>
+      <c r="ES84" s="76"/>
+      <c r="ET84" s="76"/>
+      <c r="EU84" s="76"/>
+      <c r="EV84" s="76"/>
+      <c r="EW84" s="76"/>
+      <c r="EX84" s="76"/>
+      <c r="EY84" s="76"/>
+      <c r="EZ84" s="76"/>
+      <c r="FA84" s="76"/>
+      <c r="FB84" s="76"/>
+      <c r="FC84" s="76"/>
+      <c r="FD84" s="76"/>
+      <c r="FE84" s="76"/>
+      <c r="FF84" s="76"/>
+      <c r="FG84" s="76"/>
+      <c r="FH84" s="76"/>
+      <c r="FI84" s="76"/>
+      <c r="FJ84" s="76"/>
+      <c r="FK84" s="76"/>
+      <c r="FL84" s="76"/>
+      <c r="FM84" s="76"/>
+      <c r="FN84" s="76"/>
+      <c r="FO84" s="76"/>
+      <c r="FP84" s="76"/>
+      <c r="FQ84" s="76"/>
+      <c r="FR84" s="76"/>
+      <c r="FS84" s="76"/>
+      <c r="FT84" s="76"/>
+      <c r="FU84" s="76"/>
+      <c r="FV84" s="76"/>
+      <c r="FW84" s="76"/>
+      <c r="FX84" s="76"/>
+      <c r="FY84" s="76"/>
+      <c r="FZ84" s="76"/>
+      <c r="GA84" s="76"/>
+      <c r="GB84" s="76"/>
+      <c r="GC84" s="76"/>
+      <c r="GD84" s="76"/>
+      <c r="GE84" s="76"/>
+      <c r="GF84" s="76"/>
+      <c r="GG84" s="76"/>
+      <c r="GH84" s="76"/>
+      <c r="GI84" s="76"/>
+      <c r="GJ84" s="76"/>
+      <c r="GK84" s="76"/>
+      <c r="GL84" s="76"/>
+      <c r="GM84" s="76"/>
+      <c r="GN84" s="76"/>
+      <c r="GO84" s="76"/>
+      <c r="GP84" s="76"/>
+      <c r="GQ84" s="76"/>
+      <c r="GR84" s="76"/>
+      <c r="GS84" s="76"/>
+      <c r="GT84" s="76"/>
+      <c r="GU84" s="76"/>
+      <c r="GV84" s="76"/>
+      <c r="GW84" s="76"/>
+      <c r="GX84" s="76"/>
+      <c r="GY84" s="76"/>
+      <c r="GZ84" s="76"/>
+      <c r="HA84" s="76"/>
+      <c r="HB84" s="76"/>
+      <c r="HC84" s="76"/>
+      <c r="HD84" s="76"/>
+      <c r="HE84" s="76"/>
+      <c r="HF84" s="76"/>
+      <c r="HG84" s="76"/>
+      <c r="HH84" s="76"/>
+      <c r="HI84" s="76"/>
+      <c r="HJ84" s="76"/>
+      <c r="HK84" s="76"/>
+      <c r="HL84" s="76"/>
+      <c r="HM84" s="76"/>
+      <c r="HN84" s="76"/>
+      <c r="HO84" s="76"/>
+      <c r="HP84" s="76"/>
+      <c r="HQ84" s="76"/>
+      <c r="HR84" s="76"/>
+      <c r="HS84" s="76"/>
+      <c r="HT84" s="76"/>
+      <c r="HU84" s="76"/>
+      <c r="HV84" s="76"/>
+      <c r="HW84" s="76"/>
+      <c r="HX84" s="76"/>
+      <c r="HY84" s="76"/>
+      <c r="HZ84" s="76"/>
+      <c r="IA84" s="76"/>
+      <c r="IB84" s="76"/>
+      <c r="IC84" s="76"/>
+      <c r="ID84" s="76"/>
+      <c r="IE84" s="76"/>
+      <c r="IF84" s="76"/>
+      <c r="IG84" s="76"/>
+      <c r="IH84" s="76"/>
+      <c r="II84" s="76"/>
+      <c r="IJ84" s="76"/>
+      <c r="IK84" s="76"/>
+      <c r="IL84" s="76"/>
+      <c r="IM84" s="76"/>
+      <c r="IN84" s="76"/>
+      <c r="IO84" s="76"/>
+      <c r="IP84" s="76"/>
+      <c r="IQ84" s="76"/>
+      <c r="IR84" s="76"/>
+      <c r="IS84" s="76"/>
+      <c r="IT84" s="76"/>
+      <c r="IU84" s="76"/>
+      <c r="IV84" s="76"/>
+      <c r="IW84" s="76"/>
+      <c r="IX84" s="76"/>
+      <c r="IY84" s="76"/>
+      <c r="IZ84" s="76"/>
+      <c r="JA84" s="76"/>
+      <c r="JB84" s="76"/>
+      <c r="JC84" s="76"/>
+      <c r="JD84" s="76"/>
+      <c r="JE84" s="76"/>
+      <c r="JF84" s="76"/>
+      <c r="JG84" s="76"/>
+      <c r="JH84" s="76"/>
+      <c r="JI84" s="76"/>
+      <c r="JJ84" s="76"/>
+      <c r="JK84" s="76"/>
+      <c r="JL84" s="76"/>
+      <c r="JM84" s="76"/>
+      <c r="JN84" s="76"/>
+      <c r="JO84" s="76"/>
+      <c r="JP84" s="76"/>
+      <c r="JQ84" s="76"/>
+      <c r="JR84" s="76"/>
+      <c r="JS84" s="76"/>
+      <c r="JT84" s="76"/>
+      <c r="JU84" s="76"/>
+      <c r="JV84" s="76"/>
+      <c r="JW84" s="76"/>
+      <c r="JX84" s="76"/>
+      <c r="JY84" s="76"/>
+      <c r="JZ84" s="76"/>
+      <c r="KA84" s="76"/>
+      <c r="KB84" s="76"/>
+      <c r="KC84" s="76"/>
+      <c r="KD84" s="76"/>
+      <c r="KE84" s="76"/>
+      <c r="KF84" s="76"/>
+      <c r="KG84" s="76"/>
+      <c r="KH84" s="76"/>
+      <c r="KI84" s="76"/>
+      <c r="KJ84" s="76"/>
+      <c r="KK84" s="76"/>
+      <c r="KL84" s="76"/>
+      <c r="KM84" s="76"/>
+      <c r="KN84" s="76"/>
+      <c r="KO84" s="76"/>
+      <c r="KP84" s="76"/>
+      <c r="KQ84" s="76"/>
+      <c r="KR84" s="76"/>
+      <c r="KS84" s="76"/>
+      <c r="KT84" s="76"/>
+      <c r="KU84" s="76"/>
+      <c r="KV84" s="76"/>
+      <c r="KW84" s="76"/>
+      <c r="KX84" s="76"/>
+      <c r="KY84" s="76"/>
+      <c r="KZ84" s="76"/>
+      <c r="LA84" s="76"/>
+      <c r="LB84" s="76"/>
+      <c r="LC84" s="76"/>
+      <c r="LD84" s="76"/>
+      <c r="LE84" s="76"/>
+      <c r="LF84" s="76"/>
+      <c r="LG84" s="76"/>
+      <c r="LH84" s="76"/>
+      <c r="LI84" s="76"/>
+      <c r="LJ84" s="76"/>
+      <c r="LK84" s="76"/>
+      <c r="LL84" s="76"/>
+      <c r="LM84" s="76"/>
+      <c r="LN84" s="76"/>
+      <c r="LO84" s="76"/>
+      <c r="LP84" s="76"/>
+      <c r="LQ84" s="76"/>
+      <c r="LR84" s="76"/>
+      <c r="LS84" s="76"/>
+      <c r="LT84" s="76"/>
+      <c r="LU84" s="76"/>
+      <c r="LV84" s="76"/>
+      <c r="LW84" s="76"/>
+      <c r="LX84" s="76"/>
+      <c r="LY84" s="76"/>
+      <c r="LZ84" s="76"/>
+      <c r="MA84" s="76"/>
+      <c r="MB84" s="76"/>
+      <c r="MC84" s="76"/>
+      <c r="MD84" s="76"/>
+      <c r="ME84" s="76"/>
+      <c r="MF84" s="76"/>
+      <c r="MG84" s="76"/>
+      <c r="MH84" s="76"/>
+      <c r="MI84" s="76"/>
+      <c r="MJ84" s="76"/>
+      <c r="MK84" s="76"/>
+      <c r="ML84" s="76"/>
+      <c r="MM84" s="76"/>
+      <c r="MN84" s="76"/>
+      <c r="MO84" s="76"/>
+      <c r="MP84" s="76"/>
+      <c r="MQ84" s="76"/>
+      <c r="MR84" s="76"/>
+      <c r="MS84" s="76"/>
+      <c r="MT84" s="76"/>
+      <c r="MU84" s="76"/>
+      <c r="MV84" s="76"/>
+      <c r="MW84" s="76"/>
+      <c r="MX84" s="76"/>
+      <c r="MY84" s="76"/>
+      <c r="MZ84" s="76"/>
+      <c r="NA84" s="76"/>
+      <c r="NB84" s="76"/>
+      <c r="NC84" s="76"/>
+      <c r="ND84" s="76"/>
+      <c r="NE84" s="76"/>
+      <c r="NF84" s="76"/>
+      <c r="NG84" s="76"/>
+      <c r="NH84" s="76"/>
+      <c r="NI84" s="76"/>
+      <c r="NJ84" s="76"/>
+      <c r="NK84" s="76"/>
+      <c r="NL84" s="76"/>
+      <c r="NM84" s="76"/>
+      <c r="NN84" s="76"/>
+      <c r="NO84" s="76"/>
+      <c r="NP84" s="76"/>
+      <c r="NQ84" s="76"/>
+      <c r="NR84" s="76"/>
+      <c r="NS84" s="76"/>
+      <c r="NT84" s="76"/>
+      <c r="NU84" s="76"/>
+      <c r="NV84" s="76"/>
+      <c r="NW84" s="76"/>
+      <c r="NX84" s="76"/>
+      <c r="NY84" s="76"/>
+      <c r="NZ84" s="76"/>
+      <c r="OA84" s="76"/>
+      <c r="OB84" s="76"/>
+      <c r="OC84" s="76"/>
+      <c r="OD84" s="76"/>
+      <c r="OE84" s="76"/>
+      <c r="OF84" s="76"/>
+      <c r="OG84" s="76"/>
+      <c r="OH84" s="76"/>
+      <c r="OI84" s="76"/>
+      <c r="OJ84" s="76"/>
+      <c r="OK84" s="76"/>
+      <c r="OL84" s="76"/>
+      <c r="OM84" s="76"/>
+      <c r="ON84" s="76"/>
+      <c r="OO84" s="76"/>
+      <c r="OP84" s="76"/>
+      <c r="OQ84" s="76"/>
+      <c r="OR84" s="76"/>
+      <c r="OS84" s="76"/>
+      <c r="OT84" s="76"/>
+      <c r="OU84" s="76"/>
+      <c r="OV84" s="76"/>
+      <c r="OW84" s="76"/>
+      <c r="OX84" s="76"/>
+      <c r="OY84" s="76"/>
+      <c r="OZ84" s="76"/>
+      <c r="PA84" s="76"/>
+      <c r="PB84" s="76"/>
+      <c r="PC84" s="76"/>
+      <c r="PD84" s="76"/>
+      <c r="PE84" s="76"/>
+      <c r="PF84" s="76"/>
+      <c r="PG84" s="76"/>
+      <c r="PH84" s="76"/>
+      <c r="PI84" s="76"/>
+      <c r="PJ84" s="76"/>
+      <c r="PK84" s="76"/>
+      <c r="PL84" s="76"/>
+      <c r="PM84" s="76"/>
+      <c r="PN84" s="76"/>
+      <c r="PO84" s="76"/>
+      <c r="PP84" s="76"/>
+      <c r="PQ84" s="76"/>
+      <c r="PR84" s="76"/>
+      <c r="PS84" s="76"/>
+      <c r="PT84" s="76"/>
+      <c r="PU84" s="76"/>
+      <c r="PV84" s="76"/>
+      <c r="PW84" s="76"/>
+      <c r="PX84" s="76"/>
+      <c r="PY84" s="76"/>
+      <c r="PZ84" s="76"/>
+      <c r="QA84" s="76"/>
+      <c r="QB84" s="76"/>
+      <c r="QC84" s="76"/>
+      <c r="QD84" s="76"/>
+      <c r="QE84" s="76"/>
+      <c r="QF84" s="76"/>
+      <c r="QG84" s="76"/>
+      <c r="QH84" s="76"/>
+      <c r="QI84" s="76"/>
+      <c r="QJ84" s="76"/>
+      <c r="QK84" s="76"/>
+      <c r="QL84" s="76"/>
+      <c r="QM84" s="76"/>
+      <c r="QN84" s="76"/>
+      <c r="QO84" s="76"/>
+      <c r="QP84" s="76"/>
+      <c r="QQ84" s="76"/>
+      <c r="QR84" s="76"/>
+      <c r="QS84" s="76"/>
+      <c r="QT84" s="76"/>
+      <c r="QU84" s="76"/>
+      <c r="QV84" s="76"/>
+      <c r="QW84" s="76"/>
+      <c r="QX84" s="76"/>
+      <c r="QY84" s="76"/>
+      <c r="QZ84" s="76"/>
+      <c r="RA84" s="76"/>
+      <c r="RB84" s="76"/>
+      <c r="RC84" s="76"/>
+      <c r="RD84" s="76"/>
+      <c r="RE84" s="76"/>
+      <c r="RF84" s="76"/>
+      <c r="RG84" s="76"/>
+      <c r="RH84" s="76"/>
+      <c r="RI84" s="76"/>
+      <c r="RJ84" s="76"/>
+      <c r="RK84" s="76"/>
+      <c r="RL84" s="76"/>
+      <c r="RM84" s="76"/>
+      <c r="RN84" s="76"/>
+      <c r="RO84" s="76"/>
+      <c r="RP84" s="76"/>
+      <c r="RQ84" s="76"/>
+      <c r="RR84" s="76"/>
+      <c r="RS84" s="76"/>
+      <c r="RT84" s="76"/>
+      <c r="RU84" s="76"/>
+      <c r="RV84" s="76"/>
+      <c r="RW84" s="76"/>
+      <c r="RX84" s="76"/>
+      <c r="RY84" s="76"/>
+      <c r="RZ84" s="76"/>
+      <c r="SA84" s="76"/>
+      <c r="SB84" s="76"/>
+      <c r="SC84" s="76"/>
+      <c r="SD84" s="76"/>
+      <c r="SE84" s="76"/>
+      <c r="SF84" s="76"/>
+      <c r="SG84" s="76"/>
+      <c r="SH84" s="76"/>
+      <c r="SI84" s="76"/>
+      <c r="SJ84" s="76"/>
+      <c r="SK84" s="76"/>
+      <c r="SL84" s="76"/>
+      <c r="SM84" s="76"/>
+      <c r="SN84" s="76"/>
+      <c r="SO84" s="76"/>
+      <c r="SP84" s="76"/>
+      <c r="SQ84" s="76"/>
+      <c r="SR84" s="76"/>
+      <c r="SS84" s="76"/>
+      <c r="ST84" s="76"/>
+      <c r="SU84" s="76"/>
+      <c r="SV84" s="76"/>
+      <c r="SW84" s="76"/>
+      <c r="SX84" s="76"/>
+      <c r="SY84" s="76"/>
+      <c r="SZ84" s="76"/>
+      <c r="TA84" s="76"/>
+      <c r="TB84" s="76"/>
+      <c r="TC84" s="76"/>
+      <c r="TD84" s="76"/>
+      <c r="TE84" s="76"/>
+      <c r="TF84" s="76"/>
+      <c r="TG84" s="76"/>
+      <c r="TH84" s="76"/>
+      <c r="TI84" s="76"/>
+      <c r="TJ84" s="76"/>
+      <c r="TK84" s="76"/>
+      <c r="TL84" s="76"/>
+      <c r="TM84" s="76"/>
+      <c r="TN84" s="76"/>
+      <c r="TO84" s="76"/>
+      <c r="TP84" s="76"/>
+      <c r="TQ84" s="76"/>
+      <c r="TR84" s="76"/>
+      <c r="TS84" s="76"/>
+      <c r="TT84" s="76"/>
+      <c r="TU84" s="76"/>
+      <c r="TV84" s="76"/>
+      <c r="TW84" s="76"/>
+      <c r="TX84" s="76"/>
+      <c r="TY84" s="76"/>
+      <c r="TZ84" s="76"/>
+      <c r="UA84" s="76"/>
+      <c r="UB84" s="76"/>
+      <c r="UC84" s="76"/>
+      <c r="UD84" s="76"/>
+      <c r="UE84" s="76"/>
+      <c r="UF84" s="76"/>
+      <c r="UG84" s="76"/>
+      <c r="UH84" s="76"/>
+      <c r="UI84" s="76"/>
+      <c r="UJ84" s="76"/>
+      <c r="UK84" s="76"/>
+      <c r="UL84" s="76"/>
+      <c r="UM84" s="76"/>
+      <c r="UN84" s="76"/>
+      <c r="UO84" s="76"/>
+      <c r="UP84" s="76"/>
+      <c r="UQ84" s="76"/>
+      <c r="UR84" s="76"/>
+      <c r="US84" s="76"/>
+      <c r="UT84" s="76"/>
+      <c r="UU84" s="76"/>
+      <c r="UV84" s="76"/>
+      <c r="UW84" s="76"/>
+      <c r="UX84" s="76"/>
+      <c r="UY84" s="76"/>
+      <c r="UZ84" s="76"/>
+      <c r="VA84" s="76"/>
+      <c r="VB84" s="76"/>
+      <c r="VC84" s="76"/>
+      <c r="VD84" s="76"/>
+      <c r="VE84" s="76"/>
+      <c r="VF84" s="76"/>
+      <c r="VG84" s="76"/>
+      <c r="VH84" s="76"/>
+      <c r="VI84" s="76"/>
+      <c r="VJ84" s="76"/>
+      <c r="VK84" s="76"/>
+      <c r="VL84" s="76"/>
+      <c r="VM84" s="76"/>
+      <c r="VN84" s="76"/>
+      <c r="VO84" s="76"/>
+      <c r="VP84" s="76"/>
+      <c r="VQ84" s="76"/>
+      <c r="VR84" s="76"/>
+      <c r="VS84" s="76"/>
+      <c r="VT84" s="76"/>
+      <c r="VU84" s="76"/>
+      <c r="VV84" s="76"/>
+      <c r="VW84" s="76"/>
+      <c r="VX84" s="76"/>
+      <c r="VY84" s="76"/>
+      <c r="VZ84" s="76"/>
+      <c r="WA84" s="76"/>
+      <c r="WB84" s="76"/>
+      <c r="WC84" s="76"/>
+      <c r="WD84" s="76"/>
+      <c r="WE84" s="76"/>
+      <c r="WF84" s="76"/>
+      <c r="WG84" s="76"/>
+      <c r="WH84" s="76"/>
+      <c r="WI84" s="76"/>
+      <c r="WJ84" s="76"/>
+      <c r="WK84" s="76"/>
+      <c r="WL84" s="76"/>
+      <c r="WM84" s="76"/>
+      <c r="WN84" s="76"/>
+      <c r="WO84" s="76"/>
+      <c r="WP84" s="76"/>
+      <c r="WQ84" s="76"/>
+      <c r="WR84" s="76"/>
+      <c r="WS84" s="76"/>
+      <c r="WT84" s="76"/>
+      <c r="WU84" s="76"/>
+      <c r="WV84" s="76"/>
+      <c r="WW84" s="76"/>
+      <c r="WX84" s="76"/>
+      <c r="WY84" s="76"/>
+      <c r="WZ84" s="76"/>
+      <c r="XA84" s="76"/>
+      <c r="XB84" s="76"/>
+      <c r="XC84" s="76"/>
+      <c r="XD84" s="76"/>
+      <c r="XE84" s="76"/>
+      <c r="XF84" s="76"/>
+      <c r="XG84" s="76"/>
+      <c r="XH84" s="76"/>
+      <c r="XI84" s="76"/>
+      <c r="XJ84" s="76"/>
+      <c r="XK84" s="76"/>
+      <c r="XL84" s="76"/>
+      <c r="XM84" s="76"/>
+      <c r="XN84" s="76"/>
+      <c r="XO84" s="76"/>
+      <c r="XP84" s="76"/>
+      <c r="XQ84" s="76"/>
+      <c r="XR84" s="76"/>
+      <c r="XS84" s="76"/>
+      <c r="XT84" s="76"/>
+      <c r="XU84" s="76"/>
+      <c r="XV84" s="76"/>
+      <c r="XW84" s="76"/>
+      <c r="XX84" s="76"/>
+      <c r="XY84" s="76"/>
+      <c r="XZ84" s="76"/>
+      <c r="YA84" s="76"/>
+      <c r="YB84" s="76"/>
+      <c r="YC84" s="76"/>
+      <c r="YD84" s="76"/>
+      <c r="YE84" s="76"/>
+      <c r="YF84" s="76"/>
+      <c r="YG84" s="76"/>
+      <c r="YH84" s="76"/>
+      <c r="YI84" s="76"/>
+      <c r="YJ84" s="76"/>
+      <c r="YK84" s="76"/>
+      <c r="YL84" s="76"/>
+      <c r="YM84" s="76"/>
+      <c r="YN84" s="76"/>
+      <c r="YO84" s="76"/>
+      <c r="YP84" s="76"/>
+      <c r="YQ84" s="76"/>
+      <c r="YR84" s="76"/>
+      <c r="YS84" s="76"/>
+      <c r="YT84" s="76"/>
+      <c r="YU84" s="76"/>
+      <c r="YV84" s="76"/>
+      <c r="YW84" s="76"/>
+      <c r="YX84" s="76"/>
+      <c r="YY84" s="76"/>
+      <c r="YZ84" s="76"/>
+      <c r="ZA84" s="76"/>
+      <c r="ZB84" s="76"/>
+      <c r="ZC84" s="76"/>
+      <c r="ZD84" s="76"/>
+      <c r="ZE84" s="76"/>
+      <c r="ZF84" s="76"/>
+      <c r="ZG84" s="76"/>
+      <c r="ZH84" s="76"/>
+      <c r="ZI84" s="76"/>
+      <c r="ZJ84" s="76"/>
+      <c r="ZK84" s="76"/>
+      <c r="ZL84" s="76"/>
+      <c r="ZM84" s="76"/>
+      <c r="ZN84" s="76"/>
+      <c r="ZO84" s="76"/>
+      <c r="ZP84" s="76"/>
+      <c r="ZQ84" s="76"/>
+      <c r="ZR84" s="76"/>
+      <c r="ZS84" s="76"/>
+      <c r="ZT84" s="76"/>
+      <c r="ZU84" s="76"/>
+      <c r="ZV84" s="76"/>
+      <c r="ZW84" s="76"/>
+      <c r="ZX84" s="76"/>
+      <c r="ZY84" s="76"/>
+      <c r="ZZ84" s="76"/>
+      <c r="AAA84" s="76"/>
+      <c r="AAB84" s="76"/>
+      <c r="AAC84" s="76"/>
+      <c r="AAD84" s="76"/>
+      <c r="AAE84" s="76"/>
+      <c r="AAF84" s="76"/>
+      <c r="AAG84" s="76"/>
+      <c r="AAH84" s="76"/>
+      <c r="AAI84" s="76"/>
+      <c r="AAJ84" s="76"/>
+      <c r="AAK84" s="76"/>
+      <c r="AAL84" s="76"/>
+      <c r="AAM84" s="76"/>
+      <c r="AAN84" s="76"/>
+      <c r="AAO84" s="76"/>
+      <c r="AAP84" s="76"/>
+      <c r="AAQ84" s="76"/>
+      <c r="AAR84" s="76"/>
+      <c r="AAS84" s="76"/>
+      <c r="AAT84" s="76"/>
+      <c r="AAU84" s="76"/>
+      <c r="AAV84" s="76"/>
+      <c r="AAW84" s="76"/>
+      <c r="AAX84" s="76"/>
+      <c r="AAY84" s="76"/>
+      <c r="AAZ84" s="76"/>
+      <c r="ABA84" s="76"/>
+      <c r="ABB84" s="76"/>
+      <c r="ABC84" s="76"/>
+      <c r="ABD84" s="76"/>
+      <c r="ABE84" s="76"/>
+      <c r="ABF84" s="76"/>
+      <c r="ABG84" s="76"/>
+      <c r="ABH84" s="76"/>
+      <c r="ABI84" s="76"/>
+      <c r="ABJ84" s="76"/>
+      <c r="ABK84" s="76"/>
+      <c r="ABL84" s="76"/>
+      <c r="ABM84" s="76"/>
+      <c r="ABN84" s="76"/>
+      <c r="ABO84" s="76"/>
+      <c r="ABP84" s="76"/>
+      <c r="ABQ84" s="76"/>
+      <c r="ABR84" s="76"/>
+      <c r="ABS84" s="76"/>
+      <c r="ABT84" s="76"/>
+      <c r="ABU84" s="76"/>
+      <c r="ABV84" s="76"/>
+      <c r="ABW84" s="76"/>
+      <c r="ABX84" s="76"/>
+      <c r="ABY84" s="76"/>
+      <c r="ABZ84" s="76"/>
+      <c r="ACA84" s="76"/>
+      <c r="ACB84" s="76"/>
+      <c r="ACC84" s="76"/>
+      <c r="ACD84" s="76"/>
+      <c r="ACE84" s="76"/>
+      <c r="ACF84" s="76"/>
+      <c r="ACG84" s="76"/>
+      <c r="ACH84" s="76"/>
+      <c r="ACI84" s="76"/>
+      <c r="ACJ84" s="76"/>
+      <c r="ACK84" s="76"/>
+      <c r="ACL84" s="76"/>
+      <c r="ACM84" s="76"/>
+      <c r="ACN84" s="76"/>
+      <c r="ACO84" s="76"/>
+      <c r="ACP84" s="76"/>
+      <c r="ACQ84" s="76"/>
+      <c r="ACR84" s="76"/>
+      <c r="ACS84" s="76"/>
+      <c r="ACT84" s="76"/>
+      <c r="ACU84" s="76"/>
+      <c r="ACV84" s="76"/>
+      <c r="ACW84" s="76"/>
+      <c r="ACX84" s="76"/>
+      <c r="ACY84" s="76"/>
+      <c r="ACZ84" s="76"/>
+      <c r="ADA84" s="76"/>
+      <c r="ADB84" s="76"/>
+      <c r="ADC84" s="76"/>
+      <c r="ADD84" s="76"/>
+      <c r="ADE84" s="76"/>
+      <c r="ADF84" s="76"/>
+      <c r="ADG84" s="76"/>
+      <c r="ADH84" s="76"/>
+      <c r="ADI84" s="76"/>
+      <c r="ADJ84" s="76"/>
+      <c r="ADK84" s="76"/>
+      <c r="ADL84" s="76"/>
+      <c r="ADM84" s="76"/>
+      <c r="ADN84" s="76"/>
+      <c r="ADO84" s="76"/>
+      <c r="ADP84" s="76"/>
+      <c r="ADQ84" s="76"/>
+      <c r="ADR84" s="76"/>
+      <c r="ADS84" s="76"/>
+      <c r="ADT84" s="76"/>
+      <c r="ADU84" s="76"/>
+      <c r="ADV84" s="76"/>
+      <c r="ADW84" s="76"/>
+      <c r="ADX84" s="76"/>
+      <c r="ADY84" s="76"/>
+      <c r="ADZ84" s="76"/>
+      <c r="AEA84" s="76"/>
+      <c r="AEB84" s="76"/>
+      <c r="AEC84" s="76"/>
+      <c r="AED84" s="76"/>
+      <c r="AEE84" s="76"/>
+      <c r="AEF84" s="76"/>
+      <c r="AEG84" s="76"/>
+      <c r="AEH84" s="76"/>
+      <c r="AEI84" s="76"/>
+      <c r="AEJ84" s="76"/>
+      <c r="AEK84" s="76"/>
+      <c r="AEL84" s="76"/>
+      <c r="AEM84" s="76"/>
+      <c r="AEN84" s="76"/>
+      <c r="AEO84" s="76"/>
+      <c r="AEP84" s="76"/>
+      <c r="AEQ84" s="76"/>
+      <c r="AER84" s="76"/>
+      <c r="AES84" s="76"/>
+      <c r="AET84" s="76"/>
+      <c r="AEU84" s="76"/>
+      <c r="AEV84" s="76"/>
+      <c r="AEW84" s="76"/>
+      <c r="AEX84" s="76"/>
+      <c r="AEY84" s="76"/>
+      <c r="AEZ84" s="76"/>
+      <c r="AFA84" s="76"/>
+      <c r="AFB84" s="76"/>
+      <c r="AFC84" s="76"/>
+      <c r="AFD84" s="76"/>
+      <c r="AFE84" s="76"/>
+      <c r="AFF84" s="76"/>
+      <c r="AFG84" s="76"/>
+      <c r="AFH84" s="76"/>
+      <c r="AFI84" s="76"/>
+      <c r="AFJ84" s="76"/>
+      <c r="AFK84" s="76"/>
+      <c r="AFL84" s="76"/>
+      <c r="AFM84" s="76"/>
+      <c r="AFN84" s="76"/>
+      <c r="AFO84" s="76"/>
+      <c r="AFP84" s="76"/>
+      <c r="AFQ84" s="76"/>
+      <c r="AFR84" s="76"/>
+      <c r="AFS84" s="76"/>
+      <c r="AFT84" s="76"/>
+      <c r="AFU84" s="76"/>
+      <c r="AFV84" s="76"/>
+      <c r="AFW84" s="76"/>
+      <c r="AFX84" s="76"/>
+      <c r="AFY84" s="76"/>
+      <c r="AFZ84" s="76"/>
+      <c r="AGA84" s="76"/>
+      <c r="AGB84" s="76"/>
+      <c r="AGC84" s="76"/>
+      <c r="AGD84" s="76"/>
+      <c r="AGE84" s="76"/>
+      <c r="AGF84" s="76"/>
+      <c r="AGG84" s="76"/>
+      <c r="AGH84" s="76"/>
+      <c r="AGI84" s="76"/>
+      <c r="AGJ84" s="76"/>
+      <c r="AGK84" s="76"/>
+      <c r="AGL84" s="76"/>
+      <c r="AGM84" s="76"/>
+      <c r="AGN84" s="76"/>
+      <c r="AGO84" s="76"/>
+      <c r="AGP84" s="76"/>
+      <c r="AGQ84" s="76"/>
+      <c r="AGR84" s="76"/>
+      <c r="AGS84" s="76"/>
+      <c r="AGT84" s="76"/>
+      <c r="AGU84" s="76"/>
+      <c r="AGV84" s="76"/>
+      <c r="AGW84" s="76"/>
+      <c r="AGX84" s="76"/>
+      <c r="AGY84" s="76"/>
+      <c r="AGZ84" s="76"/>
+      <c r="AHA84" s="76"/>
+      <c r="AHB84" s="76"/>
+      <c r="AHC84" s="76"/>
+      <c r="AHD84" s="76"/>
+      <c r="AHE84" s="76"/>
+      <c r="AHF84" s="76"/>
+      <c r="AHG84" s="76"/>
+      <c r="AHH84" s="76"/>
+      <c r="AHI84" s="76"/>
+      <c r="AHJ84" s="76"/>
+      <c r="AHK84" s="76"/>
+      <c r="AHL84" s="76"/>
+      <c r="AHM84" s="76"/>
+      <c r="AHN84" s="76"/>
+      <c r="AHO84" s="76"/>
+      <c r="AHP84" s="76"/>
+      <c r="AHQ84" s="76"/>
+      <c r="AHR84" s="76"/>
+      <c r="AHS84" s="76"/>
+      <c r="AHT84" s="76"/>
+      <c r="AHU84" s="76"/>
+      <c r="AHV84" s="76"/>
+      <c r="AHW84" s="76"/>
+      <c r="AHX84" s="76"/>
+      <c r="AHY84" s="76"/>
+      <c r="AHZ84" s="76"/>
+      <c r="AIA84" s="76"/>
+      <c r="AIB84" s="76"/>
+      <c r="AIC84" s="76"/>
+      <c r="AID84" s="76"/>
+      <c r="AIE84" s="76"/>
+      <c r="AIF84" s="76"/>
+      <c r="AIG84" s="76"/>
+      <c r="AIH84" s="76"/>
+      <c r="AII84" s="76"/>
+      <c r="AIJ84" s="76"/>
+      <c r="AIK84" s="76"/>
+      <c r="AIL84" s="76"/>
+      <c r="AIM84" s="76"/>
+      <c r="AIN84" s="76"/>
+      <c r="AIO84" s="76"/>
+      <c r="AIP84" s="76"/>
+      <c r="AIQ84" s="76"/>
+      <c r="AIR84" s="76"/>
+      <c r="AIS84" s="76"/>
+      <c r="AIT84" s="76"/>
+      <c r="AIU84" s="76"/>
+      <c r="AIV84" s="76"/>
+      <c r="AIW84" s="76"/>
+      <c r="AIX84" s="76"/>
+      <c r="AIY84" s="76"/>
+      <c r="AIZ84" s="76"/>
+      <c r="AJA84" s="76"/>
+      <c r="AJB84" s="76"/>
+      <c r="AJC84" s="76"/>
+      <c r="AJD84" s="76"/>
+      <c r="AJE84" s="76"/>
+      <c r="AJF84" s="76"/>
+      <c r="AJG84" s="76"/>
+      <c r="AJH84" s="76"/>
+      <c r="AJI84" s="76"/>
+      <c r="AJJ84" s="76"/>
+      <c r="AJK84" s="76"/>
+      <c r="AJL84" s="76"/>
+      <c r="AJM84" s="76"/>
+      <c r="AJN84" s="76"/>
+      <c r="AJO84" s="76"/>
+      <c r="AJP84" s="76"/>
+      <c r="AJQ84" s="76"/>
+      <c r="AJR84" s="76"/>
+      <c r="AJS84" s="76"/>
+      <c r="AJT84" s="76"/>
+      <c r="AJU84" s="76"/>
+      <c r="AJV84" s="76"/>
+      <c r="AJW84" s="76"/>
+      <c r="AJX84" s="76"/>
+      <c r="AJY84" s="76"/>
+      <c r="AJZ84" s="76"/>
+      <c r="AKA84" s="76"/>
+      <c r="AKB84" s="76"/>
+      <c r="AKC84" s="76"/>
+      <c r="AKD84" s="76"/>
+      <c r="AKE84" s="76"/>
+      <c r="AKF84" s="76"/>
+      <c r="AKG84" s="76"/>
+      <c r="AKH84" s="76"/>
+      <c r="AKI84" s="76"/>
+      <c r="AKJ84" s="76"/>
+      <c r="AKK84" s="76"/>
+      <c r="AKL84" s="76"/>
+      <c r="AKM84" s="76"/>
+      <c r="AKN84" s="76"/>
+      <c r="AKO84" s="76"/>
+      <c r="AKP84" s="76"/>
+      <c r="AKQ84" s="76"/>
+      <c r="AKR84" s="76"/>
+      <c r="AKS84" s="76"/>
+      <c r="AKT84" s="76"/>
+      <c r="AKU84" s="76"/>
+      <c r="AKV84" s="76"/>
+      <c r="AKW84" s="76"/>
+      <c r="AKX84" s="76"/>
+      <c r="AKY84" s="76"/>
+      <c r="AKZ84" s="76"/>
+      <c r="ALA84" s="76"/>
+      <c r="ALB84" s="76"/>
+      <c r="ALC84" s="76"/>
+      <c r="ALD84" s="76"/>
+      <c r="ALE84" s="76"/>
+      <c r="ALF84" s="76"/>
+      <c r="ALG84" s="76"/>
+      <c r="ALH84" s="76"/>
+      <c r="ALI84" s="76"/>
+      <c r="ALJ84" s="76"/>
+      <c r="ALK84" s="76"/>
+      <c r="ALL84" s="76"/>
+      <c r="ALM84" s="76"/>
+      <c r="ALN84" s="76"/>
+      <c r="ALO84" s="76"/>
+      <c r="ALP84" s="76"/>
+      <c r="ALQ84" s="76"/>
+      <c r="ALR84" s="76"/>
+      <c r="ALS84" s="76"/>
+      <c r="ALT84" s="76"/>
+      <c r="ALU84" s="76"/>
+      <c r="ALV84" s="76"/>
+      <c r="ALW84" s="76"/>
+      <c r="ALX84" s="76"/>
+      <c r="ALY84" s="76"/>
+      <c r="ALZ84" s="76"/>
+      <c r="AMA84" s="76"/>
+      <c r="AMB84" s="76"/>
+      <c r="AMC84" s="76"/>
+      <c r="AMD84" s="76"/>
+      <c r="AME84" s="76"/>
+      <c r="AMF84" s="76"/>
+      <c r="AMG84" s="76"/>
+      <c r="AMH84" s="76"/>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="1" t="s">
@@ -20975,7 +21005,7 @@
       </c>
     </row>
     <row r="88" s="6" customFormat="1" spans="1:1022">
-      <c r="A88" s="79" t="s">
+      <c r="A88" s="78" t="s">
         <v>149</v>
       </c>
       <c r="B88" s="27" t="s">
@@ -24143,7 +24173,7 @@
       <c r="E97" s="73"/>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="80" t="s">
+      <c r="A98" s="79" t="s">
         <v>153</v>
       </c>
       <c r="B98" s="59" t="s">
@@ -24406,7 +24436,7 @@
       </c>
     </row>
     <row r="114" ht="21" spans="1:5">
-      <c r="A114" s="81" t="s">
+      <c r="A114" s="80" t="s">
         <v>175</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -24492,7 +24522,7 @@
       <c r="E119" s="73">
         <v>0.9699</v>
       </c>
-      <c r="F119" s="76" t="s">
+      <c r="F119" s="74" t="s">
         <v>181</v>
       </c>
     </row>
@@ -24672,8 +24702,25 @@
         <v>0.9697</v>
       </c>
     </row>
-    <row r="130" spans="5:5">
-      <c r="E130" s="73"/>
+    <row r="130" spans="1:6">
+      <c r="A130" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C130" s="10">
+        <v>0.9968915</v>
+      </c>
+      <c r="D130" s="10">
+        <v>0.9679763</v>
+      </c>
+      <c r="E130" s="73">
+        <v>0.9699</v>
+      </c>
+      <c r="F130" s="74" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="131" spans="5:5">
       <c r="E131" s="73"/>

</xml_diff>

<commit_message>
fix some bugs, 0.97140
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8625" tabRatio="993"/>
+    <workbookView windowWidth="20385" windowHeight="7275" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="特征选取" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224">
   <si>
     <r>
       <rPr>
@@ -1998,6 +1998,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>添加</t>
     </r>
     <r>
@@ -2011,6 +2016,7 @@
     <r>
       <rPr>
         <sz val="8"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>个</t>
@@ -2029,11 +2035,17 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
       <t>wxr_operate_4_train_order_history_features</t>
     </r>
     <r>
       <rPr>
         <sz val="8"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>，</t>
@@ -2058,6 +2070,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>融合其他</t>
     </r>
     <r>
@@ -2071,6 +2088,7 @@
     <r>
       <rPr>
         <sz val="8"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>个</t>
@@ -2087,18 +2105,53 @@
   <si>
     <t>388</t>
   </si>
+  <si>
+    <t>fix wxr comment feature bug</t>
+  </si>
+  <si>
+    <r>
+      <t>添加额外两个特征</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+browse_num_after_last_order</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t>open_num_after_last_order</t>
+    </r>
+  </si>
+  <si>
+    <t>380</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.00000_ "/>
+    <numFmt numFmtId="176" formatCode="0.0000000_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.0000000_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0.00000_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -2148,15 +2201,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2164,7 +2218,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2178,7 +2232,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2192,17 +2277,44 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2218,65 +2330,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -2285,16 +2338,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2398,31 +2451,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2434,25 +2493,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2464,7 +2511,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2482,13 +2529,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2500,7 +2607,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2512,73 +2631,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2592,26 +2645,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2640,26 +2693,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2675,17 +2708,37 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2694,137 +2747,137 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="37" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2860,16 +2913,16 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -2890,7 +2943,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2905,7 +2958,7 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2914,13 +2967,13 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2932,40 +2985,40 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -2989,10 +3042,10 @@
     <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3001,7 +3054,7 @@
     <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3010,7 +3063,7 @@
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3025,31 +3078,31 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -3062,7 +3115,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3393,8 +3446,8 @@
   <sheetPr/>
   <dimension ref="A1:AMH209"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="A146" sqref="A146"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="F147" sqref="F147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -25166,7 +25219,7 @@
       </c>
     </row>
     <row r="142" spans="1:5">
-      <c r="A142" s="77" t="s">
+      <c r="A142" s="15" t="s">
         <v>213</v>
       </c>
       <c r="B142" s="1" t="s">
@@ -25200,24 +25253,24 @@
       </c>
     </row>
     <row r="144" spans="1:5">
-      <c r="A144" s="1" t="s">
+      <c r="A144" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="B144" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="C144" s="10">
+      <c r="C144" s="28">
         <v>0.9960942</v>
       </c>
-      <c r="D144" s="10">
+      <c r="D144" s="28">
         <v>0.9686654</v>
       </c>
-      <c r="E144" s="71">
+      <c r="E144" s="39">
         <v>0.9714</v>
       </c>
     </row>
     <row r="145" spans="1:5">
-      <c r="A145" s="77" t="s">
+      <c r="A145" s="15" t="s">
         <v>219</v>
       </c>
       <c r="B145" s="1" t="s">
@@ -25233,11 +25286,42 @@
         <v>0.9703</v>
       </c>
     </row>
-    <row r="146" spans="5:5">
-      <c r="E146" s="71"/>
+    <row r="146" spans="1:5">
+      <c r="A146" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C146" s="10">
+        <v>0.9975073</v>
+      </c>
+      <c r="D146" s="10">
+        <v>0.9687168</v>
+      </c>
+      <c r="E146" s="71">
+        <v>0.97119</v>
+      </c>
     </row>
-    <row r="147" spans="5:5">
-      <c r="E147" s="71"/>
+    <row r="147" ht="31.5" spans="1:6">
+      <c r="A147" s="77" t="s">
+        <v>222</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C147" s="10">
+        <v>0.9964838</v>
+      </c>
+      <c r="D147" s="10">
+        <v>0.9685926</v>
+      </c>
+      <c r="E147" s="71">
+        <v>0.9714</v>
+      </c>
+      <c r="F147" s="11" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="148" spans="5:5">
       <c r="E148" s="71"/>

</xml_diff>

<commit_message>
back to newbaseline 0.97170
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246">
   <si>
     <r>
       <rPr>
@@ -1906,7 +1906,32 @@
     <t>337</t>
   </si>
   <si>
-    <t>多次订单 &gt;1 并且有精品的老用户multi_order_has_good_order</t>
+    <r>
+      <t>多次订单</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <charset val="134"/>
+      </rPr>
+      <t>并且有精品的老用户</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>multi_order_has_good_order</t>
+    </r>
   </si>
   <si>
     <t>卡label为0 的概率规则 trick！</t>
@@ -2288,6 +2313,9 @@
     </r>
   </si>
   <si>
+    <t>连续特征离散化测试</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="8"/>
@@ -2312,54 +2340,44 @@
     <t>391</t>
   </si>
   <si>
-    <t>连续特征离散化处理</t>
+    <t>timespanthred = 600</t>
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="DejaVu Sans Mono"/>
-        <charset val="134"/>
-      </rPr>
-      <t>eta: 0.05</t>
+      <t xml:space="preserve">one-hot </t>
     </r>
     <r>
       <rPr>
         <sz val="8"/>
-        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="DejaVu Sans Mono"/>
-        <charset val="134"/>
-      </rPr>
-      <t>num_boost_round=1000</t>
+      <t>测试</t>
     </r>
   </si>
   <si>
-    <t>1</t>
+    <t>last_time_order_year, weekofyear
+'last_time_continent, country, city' one-hot</t>
   </si>
   <si>
-    <t>browse_product_ratio</t>
+    <t>695</t>
   </si>
   <si>
-    <t>0.75</t>
+    <t>last_time_continent, country, city' one-hot</t>
   </si>
   <si>
-    <t>browse_product2_ratio</t>
+    <t>640</t>
   </si>
   <si>
-    <t>0.7</t>
+    <t>特征交叉测试</t>
   </si>
   <si>
-    <t>fillin_form5_ratio</t>
+    <t>has_good_order_x_country_rich</t>
   </si>
   <si>
-    <t>0.95</t>
+    <t>392</t>
+  </si>
+  <si>
+    <t>可能存在共线性问题</t>
   </si>
 </sst>
 </file>
@@ -2374,7 +2392,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="36">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2414,6 +2432,15 @@
       <sz val="8"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2964,142 +2991,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3331,7 +3358,19 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
@@ -3661,15 +3700,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AMH206"/>
+  <dimension ref="A1:AMH211"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="A160" sqref="A160"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="E162" sqref="E162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
   <cols>
-    <col min="1" max="1" width="39.65" style="1" customWidth="1"/>
+    <col min="1" max="1" width="42.55" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.775" style="1"/>
     <col min="3" max="3" width="10.3" style="10" customWidth="1"/>
     <col min="4" max="4" width="9.325" style="10" customWidth="1"/>
@@ -8979,7 +9018,7 @@
       <c r="AMH13" s="47"/>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:1022">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="82" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="19" t="s">
@@ -21539,7 +21578,7 @@
       </c>
     </row>
     <row r="88" s="6" customFormat="1" spans="1:1022">
-      <c r="A88" s="79" t="s">
+      <c r="A88" s="83" t="s">
         <v>149</v>
       </c>
       <c r="B88" s="27" t="s">
@@ -24707,7 +24746,7 @@
       <c r="E97" s="71"/>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="80" t="s">
+      <c r="A98" s="84" t="s">
         <v>153</v>
       </c>
       <c r="B98" s="59" t="s">
@@ -24970,7 +25009,7 @@
       </c>
     </row>
     <row r="114" ht="21" spans="1:5">
-      <c r="A114" s="81" t="s">
+      <c r="A114" s="85" t="s">
         <v>175</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -25274,7 +25313,7 @@
       </c>
     </row>
     <row r="132" spans="1:6">
-      <c r="A132" s="31" t="s">
+      <c r="A132" s="77" t="s">
         <v>198</v>
       </c>
       <c r="B132" s="19" t="s">
@@ -25575,7 +25614,7 @@
       </c>
     </row>
     <row r="150" spans="1:5">
-      <c r="A150" s="77"/>
+      <c r="A150" s="78"/>
       <c r="E150" s="71"/>
     </row>
     <row r="151" spans="1:5">
@@ -25644,12 +25683,15 @@
     <row r="156" spans="5:5">
       <c r="E156" s="71"/>
     </row>
-    <row r="157" spans="5:5">
+    <row r="157" spans="1:5">
+      <c r="A157" s="79" t="s">
+        <v>232</v>
+      </c>
       <c r="E157" s="71"/>
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="27" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B158" s="27" t="s">
         <v>223</v>
@@ -25664,117 +25706,125 @@
         <v>0.97159</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
-      <c r="A159" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B159" s="1" t="s">
+    <row r="159" spans="1:6">
+      <c r="A159" s="27" t="s">
         <v>234</v>
       </c>
-      <c r="C159" s="10">
+      <c r="B159" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="C159" s="28">
         <v>0.9970582</v>
       </c>
-      <c r="D159" s="10">
+      <c r="D159" s="28">
         <v>0.969019</v>
       </c>
-      <c r="E159" s="71">
+      <c r="E159" s="39">
         <v>0.9717</v>
       </c>
+      <c r="F159" s="20" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="160" spans="5:5">
-      <c r="E160" s="71"/>
+    <row r="160" spans="1:6">
+      <c r="A160" s="56" t="s">
+        <v>236</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C160" s="10">
+        <v>0.997552</v>
+      </c>
+      <c r="D160" s="10">
+        <v>0.9690566</v>
+      </c>
+      <c r="E160" s="68">
+        <v>0.9716</v>
+      </c>
+      <c r="F160" s="80"/>
     </row>
     <row r="161" spans="5:5">
       <c r="E161" s="71"/>
     </row>
-    <row r="162" spans="5:5">
+    <row r="162" spans="1:5">
+      <c r="A162" s="24" t="s">
+        <v>237</v>
+      </c>
       <c r="E162" s="71"/>
     </row>
-    <row r="163" spans="5:5">
+    <row r="163" ht="21" spans="1:5">
+      <c r="A163" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>239</v>
+      </c>
       <c r="E163" s="71"/>
     </row>
-    <row r="164" spans="5:5">
-      <c r="E164" s="71"/>
+    <row r="164" spans="1:5">
+      <c r="A164" s="83" t="s">
+        <v>240</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C164" s="10">
+        <v>0.9968468</v>
+      </c>
+      <c r="D164" s="10">
+        <v>0.9690211</v>
+      </c>
+      <c r="E164" s="71">
+        <v>0.9717</v>
+      </c>
     </row>
     <row r="165" spans="5:5">
       <c r="E165" s="71"/>
     </row>
-    <row r="166" spans="5:5">
+    <row r="166" spans="1:5">
+      <c r="A166" s="79" t="s">
+        <v>242</v>
+      </c>
       <c r="E166" s="71"/>
     </row>
-    <row r="167" spans="1:5">
-      <c r="A167" s="15" t="s">
-        <v>235</v>
+    <row r="167" spans="1:6">
+      <c r="A167" s="56" t="s">
+        <v>243</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C167" s="1"/>
-      <c r="D167" s="1"/>
-      <c r="E167" s="1"/>
+        <v>244</v>
+      </c>
+      <c r="C167" s="10">
+        <v>0.9969679</v>
+      </c>
+      <c r="D167" s="10">
+        <v>0.9690449</v>
+      </c>
+      <c r="E167" s="71">
+        <v>0.9716</v>
+      </c>
+      <c r="F167" s="81" t="s">
+        <v>245</v>
+      </c>
     </row>
-    <row r="168" spans="1:5">
-      <c r="A168" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C168" s="10">
-        <v>0.9965687</v>
-      </c>
-      <c r="D168" s="10">
-        <v>0.9678254</v>
-      </c>
+    <row r="168" spans="5:5">
       <c r="E168" s="71"/>
     </row>
-    <row r="169" spans="1:5">
-      <c r="A169" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C169" s="10">
-        <v>0.9980355</v>
-      </c>
-      <c r="D169" s="10">
-        <v>0.9681056</v>
-      </c>
+    <row r="169" spans="5:5">
       <c r="E169" s="71"/>
     </row>
-    <row r="170" spans="1:5">
-      <c r="A170" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C170" s="10">
-        <v>0.9966559</v>
-      </c>
-      <c r="D170" s="10">
-        <v>0.9681643</v>
-      </c>
+    <row r="170" spans="5:5">
       <c r="E170" s="71"/>
     </row>
-    <row r="171" spans="1:5">
-      <c r="A171" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C171" s="10">
-        <v>0.997926</v>
-      </c>
-      <c r="D171" s="10">
-        <v>0.9681989</v>
-      </c>
+    <row r="171" spans="5:5">
       <c r="E171" s="71"/>
     </row>
-    <row r="172" spans="5:5">
-      <c r="E172" s="71"/>
+    <row r="172" spans="1:5">
+      <c r="A172" s="15"/>
+      <c r="C172" s="1"/>
+      <c r="D172" s="1"/>
+      <c r="E172" s="1"/>
     </row>
     <row r="173" spans="5:5">
       <c r="E173" s="71"/>
@@ -25878,10 +25928,25 @@
     <row r="206" spans="5:5">
       <c r="E206" s="71"/>
     </row>
+    <row r="207" spans="5:5">
+      <c r="E207" s="71"/>
+    </row>
+    <row r="208" spans="5:5">
+      <c r="E208" s="71"/>
+    </row>
+    <row r="209" spans="5:5">
+      <c r="E209" s="71"/>
+    </row>
+    <row r="210" spans="5:5">
+      <c r="E210" s="71"/>
+    </row>
+    <row r="211" spans="5:5">
+      <c r="E211" s="71"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A32:G32"/>
-    <mergeCell ref="B167:E167"/>
+    <mergeCell ref="B172:E172"/>
   </mergeCells>
   <pageMargins left="0.697916666666667" right="0.697916666666667" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
back to new baseline, 0.97210
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8625" tabRatio="993"/>
+    <workbookView windowWidth="28695" windowHeight="13305" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="特征选取" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271">
   <si>
     <r>
       <rPr>
@@ -2655,11 +2655,17 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
       <t>last_order_time_minus_action1</t>
     </r>
     <r>
       <rPr>
         <sz val="8"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>，</t>
@@ -2675,6 +2681,7 @@
     <r>
       <rPr>
         <sz val="8"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>，</t>
@@ -2688,6 +2695,114 @@
       <t>6_delta</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>添加国哥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> stage one </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的特征</t>
+    </r>
+  </si>
+  <si>
+    <t>464</t>
+  </si>
+  <si>
+    <r>
+      <t>添加国哥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> stage one </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的特征，筛选一些特征</t>
+    </r>
+  </si>
+  <si>
+    <t>428</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">添加 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t>actiontype_statistic</t>
+    </r>
+  </si>
+  <si>
+    <t>415</t>
+  </si>
+  <si>
+    <t>actiontype_timedelta_statistic2</t>
+  </si>
+  <si>
+    <r>
+      <t>添加</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> actiontypedelta_statistic</t>
+    </r>
+  </si>
+  <si>
+    <t>427</t>
+  </si>
+  <si>
+    <r>
+      <t>previous_latest_action_statistic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <charset val="134"/>
+      </rPr>
+      <t>个</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -2695,11 +2810,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="0.00000_ "/>
+    <numFmt numFmtId="177" formatCode="0.0000000_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.0000000_ "/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -2744,9 +2859,21 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="8"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2769,14 +2896,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2790,11 +2910,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2805,16 +2924,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2822,9 +2934,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2842,9 +2954,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2858,6 +2977,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -2865,30 +3007,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2937,12 +3056,8 @@
       <name val="DejaVu Sans Mono"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="42">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2999,13 +3114,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3017,67 +3192,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3095,7 +3240,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3107,67 +3282,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3179,13 +3294,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3214,11 +3323,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3227,7 +3342,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3262,21 +3377,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -3284,6 +3384,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3301,137 +3410,137 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3671,10 +3780,10 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
@@ -4006,8 +4115,8 @@
   <sheetPr/>
   <dimension ref="A1:AMH207"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="B179" sqref="B179"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="F177" sqref="F177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -26046,7 +26155,7 @@
       <c r="E160" s="68">
         <v>0.9716</v>
       </c>
-      <c r="F160" s="78"/>
+      <c r="F160" s="79"/>
     </row>
     <row r="161" spans="5:5">
       <c r="E161" s="71"/>
@@ -26217,7 +26326,7 @@
     <row r="175" spans="5:5">
       <c r="E175" s="71"/>
     </row>
-    <row r="176" ht="21" spans="1:5">
+    <row r="176" ht="21" spans="1:6">
       <c r="A176" s="22" t="s">
         <v>256</v>
       </c>
@@ -26232,6 +26341,9 @@
       </c>
       <c r="E176" s="39">
         <v>0.9721</v>
+      </c>
+      <c r="F176" s="11" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="177" ht="31.5" spans="1:5">
@@ -26264,27 +26376,111 @@
       <c r="D178" s="28">
         <v>0.9691257</v>
       </c>
-      <c r="E178" s="79">
+      <c r="E178" s="67">
         <v>0.9715</v>
       </c>
     </row>
-    <row r="179" spans="5:5">
-      <c r="E179" s="71"/>
+    <row r="179" spans="1:5">
+      <c r="A179" s="78" t="s">
+        <v>261</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C179" s="10">
+        <v>0.9977735</v>
+      </c>
+      <c r="D179" s="10">
+        <v>0.9689449</v>
+      </c>
+      <c r="E179" s="71">
+        <v>0.972</v>
+      </c>
     </row>
-    <row r="180" spans="5:5">
-      <c r="E180" s="71"/>
+    <row r="180" spans="1:5">
+      <c r="A180" s="78" t="s">
+        <v>263</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C180" s="10">
+        <v>0.9973033</v>
+      </c>
+      <c r="D180" s="10">
+        <v>0.9690565</v>
+      </c>
+      <c r="E180" s="67">
+        <v>0.9718</v>
+      </c>
     </row>
-    <row r="181" spans="5:5">
-      <c r="E181" s="71"/>
+    <row r="181" spans="1:5">
+      <c r="A181" s="78" t="s">
+        <v>265</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C181" s="10">
+        <v>0.9972382</v>
+      </c>
+      <c r="D181" s="28">
+        <v>0.969112</v>
+      </c>
+      <c r="E181" s="67">
+        <v>0.9714</v>
+      </c>
     </row>
-    <row r="182" spans="5:5">
-      <c r="E182" s="71"/>
+    <row r="182" spans="1:5">
+      <c r="A182" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C182" s="10">
+        <v>0.9975042</v>
+      </c>
+      <c r="D182" s="28">
+        <v>0.9691493</v>
+      </c>
+      <c r="E182" s="68">
+        <v>0.9717</v>
+      </c>
     </row>
-    <row r="183" spans="5:5">
-      <c r="E183" s="71"/>
+    <row r="183" spans="1:5">
+      <c r="A183" s="78" t="s">
+        <v>268</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C183" s="10">
+        <v>0.9973661</v>
+      </c>
+      <c r="D183" s="28">
+        <v>0.96912</v>
+      </c>
+      <c r="E183" s="68">
+        <v>0.972</v>
+      </c>
     </row>
-    <row r="184" spans="5:5">
-      <c r="E184" s="71"/>
+    <row r="184" spans="1:5">
+      <c r="A184" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C184" s="10">
+        <v>0.9970481</v>
+      </c>
+      <c r="D184" s="10">
+        <v>0.9690309</v>
+      </c>
+      <c r="E184" s="71">
+        <v>0.9717</v>
+      </c>
     </row>
     <row r="185" spans="5:5">
       <c r="E185" s="71"/>

</xml_diff>

<commit_message>
back to baseline, add some code
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277">
   <si>
     <r>
       <rPr>
@@ -1626,13 +1626,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="9" tint="-0.25"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
       <t>设置</t>
     </r>
     <r>
@@ -2833,15 +2826,23 @@
     </r>
   </si>
   <si>
+    <t>last_action_timestamp， 9个</t>
+  </si>
+  <si>
+    <t>422</t>
+  </si>
+  <si>
+    <t>last_actiontype_is_6|7, 2个</t>
+  </si>
+  <si>
+    <t>571 all features</t>
+  </si>
+  <si>
+    <t>571</t>
+  </si>
+  <si>
     <r>
-      <t>last_action_timestamp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <charset val="134"/>
-      </rPr>
-      <t>，</t>
+      <t>贪心算法</t>
     </r>
     <r>
       <rPr>
@@ -2849,29 +2850,14 @@
         <rFont val="DejaVu Sans Mono"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve"> 9</t>
+      <t xml:space="preserve"> remove </t>
     </r>
     <r>
       <rPr>
         <sz val="8"/>
         <charset val="134"/>
       </rPr>
-      <t>个</t>
-    </r>
-  </si>
-  <si>
-    <t>422</t>
-  </si>
-  <si>
-    <r>
-      <t>last_actiontype_is_6|7, 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <charset val="134"/>
-      </rPr>
-      <t>个</t>
+      <t>不重要的特征，remove_ratio = 0.3</t>
     </r>
   </si>
 </sst>
@@ -2880,11 +2866,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.0000000_ "/>
+    <numFmt numFmtId="176" formatCode="0.00000_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0.0000000_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.00000_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="35">
@@ -2919,7 +2905,6 @@
       <b/>
       <sz val="8"/>
       <color theme="9" tint="-0.25"/>
-      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2930,9 +2915,21 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="8"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2942,6 +2939,21 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2960,8 +2972,15 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2970,13 +2989,37 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2990,30 +3033,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3027,8 +3047,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3041,41 +3062,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3121,10 +3110,6 @@
       <sz val="8"/>
       <color rgb="FFFF0000"/>
       <name val="DejaVu Sans Mono"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -3185,7 +3170,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3203,24 +3194,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -3233,7 +3206,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3245,61 +3320,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3311,61 +3344,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3376,6 +3361,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -3395,40 +3419,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3461,162 +3461,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3647,16 +3632,16 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -3677,7 +3662,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3692,7 +3677,7 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3701,13 +3686,13 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3719,40 +3704,40 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -3776,10 +3761,10 @@
     <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3788,7 +3773,7 @@
     <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3797,7 +3782,7 @@
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3812,31 +3797,31 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -3851,7 +3836,19 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
@@ -4183,8 +4180,8 @@
   <sheetPr/>
   <dimension ref="A1:AMH207"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="D188" sqref="D188"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="A194" sqref="A194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -9499,7 +9496,7 @@
       <c r="AMH13" s="47"/>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:1022">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="83" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="19" t="s">
@@ -22059,7 +22056,7 @@
       </c>
     </row>
     <row r="88" s="6" customFormat="1" spans="1:1022">
-      <c r="A88" s="80" t="s">
+      <c r="A88" s="84" t="s">
         <v>149</v>
       </c>
       <c r="B88" s="27" t="s">
@@ -25227,7 +25224,7 @@
       <c r="E97" s="71"/>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="81" t="s">
+      <c r="A98" s="85" t="s">
         <v>153</v>
       </c>
       <c r="B98" s="59" t="s">
@@ -25490,7 +25487,7 @@
       </c>
     </row>
     <row r="114" ht="21" spans="1:5">
-      <c r="A114" s="82" t="s">
+      <c r="A114" s="86" t="s">
         <v>175</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -26223,7 +26220,7 @@
       <c r="E160" s="68">
         <v>0.9716</v>
       </c>
-      <c r="F160" s="78"/>
+      <c r="F160" s="80"/>
     </row>
     <row r="161" spans="5:5">
       <c r="E161" s="71"/>
@@ -26244,7 +26241,7 @@
       <c r="E163" s="71"/>
     </row>
     <row r="164" spans="1:5">
-      <c r="A164" s="80" t="s">
+      <c r="A164" s="84" t="s">
         <v>240</v>
       </c>
       <c r="B164" s="1" t="s">
@@ -26590,19 +26587,47 @@
     <row r="188" spans="5:5">
       <c r="E188" s="71"/>
     </row>
-    <row r="189" spans="5:5">
-      <c r="E189" s="71"/>
+    <row r="189" spans="1:5">
+      <c r="A189" s="78" t="s">
+        <v>274</v>
+      </c>
+      <c r="B189" s="78" t="s">
+        <v>275</v>
+      </c>
+      <c r="C189" s="79">
+        <v>0.9972154</v>
+      </c>
+      <c r="D189" s="79">
+        <v>0.9689785</v>
+      </c>
+      <c r="E189" s="81">
+        <v>0.9707</v>
+      </c>
     </row>
     <row r="190" spans="5:5">
       <c r="E190" s="71"/>
     </row>
-    <row r="191" spans="5:5">
-      <c r="E191" s="71"/>
+    <row r="192" spans="1:5">
+      <c r="A192" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="B192" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="C192" s="28">
+        <v>0.9974912</v>
+      </c>
+      <c r="D192" s="28">
+        <v>0.9690679</v>
+      </c>
+      <c r="E192" s="39">
+        <v>0.9721</v>
+      </c>
     </row>
-    <row r="192" spans="5:5">
-      <c r="E192" s="71"/>
-    </row>
-    <row r="193" spans="5:5">
+    <row r="193" spans="1:5">
+      <c r="A193" s="82" t="s">
+        <v>276</v>
+      </c>
       <c r="E193" s="71"/>
     </row>
     <row r="194" spans="5:5">

</xml_diff>

<commit_message>
back to baseline, 0.97210, add set 1 trick, 0.97210
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -2572,11 +2572,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="DejaVu Sans Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">last_openapp_browse_count
 </t>
     </r>
@@ -2648,11 +2643,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="DejaVu Sans Mono"/>
-        <charset val="134"/>
-      </rPr>
       <t>last_order_time_minus_action1</t>
     </r>
     <r>
@@ -2841,24 +2831,7 @@
     <t>571</t>
   </si>
   <si>
-    <r>
-      <t>贪心算法</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="DejaVu Sans Mono"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> remove </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <charset val="134"/>
-      </rPr>
-      <t>不重要的特征，remove_ratio = 0.3</t>
-    </r>
+    <t>new baseline，fuck！</t>
   </si>
 </sst>
 </file>
@@ -4180,8 +4153,8 @@
   <sheetPr/>
   <dimension ref="A1:AMH207"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="A194" sqref="A194"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="E194" sqref="E194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -26628,7 +26601,18 @@
       <c r="A193" s="82" t="s">
         <v>276</v>
       </c>
-      <c r="E193" s="71"/>
+      <c r="B193" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C193" s="10">
+        <v>0.9965768</v>
+      </c>
+      <c r="D193" s="10">
+        <v>0.9688926</v>
+      </c>
+      <c r="E193" s="71">
+        <v>0.9712</v>
+      </c>
     </row>
     <row r="194" spans="5:5">
       <c r="E194" s="71"/>

</xml_diff>

<commit_message>
back to baseline, 0.97210
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280">
   <si>
     <r>
       <rPr>
@@ -1626,6 +1626,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="9" tint="-0.25"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>设置</t>
     </r>
     <r>
@@ -2572,6 +2579,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">last_openapp_browse_count
 </t>
     </r>
@@ -2643,6 +2655,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
       <t>last_order_time_minus_action1</t>
     </r>
     <r>
@@ -2830,18 +2847,52 @@
   <si>
     <t>571</t>
   </si>
+  <si>
+    <r>
+      <t>去掉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> '6_7_diff_time', '7_8_diff_time', '8_9_diff_time',
+ 'last_openapp_browse_count', 'user_rating_std'</t>
+    </r>
+  </si>
+  <si>
+    <t>408</t>
+  </si>
+  <si>
+    <r>
+      <t>再去掉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> '2016_2017_first_last_ordertype',
+ 'total_good_order_ratio', '2017_good_order_ratio'</t>
+    </r>
+  </si>
+  <si>
+    <t>405</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.00000_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.0000000_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.0000000_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0.00000_ "/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -2875,6 +2926,7 @@
       <b/>
       <sz val="8"/>
       <color theme="9" tint="-0.25"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2889,17 +2941,70 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2915,73 +3020,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2995,8 +3039,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3011,15 +3056,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3032,11 +3076,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3146,19 +3198,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3176,7 +3240,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3188,43 +3300,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3236,73 +3348,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3314,13 +3372,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3334,11 +3386,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3373,6 +3431,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3388,28 +3457,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3426,8 +3478,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3436,137 +3488,137 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3602,16 +3654,16 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -3632,7 +3684,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3647,7 +3699,7 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3656,13 +3708,13 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3674,40 +3726,40 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -3731,10 +3783,10 @@
     <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3743,7 +3795,7 @@
     <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3752,7 +3804,7 @@
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3767,31 +3819,31 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -3809,17 +3861,17 @@
     <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4151,7 +4203,7 @@
   <dimension ref="A1:AMH207"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="A193" sqref="A193:E193"/>
+      <selection activeCell="A197" sqref="A195:A197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -26594,15 +26646,39 @@
         <v>0.9721</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
-      <c r="A193" s="82"/>
-      <c r="B193" s="1"/>
-      <c r="C193" s="10"/>
-      <c r="D193" s="10"/>
-      <c r="E193" s="71"/>
+    <row r="193" ht="21" spans="1:5">
+      <c r="A193" s="82" t="s">
+        <v>276</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C193" s="10">
+        <v>0.9973749</v>
+      </c>
+      <c r="D193" s="10">
+        <v>0.9690738</v>
+      </c>
+      <c r="E193" s="71">
+        <v>0.9716</v>
+      </c>
     </row>
-    <row r="194" spans="5:5">
-      <c r="E194" s="71"/>
+    <row r="194" ht="31.5" spans="1:5">
+      <c r="A194" s="82" t="s">
+        <v>278</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C194" s="10">
+        <v>0.9975622</v>
+      </c>
+      <c r="D194" s="10">
+        <v>0.9691027</v>
+      </c>
+      <c r="E194" s="71">
+        <v>0.9715</v>
+      </c>
     </row>
     <row r="195" spans="5:5">
       <c r="E195" s="71"/>

</xml_diff>

<commit_message>
xgboost check removed features
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13305" tabRatio="993"/>
+    <workbookView windowWidth="20385" windowHeight="8625" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="特征选取" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328">
   <si>
     <r>
       <rPr>
@@ -3465,11 +3465,17 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">B </t>
     </r>
     <r>
       <rPr>
         <sz val="8"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>榜</t>
@@ -3484,6 +3490,43 @@
   </si>
   <si>
     <t>537</t>
+  </si>
+  <si>
+    <t>current baseline</t>
+  </si>
+  <si>
+    <t>diff_action_type_time_delta 68</t>
+  </si>
+  <si>
+    <t>559</t>
+  </si>
+  <si>
+    <t>diff_action_type_time_delta 27</t>
+  </si>
+  <si>
+    <t>diff_action_type_time_delta 36</t>
+  </si>
+  <si>
+    <t>diff_action_type_time_delta 26</t>
+  </si>
+  <si>
+    <t>diff_action_type_time_delta 15</t>
+  </si>
+  <si>
+    <t>diff_action_type_time_delta 14</t>
+  </si>
+  <si>
+    <t>diff_action_type_time_delta 13</t>
+  </si>
+  <si>
+    <t>diff_action_type_time_delta 68,27,36,26,15,14,13</t>
+  </si>
+  <si>
+    <t>576</t>
+  </si>
+  <si>
+    <t>0.97299 + diff_action_type_time_delta 
+68,27,36,26,15,14,13</t>
   </si>
 </sst>
 </file>
@@ -3491,14 +3534,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.0000000_ "/>
+    <numFmt numFmtId="176" formatCode="0.00000_ "/>
+    <numFmt numFmtId="177" formatCode="0.0000000_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.00000_ "/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="35">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3547,16 +3590,92 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3586,31 +3705,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3618,29 +3713,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3653,48 +3733,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3738,10 +3781,6 @@
       <sz val="8"/>
       <color rgb="FFFF0000"/>
       <name val="DejaVu Sans Mono"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -3808,31 +3847,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3844,19 +3859,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3868,19 +3871,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3892,61 +3895,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3964,13 +3913,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3982,7 +3967,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3993,6 +4032,80 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -4014,82 +4127,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4098,137 +4137,137 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4264,19 +4303,19 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -4297,7 +4336,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4312,7 +4351,7 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4321,13 +4360,13 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4339,40 +4378,40 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -4396,10 +4435,10 @@
     <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4408,7 +4447,7 @@
     <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4417,7 +4456,7 @@
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4432,28 +4471,28 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -4471,22 +4510,22 @@
     <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
@@ -4816,10 +4855,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AMH216"/>
+  <dimension ref="A1:AMH228"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="A207" workbookViewId="0">
-      <selection activeCell="E218" sqref="E218"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="C228" sqref="C228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -27585,6 +27624,125 @@
         <v>0.9735</v>
       </c>
     </row>
+    <row r="218" spans="1:4">
+      <c r="A218" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C218" s="10">
+        <v>0.9984021</v>
+      </c>
+      <c r="D218" s="10">
+        <v>0.9608295</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
+      <c r="A219" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C219" s="10">
+        <v>0.997123</v>
+      </c>
+      <c r="D219" s="10">
+        <v>0.9609962</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4">
+      <c r="A220" s="28" t="s">
+        <v>319</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C220" s="10">
+        <v>0.997867</v>
+      </c>
+      <c r="D220" s="10">
+        <v>0.9611265</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4">
+      <c r="A221" s="28" t="s">
+        <v>320</v>
+      </c>
+      <c r="C221" s="10">
+        <v>0.9976841</v>
+      </c>
+      <c r="D221" s="10">
+        <v>0.9612175</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4">
+      <c r="A222" s="28" t="s">
+        <v>321</v>
+      </c>
+      <c r="C222" s="10">
+        <v>0.9976798</v>
+      </c>
+      <c r="D222" s="10">
+        <v>0.9612306</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4">
+      <c r="A223" s="28" t="s">
+        <v>322</v>
+      </c>
+      <c r="C223" s="10">
+        <v>0.9975381</v>
+      </c>
+      <c r="D223" s="10">
+        <v>0.960906</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4">
+      <c r="A224" s="28" t="s">
+        <v>323</v>
+      </c>
+      <c r="C224" s="10">
+        <v>0.9989328</v>
+      </c>
+      <c r="D224" s="10">
+        <v>0.9611494</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4">
+      <c r="A225" s="28" t="s">
+        <v>324</v>
+      </c>
+      <c r="C225" s="10">
+        <v>0.9986115</v>
+      </c>
+      <c r="D225" s="10">
+        <v>0.9610515</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4">
+      <c r="A226" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C226" s="10">
+        <v>0.9985246</v>
+      </c>
+      <c r="D226" s="10">
+        <v>0.9697816</v>
+      </c>
+    </row>
+    <row r="228" ht="21" spans="1:2">
+      <c r="A228" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A32:G32"/>

</xml_diff>

<commit_message>
add some model roof
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345">
   <si>
     <r>
       <rPr>
@@ -3648,6 +3648,42 @@
         <charset val="134"/>
       </rPr>
       <t>的特征</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>黄麟的数据</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <charset val="134"/>
+      </rPr>
+      <t>调优参数</t>
+    </r>
+  </si>
+  <si>
+    <t>368</t>
+  </si>
+  <si>
+    <r>
+      <t>黄麟的数据</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> xgboost  xgboost_huang_lin.csv</t>
     </r>
   </si>
 </sst>
@@ -4410,7 +4446,7 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4667,6 +4703,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -5008,10 +5047,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AMH238"/>
+  <dimension ref="A1:AMH241"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="E238" sqref="E238"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="A244" sqref="A244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -10326,7 +10365,7 @@
       <c r="AMH13" s="48"/>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:1022">
-      <c r="A14" s="90" t="s">
+      <c r="A14" s="91" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="20" t="s">
@@ -22885,7 +22924,7 @@
       </c>
     </row>
     <row r="88" s="6" customFormat="1" spans="1:1022">
-      <c r="A88" s="91" t="s">
+      <c r="A88" s="92" t="s">
         <v>149</v>
       </c>
       <c r="B88" s="28" t="s">
@@ -26050,7 +26089,7 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="92" t="s">
+      <c r="A98" s="93" t="s">
         <v>153</v>
       </c>
       <c r="B98" s="60" t="s">
@@ -26308,7 +26347,7 @@
       </c>
     </row>
     <row r="114" ht="21" spans="1:5">
-      <c r="A114" s="93" t="s">
+      <c r="A114" s="94" t="s">
         <v>175</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -27044,7 +27083,7 @@
       </c>
     </row>
     <row r="164" spans="1:5">
-      <c r="A164" s="91" t="s">
+      <c r="A164" s="92" t="s">
         <v>240</v>
       </c>
       <c r="B164" s="1" t="s">
@@ -27492,7 +27531,7 @@
       <c r="B200" s="82"/>
       <c r="C200" s="82"/>
       <c r="D200" s="82"/>
-      <c r="E200" s="86"/>
+      <c r="E200" s="87"/>
     </row>
     <row r="201" ht="12" spans="1:6">
       <c r="A201" s="16" t="s">
@@ -27618,7 +27657,7 @@
       <c r="D207" s="10">
         <v>0.9696725</v>
       </c>
-      <c r="E207" s="87"/>
+      <c r="E207" s="88"/>
     </row>
     <row r="208" spans="1:5">
       <c r="A208" s="23" t="s">
@@ -27935,7 +27974,7 @@
       <c r="D231" s="84">
         <v>0.9710983</v>
       </c>
-      <c r="E231" s="88">
+      <c r="E231" s="89">
         <v>0.97329</v>
       </c>
       <c r="F231" s="12">
@@ -27972,7 +28011,7 @@
       <c r="D233" s="10">
         <v>0.9712821</v>
       </c>
-      <c r="E233" s="89">
+      <c r="E233" s="90">
         <v>0.97239</v>
       </c>
       <c r="F233" s="12">
@@ -28042,6 +28081,38 @@
       </c>
       <c r="D238" s="10">
         <v>0.9707639</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6">
+      <c r="A240" s="86" t="s">
+        <v>342</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D240" s="10">
+        <v>0.971064</v>
+      </c>
+      <c r="E240" s="67"/>
+      <c r="F240" s="12">
+        <v>0.161003</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6">
+      <c r="A241" s="85" t="s">
+        <v>344</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C241" s="10">
+        <v>0.9978451</v>
+      </c>
+      <c r="D241" s="10">
+        <v>0.9719596</v>
+      </c>
+      <c r="F241" s="12">
+        <v>0.158632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add qian-guo model roof
</commit_message>
<xml_diff>
--- a/Feature Engineering.xlsx
+++ b/Feature Engineering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347">
   <si>
     <r>
       <rPr>
@@ -3557,11 +3557,17 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
       <t>lgbm</t>
     </r>
     <r>
       <rPr>
         <sz val="8"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>调参</t>
@@ -3572,6 +3578,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>根据</t>
     </r>
     <r>
@@ -3585,6 +3596,7 @@
     <r>
       <rPr>
         <sz val="8"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>取出为</t>
@@ -3600,6 +3612,7 @@
     <r>
       <rPr>
         <sz val="8"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>的特征</t>
@@ -3610,11 +3623,17 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
       <t>lgbm</t>
     </r>
     <r>
       <rPr>
         <sz val="8"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>调参</t>
@@ -3630,6 +3649,7 @@
     <r>
       <rPr>
         <sz val="8"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>去除</t>
@@ -3645,6 +3665,7 @@
     <r>
       <rPr>
         <sz val="8"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>的特征</t>
@@ -3652,6 +3673,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>黄麟的数据</t>
     </r>
     <r>
@@ -3665,6 +3691,7 @@
     <r>
       <rPr>
         <sz val="8"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>调优参数</t>
@@ -3675,6 +3702,11 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>黄麟的数据</t>
     </r>
     <r>
@@ -3685,6 +3717,55 @@
       </rPr>
       <t xml:space="preserve"> xgboost  xgboost_huang_lin.csv</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>max_depth': 10
+'scale_pos_weight': 0.8
+120</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <charset val="134"/>
+      </rPr>
+      <t>模型</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t>+46</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <charset val="134"/>
+      </rPr>
+      <t>重要的特征</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">+ xgb </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <charset val="134"/>
+      </rPr>
+      <t>stacking</t>
+    </r>
+  </si>
+  <si>
+    <t>166</t>
   </si>
 </sst>
 </file>
@@ -3692,12 +3773,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.0000000_ "/>
+    <numFmt numFmtId="176" formatCode="0.00000_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0.0000000_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.00000_ "/>
   </numFmts>
   <fonts count="36">
     <font>
@@ -3748,8 +3829,20 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="8"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3773,11 +3866,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3785,22 +3885,6 @@
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3819,15 +3903,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3842,15 +3936,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -3858,22 +3944,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3887,19 +3965,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3945,8 +4022,12 @@
       <name val="DejaVu Sans Mono"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="43">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4015,12 +4096,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -4033,7 +4108,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4045,7 +4234,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4057,145 +4270,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4206,6 +4281,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -4220,6 +4304,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4268,26 +4361,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4311,142 +4386,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="39" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4477,19 +4552,19 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -4510,7 +4585,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4525,7 +4600,7 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4534,13 +4609,13 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4552,40 +4627,40 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -4609,10 +4684,10 @@
     <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4621,7 +4696,7 @@
     <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4630,7 +4705,7 @@
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4645,28 +4720,28 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="177" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -4684,40 +4759,28 @@
     <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
@@ -4730,6 +4793,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5047,10 +5113,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AMH241"/>
+  <dimension ref="A1:AMH244"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="E242" sqref="E242"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A239" workbookViewId="0">
+      <selection activeCell="E247" sqref="E247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -10365,7 +10431,7 @@
       <c r="AMH13" s="48"/>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:1022">
-      <c r="A14" s="91" t="s">
+      <c r="A14" s="87" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="20" t="s">
@@ -22924,7 +22990,7 @@
       </c>
     </row>
     <row r="88" s="6" customFormat="1" spans="1:1022">
-      <c r="A88" s="92" t="s">
+      <c r="A88" s="88" t="s">
         <v>149</v>
       </c>
       <c r="B88" s="28" t="s">
@@ -26089,7 +26155,7 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="93" t="s">
+      <c r="A98" s="89" t="s">
         <v>153</v>
       </c>
       <c r="B98" s="60" t="s">
@@ -26347,7 +26413,7 @@
       </c>
     </row>
     <row r="114" ht="21" spans="1:5">
-      <c r="A114" s="94" t="s">
+      <c r="A114" s="90" t="s">
         <v>175</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -27083,7 +27149,7 @@
       </c>
     </row>
     <row r="164" spans="1:5">
-      <c r="A164" s="92" t="s">
+      <c r="A164" s="88" t="s">
         <v>240</v>
       </c>
       <c r="B164" s="1" t="s">
@@ -27531,7 +27597,7 @@
       <c r="B200" s="82"/>
       <c r="C200" s="82"/>
       <c r="D200" s="82"/>
-      <c r="E200" s="87"/>
+      <c r="E200" s="84"/>
     </row>
     <row r="201" ht="12" spans="1:6">
       <c r="A201" s="16" t="s">
@@ -27657,7 +27723,7 @@
       <c r="D207" s="10">
         <v>0.9696725</v>
       </c>
-      <c r="E207" s="88"/>
+      <c r="E207" s="85"/>
     </row>
     <row r="208" spans="1:5">
       <c r="A208" s="23" t="s">
@@ -27968,13 +28034,13 @@
       <c r="B231" s="20" t="s">
         <v>330</v>
       </c>
-      <c r="C231" s="84">
+      <c r="C231" s="21">
         <v>0.997871</v>
       </c>
-      <c r="D231" s="84">
+      <c r="D231" s="21">
         <v>0.9710983</v>
       </c>
-      <c r="E231" s="89">
+      <c r="E231" s="36">
         <v>0.97329</v>
       </c>
       <c r="F231" s="12">
@@ -28011,7 +28077,7 @@
       <c r="D233" s="10">
         <v>0.9712821</v>
       </c>
-      <c r="E233" s="90">
+      <c r="E233" s="86">
         <v>0.97239</v>
       </c>
       <c r="F233" s="12">
@@ -28053,7 +28119,7 @@
       </c>
     </row>
     <row r="237" spans="1:6">
-      <c r="A237" s="85" t="s">
+      <c r="A237" s="16" t="s">
         <v>339</v>
       </c>
       <c r="B237" s="1" t="s">
@@ -28084,7 +28150,7 @@
       </c>
     </row>
     <row r="240" spans="1:6">
-      <c r="A240" s="86" t="s">
+      <c r="A240" s="75" t="s">
         <v>342</v>
       </c>
       <c r="B240" s="1" t="s">
@@ -28099,7 +28165,7 @@
       </c>
     </row>
     <row r="241" spans="1:6">
-      <c r="A241" s="85" t="s">
+      <c r="A241" s="16" t="s">
         <v>344</v>
       </c>
       <c r="B241" s="1" t="s">
@@ -28116,6 +28182,26 @@
       </c>
       <c r="F241" s="12">
         <v>0.158632</v>
+      </c>
+    </row>
+    <row r="244" ht="31.5" spans="1:6">
+      <c r="A244" s="91" t="s">
+        <v>345</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C244" s="10">
+        <v>0.9889657</v>
+      </c>
+      <c r="D244" s="10">
+        <v>0.9736491</v>
+      </c>
+      <c r="E244" s="40">
+        <v>0.97339</v>
+      </c>
+      <c r="F244" s="12">
+        <v>0.158151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>